<commit_message>
add content to index, javascript
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="467">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -2347,6 +2347,23 @@
     <t>Web Framework Category:
 [Action-based framework]Apache Structs, Spring 
 [Component-based Framework]Apache Tapestry, Apache Wicket, JSF</t>
+  </si>
+  <si>
+    <t>Http protocol</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIME</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>* HTTP Protocol是可運行在TCP/IP傳輸框架下的其中一種Protocol (其同伴還有FTP, POP3等等).
+* 在Web developing中, Http的幀由其Header分成兩種: Request 和 Response, 各有結構相似之處.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>多媒體格式的結構化表示形式, Tika呀, Http Request的Request header中都會有要求你給出當前處理的數据是哪種MIME的要求, 常見的有text/html, application/json, 等等</t>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2911,9 +2928,6 @@
     <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2957,6 +2971,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3320,10 +3337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F189"/>
+  <dimension ref="A1:F191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C187" sqref="C187"/>
+    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C190" sqref="C190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3497,7 +3514,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="86" t="s">
+      <c r="B21" s="101" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -3505,7 +3522,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="86"/>
+      <c r="B22" s="101"/>
       <c r="C22" s="9" t="s">
         <v>165</v>
       </c>
@@ -5072,6 +5089,28 @@
       </c>
       <c r="C189" s="83" t="s">
         <v>335</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -5102,16 +5141,16 @@
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6427,72 +6466,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="87"/>
-      <c r="B1" s="87" t="s">
+      <c r="A1" s="86"/>
+      <c r="B1" s="86" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="154.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="87" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="88" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="89" t="s">
         <v>339</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="89" t="s">
         <v>341</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="90" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="90" t="s">
+      <c r="A5" s="89" t="s">
         <v>343</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="90" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="87" t="s">
         <v>345</v>
       </c>
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="90" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="90" t="s">
+      <c r="A7" s="89" t="s">
         <v>347</v>
       </c>
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="90" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="90" t="s">
+      <c r="A8" s="89" t="s">
         <v>349</v>
       </c>
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="90" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="88" t="s">
+      <c r="A9" s="87" t="s">
         <v>351</v>
       </c>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="90" t="s">
         <v>352</v>
       </c>
     </row>
@@ -6520,694 +6559,694 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="91" t="s">
         <v>353</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="92" t="s">
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="91" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="87"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="95" t="s">
+      <c r="A2" s="86"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="94" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="86" t="s">
         <v>355</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="D3" s="87" t="s">
+      <c r="D3" s="86" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="86" t="s">
         <v>359</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="86" t="s">
         <v>360</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="86" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="95" t="s">
         <v>362</v>
       </c>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C5" s="87" t="s">
+      <c r="C5" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="D5" s="87" t="s">
+      <c r="D5" s="86" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="86" t="s">
         <v>365</v>
       </c>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C6" s="87" t="s">
+      <c r="C6" s="86" t="s">
         <v>366</v>
       </c>
-      <c r="D6" s="87" t="s">
+      <c r="D6" s="86" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="86" t="s">
         <v>368</v>
       </c>
-      <c r="B7" s="87" t="s">
+      <c r="B7" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C7" s="87" t="s">
+      <c r="C7" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="D7" s="87" t="s">
+      <c r="D7" s="86" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="86" t="s">
         <v>370</v>
       </c>
-      <c r="B8" s="87" t="s">
+      <c r="B8" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C8" s="87" t="s">
+      <c r="C8" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="87" t="s">
+      <c r="D8" s="86" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="96" t="s">
         <v>372</v>
       </c>
-      <c r="B9" s="87" t="s">
+      <c r="B9" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="86" t="s">
         <v>373</v>
       </c>
-      <c r="D9" s="87" t="s">
+      <c r="D9" s="86" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="97" t="s">
+      <c r="A10" s="96" t="s">
         <v>375</v>
       </c>
-      <c r="B10" s="87" t="s">
+      <c r="B10" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C10" s="87" t="s">
+      <c r="C10" s="86" t="s">
         <v>366</v>
       </c>
-      <c r="D10" s="87" t="s">
+      <c r="D10" s="86" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="97" t="s">
+      <c r="A11" s="96" t="s">
         <v>377</v>
       </c>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C11" s="87" t="s">
+      <c r="C11" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="D11" s="87" t="s">
+      <c r="D11" s="86" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="97" t="s">
+      <c r="A12" s="96" t="s">
         <v>379</v>
       </c>
-      <c r="B12" s="87" t="s">
+      <c r="B12" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C12" s="87" t="s">
+      <c r="C12" s="86" t="s">
         <v>360</v>
       </c>
-      <c r="D12" s="87" t="s">
+      <c r="D12" s="86" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="96" t="s">
         <v>381</v>
       </c>
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C13" s="87" t="s">
+      <c r="C13" s="86" t="s">
         <v>382</v>
       </c>
-      <c r="D13" s="87" t="s">
+      <c r="D13" s="86" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="97" t="s">
+      <c r="A14" s="96" t="s">
         <v>384</v>
       </c>
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="86" t="s">
         <v>385</v>
       </c>
-      <c r="D14" s="87" t="s">
+      <c r="D14" s="86" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="96" t="s">
         <v>387</v>
       </c>
-      <c r="B15" s="87" t="s">
+      <c r="B15" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C15" s="87" t="s">
+      <c r="C15" s="86" t="s">
         <v>366</v>
       </c>
-      <c r="D15" s="87" t="s">
+      <c r="D15" s="86" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="97" t="s">
+      <c r="A16" s="96" t="s">
         <v>389</v>
       </c>
-      <c r="B16" s="87" t="s">
+      <c r="B16" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C16" s="87" t="s">
+      <c r="C16" s="86" t="s">
         <v>390</v>
       </c>
-      <c r="D16" s="87" t="s">
+      <c r="D16" s="86" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="87" t="s">
+      <c r="A17" s="86" t="s">
         <v>392</v>
       </c>
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C17" s="87" t="s">
+      <c r="C17" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="D17" s="87" t="s">
+      <c r="D17" s="86" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="87" t="s">
+      <c r="A18" s="86" t="s">
         <v>394</v>
       </c>
-      <c r="B18" s="87" t="s">
+      <c r="B18" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87" t="s">
+      <c r="C18" s="86"/>
+      <c r="D18" s="86" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="96" t="s">
+      <c r="A19" s="95" t="s">
         <v>396</v>
       </c>
-      <c r="B19" s="87" t="s">
+      <c r="B19" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C19" s="97" t="s">
+      <c r="C19" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="97" t="s">
+      <c r="D19" s="96" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="87" t="s">
+      <c r="A20" s="86" t="s">
         <v>398</v>
       </c>
-      <c r="B20" s="87" t="s">
+      <c r="B20" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C20" s="87" t="s">
+      <c r="C20" s="86" t="s">
         <v>399</v>
       </c>
-      <c r="D20" s="87" t="s">
+      <c r="D20" s="86" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="98" t="s">
+      <c r="A21" s="97" t="s">
         <v>401</v>
       </c>
-      <c r="B21" s="87" t="s">
+      <c r="B21" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C21" s="87" t="s">
+      <c r="C21" s="86" t="s">
         <v>390</v>
       </c>
-      <c r="D21" s="87" t="s">
+      <c r="D21" s="86" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="86" t="s">
         <v>403</v>
       </c>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C22" s="87" t="s">
+      <c r="C22" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="D22" s="87" t="s">
+      <c r="D22" s="86" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="87" t="s">
+      <c r="A23" s="86" t="s">
         <v>405</v>
       </c>
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="D23" s="87" t="s">
+      <c r="D23" s="86" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="87" t="s">
+      <c r="A24" s="86" t="s">
         <v>407</v>
       </c>
-      <c r="B24" s="87" t="s">
+      <c r="B24" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C24" s="87" t="s">
+      <c r="C24" s="86" t="s">
         <v>408</v>
       </c>
-      <c r="D24" s="87" t="s">
+      <c r="D24" s="86" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="87" t="s">
+      <c r="A25" s="86" t="s">
         <v>410</v>
       </c>
-      <c r="B25" s="87" t="s">
+      <c r="B25" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C25" s="87"/>
-      <c r="D25" s="87" t="s">
+      <c r="C25" s="86"/>
+      <c r="D25" s="86" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="87" t="s">
+      <c r="A26" s="86" t="s">
         <v>412</v>
       </c>
-      <c r="B26" s="87" t="s">
+      <c r="B26" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C26" s="87" t="s">
+      <c r="C26" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="87" t="s">
+      <c r="D26" s="86" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="87" t="s">
+      <c r="A27" s="86" t="s">
         <v>414</v>
       </c>
-      <c r="B27" s="87" t="s">
+      <c r="B27" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C27" s="87" t="s">
+      <c r="C27" s="86" t="s">
         <v>415</v>
       </c>
-      <c r="D27" s="87" t="s">
+      <c r="D27" s="86" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="87" t="s">
+      <c r="A28" s="86" t="s">
         <v>417</v>
       </c>
-      <c r="B28" s="87" t="s">
+      <c r="B28" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C28" s="87" t="s">
+      <c r="C28" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="87" t="s">
+      <c r="D28" s="86" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="98" t="s">
+      <c r="A29" s="97" t="s">
         <v>419</v>
       </c>
-      <c r="B29" s="87" t="s">
+      <c r="B29" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C29" s="87" t="s">
+      <c r="C29" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="87" t="s">
+      <c r="D29" s="86" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="87" t="s">
+      <c r="A30" s="86" t="s">
         <v>421</v>
       </c>
-      <c r="B30" s="87" t="s">
+      <c r="B30" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C30" s="87" t="s">
+      <c r="C30" s="86" t="s">
         <v>366</v>
       </c>
-      <c r="D30" s="87" t="s">
+      <c r="D30" s="86" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="87" t="s">
+      <c r="A31" s="86" t="s">
         <v>423</v>
       </c>
-      <c r="B31" s="87" t="s">
+      <c r="B31" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C31" s="87"/>
-      <c r="D31" s="87" t="s">
+      <c r="C31" s="86"/>
+      <c r="D31" s="86" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="87" t="s">
+      <c r="A32" s="86" t="s">
         <v>425</v>
       </c>
-      <c r="B32" s="87" t="s">
+      <c r="B32" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C32" s="87" t="s">
+      <c r="C32" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="D32" s="87" t="s">
+      <c r="D32" s="86" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="87" t="s">
+      <c r="A33" s="86" t="s">
         <v>427</v>
       </c>
-      <c r="B33" s="87" t="s">
+      <c r="B33" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C33" s="87" t="s">
+      <c r="C33" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="D33" s="87" t="s">
+      <c r="D33" s="86" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="87" t="s">
+      <c r="A34" s="86" t="s">
         <v>429</v>
       </c>
-      <c r="B34" s="87" t="s">
+      <c r="B34" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C34" s="87" t="s">
+      <c r="C34" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="D34" s="87" t="s">
+      <c r="D34" s="86" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="87" t="s">
+      <c r="A35" s="86" t="s">
         <v>431</v>
       </c>
-      <c r="B35" s="87" t="s">
+      <c r="B35" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C35" s="87" t="s">
+      <c r="C35" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="D35" s="87" t="s">
+      <c r="D35" s="86" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="96" t="s">
+      <c r="A36" s="95" t="s">
         <v>433</v>
       </c>
-      <c r="B36" s="87" t="s">
+      <c r="B36" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C36" s="97" t="s">
+      <c r="C36" s="96" t="s">
         <v>366</v>
       </c>
-      <c r="D36" s="97" t="s">
+      <c r="D36" s="96" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="87" t="s">
+      <c r="A37" s="86" t="s">
         <v>435</v>
       </c>
-      <c r="B37" s="87" t="s">
+      <c r="B37" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C37" s="87" t="s">
+      <c r="C37" s="86" t="s">
         <v>366</v>
       </c>
-      <c r="D37" s="87" t="s">
+      <c r="D37" s="86" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="87" t="s">
+      <c r="A38" s="86" t="s">
         <v>437</v>
       </c>
-      <c r="B38" s="87" t="s">
+      <c r="B38" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C38" s="87" t="s">
+      <c r="C38" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="D38" s="87" t="s">
+      <c r="D38" s="86" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="97" t="s">
+      <c r="A39" s="96" t="s">
         <v>439</v>
       </c>
-      <c r="B39" s="87" t="s">
+      <c r="B39" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C39" s="87" t="s">
+      <c r="C39" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="D39" s="87" t="s">
+      <c r="D39" s="86" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="87" t="s">
+      <c r="A40" s="86" t="s">
         <v>441</v>
       </c>
-      <c r="B40" s="87" t="s">
+      <c r="B40" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C40" s="87" t="s">
+      <c r="C40" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="D40" s="87" t="s">
+      <c r="D40" s="86" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="87" t="s">
+      <c r="A41" s="86" t="s">
         <v>443</v>
       </c>
-      <c r="B41" s="87" t="s">
+      <c r="B41" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C41" s="87" t="s">
+      <c r="C41" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="D41" s="87" t="s">
+      <c r="D41" s="86" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="98" t="s">
+      <c r="A42" s="97" t="s">
         <v>445</v>
       </c>
-      <c r="B42" s="87" t="s">
+      <c r="B42" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C42" s="87" t="s">
+      <c r="C42" s="86" t="s">
         <v>357</v>
       </c>
-      <c r="D42" s="87" t="s">
+      <c r="D42" s="86" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="98" t="s">
+      <c r="A43" s="97" t="s">
         <v>447</v>
       </c>
-      <c r="B43" s="87" t="s">
+      <c r="B43" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C43" s="99"/>
-      <c r="D43" s="97" t="s">
+      <c r="C43" s="98"/>
+      <c r="D43" s="96" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="96" t="s">
+      <c r="A44" s="95" t="s">
         <v>449</v>
       </c>
-      <c r="B44" s="87" t="s">
+      <c r="B44" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C44" s="87" t="s">
+      <c r="C44" s="86" t="s">
         <v>390</v>
       </c>
-      <c r="D44" s="87" t="s">
+      <c r="D44" s="86" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="87" t="s">
+      <c r="A45" s="86" t="s">
         <v>451</v>
       </c>
-      <c r="B45" s="87" t="s">
+      <c r="B45" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C45" s="87" t="s">
+      <c r="C45" s="86" t="s">
         <v>363</v>
       </c>
-      <c r="D45" s="87" t="s">
+      <c r="D45" s="86" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="98" t="s">
+      <c r="A46" s="97" t="s">
         <v>453</v>
       </c>
-      <c r="B46" s="87" t="s">
+      <c r="B46" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C46" s="97" t="s">
+      <c r="C46" s="96" t="s">
         <v>366</v>
       </c>
-      <c r="D46" s="97" t="s">
+      <c r="D46" s="96" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="87" t="s">
+      <c r="A47" s="86" t="s">
         <v>455</v>
       </c>
-      <c r="B47" s="87" t="s">
+      <c r="B47" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C47" s="87"/>
-      <c r="D47" s="87" t="s">
+      <c r="C47" s="86"/>
+      <c r="D47" s="86" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="87" t="s">
+      <c r="A48" s="86" t="s">
         <v>457</v>
       </c>
-      <c r="B48" s="87" t="s">
+      <c r="B48" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="C48" s="99"/>
-      <c r="D48" s="97" t="s">
+      <c r="C48" s="98"/>
+      <c r="D48" s="96" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="87"/>
-      <c r="B49" s="87"/>
-      <c r="C49" s="99"/>
-      <c r="D49" s="99"/>
+      <c r="A49" s="86"/>
+      <c r="B49" s="86"/>
+      <c r="C49" s="98"/>
+      <c r="D49" s="98"/>
     </row>
     <row r="50" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="87"/>
-      <c r="B50" s="87"/>
-      <c r="C50" s="87"/>
-      <c r="D50" s="87"/>
+      <c r="A50" s="86"/>
+      <c r="B50" s="86"/>
+      <c r="C50" s="86"/>
+      <c r="D50" s="86"/>
     </row>
     <row r="51" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="100" t="s">
+      <c r="A51" s="99" t="s">
         <v>459</v>
       </c>
-      <c r="B51" s="87"/>
-      <c r="C51" s="87"/>
-      <c r="D51" s="100" t="s">
+      <c r="B51" s="86"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="99" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="100" t="s">
+      <c r="A52" s="99" t="s">
         <v>459</v>
       </c>
-      <c r="B52" s="87"/>
-      <c r="C52" s="87"/>
-      <c r="D52" s="101" t="s">
+      <c r="B52" s="86"/>
+      <c r="C52" s="86"/>
+      <c r="D52" s="100" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="100" t="s">
+      <c r="A53" s="99" t="s">
         <v>459</v>
       </c>
-      <c r="B53" s="87"/>
-      <c r="C53" s="87"/>
-      <c r="D53" s="101" t="s">
+      <c r="B53" s="86"/>
+      <c r="C53" s="86"/>
+      <c r="D53" s="100" t="s">
         <v>462</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add content to index and java_lib
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="471">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -2363,6 +2363,23 @@
   </si>
   <si>
     <t>多媒體格式的結構化表示形式, Tika呀, Http Request的Request header中都會有要求你給出當前處理的數据是哪種MIME的要求, 常見的有text/html, application/json, 等等</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maven</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Great Maven Repo Search Site: search.maven.org</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>GSON</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>* Gson 在少量數据量的JSON翻釋速度較其他同類library快, 但巨量數据下則最慢(最快為Jackson)
+* Gson 的fromJson方法允許input的Json有數据不完整性存在.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -3337,10 +3354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F191"/>
+  <dimension ref="A1:F193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C190" sqref="C190"/>
+    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B194" sqref="B194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5111,6 +5128,28 @@
       </c>
       <c r="C191" s="1" t="s">
         <v>466</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add index and java
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -15,14 +15,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'AS400 Version'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$131</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="475">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -2393,6 +2393,10 @@
 D/COPY CFSORC,SRW000
 C/COPY CFSORC,SRP001
 那麼在源碼中便可直接用EXSR SRP009來使用了, 當然必先設定Input的值.</t>
+  </si>
+  <si>
+    <t>之前已有總結Encoding的結構, 再結合今天在Java上的String Encoding測試, 更加深了認識. Java的String.getByte方法會以字符的內容為基準, 按你注入的Charset Name返回相應的Byte值, 換句話講, 是面向字符內容而非面向Byte的, 不變的是內容, 變的是Byte值, 這是他的邏輯. 
+* 信息弄失在以某種大信息集的字符轉換到小信息集時, 小信息集會把不能承載的信息弄棄.</t>
   </si>
 </sst>
 </file>
@@ -2706,7 +2710,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2991,6 +2995,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3039,13 +3046,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4202207</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>593914</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>414618</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>102264</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3361,7 +3368,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F196"/>
+  <dimension ref="A1:F197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -3390,304 +3397,304 @@
       <c r="B2" s="98"/>
       <c r="C2" s="98"/>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="60">
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="105">
       <c r="A3" s="2">
         <v>42459</v>
       </c>
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="100" t="s">
+        <v>471</v>
+      </c>
+      <c r="C3" s="100" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="4" customFormat="1" ht="60">
+      <c r="A4" s="2">
+        <v>42459</v>
+      </c>
+      <c r="B4" s="99" t="s">
         <v>242</v>
       </c>
-      <c r="C3" s="99" t="s">
+      <c r="C4" s="99" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1">
-      <c r="A4" s="2">
+    <row r="5" spans="1:3" s="4" customFormat="1">
+      <c r="A5" s="2">
         <v>42458</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B5" s="98" t="s">
         <v>471</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C5" s="9" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="105">
-      <c r="A5" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B5" s="98" t="s">
-        <v>255</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="60">
+    <row r="6" spans="1:3" ht="105">
       <c r="A6" s="2">
         <v>42456</v>
       </c>
       <c r="B6" s="98" t="s">
-        <v>463</v>
+        <v>255</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="45">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60">
       <c r="A7" s="2">
         <v>42456</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>464</v>
+      <c r="B7" s="98" t="s">
+        <v>463</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45">
       <c r="A8" s="2">
         <v>42456</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="45">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2">
         <v>42456</v>
       </c>
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="45">
+      <c r="A10" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B10" s="98" t="s">
         <v>469</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="77.25">
-      <c r="A10" s="81">
-        <v>42453</v>
-      </c>
-      <c r="B10" s="80" t="s">
-        <v>265</v>
-      </c>
-      <c r="C10" s="80" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="26.25">
+    <row r="11" spans="1:3" ht="77.25">
       <c r="A11" s="81">
         <v>42453</v>
       </c>
       <c r="B11" s="80" t="s">
+        <v>265</v>
+      </c>
+      <c r="C11" s="80" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="26.25">
+      <c r="A12" s="81">
+        <v>42453</v>
+      </c>
+      <c r="B12" s="80" t="s">
         <v>263</v>
       </c>
-      <c r="C11" s="80" t="s">
+      <c r="C12" s="80" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="39">
-      <c r="A12" s="81">
+    <row r="13" spans="1:3" ht="39">
+      <c r="A13" s="81">
         <v>42452</v>
       </c>
-      <c r="B12" s="80" t="s">
+      <c r="B13" s="80" t="s">
         <v>261</v>
       </c>
-      <c r="C12" s="80" t="s">
+      <c r="C13" s="80" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="165">
-      <c r="A13" s="77">
+    <row r="14" spans="1:3" ht="165">
+      <c r="A14" s="77">
         <v>42451</v>
       </c>
-      <c r="B13" s="76" t="s">
+      <c r="B14" s="76" t="s">
         <v>248</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45">
-      <c r="A14" s="2">
-        <v>42451</v>
-      </c>
-      <c r="B14" s="98" t="s">
-        <v>250</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30">
+    <row r="15" spans="1:3" ht="45">
       <c r="A15" s="2">
         <v>42451</v>
       </c>
       <c r="B15" s="98" t="s">
-        <v>196</v>
+        <v>250</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="165">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30">
       <c r="A16" s="2">
         <v>42451</v>
       </c>
       <c r="B16" s="98" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="165">
+      <c r="A17" s="2">
+        <v>42451</v>
+      </c>
+      <c r="B17" s="98" t="s">
         <v>254</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="64.5">
-      <c r="A17" s="81">
-        <v>42451</v>
-      </c>
-      <c r="B17" s="80" t="s">
-        <v>254</v>
-      </c>
-      <c r="C17" s="80" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="64.5">
       <c r="A18" s="81">
+        <v>42451</v>
+      </c>
+      <c r="B18" s="80" t="s">
+        <v>254</v>
+      </c>
+      <c r="C18" s="80" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="64.5">
+      <c r="A19" s="81">
         <v>42447</v>
       </c>
-      <c r="B18" s="80" t="s">
+      <c r="B19" s="80" t="s">
         <v>258</v>
       </c>
-      <c r="C18" s="80" t="s">
+      <c r="C19" s="80" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="2">
+    <row r="20" spans="1:3">
+      <c r="A20" s="2">
         <v>42440</v>
       </c>
-      <c r="B19" s="98" t="s">
+      <c r="B20" s="98" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="75">
-      <c r="A20" s="2">
+    <row r="21" spans="1:3" ht="75">
+      <c r="A21" s="2">
         <v>42436</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="39">
-      <c r="A21" s="81">
-        <v>42431</v>
-      </c>
-      <c r="B21" s="80" t="s">
-        <v>275</v>
-      </c>
-      <c r="C21" s="80" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="26.25">
+    <row r="22" spans="1:3" ht="39">
       <c r="A22" s="81">
         <v>42431</v>
       </c>
       <c r="B22" s="80" t="s">
+        <v>275</v>
+      </c>
+      <c r="C22" s="80" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="26.25">
+      <c r="A23" s="81">
+        <v>42431</v>
+      </c>
+      <c r="B23" s="80" t="s">
         <v>273</v>
       </c>
-      <c r="C22" s="80" t="s">
+      <c r="C23" s="80" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="51.75">
-      <c r="A23" s="81">
+    <row r="24" spans="1:3" ht="51.75">
+      <c r="A24" s="81">
         <v>42430</v>
       </c>
-      <c r="B23" s="80" t="s">
+      <c r="B24" s="80" t="s">
         <v>271</v>
       </c>
-      <c r="C23" s="80" t="s">
+      <c r="C24" s="80" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="26.25">
-      <c r="A24" s="81">
+    <row r="25" spans="1:3" ht="26.25">
+      <c r="A25" s="81">
         <v>42428</v>
       </c>
-      <c r="B24" s="80" t="s">
+      <c r="B25" s="80" t="s">
         <v>269</v>
       </c>
-      <c r="C24" s="80" t="s">
+      <c r="C25" s="80" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30">
-      <c r="A25" s="2">
+    <row r="26" spans="1:3" ht="30">
+      <c r="A26" s="2">
         <v>42426</v>
       </c>
-      <c r="B25" s="98" t="s">
+      <c r="B26" s="98" t="s">
         <v>186</v>
       </c>
-      <c r="C25" s="98" t="s">
+      <c r="C26" s="98" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="77.25">
-      <c r="A26" s="81">
+    <row r="27" spans="1:3" ht="77.25">
+      <c r="A27" s="81">
         <v>42426</v>
       </c>
-      <c r="B26" s="80" t="s">
+      <c r="B27" s="80" t="s">
         <v>267</v>
       </c>
-      <c r="C26" s="80" t="s">
+      <c r="C27" s="80" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="2">
-        <v>42425</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="30">
+    <row r="28" spans="1:3">
       <c r="A28" s="2">
         <v>42425</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30">
+      <c r="A29" s="2">
+        <v>42425</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="26.25">
-      <c r="A29" s="81">
-        <v>42425</v>
-      </c>
-      <c r="B29" s="80" t="s">
-        <v>277</v>
-      </c>
-      <c r="C29" s="80" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" ht="26.25">
       <c r="A30" s="81">
         <v>42425</v>
       </c>
@@ -3695,261 +3702,261 @@
         <v>277</v>
       </c>
       <c r="C30" s="80" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="26.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="81">
         <v>42425</v>
       </c>
       <c r="B31" s="80" t="s">
+        <v>277</v>
+      </c>
+      <c r="C31" s="80" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="26.25">
+      <c r="A32" s="81">
+        <v>42425</v>
+      </c>
+      <c r="B32" s="80" t="s">
         <v>280</v>
       </c>
-      <c r="C31" s="80" t="s">
+      <c r="C32" s="80" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="165">
-      <c r="A32" s="2">
+    <row r="33" spans="1:3" ht="165">
+      <c r="A33" s="2">
         <v>42424</v>
       </c>
-      <c r="B32" s="98" t="s">
+      <c r="B33" s="98" t="s">
         <v>239</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C33" s="12" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="45">
-      <c r="A33" s="2">
+    <row r="34" spans="1:3" ht="45">
+      <c r="A34" s="2">
         <v>42423</v>
       </c>
-      <c r="B33" s="98" t="s">
+      <c r="B34" s="98" t="s">
         <v>196</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C34" s="13" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="81">
+    <row r="35" spans="1:3">
+      <c r="A35" s="81">
         <v>42423</v>
       </c>
-      <c r="B34" s="80" t="s">
+      <c r="B35" s="80" t="s">
         <v>282</v>
       </c>
-      <c r="C34" s="80" t="s">
+      <c r="C35" s="80" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="90">
-      <c r="A35" s="2">
+    <row r="36" spans="1:3" ht="90">
+      <c r="A36" s="2">
         <v>42422</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B36" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="C35" s="38" t="s">
+      <c r="C36" s="38" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="60">
-      <c r="A36" s="2">
+    <row r="37" spans="1:3" ht="60">
+      <c r="A37" s="2">
         <v>42419</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B37" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C37" s="20" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="195">
-      <c r="A37" s="2">
+    <row r="38" spans="1:3" ht="195">
+      <c r="A38" s="2">
         <v>42418</v>
       </c>
-      <c r="B37" s="98" t="s">
+      <c r="B38" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C38" s="13" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="45">
-      <c r="A38" s="2">
-        <v>42403</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="75">
+    <row r="39" spans="1:3" ht="45">
       <c r="A39" s="2">
         <v>42403</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="90">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="75">
       <c r="A40" s="2">
         <v>42403</v>
       </c>
-      <c r="B40" s="13"/>
+      <c r="B40" s="13" t="s">
+        <v>230</v>
+      </c>
       <c r="C40" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="90">
       <c r="A41" s="2">
-        <v>42398</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>196</v>
-      </c>
+        <v>42403</v>
+      </c>
+      <c r="B41" s="13"/>
       <c r="C41" s="13" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="45">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="90">
       <c r="A42" s="2">
         <v>42398</v>
       </c>
-      <c r="B42" s="98" t="s">
+      <c r="B42" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="45">
+      <c r="A43" s="2">
+        <v>42398</v>
+      </c>
+      <c r="B43" s="98" t="s">
         <v>226</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C43" s="15" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="2">
+    <row r="44" spans="1:3">
+      <c r="A44" s="2">
         <v>42397</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B44" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C44" s="13" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="45">
-      <c r="A44" s="2">
-        <v>42396</v>
-      </c>
-      <c r="B44" s="98" t="s">
-        <v>196</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="30">
+    <row r="45" spans="1:3" ht="45">
       <c r="A45" s="2">
         <v>42396</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="98" t="s">
+        <v>196</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30">
+      <c r="A46" s="2">
+        <v>42396</v>
+      </c>
+      <c r="B46" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C46" s="15" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="128.25">
-      <c r="A46" s="81">
-        <v>42386</v>
-      </c>
-      <c r="B46" s="80" t="s">
-        <v>284</v>
-      </c>
-      <c r="C46" s="80" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="64.5">
+    <row r="47" spans="1:3" ht="128.25">
       <c r="A47" s="81">
         <v>42386</v>
       </c>
       <c r="B47" s="80" t="s">
+        <v>284</v>
+      </c>
+      <c r="C47" s="80" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="64.5">
+      <c r="A48" s="81">
+        <v>42386</v>
+      </c>
+      <c r="B48" s="80" t="s">
         <v>286</v>
       </c>
-      <c r="C47" s="80" t="s">
+      <c r="C48" s="80" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="45">
-      <c r="A48" s="2">
+    <row r="49" spans="1:3" ht="45">
+      <c r="A49" s="2">
         <v>42384</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B49" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="C49" s="15" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="180">
-      <c r="A49" s="2">
+    <row r="50" spans="1:3" ht="180">
+      <c r="A50" s="2">
         <v>42382</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B50" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="C50" s="17" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="64.5">
-      <c r="A50" s="81">
+    <row r="51" spans="1:3" ht="64.5">
+      <c r="A51" s="81">
         <v>42382</v>
       </c>
-      <c r="B50" s="80" t="s">
+      <c r="B51" s="80" t="s">
         <v>288</v>
       </c>
-      <c r="C50" s="80" t="s">
+      <c r="C51" s="80" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="30">
-      <c r="A51" s="2">
+    <row r="52" spans="1:3" ht="30">
+      <c r="A52" s="2">
         <v>42381</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B52" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="C51" s="18" t="s">
+      <c r="C52" s="18" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="45">
-      <c r="A52" s="2">
-        <v>42380</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="75">
+    <row r="53" spans="1:3" ht="45">
       <c r="A53" s="2">
         <v>42380</v>
       </c>
-      <c r="B53" s="52" t="s">
-        <v>195</v>
-      </c>
-      <c r="C53" s="20" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="180">
+      <c r="B53" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="75">
       <c r="A54" s="2">
         <v>42380</v>
       </c>
@@ -3957,29 +3964,29 @@
         <v>195</v>
       </c>
       <c r="C54" s="20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="180">
+      <c r="A55" s="2">
+        <v>42380</v>
+      </c>
+      <c r="B55" s="52" t="s">
+        <v>195</v>
+      </c>
+      <c r="C55" s="20" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="217.5">
-      <c r="A55" s="81">
+    <row r="56" spans="1:3" ht="217.5">
+      <c r="A56" s="81">
         <v>42380</v>
       </c>
-      <c r="B55" s="80" t="s">
+      <c r="B56" s="80" t="s">
         <v>289</v>
       </c>
-      <c r="C55" s="80" t="s">
+      <c r="C56" s="80" t="s">
         <v>290</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="102.75">
-      <c r="A56" s="81">
-        <v>42378</v>
-      </c>
-      <c r="B56" s="80" t="s">
-        <v>292</v>
-      </c>
-      <c r="C56" s="80" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="102.75">
@@ -3987,24 +3994,24 @@
         <v>42378</v>
       </c>
       <c r="B57" s="80" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C57" s="80" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="141">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="102.75">
       <c r="A58" s="81">
         <v>42378</v>
       </c>
       <c r="B58" s="80" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C58" s="80" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="77.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="141">
       <c r="A59" s="81">
         <v>42378</v>
       </c>
@@ -4012,169 +4019,169 @@
         <v>298</v>
       </c>
       <c r="C59" s="80" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="102.75">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="77.25">
       <c r="A60" s="81">
         <v>42378</v>
       </c>
       <c r="B60" s="80" t="s">
+        <v>298</v>
+      </c>
+      <c r="C60" s="80" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="102.75">
+      <c r="A61" s="81">
+        <v>42378</v>
+      </c>
+      <c r="B61" s="80" t="s">
         <v>296</v>
       </c>
-      <c r="C60" s="80" t="s">
+      <c r="C61" s="80" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="60">
-      <c r="A61" s="2">
+    <row r="62" spans="1:3" ht="60">
+      <c r="A62" s="2">
         <v>42377</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C61" s="98" t="s">
+      <c r="C62" s="98" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="77.25">
-      <c r="A62" s="81">
+    <row r="63" spans="1:3" ht="77.25">
+      <c r="A63" s="81">
         <v>42376</v>
       </c>
-      <c r="B62" s="80" t="s">
+      <c r="B63" s="80" t="s">
         <v>301</v>
       </c>
-      <c r="C62" s="80" t="s">
+      <c r="C63" s="80" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="45">
-      <c r="A63" s="2">
+    <row r="64" spans="1:3" ht="45">
+      <c r="A64" s="2">
         <v>42375</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="B64" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C63" s="21" t="s">
+      <c r="C64" s="21" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="2">
+    <row r="65" spans="1:3">
+      <c r="A65" s="2">
         <v>42369</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C64" s="21" t="s">
+      <c r="C65" s="21" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="195">
-      <c r="A65" s="2">
-        <v>42368</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C65" s="22" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="135">
+    <row r="66" spans="1:3" ht="195">
       <c r="A66" s="2">
         <v>42368</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="45">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="135">
       <c r="A67" s="2">
         <v>42368</v>
       </c>
-      <c r="B67" s="22" t="s">
+      <c r="B67" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="45">
+      <c r="A68" s="2">
+        <v>42368</v>
+      </c>
+      <c r="B68" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="C67" s="22" t="s">
+      <c r="C68" s="22" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="30">
-      <c r="A68" s="2">
-        <v>42366</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C68" s="22" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="30">
       <c r="A69" s="2">
         <v>42366</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="22" t="s">
         <v>49</v>
       </c>
       <c r="C69" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="30">
+      <c r="A70" s="2">
+        <v>42366</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C70" s="22" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="150">
-      <c r="A70" s="2">
-        <v>42361</v>
-      </c>
-      <c r="C70" s="22" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="30">
+    <row r="71" spans="1:3" ht="150">
       <c r="A71" s="2">
         <v>42361</v>
       </c>
-      <c r="C71" s="24" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="270">
+      <c r="C71" s="22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="30">
       <c r="A72" s="2">
         <v>42361</v>
       </c>
-      <c r="B72" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="C72" s="22" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="30">
+      <c r="C72" s="24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="270">
       <c r="A73" s="2">
         <v>42361</v>
       </c>
-      <c r="B73" s="98" t="s">
-        <v>53</v>
-      </c>
-      <c r="C73" s="23" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="B73" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="30">
       <c r="A74" s="2">
         <v>42361</v>
       </c>
-      <c r="B74" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="C74" s="24" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="225">
+      <c r="B74" s="98" t="s">
+        <v>53</v>
+      </c>
+      <c r="C74" s="23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" s="2">
         <v>42361</v>
       </c>
@@ -4182,51 +4189,51 @@
         <v>186</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="60">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="225">
       <c r="A76" s="2">
         <v>42361</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>49</v>
+      <c r="B76" s="37" t="s">
+        <v>186</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="90">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="60">
       <c r="A77" s="2">
         <v>42361</v>
       </c>
-      <c r="B77" s="26" t="s">
-        <v>196</v>
-      </c>
-      <c r="C77" s="26" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="60">
+      <c r="B77" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C77" s="24" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="90">
       <c r="A78" s="2">
         <v>42361</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="26" t="s">
         <v>196</v>
       </c>
       <c r="C78" s="26" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="60">
+      <c r="A79" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C79" s="26" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="42">
-        <v>42360</v>
-      </c>
-      <c r="B79" s="52" t="s">
-        <v>195</v>
-      </c>
-      <c r="C79" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -4237,85 +4244,85 @@
         <v>195</v>
       </c>
       <c r="C80" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="42">
+        <v>42360</v>
+      </c>
+      <c r="B81" s="52" t="s">
+        <v>195</v>
+      </c>
+      <c r="C81" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="102.75">
-      <c r="A81" s="82">
+    <row r="82" spans="1:3" ht="102.75">
+      <c r="A82" s="82">
         <v>42360</v>
       </c>
-      <c r="B81" s="80" t="s">
+      <c r="B82" s="80" t="s">
         <v>303</v>
       </c>
-      <c r="C81" s="80" t="s">
+      <c r="C82" s="80" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="30">
-      <c r="A82" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B82" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C82" s="25" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" ht="30">
       <c r="A83" s="2">
         <v>42356</v>
       </c>
-      <c r="B83" s="27" t="s">
-        <v>202</v>
-      </c>
-      <c r="C83" s="27" t="s">
-        <v>181</v>
+      <c r="B83" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C83" s="25" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="2">
         <v>42356</v>
       </c>
-      <c r="B84" s="98" t="s">
-        <v>201</v>
+      <c r="B84" s="27" t="s">
+        <v>202</v>
       </c>
       <c r="C84" s="27" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="30">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" s="2">
         <v>42356</v>
       </c>
-      <c r="B85" s="98"/>
-      <c r="C85" s="28" t="s">
+      <c r="B85" s="98" t="s">
+        <v>201</v>
+      </c>
+      <c r="C85" s="27" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="30">
+      <c r="A86" s="2">
+        <v>42356</v>
+      </c>
+      <c r="B86" s="98"/>
+      <c r="C86" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="60">
-      <c r="A86" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B86" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="C86" s="31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" ht="60">
       <c r="A87" s="2">
         <v>42355</v>
       </c>
-      <c r="B87" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C87" s="28" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="150">
+      <c r="B87" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C87" s="31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88" s="2">
         <v>42355</v>
       </c>
@@ -4323,76 +4330,76 @@
         <v>33</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="120">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="150">
       <c r="A89" s="2">
         <v>42355</v>
       </c>
-      <c r="B89" s="98" t="s">
-        <v>168</v>
-      </c>
-      <c r="C89" s="30" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="30">
+      <c r="B89" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C89" s="28" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="120">
       <c r="A90" s="2">
         <v>42355</v>
       </c>
-      <c r="B90" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C90" s="31" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="B90" s="98" t="s">
+        <v>168</v>
+      </c>
+      <c r="C90" s="30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="30">
       <c r="A91" s="2">
         <v>42355</v>
       </c>
       <c r="B91" s="31" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="C91" s="31" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="75">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
       <c r="A92" s="2">
         <v>42355</v>
       </c>
-      <c r="B92" s="16" t="s">
-        <v>43</v>
+      <c r="B92" s="31" t="s">
+        <v>171</v>
       </c>
       <c r="C92" s="31" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="135">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="75">
       <c r="A93" s="2">
         <v>42355</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C93" s="44" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="75">
+      <c r="B93" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C93" s="31" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="135">
       <c r="A94" s="2">
         <v>42355</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C94" s="32" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="30">
+      <c r="C94" s="44" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="75">
       <c r="A95" s="2">
         <v>42355</v>
       </c>
@@ -4400,16 +4407,18 @@
         <v>173</v>
       </c>
       <c r="C95" s="32" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="30">
       <c r="A96" s="2">
         <v>42355</v>
       </c>
-      <c r="B96" s="44"/>
+      <c r="B96" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="C96" s="32" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -4418,7 +4427,7 @@
       </c>
       <c r="B97" s="44"/>
       <c r="C97" s="32" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -4427,92 +4436,92 @@
       </c>
       <c r="B98" s="44"/>
       <c r="C98" s="32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="2">
+        <v>42355</v>
+      </c>
+      <c r="B99" s="44"/>
+      <c r="C99" s="32" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="75">
-      <c r="A99" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B99" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="C99" s="33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="30">
+    <row r="100" spans="1:6" ht="75">
       <c r="A100" s="2">
         <v>42352</v>
       </c>
-      <c r="B100" s="28"/>
-      <c r="C100" s="72" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="75">
+      <c r="B100" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C100" s="33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="30">
       <c r="A101" s="2">
         <v>42352</v>
       </c>
       <c r="B101" s="28"/>
-      <c r="C101" s="34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
+      <c r="C101" s="72" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="75">
       <c r="A102" s="2">
         <v>42352</v>
       </c>
-      <c r="B102" s="98"/>
-      <c r="C102" s="35" t="s">
-        <v>69</v>
+      <c r="B102" s="28"/>
+      <c r="C102" s="34" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="2">
         <v>42352</v>
       </c>
-      <c r="B103" s="36"/>
-      <c r="C103" s="36" t="s">
-        <v>75</v>
+      <c r="B103" s="98"/>
+      <c r="C103" s="35" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="2">
         <v>42352</v>
       </c>
-      <c r="B104" s="98" t="s">
-        <v>71</v>
-      </c>
+      <c r="B104" s="36"/>
       <c r="C104" s="36" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="2">
         <v>42352</v>
       </c>
-      <c r="B105" s="98"/>
-      <c r="C105" s="39" t="s">
-        <v>73</v>
+      <c r="B105" s="98" t="s">
+        <v>71</v>
+      </c>
+      <c r="C105" s="36" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="2">
         <v>42352</v>
       </c>
-      <c r="B106" s="39"/>
+      <c r="B106" s="98"/>
       <c r="C106" s="39" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="30">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" s="2">
         <v>42352</v>
       </c>
-      <c r="B107" s="98"/>
-      <c r="C107" s="98" t="s">
-        <v>76</v>
+      <c r="B107" s="39"/>
+      <c r="C107" s="39" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="30">
@@ -4521,270 +4530,268 @@
       </c>
       <c r="B108" s="98"/>
       <c r="C108" s="98" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="30">
       <c r="A109" s="2">
         <v>42352</v>
       </c>
-      <c r="B109" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C109" s="41" t="s">
-        <v>79</v>
+      <c r="B109" s="98"/>
+      <c r="C109" s="98" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="45">
       <c r="A110" s="2">
         <v>42352</v>
       </c>
-      <c r="B110" s="40"/>
-      <c r="C110" s="58" t="s">
-        <v>80</v>
-      </c>
-      <c r="F110" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="30">
+      <c r="B110" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C110" s="41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="45">
       <c r="A111" s="2">
         <v>42352</v>
       </c>
-      <c r="B111" s="43"/>
-      <c r="C111" s="43" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="75">
+      <c r="B111" s="40"/>
+      <c r="C111" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="F111" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="30">
       <c r="A112" s="2">
         <v>42352</v>
       </c>
       <c r="B112" s="43"/>
       <c r="C112" s="43" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="75">
       <c r="A113" s="2">
         <v>42352</v>
       </c>
-      <c r="B113" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C113" s="45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="30">
+      <c r="B113" s="43"/>
+      <c r="C113" s="43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="45">
       <c r="A114" s="2">
         <v>42352</v>
       </c>
-      <c r="B114" s="46"/>
-      <c r="C114" s="46" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="45">
+      <c r="B114" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C114" s="45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="30">
       <c r="A115" s="2">
         <v>42352</v>
       </c>
-      <c r="B115" s="47"/>
-      <c r="C115" s="48" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="30">
+      <c r="B115" s="46"/>
+      <c r="C115" s="46" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="45">
       <c r="A116" s="2">
         <v>42352</v>
       </c>
-      <c r="B116" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="C116" s="49" t="s">
-        <v>86</v>
+      <c r="B116" s="47"/>
+      <c r="C116" s="48" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="30">
       <c r="A117" s="2">
         <v>42352</v>
       </c>
-      <c r="B117" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C117" s="50" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
+      <c r="B117" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C117" s="49" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="30">
       <c r="A118" s="2">
         <v>42352</v>
       </c>
-      <c r="B118" s="51" t="s">
+      <c r="B118" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C118" s="50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B119" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="C118" s="51" t="s">
+      <c r="C119" s="51" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="135">
-      <c r="A119" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B119" s="53"/>
-      <c r="C119" s="53" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="60">
+    <row r="120" spans="1:3" ht="135">
       <c r="A120" s="2">
         <v>42349</v>
       </c>
-      <c r="B120" s="98" t="s">
-        <v>53</v>
-      </c>
-      <c r="C120" s="55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="30">
+      <c r="B120" s="53"/>
+      <c r="C120" s="53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="60">
       <c r="A121" s="2">
         <v>42349</v>
       </c>
-      <c r="B121" s="98"/>
+      <c r="B121" s="98" t="s">
+        <v>53</v>
+      </c>
       <c r="C121" s="55" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="120">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="30">
       <c r="A122" s="2">
         <v>42349</v>
       </c>
-      <c r="B122" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C122" s="54" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="150">
+      <c r="B122" s="98"/>
+      <c r="C122" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="120">
       <c r="A123" s="2">
         <v>42349</v>
       </c>
-      <c r="B123" s="56"/>
-      <c r="C123" s="56" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="30">
+      <c r="B123" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C123" s="54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="150">
       <c r="A124" s="2">
         <v>42349</v>
       </c>
-      <c r="B124" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C124" s="57" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
+      <c r="B124" s="56"/>
+      <c r="C124" s="56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="30">
       <c r="A125" s="2">
         <v>42349</v>
       </c>
       <c r="B125" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C125" s="59" t="s">
-        <v>61</v>
+      <c r="C125" s="57" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="2">
         <v>42349</v>
       </c>
-      <c r="B126" s="60"/>
-      <c r="C126" s="60" t="s">
-        <v>78</v>
+      <c r="B126" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C126" s="59" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="2">
         <v>42349</v>
       </c>
-      <c r="B127" s="61"/>
-      <c r="C127" s="61" t="s">
-        <v>62</v>
+      <c r="B127" s="60"/>
+      <c r="C127" s="60" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="2">
         <v>42349</v>
       </c>
-      <c r="B128" s="62"/>
-      <c r="C128" s="62" t="s">
-        <v>70</v>
+      <c r="B128" s="61"/>
+      <c r="C128" s="61" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="2">
         <v>42349</v>
       </c>
-      <c r="B129" s="63"/>
-      <c r="C129" s="63" t="s">
-        <v>64</v>
+      <c r="B129" s="62"/>
+      <c r="C129" s="62" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="2">
         <v>42349</v>
       </c>
-      <c r="B130" s="64"/>
-      <c r="C130" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="60">
+      <c r="B130" s="63"/>
+      <c r="C130" s="63" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
       <c r="A131" s="2">
         <v>42349</v>
       </c>
-      <c r="B131" s="64" t="s">
+      <c r="B131" s="64"/>
+      <c r="C131" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="60">
+      <c r="A132" s="2">
+        <v>42349</v>
+      </c>
+      <c r="B132" s="64" t="s">
         <v>168</v>
       </c>
-      <c r="C131" s="64" t="s">
+      <c r="C132" s="64" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="90">
-      <c r="A132" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C132" s="64" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="30">
+    <row r="133" spans="1:3" ht="90">
       <c r="A133" s="2">
         <v>42345</v>
       </c>
-      <c r="B133" s="65" t="s">
+      <c r="B133" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C133" s="65" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
+      <c r="C133" s="64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="30">
       <c r="A134" s="2">
         <v>42345</v>
       </c>
-      <c r="B134" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C134" s="66" t="s">
-        <v>28</v>
+      <c r="B134" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="C134" s="65" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -4794,162 +4801,162 @@
       <c r="B135" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C135" s="67" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="30">
+      <c r="C135" s="66" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
       <c r="A136" s="2">
         <v>42345</v>
       </c>
       <c r="B136" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C136" s="68" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="195">
+      <c r="C136" s="67" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="30">
       <c r="A137" s="2">
         <v>42345</v>
       </c>
-      <c r="B137" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C137" s="69" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="135">
+      <c r="B137" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C137" s="68" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="195">
       <c r="A138" s="2">
         <v>42345</v>
       </c>
-      <c r="B138" s="71" t="s">
-        <v>31</v>
-      </c>
-      <c r="C138" s="70" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="75">
+      <c r="B138" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C138" s="69" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="135">
       <c r="A139" s="2">
         <v>42345</v>
       </c>
       <c r="B139" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="C139" s="71" t="s">
-        <v>32</v>
+      <c r="C139" s="70" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="75">
       <c r="A140" s="2">
         <v>42345</v>
       </c>
-      <c r="B140" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C140" s="75" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="30">
+      <c r="B140" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="C140" s="71" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="75">
       <c r="A141" s="2">
         <v>42345</v>
       </c>
-      <c r="B141" s="73" t="s">
-        <v>12</v>
+      <c r="B141" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="C141" s="75" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="30">
       <c r="A142" s="2">
         <v>42345</v>
       </c>
-      <c r="B142" s="74" t="s">
-        <v>39</v>
+      <c r="B142" s="73" t="s">
+        <v>12</v>
       </c>
       <c r="C142" s="75" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="2">
         <v>42345</v>
       </c>
-      <c r="B143" s="98" t="s">
+      <c r="B143" s="74" t="s">
         <v>39</v>
       </c>
       <c r="C143" s="75" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="60">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
       <c r="A144" s="2">
         <v>42345</v>
       </c>
-      <c r="B144" s="75" t="s">
+      <c r="B144" s="98" t="s">
         <v>39</v>
       </c>
       <c r="C144" s="75" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="150">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="60">
       <c r="A145" s="2">
         <v>42345</v>
       </c>
-      <c r="B145" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C145" s="78" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="45">
+      <c r="B145" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C145" s="75" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="150">
       <c r="A146" s="2">
         <v>42345</v>
       </c>
-      <c r="B146" s="79" t="s">
-        <v>39</v>
-      </c>
-      <c r="C146" s="79" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" ht="60">
+      <c r="B146" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C146" s="78" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="45">
       <c r="A147" s="2">
         <v>42345</v>
       </c>
-      <c r="B147" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="105">
+      <c r="B147" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C147" s="79" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="60">
       <c r="A148" s="2">
         <v>42345</v>
       </c>
-      <c r="B148" s="98" t="s">
-        <v>12</v>
-      </c>
-      <c r="C148" s="98" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3">
+      <c r="B148" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="105">
       <c r="A149" s="2">
         <v>42345</v>
       </c>
       <c r="B149" s="98" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C149" s="98" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -4960,10 +4967,10 @@
         <v>49</v>
       </c>
       <c r="C150" s="98" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="75">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
       <c r="A151" s="2">
         <v>42345</v>
       </c>
@@ -4971,54 +4978,54 @@
         <v>49</v>
       </c>
       <c r="C151" s="98" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="75">
       <c r="A152" s="2">
         <v>42345</v>
       </c>
       <c r="B152" s="98" t="s">
+        <v>49</v>
+      </c>
+      <c r="C152" s="98" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="45">
+      <c r="A153" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B153" s="98" t="s">
         <v>53</v>
       </c>
-      <c r="C152" s="98" t="s">
+      <c r="C153" s="98" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="141">
-      <c r="A153" s="82">
+    <row r="154" spans="1:3" ht="141">
+      <c r="A154" s="82">
         <v>42345</v>
       </c>
-      <c r="B153" s="80" t="s">
+      <c r="B154" s="80" t="s">
         <v>304</v>
       </c>
-      <c r="C153" s="80" t="s">
+      <c r="C154" s="80" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="105">
-      <c r="A154" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C154" s="98" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="90">
+    <row r="155" spans="1:3" ht="105">
       <c r="A155" s="2">
         <v>42341</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C155" s="98" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="75">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="90">
       <c r="A156" s="2">
         <v>42341</v>
       </c>
@@ -5026,10 +5033,10 @@
         <v>15</v>
       </c>
       <c r="C156" s="98" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="75">
       <c r="A157" s="2">
         <v>42341</v>
       </c>
@@ -5037,7 +5044,7 @@
         <v>15</v>
       </c>
       <c r="C157" s="98" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="30">
@@ -5048,10 +5055,10 @@
         <v>15</v>
       </c>
       <c r="C158" s="98" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="30">
       <c r="A159" s="2">
         <v>42341</v>
       </c>
@@ -5059,32 +5066,32 @@
         <v>15</v>
       </c>
       <c r="C159" s="98" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="90">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="45">
       <c r="A160" s="2">
         <v>42341</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C160" s="98" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="90">
       <c r="A161" s="2">
         <v>42341</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C161" s="98" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="150">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="30">
       <c r="A162" s="2">
         <v>42341</v>
       </c>
@@ -5092,10 +5099,10 @@
         <v>15</v>
       </c>
       <c r="C162" s="98" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="75">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="150">
       <c r="A163" s="2">
         <v>42341</v>
       </c>
@@ -5103,40 +5110,40 @@
         <v>15</v>
       </c>
       <c r="C163" s="98" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="90">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="75">
       <c r="A164" s="2">
         <v>42341</v>
       </c>
-      <c r="B164" s="98" t="s">
-        <v>12</v>
+      <c r="B164" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C164" s="98" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="90">
       <c r="A165" s="2">
         <v>42341</v>
       </c>
       <c r="B165" s="98" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C165" s="98" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="60">
       <c r="A166" s="2">
         <v>42341</v>
       </c>
       <c r="B166" s="98" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C166" s="98" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -5144,10 +5151,10 @@
         <v>42341</v>
       </c>
       <c r="B167" s="98" t="s">
-        <v>15</v>
-      </c>
-      <c r="C167" s="7" t="s">
-        <v>34</v>
+        <v>12</v>
+      </c>
+      <c r="C167" s="98" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -5158,7 +5165,7 @@
         <v>15</v>
       </c>
       <c r="C168" s="7" t="s">
-        <v>166</v>
+        <v>34</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -5168,8 +5175,8 @@
       <c r="B169" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="C169" s="9" t="s">
-        <v>165</v>
+      <c r="C169" s="7" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -5180,67 +5187,69 @@
         <v>15</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" ht="75">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
       <c r="A171" s="2">
         <v>42341</v>
       </c>
       <c r="B171" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="C171" s="98" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" ht="60">
+      <c r="C171" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="75">
       <c r="A172" s="2">
         <v>42341</v>
       </c>
       <c r="B172" s="98" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C172" s="98" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="60">
       <c r="A173" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B173" s="98"/>
+        <v>42341</v>
+      </c>
+      <c r="B173" s="98" t="s">
+        <v>12</v>
+      </c>
       <c r="C173" s="98" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="60">
       <c r="A174" s="2">
         <v>42340</v>
       </c>
       <c r="B174" s="98"/>
       <c r="C174" s="98" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" ht="60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="45">
       <c r="A175" s="2">
         <v>42340</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="B175" s="98"/>
+      <c r="C175" s="98" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="60">
+      <c r="A176" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C175" s="98" t="s">
+      <c r="C176" s="98" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3">
-      <c r="A176" s="2">
-        <v>42339</v>
-      </c>
-      <c r="B176" s="2"/>
-      <c r="C176" s="98" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -5249,131 +5258,129 @@
       </c>
       <c r="B177" s="2"/>
       <c r="C177" s="98" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" s="2">
+        <v>42339</v>
+      </c>
+      <c r="B178" s="2"/>
+      <c r="C178" s="98" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="64.5">
-      <c r="A178" s="82">
-        <v>42334</v>
-      </c>
-      <c r="B178" s="80" t="s">
-        <v>310</v>
-      </c>
-      <c r="C178" s="80" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="26.25">
+    <row r="179" spans="1:3" ht="64.5">
       <c r="A179" s="82">
         <v>42334</v>
       </c>
       <c r="B179" s="80" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C179" s="80" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="39">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="26.25">
       <c r="A180" s="82">
         <v>42334</v>
       </c>
       <c r="B180" s="80" t="s">
+        <v>308</v>
+      </c>
+      <c r="C180" s="80" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="39">
+      <c r="A181" s="82">
+        <v>42334</v>
+      </c>
+      <c r="B181" s="80" t="s">
         <v>273</v>
       </c>
-      <c r="C180" s="80" t="s">
+      <c r="C181" s="80" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="128.25">
-      <c r="A181" s="82">
-        <v>42333</v>
-      </c>
-      <c r="B181" s="80" t="s">
-        <v>269</v>
-      </c>
-      <c r="C181" s="80" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" ht="51.75">
+    <row r="182" spans="1:3" ht="128.25">
       <c r="A182" s="82">
         <v>42333</v>
       </c>
       <c r="B182" s="80" t="s">
+        <v>269</v>
+      </c>
+      <c r="C182" s="80" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="51.75">
+      <c r="A183" s="82">
+        <v>42333</v>
+      </c>
+      <c r="B183" s="80" t="s">
         <v>216</v>
       </c>
-      <c r="C182" s="80" t="s">
+      <c r="C183" s="80" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="26.25">
-      <c r="A183" s="82">
+    <row r="184" spans="1:3" ht="26.25">
+      <c r="A184" s="82">
         <v>42331</v>
       </c>
-      <c r="B183" s="80" t="s">
+      <c r="B184" s="80" t="s">
         <v>314</v>
       </c>
-      <c r="C183" s="80" t="s">
+      <c r="C184" s="80" t="s">
         <v>313</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" ht="39">
-      <c r="A184" s="82">
-        <v>42329</v>
-      </c>
-      <c r="B184" s="80" t="s">
-        <v>316</v>
-      </c>
-      <c r="C184" s="80" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="39">
       <c r="A185" s="82">
-        <v>42328</v>
+        <v>42329</v>
       </c>
       <c r="B185" s="80" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="C185" s="80" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="26.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="39">
       <c r="A186" s="82">
         <v>42328</v>
       </c>
       <c r="B186" s="80" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C186" s="80" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="115.5">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="26.25">
       <c r="A187" s="82">
         <v>42328</v>
       </c>
       <c r="B187" s="80" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C187" s="80" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" ht="90">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="115.5">
       <c r="A188" s="82">
         <v>42328</v>
       </c>
       <c r="B188" s="80" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C188" s="80" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" ht="153.75">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="90">
       <c r="A189" s="82">
         <v>42328</v>
       </c>
@@ -5381,32 +5388,32 @@
         <v>318</v>
       </c>
       <c r="C189" s="80" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="153.75">
+      <c r="A190" s="82">
+        <v>42328</v>
+      </c>
+      <c r="B190" s="80" t="s">
+        <v>318</v>
+      </c>
+      <c r="C190" s="80" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="102.75">
-      <c r="A190" s="82">
+    <row r="191" spans="1:3" ht="102.75">
+      <c r="A191" s="82">
         <v>42324</v>
       </c>
-      <c r="B190" s="80" t="s">
+      <c r="B191" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="C190" s="80" t="s">
+      <c r="C191" s="80" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="90">
-      <c r="A191" s="82">
-        <v>42321</v>
-      </c>
-      <c r="B191" s="80" t="s">
-        <v>328</v>
-      </c>
-      <c r="C191" s="80" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" ht="26.25">
+    <row r="192" spans="1:3" ht="90">
       <c r="A192" s="82">
         <v>42321</v>
       </c>
@@ -5414,65 +5421,76 @@
         <v>328</v>
       </c>
       <c r="C192" s="80" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="26.25">
+      <c r="A193" s="82">
+        <v>42321</v>
+      </c>
+      <c r="B193" s="80" t="s">
+        <v>328</v>
+      </c>
+      <c r="C193" s="80" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="77.25">
-      <c r="A193" s="81">
+    <row r="194" spans="1:3" ht="77.25">
+      <c r="A194" s="81">
         <v>42318</v>
       </c>
-      <c r="B193" s="80" t="s">
+      <c r="B194" s="80" t="s">
         <v>331</v>
       </c>
-      <c r="C193" s="80" t="s">
+      <c r="C194" s="80" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="115.5">
-      <c r="A194" s="81">
+    <row r="195" spans="1:3" ht="115.5">
+      <c r="A195" s="81">
         <v>42311</v>
-      </c>
-      <c r="B194" s="80" t="s">
-        <v>216</v>
-      </c>
-      <c r="C194" s="80" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="77.25">
-      <c r="A195" s="81">
-        <v>42310</v>
       </c>
       <c r="B195" s="80" t="s">
         <v>216</v>
       </c>
       <c r="C195" s="80" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="77.25">
+      <c r="A196" s="81">
+        <v>42310</v>
+      </c>
+      <c r="B196" s="80" t="s">
+        <v>216</v>
+      </c>
+      <c r="C196" s="80" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="51.75">
-      <c r="A196" s="81">
+    <row r="197" spans="1:3" ht="51.75">
+      <c r="A197" s="81">
         <v>42306</v>
       </c>
-      <c r="B196" s="80" t="s">
+      <c r="B197" s="80" t="s">
         <v>334</v>
       </c>
-      <c r="C196" s="80" t="s">
+      <c r="C197" s="80" t="s">
         <v>335</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C130">
+  <autoFilter ref="A1:C131">
     <sortState ref="A2:C193">
       <sortCondition descending="1" ref="A1:A127"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C169" r:id="rId1"/>
-    <hyperlink ref="C130" r:id="rId2"/>
-    <hyperlink ref="C170" r:id="rId3"/>
-    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="C170" r:id="rId1"/>
+    <hyperlink ref="C131" r:id="rId2"/>
+    <hyperlink ref="C171" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -5491,16 +5509,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="60.75" customHeight="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add jquery jsonp & callback
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -15,14 +15,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'AS400 Version'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$218</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$222</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="513">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -2624,6 +2624,12 @@
 /etc/nginx/ 放置設置文檔
 /usr/sbin/nginx 軟件的不變程式
 /usr/share/nginx 預設放置網站之處 (也可以通過設定放到別處啦)</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>關於NGINX的分流選擇方式, 官網上寫明:
+When nginx selects a location block to serve a request it first checks location directives that specify prefixes, remembering location with the longest prefix, and then checks regular expressions. If there is a match with a regular expression, nginx picks this location or, otherwise, it picks the one remembered earlier.
+優先正則擊中, 次為最長匹配</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -2953,7 +2959,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3254,6 +3260,9 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3316,13 +3325,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4202207</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>593914</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>414618</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>102265</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3640,10 +3649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F218"/>
+  <dimension ref="A1:F222"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3669,860 +3678,842 @@
       <c r="B2" s="100"/>
       <c r="C2" s="100"/>
     </row>
-    <row r="3" spans="1:3" s="102" customFormat="1" ht="126" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="110"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="110"/>
+    </row>
+    <row r="4" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="110"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="110"/>
+    </row>
+    <row r="5" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="110"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="110"/>
+    </row>
+    <row r="6" spans="1:3" s="102" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>42478</v>
+      </c>
+      <c r="B6" s="110" t="s">
+        <v>510</v>
+      </c>
+      <c r="C6" s="110" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="102" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>42477</v>
       </c>
-      <c r="B3" s="109" t="s">
+      <c r="B7" s="109" t="s">
         <v>510</v>
       </c>
-      <c r="C3" s="109" t="s">
+      <c r="C7" s="109" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="102" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="8" spans="1:3" s="102" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>42477</v>
       </c>
-      <c r="B4" s="108" t="s">
+      <c r="B8" s="108" t="s">
         <v>508</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="C8" s="108" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="9" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>42473</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B9" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="106" t="s">
+      <c r="C9" s="106" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="102" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="10" spans="1:3" s="102" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>42473</v>
       </c>
-      <c r="B6" s="106" t="s">
+      <c r="B10" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="107" t="s">
+      <c r="C10" s="107" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="11" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>42469</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="B11" s="105" t="s">
         <v>505</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C11" s="8" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="102" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B8" s="104" t="s">
-        <v>498</v>
-      </c>
-      <c r="C8" s="104" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="102" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B9" s="104" t="s">
-        <v>500</v>
-      </c>
-      <c r="C9" s="104" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B10" s="104" t="s">
-        <v>502</v>
-      </c>
-      <c r="C10" s="104" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="102" customFormat="1" ht="126" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B11" s="100" t="s">
-        <v>494</v>
-      </c>
-      <c r="C11" s="100" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="102" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="102" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>42463</v>
       </c>
-      <c r="B12" s="103" t="s">
-        <v>493</v>
-      </c>
-      <c r="C12" s="103" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="102" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="104" t="s">
+        <v>498</v>
+      </c>
+      <c r="C12" s="104" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="102" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>42463</v>
       </c>
-      <c r="B13" s="101" t="s">
-        <v>490</v>
-      </c>
-      <c r="C13" s="101" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="102" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="B13" s="104" t="s">
+        <v>500</v>
+      </c>
+      <c r="C13" s="104" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42463</v>
       </c>
-      <c r="B14" s="101" t="s">
+      <c r="B14" s="104" t="s">
+        <v>502</v>
+      </c>
+      <c r="C14" s="104" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="102" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B15" s="100" t="s">
+        <v>494</v>
+      </c>
+      <c r="C15" s="100" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="102" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B16" s="103" t="s">
+        <v>493</v>
+      </c>
+      <c r="C16" s="103" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="102" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B17" s="101" t="s">
+        <v>490</v>
+      </c>
+      <c r="C17" s="101" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="102" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B18" s="101" t="s">
         <v>489</v>
       </c>
-      <c r="C14" s="101" t="s">
+      <c r="C18" s="101" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="102" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="19" spans="1:3" s="102" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>42462</v>
       </c>
-      <c r="B15" s="100" t="s">
+      <c r="B19" s="100" t="s">
         <v>487</v>
       </c>
-      <c r="C15" s="100" t="s">
+      <c r="C19" s="100" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="102" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="20" spans="1:3" s="102" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>42462</v>
       </c>
-      <c r="B16" s="100" t="s">
+      <c r="B20" s="100" t="s">
         <v>485</v>
       </c>
-      <c r="C16" s="100" t="s">
+      <c r="C20" s="100" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="102" customFormat="1" ht="236.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+    <row r="21" spans="1:3" s="102" customFormat="1" ht="236.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>42462</v>
       </c>
-      <c r="B17" s="100" t="s">
+      <c r="B21" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="C17" s="100" t="s">
+      <c r="C21" s="100" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="102" customFormat="1" ht="126" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="22" spans="1:3" s="102" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>42462</v>
       </c>
-      <c r="B18" s="100" t="s">
+      <c r="B22" s="100" t="s">
         <v>481</v>
       </c>
-      <c r="C18" s="100" t="s">
+      <c r="C22" s="100" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="23" spans="1:3" s="4" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>42460</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="B23" s="99" t="s">
         <v>478</v>
       </c>
-      <c r="C19" s="99" t="s">
+      <c r="C23" s="99" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="24" spans="1:3" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>42460</v>
       </c>
-      <c r="B20" s="99" t="s">
+      <c r="B24" s="99" t="s">
         <v>477</v>
       </c>
-      <c r="C20" s="99" t="s">
+      <c r="C24" s="99" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+    <row r="25" spans="1:3" s="4" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>42460</v>
       </c>
-      <c r="B21" s="99" t="s">
+      <c r="B25" s="99" t="s">
         <v>476</v>
       </c>
-      <c r="C21" s="99" t="s">
+      <c r="C25" s="99" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+    <row r="26" spans="1:3" s="4" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>42460</v>
       </c>
-      <c r="B22" s="99" t="s">
+      <c r="B26" s="99" t="s">
         <v>479</v>
       </c>
-      <c r="C22" s="99" t="s">
+      <c r="C26" s="99" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+    <row r="27" spans="1:3" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>42459</v>
       </c>
-      <c r="B23" s="99" t="s">
+      <c r="B27" s="99" t="s">
         <v>471</v>
       </c>
-      <c r="C23" s="98" t="s">
+      <c r="C27" s="98" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="28" spans="1:3" s="4" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>42459</v>
       </c>
-      <c r="B24" s="99" t="s">
+      <c r="B28" s="99" t="s">
         <v>242</v>
       </c>
-      <c r="C24" s="99" t="s">
+      <c r="C28" s="99" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>42458</v>
       </c>
-      <c r="B25" s="97" t="s">
+      <c r="B29" s="97" t="s">
         <v>471</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B26" s="96" t="s">
-        <v>255</v>
-      </c>
-      <c r="C26" s="100" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B27" s="96" t="s">
-        <v>463</v>
-      </c>
-      <c r="C27" s="44" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B28" s="96" t="s">
-        <v>464</v>
-      </c>
-      <c r="C28" s="44" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="C29" s="44" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>42456</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="96" t="s">
+        <v>255</v>
+      </c>
+      <c r="C30" s="100" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B31" s="96" t="s">
+        <v>463</v>
+      </c>
+      <c r="C31" s="44" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B32" s="96" t="s">
+        <v>464</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C33" s="44" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="C30" s="44" t="s">
+      <c r="C34" s="44" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="79">
+    <row r="35" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="79">
         <v>42453</v>
       </c>
-      <c r="B31" s="78" t="s">
+      <c r="B35" s="78" t="s">
         <v>265</v>
       </c>
-      <c r="C31" s="78" t="s">
+      <c r="C35" s="78" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="79">
+    <row r="36" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="79">
         <v>42453</v>
       </c>
-      <c r="B32" s="78" t="s">
+      <c r="B36" s="78" t="s">
         <v>263</v>
       </c>
-      <c r="C32" s="78" t="s">
+      <c r="C36" s="78" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="79">
+    <row r="37" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="79">
         <v>42452</v>
       </c>
-      <c r="B33" s="78" t="s">
+      <c r="B37" s="78" t="s">
         <v>261</v>
       </c>
-      <c r="C33" s="78" t="s">
+      <c r="C37" s="78" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="75">
+    <row r="38" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="75">
         <v>42451</v>
       </c>
-      <c r="B34" s="74" t="s">
+      <c r="B38" s="74" t="s">
         <v>248</v>
       </c>
-      <c r="C34" s="100" t="s">
+      <c r="C38" s="100" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+    <row r="39" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
         <v>42451</v>
       </c>
-      <c r="B35" s="100" t="s">
+      <c r="B39" s="100" t="s">
         <v>250</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
         <v>42451</v>
       </c>
-      <c r="B36" s="96" t="s">
+      <c r="B40" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+    <row r="41" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
         <v>42451</v>
       </c>
-      <c r="B37" s="96" t="s">
+      <c r="B41" s="96" t="s">
         <v>254</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="79">
+    <row r="42" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="79">
         <v>42451</v>
       </c>
-      <c r="B38" s="78" t="s">
+      <c r="B42" s="78" t="s">
         <v>254</v>
       </c>
-      <c r="C38" s="78" t="s">
+      <c r="C42" s="78" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="79">
+    <row r="43" spans="1:3" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="79">
         <v>42447</v>
       </c>
-      <c r="B39" s="78" t="s">
+      <c r="B43" s="78" t="s">
         <v>258</v>
       </c>
-      <c r="C39" s="78" t="s">
+      <c r="C43" s="78" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
         <v>42440</v>
       </c>
-      <c r="B40" s="100" t="s">
+      <c r="B44" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="100" t="s">
+      <c r="C44" s="100" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+    <row r="45" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
         <v>42436</v>
       </c>
-      <c r="B41" s="96" t="s">
+      <c r="B45" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A42" s="79">
+    <row r="46" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A46" s="79">
         <v>42431</v>
       </c>
-      <c r="B42" s="78" t="s">
+      <c r="B46" s="78" t="s">
         <v>275</v>
       </c>
-      <c r="C42" s="78" t="s">
+      <c r="C46" s="78" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="79">
+    <row r="47" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A47" s="79">
         <v>42431</v>
       </c>
-      <c r="B43" s="78" t="s">
+      <c r="B47" s="78" t="s">
         <v>273</v>
       </c>
-      <c r="C43" s="78" t="s">
+      <c r="C47" s="78" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="79">
+    <row r="48" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="79">
         <v>42430</v>
       </c>
-      <c r="B44" s="78" t="s">
+      <c r="B48" s="78" t="s">
         <v>271</v>
       </c>
-      <c r="C44" s="78" t="s">
+      <c r="C48" s="78" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="79">
+    <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="79">
         <v>42428</v>
       </c>
-      <c r="B45" s="78" t="s">
+      <c r="B49" s="78" t="s">
         <v>269</v>
       </c>
-      <c r="C45" s="78" t="s">
+      <c r="C49" s="78" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
         <v>42426</v>
       </c>
-      <c r="B46" s="100" t="s">
+      <c r="B50" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="C46" s="100" t="s">
+      <c r="C50" s="100" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="79">
+    <row r="51" spans="1:3" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="79">
         <v>42426</v>
       </c>
-      <c r="B47" s="78" t="s">
+      <c r="B51" s="78" t="s">
         <v>267</v>
       </c>
-      <c r="C47" s="78" t="s">
+      <c r="C51" s="78" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
         <v>42425</v>
       </c>
-      <c r="B48" s="100" t="s">
+      <c r="B52" s="100" t="s">
         <v>242</v>
       </c>
-      <c r="C48" s="100" t="s">
+      <c r="C52" s="100" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+    <row r="53" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
         <v>42425</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="79">
+    <row r="54" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A54" s="79">
         <v>42425</v>
       </c>
-      <c r="B50" s="78" t="s">
+      <c r="B54" s="78" t="s">
         <v>277</v>
       </c>
-      <c r="C50" s="78" t="s">
+      <c r="C54" s="78" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="79">
-        <v>42425</v>
-      </c>
-      <c r="B51" s="78" t="s">
-        <v>277</v>
-      </c>
-      <c r="C51" s="78" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="79">
-        <v>42425</v>
-      </c>
-      <c r="B52" s="78" t="s">
-        <v>280</v>
-      </c>
-      <c r="C52" s="78" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
-        <v>42424</v>
-      </c>
-      <c r="B53" s="100" t="s">
-        <v>239</v>
-      </c>
-      <c r="C53" s="100" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
-        <v>42423</v>
-      </c>
-      <c r="B54" s="96" t="s">
-        <v>196</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="79">
+        <v>42425</v>
+      </c>
+      <c r="B55" s="78" t="s">
+        <v>277</v>
+      </c>
+      <c r="C55" s="78" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A56" s="79">
+        <v>42425</v>
+      </c>
+      <c r="B56" s="78" t="s">
+        <v>280</v>
+      </c>
+      <c r="C56" s="78" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>42424</v>
+      </c>
+      <c r="B57" s="100" t="s">
+        <v>239</v>
+      </c>
+      <c r="C57" s="100" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
         <v>42423</v>
       </c>
-      <c r="B55" s="78" t="s">
+      <c r="B58" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="79">
+        <v>42423</v>
+      </c>
+      <c r="B59" s="78" t="s">
         <v>282</v>
       </c>
-      <c r="C55" s="78" t="s">
+      <c r="C59" s="78" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+    <row r="60" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
         <v>42422</v>
       </c>
-      <c r="B56" s="100" t="s">
+      <c r="B60" s="100" t="s">
         <v>236</v>
       </c>
-      <c r="C56" s="100" t="s">
+      <c r="C60" s="100" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+    <row r="61" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
         <v>42419</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B61" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="C57" s="36" t="s">
+      <c r="C61" s="36" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="189" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+    <row r="62" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
         <v>42418</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B62" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C62" s="18" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
-        <v>42403</v>
-      </c>
-      <c r="B59" s="96" t="s">
-        <v>229</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
-        <v>42403</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
-        <v>42403</v>
-      </c>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>42398</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B63" s="96" t="s">
+        <v>229</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
         <v>42398</v>
       </c>
-      <c r="B63" s="12" t="s">
+      <c r="B66" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>42398</v>
+      </c>
+      <c r="B67" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C67" s="12" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
         <v>42397</v>
       </c>
-      <c r="B64" s="96" t="s">
+      <c r="B68" s="96" t="s">
         <v>201</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C68" s="14" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
-        <v>42396</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
-        <v>42396</v>
-      </c>
-      <c r="B66" s="96" t="s">
-        <v>39</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="128.25" x14ac:dyDescent="0.25">
-      <c r="A67" s="79">
-        <v>42386</v>
-      </c>
-      <c r="B67" s="78" t="s">
-        <v>284</v>
-      </c>
-      <c r="C67" s="78" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="79">
-        <v>42386</v>
-      </c>
-      <c r="B68" s="78" t="s">
-        <v>286</v>
-      </c>
-      <c r="C68" s="78" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>42384</v>
-      </c>
-      <c r="B69" s="100" t="s">
-        <v>220</v>
-      </c>
-      <c r="C69" s="100" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+        <v>42396</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>42382</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>219</v>
+        <v>42396</v>
+      </c>
+      <c r="B70" s="96" t="s">
+        <v>39</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="64.5" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A71" s="79">
-        <v>42382</v>
+        <v>42386</v>
       </c>
       <c r="B71" s="78" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C71" s="78" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
-        <v>42381</v>
-      </c>
-      <c r="B72" s="100" t="s">
-        <v>216</v>
-      </c>
-      <c r="C72" s="100" t="s">
-        <v>217</v>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="79">
+        <v>42386</v>
+      </c>
+      <c r="B72" s="78" t="s">
+        <v>286</v>
+      </c>
+      <c r="C72" s="78" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
+        <v>42384</v>
+      </c>
+      <c r="B73" s="100" t="s">
+        <v>220</v>
+      </c>
+      <c r="C73" s="100" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>42382</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="79">
+        <v>42382</v>
+      </c>
+      <c r="B75" s="78" t="s">
+        <v>288</v>
+      </c>
+      <c r="C75" s="78" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>42381</v>
+      </c>
+      <c r="B76" s="100" t="s">
+        <v>216</v>
+      </c>
+      <c r="C76" s="100" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
         <v>42380</v>
       </c>
-      <c r="B73" s="16" t="s">
+      <c r="B77" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C73" s="16" t="s">
+      <c r="C77" s="16" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
+    <row r="78" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
         <v>42380</v>
       </c>
-      <c r="B74" s="50" t="s">
+      <c r="B78" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C74" s="17" t="s">
+      <c r="C78" s="17" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="189" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
+    <row r="79" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
         <v>42380</v>
       </c>
-      <c r="B75" s="50" t="s">
+      <c r="B79" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C75" s="18" t="s">
+      <c r="C79" s="18" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="230.25" x14ac:dyDescent="0.25">
-      <c r="A76" s="79">
+    <row r="80" spans="1:3" ht="230.25" x14ac:dyDescent="0.25">
+      <c r="A80" s="79">
         <v>42380</v>
       </c>
-      <c r="B76" s="78" t="s">
+      <c r="B80" s="78" t="s">
         <v>289</v>
       </c>
-      <c r="C76" s="78" t="s">
+      <c r="C80" s="78" t="s">
         <v>290</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="102.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B77" s="78" t="s">
-        <v>292</v>
-      </c>
-      <c r="C77" s="78" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="102.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B78" s="78" t="s">
-        <v>294</v>
-      </c>
-      <c r="C78" s="78" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="128.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B79" s="78" t="s">
-        <v>298</v>
-      </c>
-      <c r="C79" s="78" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B80" s="78" t="s">
-        <v>298</v>
-      </c>
-      <c r="C80" s="78" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="102.75" x14ac:dyDescent="0.25">
@@ -4530,1037 +4521,1037 @@
         <v>42378</v>
       </c>
       <c r="B81" s="78" t="s">
+        <v>292</v>
+      </c>
+      <c r="C81" s="78" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="102.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B82" s="78" t="s">
+        <v>294</v>
+      </c>
+      <c r="C82" s="78" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A83" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B83" s="78" t="s">
+        <v>298</v>
+      </c>
+      <c r="C83" s="78" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A84" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B84" s="78" t="s">
+        <v>298</v>
+      </c>
+      <c r="C84" s="78" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="102.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B85" s="78" t="s">
         <v>296</v>
       </c>
-      <c r="C81" s="78" t="s">
+      <c r="C85" s="78" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="63" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+    <row r="86" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
         <v>42377</v>
       </c>
-      <c r="B82" s="100" t="s">
+      <c r="B86" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="C82" s="100" t="s">
+      <c r="C86" s="100" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="79">
+    <row r="87" spans="1:3" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A87" s="79">
         <v>42376</v>
       </c>
-      <c r="B83" s="78" t="s">
+      <c r="B87" s="78" t="s">
         <v>301</v>
       </c>
-      <c r="C83" s="78" t="s">
+      <c r="C87" s="78" t="s">
         <v>300</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
-        <v>42375</v>
-      </c>
-      <c r="B84" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C84" s="100" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
-        <v>42369</v>
-      </c>
-      <c r="B85" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="C85" s="19" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="189" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
-        <v>42368</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C86" s="19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="126" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
-        <v>42368</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C87" s="20" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>42368</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C88" s="20" t="s">
-        <v>208</v>
+        <v>42375</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88" s="100" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
+        <v>42369</v>
+      </c>
+      <c r="B89" s="100" t="s">
+        <v>202</v>
+      </c>
+      <c r="C89" s="19" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>42368</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C90" s="19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>42368</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C91" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>42368</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C92" s="20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
         <v>42366</v>
       </c>
-      <c r="B89" s="20" t="s">
+      <c r="B93" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C89" s="20" t="s">
+      <c r="C93" s="20" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
-        <v>42366</v>
-      </c>
-      <c r="B90" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C90" s="20" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
-        <v>42361</v>
-      </c>
-      <c r="C91" s="20" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
-        <v>42361</v>
-      </c>
-      <c r="C92" s="20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="283.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
-        <v>42361</v>
-      </c>
-      <c r="B93" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C93" s="22" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>42361</v>
-      </c>
-      <c r="B94" s="100" t="s">
-        <v>53</v>
+        <v>42366</v>
+      </c>
+      <c r="B94" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="C94" s="20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>42361</v>
       </c>
-      <c r="B95" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C95" s="21" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="236.25" x14ac:dyDescent="0.25">
+      <c r="C95" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>42361</v>
       </c>
-      <c r="B96" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C96" s="22" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="C96" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="283.5" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>42361</v>
       </c>
-      <c r="B97" s="100" t="s">
-        <v>49</v>
+      <c r="B97" s="35" t="s">
+        <v>186</v>
       </c>
       <c r="C97" s="22" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>42361</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C98" s="22" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="B98" s="100" t="s">
+        <v>53</v>
+      </c>
+      <c r="C98" s="20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>42361</v>
       </c>
-      <c r="B99" s="24" t="s">
+      <c r="B99" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C99" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="236.25" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B100" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C100" s="22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B101" s="100" t="s">
+        <v>49</v>
+      </c>
+      <c r="C101" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C99" s="24" t="s">
+      <c r="C102" s="22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B103" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C103" s="24" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="40">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="40">
         <v>42360</v>
       </c>
-      <c r="B100" s="50" t="s">
+      <c r="B104" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C104" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="40">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="40">
         <v>42360</v>
       </c>
-      <c r="B101" s="50" t="s">
+      <c r="B105" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C105" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="102.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="80">
+    <row r="106" spans="1:3" ht="102.75" x14ac:dyDescent="0.25">
+      <c r="A106" s="80">
         <v>42360</v>
       </c>
-      <c r="B102" s="78" t="s">
+      <c r="B106" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="C102" s="78" t="s">
+      <c r="C106" s="78" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A103" s="2">
+    <row r="107" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
         <v>42356</v>
       </c>
-      <c r="B103" s="100" t="s">
+      <c r="B107" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="C103" s="100" t="s">
+      <c r="C107" s="100" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B104" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="C104" s="23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B105" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="C105" s="25" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A106" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B106" s="96"/>
-      <c r="C106" s="25" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A107" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B107" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="C107" s="26" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B108" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C108" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+        <v>42356</v>
+      </c>
+      <c r="B108" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="C108" s="23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B109" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C109" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+        <v>42356</v>
+      </c>
+      <c r="B109" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C109" s="25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B110" s="100" t="s">
-        <v>168</v>
-      </c>
-      <c r="C110" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>42356</v>
+      </c>
+      <c r="B110" s="96"/>
+      <c r="C110" s="25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>42355</v>
       </c>
       <c r="B111" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C111" s="28" t="s">
-        <v>169</v>
+        <v>91</v>
+      </c>
+      <c r="C111" s="26" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>42355</v>
       </c>
-      <c r="B112" s="29" t="s">
-        <v>171</v>
+      <c r="B112" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="C112" s="29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>42355</v>
       </c>
-      <c r="B113" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C113" s="29" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="B113" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C113" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>42355</v>
       </c>
       <c r="B114" s="100" t="s">
-        <v>173</v>
-      </c>
-      <c r="C114" s="29" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="C114" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>42355</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C115" s="42" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B115" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C115" s="28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>42355</v>
       </c>
-      <c r="B116" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C116" s="30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B116" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C116" s="29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>42355</v>
       </c>
-      <c r="C117" s="30" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B117" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C117" s="29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>42355</v>
       </c>
-      <c r="B118" s="42"/>
-      <c r="C118" s="30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B118" s="100" t="s">
+        <v>173</v>
+      </c>
+      <c r="C118" s="29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>42355</v>
       </c>
-      <c r="B119" s="42"/>
-      <c r="C119" s="30" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="B119" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C119" s="42" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B120" s="42" t="s">
-        <v>189</v>
+        <v>42355</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="C120" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B121" s="26"/>
-      <c r="C121" s="31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+        <v>42355</v>
+      </c>
+      <c r="C121" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B122" s="26"/>
-      <c r="C122" s="70" t="s">
-        <v>66</v>
+        <v>42355</v>
+      </c>
+      <c r="B122" s="42"/>
+      <c r="C122" s="30" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B123" s="26"/>
-      <c r="C123" s="32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42355</v>
+      </c>
+      <c r="B123" s="42"/>
+      <c r="C123" s="30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>42352</v>
       </c>
-      <c r="B124" s="96"/>
-      <c r="C124" s="33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B124" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C124" s="30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>42352</v>
       </c>
-      <c r="B125" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C125" s="34" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B125" s="26"/>
+      <c r="C125" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>42352</v>
       </c>
-      <c r="B126" s="96"/>
-      <c r="C126" s="34" t="s">
-        <v>73</v>
+      <c r="B126" s="26"/>
+      <c r="C126" s="70" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>42352</v>
       </c>
-      <c r="B127" s="96"/>
-      <c r="C127" s="37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B127" s="26"/>
+      <c r="C127" s="32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>42352</v>
       </c>
-      <c r="B128" s="37"/>
-      <c r="C128" s="37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B128" s="96"/>
+      <c r="C128" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>42352</v>
       </c>
-      <c r="B129" s="96"/>
-      <c r="C129" s="96" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B129" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C129" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>42352</v>
       </c>
-      <c r="B130" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C130" s="96" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B130" s="96"/>
+      <c r="C130" s="34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>42352</v>
       </c>
-      <c r="B131" s="100"/>
-      <c r="C131" s="39" t="s">
-        <v>80</v>
+      <c r="B131" s="96"/>
+      <c r="C131" s="37" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>42352</v>
       </c>
-      <c r="B132" s="38"/>
-      <c r="C132" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="F132" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B132" s="37"/>
+      <c r="C132" s="37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>42352</v>
       </c>
-      <c r="B133" s="41"/>
-      <c r="C133" s="41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B133" s="96"/>
+      <c r="C133" s="96" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>42352</v>
       </c>
-      <c r="B134" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C134" s="41" t="s">
-        <v>90</v>
+      <c r="B134" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C134" s="96" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>42352</v>
       </c>
-      <c r="B135" s="43"/>
-      <c r="C135" s="43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B135" s="100"/>
+      <c r="C135" s="39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>42352</v>
       </c>
-      <c r="B136" s="44"/>
-      <c r="C136" s="44" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B136" s="38"/>
+      <c r="C136" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="F136" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>42352</v>
       </c>
-      <c r="B137" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="C137" s="46" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B137" s="41"/>
+      <c r="C137" s="41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>42352</v>
       </c>
-      <c r="B138" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C138" s="47" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B138" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C138" s="41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>42352</v>
       </c>
-      <c r="B139" s="100" t="s">
+      <c r="B139" s="43"/>
+      <c r="C139" s="43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B140" s="44"/>
+      <c r="C140" s="44" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B141" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C141" s="46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B142" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C142" s="47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B143" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="C139" s="48" t="s">
+      <c r="C143" s="48" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A140" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B140" s="49"/>
-      <c r="C140" s="49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" ht="63" x14ac:dyDescent="0.25">
-      <c r="A141" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B141" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="C141" s="51" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B142" s="96"/>
-      <c r="C142" s="53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A143" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B143" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C143" s="53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>42349</v>
       </c>
-      <c r="B144" s="52"/>
-      <c r="C144" s="52" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B144" s="49"/>
+      <c r="C144" s="49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>42349</v>
       </c>
-      <c r="B145" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C145" s="54" t="s">
-        <v>60</v>
+      <c r="B145" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C145" s="51" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>42349</v>
       </c>
-      <c r="B146" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C146" s="55" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B146" s="96"/>
+      <c r="C146" s="53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>42349</v>
       </c>
-      <c r="B147" s="100"/>
-      <c r="C147" s="57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B147" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C147" s="53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>42349</v>
       </c>
-      <c r="B148" s="58"/>
-      <c r="C148" s="58" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B148" s="52"/>
+      <c r="C148" s="52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>42349</v>
       </c>
-      <c r="B149" s="59"/>
-      <c r="C149" s="59" t="s">
-        <v>70</v>
+      <c r="B149" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C149" s="54" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>42349</v>
       </c>
-      <c r="B150" s="60"/>
-      <c r="C150" s="60" t="s">
-        <v>64</v>
+      <c r="B150" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C150" s="55" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>42349</v>
       </c>
-      <c r="B151" s="61"/>
-      <c r="C151" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="B151" s="100"/>
+      <c r="C151" s="57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>42349</v>
       </c>
-      <c r="B152" s="62" t="s">
-        <v>168</v>
-      </c>
-      <c r="C152" s="100" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="B152" s="58"/>
+      <c r="C152" s="58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B153" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C153" s="62" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>42349</v>
+      </c>
+      <c r="B153" s="59"/>
+      <c r="C153" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C154" s="62" t="s">
-        <v>36</v>
+        <v>42349</v>
+      </c>
+      <c r="B154" s="60"/>
+      <c r="C154" s="60" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B155" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C155" s="63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42349</v>
+      </c>
+      <c r="B155" s="61"/>
+      <c r="C155" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B156" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C156" s="64" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>42349</v>
+      </c>
+      <c r="B156" s="62" t="s">
+        <v>168</v>
+      </c>
+      <c r="C156" s="100" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>42345</v>
       </c>
-      <c r="B157" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C157" s="65" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+      <c r="B157" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C157" s="62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>42345</v>
       </c>
-      <c r="B158" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C158" s="66" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="B158" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C158" s="62" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>42345</v>
       </c>
-      <c r="B159" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="C159" s="67" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B159" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C159" s="63" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>42345</v>
       </c>
-      <c r="B160" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="C160" s="68" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B160" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C160" s="64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>42345</v>
       </c>
-      <c r="B161" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C161" s="69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B161" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C161" s="65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>42345</v>
       </c>
-      <c r="B162" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C162" s="73" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B162" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C162" s="66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>42345</v>
       </c>
-      <c r="B163" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="C163" s="73" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B163" s="100" t="s">
+        <v>31</v>
+      </c>
+      <c r="C163" s="67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>42345</v>
       </c>
-      <c r="B164" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="C164" s="73" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B164" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C164" s="68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>42345</v>
       </c>
-      <c r="B165" s="96" t="s">
-        <v>39</v>
-      </c>
-      <c r="C165" s="73" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="B165" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C165" s="69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>42345</v>
       </c>
-      <c r="B166" s="15" t="s">
-        <v>43</v>
+      <c r="B166" s="100" t="s">
+        <v>12</v>
       </c>
       <c r="C166" s="73" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>42345</v>
       </c>
-      <c r="B167" s="100" t="s">
+      <c r="B167" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="C167" s="76" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="C167" s="73" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>42345</v>
       </c>
-      <c r="B168" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C168" s="77" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="B168" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C168" s="73" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>42345</v>
       </c>
-      <c r="B169" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B169" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="C169" s="73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>42345</v>
       </c>
-      <c r="B170" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C170" s="96" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B170" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C170" s="73" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>42345</v>
       </c>
-      <c r="B171" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C171" s="96" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B171" s="100" t="s">
+        <v>39</v>
+      </c>
+      <c r="C171" s="76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>42345</v>
       </c>
-      <c r="B172" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C172" s="96" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B172" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C172" s="77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>42345</v>
       </c>
-      <c r="B173" s="96" t="s">
+      <c r="B173" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B174" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C174" s="96" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B175" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C175" s="96" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B176" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C176" s="96" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B177" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C173" s="96" t="s">
+      <c r="C177" s="96" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="141" x14ac:dyDescent="0.25">
-      <c r="A174" s="80">
+    <row r="178" spans="1:3" ht="141" x14ac:dyDescent="0.25">
+      <c r="A178" s="80">
         <v>42345</v>
       </c>
-      <c r="B174" s="78" t="s">
+      <c r="B178" s="78" t="s">
         <v>304</v>
       </c>
-      <c r="C174" s="78" t="s">
+      <c r="C178" s="78" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A175" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C175" s="100" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A176" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C176" s="96" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A177" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C177" s="96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A178" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C178" s="96" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>42341</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C179" s="96" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C179" s="100" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>42341</v>
       </c>
@@ -5568,18 +5559,18 @@
         <v>15</v>
       </c>
       <c r="C180" s="96" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>42341</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C181" s="96" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -5590,10 +5581,10 @@
         <v>15</v>
       </c>
       <c r="C182" s="96" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>42341</v>
       </c>
@@ -5601,10 +5592,10 @@
         <v>15</v>
       </c>
       <c r="C183" s="96" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>42341</v>
       </c>
@@ -5612,73 +5603,73 @@
         <v>15</v>
       </c>
       <c r="C184" s="96" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>42341</v>
       </c>
-      <c r="B185" s="100" t="s">
-        <v>12</v>
+      <c r="B185" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C185" s="96" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>42341</v>
       </c>
-      <c r="B186" s="96" t="s">
+      <c r="B186" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C186" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>42341</v>
       </c>
-      <c r="B187" s="96" t="s">
-        <v>12</v>
+      <c r="B187" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C187" s="96" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>42341</v>
       </c>
-      <c r="B188" s="96" t="s">
+      <c r="B188" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C188" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C188" s="96" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>42341</v>
       </c>
-      <c r="B189" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C189" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B189" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C189" s="96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>42341</v>
       </c>
       <c r="B190" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C190" s="8" t="s">
-        <v>165</v>
+      <c r="C190" s="96" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -5686,309 +5677,353 @@
         <v>42341</v>
       </c>
       <c r="B191" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C191" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C191" s="96" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>42341</v>
       </c>
       <c r="B192" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C192" s="100" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="C192" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>42341</v>
       </c>
       <c r="B193" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C193" s="96" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C193" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B194" s="96"/>
-      <c r="C194" s="96" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>42341</v>
+      </c>
+      <c r="B194" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C194" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B195" s="96"/>
-      <c r="C195" s="96" t="s">
-        <v>8</v>
+        <v>42341</v>
+      </c>
+      <c r="B195" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C195" s="8" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B196" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C196" s="100" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B197" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C197" s="96" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
         <v>42340</v>
       </c>
-      <c r="B196" s="2" t="s">
+      <c r="B198" s="96"/>
+      <c r="C198" s="96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B199" s="96"/>
+      <c r="C199" s="96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B200" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C196" s="96" t="s">
+      <c r="C200" s="96" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="2">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
         <v>42339</v>
       </c>
-      <c r="B197" s="2"/>
-      <c r="C197" s="96" t="s">
+      <c r="B201" s="2"/>
+      <c r="C201" s="96" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" s="2">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
         <v>42339</v>
       </c>
-      <c r="B198" s="2"/>
-      <c r="C198" s="96" t="s">
+      <c r="B202" s="2"/>
+      <c r="C202" s="96" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A199" s="80">
+    <row r="203" spans="1:3" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A203" s="80">
         <v>42334</v>
       </c>
-      <c r="B199" s="78" t="s">
+      <c r="B203" s="78" t="s">
         <v>310</v>
       </c>
-      <c r="C199" s="78" t="s">
+      <c r="C203" s="78" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A200" s="80">
+    <row r="204" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A204" s="80">
         <v>42334</v>
       </c>
-      <c r="B200" s="78" t="s">
+      <c r="B204" s="78" t="s">
         <v>308</v>
       </c>
-      <c r="C200" s="78" t="s">
+      <c r="C204" s="78" t="s">
         <v>307</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A201" s="80">
-        <v>42334</v>
-      </c>
-      <c r="B201" s="78" t="s">
-        <v>273</v>
-      </c>
-      <c r="C201" s="78" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="128.25" x14ac:dyDescent="0.25">
-      <c r="A202" s="80">
-        <v>42333</v>
-      </c>
-      <c r="B202" s="78" t="s">
-        <v>269</v>
-      </c>
-      <c r="C202" s="78" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A203" s="80">
-        <v>42333</v>
-      </c>
-      <c r="B203" s="78" t="s">
-        <v>216</v>
-      </c>
-      <c r="C203" s="78" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="80">
-        <v>42331</v>
-      </c>
-      <c r="B204" s="78" t="s">
-        <v>314</v>
-      </c>
-      <c r="C204" s="78" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A205" s="80">
+        <v>42334</v>
+      </c>
+      <c r="B205" s="78" t="s">
+        <v>273</v>
+      </c>
+      <c r="C205" s="78" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A206" s="80">
+        <v>42333</v>
+      </c>
+      <c r="B206" s="78" t="s">
+        <v>269</v>
+      </c>
+      <c r="C206" s="78" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A207" s="80">
+        <v>42333</v>
+      </c>
+      <c r="B207" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="C207" s="78" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="80">
+        <v>42331</v>
+      </c>
+      <c r="B208" s="78" t="s">
+        <v>314</v>
+      </c>
+      <c r="C208" s="78" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A209" s="80">
         <v>42329</v>
       </c>
-      <c r="B205" s="78" t="s">
+      <c r="B209" s="78" t="s">
         <v>316</v>
       </c>
-      <c r="C205" s="78" t="s">
+      <c r="C209" s="78" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A206" s="80">
-        <v>42328</v>
-      </c>
-      <c r="B206" s="78" t="s">
-        <v>325</v>
-      </c>
-      <c r="C206" s="78" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A207" s="80">
-        <v>42328</v>
-      </c>
-      <c r="B207" s="78" t="s">
-        <v>323</v>
-      </c>
-      <c r="C207" s="78" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="102.75" x14ac:dyDescent="0.25">
-      <c r="A208" s="80">
-        <v>42328</v>
-      </c>
-      <c r="B208" s="78" t="s">
-        <v>321</v>
-      </c>
-      <c r="C208" s="78" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A209" s="80">
-        <v>42328</v>
-      </c>
-      <c r="B209" s="78" t="s">
-        <v>318</v>
-      </c>
-      <c r="C209" s="78" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" ht="141" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A210" s="80">
         <v>42328</v>
       </c>
       <c r="B210" s="78" t="s">
+        <v>325</v>
+      </c>
+      <c r="C210" s="78" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A211" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B211" s="78" t="s">
+        <v>323</v>
+      </c>
+      <c r="C211" s="78" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="102.75" x14ac:dyDescent="0.25">
+      <c r="A212" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B212" s="78" t="s">
+        <v>321</v>
+      </c>
+      <c r="C212" s="78" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A213" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B213" s="78" t="s">
         <v>318</v>
       </c>
-      <c r="C210" s="78" t="s">
+      <c r="C213" s="78" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" ht="141" x14ac:dyDescent="0.25">
+      <c r="A214" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B214" s="78" t="s">
+        <v>318</v>
+      </c>
+      <c r="C214" s="78" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A211" s="80">
+    <row r="215" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A215" s="80">
         <v>42324</v>
       </c>
-      <c r="B211" s="78" t="s">
+      <c r="B215" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="C211" s="78" t="s">
+      <c r="C215" s="78" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A212" s="80">
+    <row r="216" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A216" s="80">
         <v>42321</v>
       </c>
-      <c r="B212" s="78" t="s">
+      <c r="B216" s="78" t="s">
         <v>328</v>
       </c>
-      <c r="C212" s="78" t="s">
+      <c r="C216" s="78" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A213" s="80">
+    <row r="217" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A217" s="80">
         <v>42321</v>
       </c>
-      <c r="B213" s="78" t="s">
+      <c r="B217" s="78" t="s">
         <v>328</v>
       </c>
-      <c r="C213" s="78" t="s">
+      <c r="C217" s="78" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A214" s="79">
+    <row r="218" spans="1:3" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A218" s="79">
         <v>42318</v>
       </c>
-      <c r="B214" s="78" t="s">
+      <c r="B218" s="78" t="s">
         <v>331</v>
       </c>
-      <c r="C214" s="78" t="s">
+      <c r="C218" s="78" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
-      <c r="A215" s="79">
+    <row r="219" spans="1:3" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A219" s="79">
         <v>42311</v>
       </c>
-      <c r="B215" s="78" t="s">
+      <c r="B219" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C215" s="78" t="s">
+      <c r="C219" s="78" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A216" s="79">
+    <row r="220" spans="1:3" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A220" s="79">
         <v>42310</v>
       </c>
-      <c r="B216" s="78" t="s">
+      <c r="B220" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C216" s="78" t="s">
+      <c r="C220" s="78" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A217" s="79">
+    <row r="221" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A221" s="79">
         <v>42306</v>
       </c>
-      <c r="B217" s="78" t="s">
+      <c r="B221" s="78" t="s">
         <v>334</v>
       </c>
-      <c r="C217" s="78" t="s">
+      <c r="C221" s="78" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A218" s="100"/>
-      <c r="B218" s="100"/>
-      <c r="C218" s="100"/>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="100"/>
+      <c r="B222" s="100"/>
+      <c r="C222" s="100"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C218">
+  <autoFilter ref="A1:C222">
     <sortState ref="A2:C201">
       <sortCondition descending="1" ref="A1:A201"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C190" r:id="rId1"/>
-    <hyperlink ref="C151" r:id="rId2"/>
-    <hyperlink ref="C191" r:id="rId3"/>
-    <hyperlink ref="C25" r:id="rId4"/>
-    <hyperlink ref="C10" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C194" r:id="rId1"/>
+    <hyperlink ref="C155" r:id="rId2"/>
+    <hyperlink ref="C195" r:id="rId3"/>
+    <hyperlink ref="C29" r:id="rId4"/>
+    <hyperlink ref="C14" r:id="rId5"/>
+    <hyperlink ref="C11" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -6007,16 +6042,16 @@
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add aandroid studio install message note
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="532">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -2729,6 +2729,21 @@
 2. 於UEFI找到Intel Virtualiztion Technology (有時Wording不一樣, 如VTX等)Enable佢
 3. F10 Save and Restart 就可以了
 且另外誤打誤撞, 在Enable完VTX後之前行不了的VMWare player也可以運行kali linus了!</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android Studio</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android Studio安裝時之MSG:
+C:\Program Files\Android\Android Studio
+Android SDK Installation Location:
+C:\Users\user\AppData\Local\Android\sdk
+Running Intel® HAXM installer
+HAXM installation failed. To install HAXM follow the instructions found at: https://software.intel.com/android/articles/installation-instructions-for-intel-hardware-accelerated-execution-manager-windowsCreating Android virtual device
+Unable to create a virtual device: Unable to create Android virtual device
+p.s 要安裝HAXM, 需到SDK Manager的SDK Tool中勾選installer並安裝.</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -3781,7 +3796,7 @@
   <dimension ref="A1:F231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3807,10 +3822,14 @@
       <c r="B2" s="100"/>
       <c r="C2" s="100"/>
     </row>
-    <row r="3" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="102" customFormat="1" ht="189" x14ac:dyDescent="0.25">
       <c r="A3" s="120"/>
-      <c r="B3" s="120"/>
-      <c r="C3" s="120"/>
+      <c r="B3" s="120" t="s">
+        <v>530</v>
+      </c>
+      <c r="C3" s="120" t="s">
+        <v>531</v>
+      </c>
     </row>
     <row r="4" spans="1:3" s="102" customFormat="1" ht="126" x14ac:dyDescent="0.25">
       <c r="A4" s="2">

</xml_diff>

<commit_message>
Add indexs and maven
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -15,14 +15,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'AS400 Version'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$233</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$237</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="542">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -2744,6 +2744,48 @@
   </si>
   <si>
     <t xml:space="preserve">在兩三周前看完了這本英文書, 感覺世界改變, 對於很多網絡安全的事情清淅了也更恐懼, 就像初入行的小醫生看到處處都是病機一樣的感覺. 書大概介紹了Kali linux, Metasploit, 各種Module及其相容Payload, 市面上(見光的) 漏洞數據庫. 又順道介紹了小工具如Netcat, nmap, wireshark, 等等, man-in-the-middle原理, stack-overflow-attack原理等等. 分兩個入侵理念的server side attack和client side attack.. Wireless hacking及Mobile Hacking都有講解. </t>
+  </si>
+  <si>
+    <t>docker</t>
+  </si>
+  <si>
+    <t>Popular server-end open-source tools</t>
+  </si>
+  <si>
+    <t>Spark the neat web app framework</t>
+  </si>
+  <si>
+    <t>Android concept</t>
+  </si>
+  <si>
+    <t>Android is a smart phone framework build on Linux, different managers live in the framework and collaborate android behavior. Every app run on the system is build seperately and each has 4 main componenet:
+1. Activity 
+2. Service
+3. Content provider
+4. Broadcast provider
+The interaction between each components are carried by the Intent system. I am working on a notebook for android developemnt learning. Detail refers to it.</t>
+  </si>
+  <si>
+    <t>Spark web framework(java) is always confused with the apcahe spark (which is a distributed storage strategy). Spark is a simple web framework and it can run alone as the web server itself to listen on ports and return informations.
+* It can also work with servers such as tomcat.</t>
+  </si>
+  <si>
+    <t>In the "Docker book", I learn about these useful tools:
+1. Redis: A key-pair database
+2. Sanatra: A server tool to receive http request and JSONize parameter.
+3. Jenkins: 管家for continural integration
+4. Jekyll: 化身博士 for css/ content seperated website/blog builder.</t>
+  </si>
+  <si>
+    <t>* Main component:
+    1. Docker file: The author, the environment vars, the action, the entrypoint, etc.
+* Deployment process:
+    1. Build the container using docker command
+    2. Run the container with docker command(定何port, 何卷, 連接, priviledge等)
+* Docker important feature:
+    1. Volume(卷): A way to mount a folder to container from host machine(this allows awesome code-environ seperation)
+    2. Link(連接): Simulate a LAN within the host machine and containers so that the communication is secured.
+    3. Priviledge: Grant priviledge to container to run docker on itself recursively.</t>
   </si>
 </sst>
 </file>
@@ -3428,10 +3470,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3466,13 +3508,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4202207</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>593914</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>414618</xdr:colOff>
-      <xdr:row>124</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>102264</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3789,16 +3831,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F233"/>
+  <dimension ref="A1:F237"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" customWidth="1"/>
     <col min="3" max="3" width="77" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3818,1023 +3860,1023 @@
       <c r="B2" s="100"/>
       <c r="C2" s="100"/>
     </row>
-    <row r="3" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A3" s="122">
+    <row r="3" spans="1:3" s="102" customFormat="1" ht="135">
+      <c r="A3" s="121">
+        <v>42562</v>
+      </c>
+      <c r="B3" s="120" t="s">
+        <v>537</v>
+      </c>
+      <c r="C3" s="120" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A4" s="121">
+        <v>42562</v>
+      </c>
+      <c r="B4" s="120" t="s">
+        <v>536</v>
+      </c>
+      <c r="C4" s="120" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="102" customFormat="1" ht="75">
+      <c r="A5" s="121">
+        <v>42562</v>
+      </c>
+      <c r="B5" s="120" t="s">
+        <v>535</v>
+      </c>
+      <c r="C5" s="120" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="102" customFormat="1" ht="165">
+      <c r="A6" s="121">
+        <v>42562</v>
+      </c>
+      <c r="B6" s="120" t="s">
+        <v>534</v>
+      </c>
+      <c r="C6" s="120" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A7" s="121">
         <v>42557</v>
       </c>
-      <c r="B3" s="121" t="s">
+      <c r="B7" s="120" t="s">
         <v>525</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="C7" s="120" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="102" customFormat="1" ht="180">
-      <c r="A4" s="121"/>
-      <c r="B4" s="121" t="s">
+    <row r="8" spans="1:3" s="102" customFormat="1" ht="180">
+      <c r="A8" s="120"/>
+      <c r="B8" s="120" t="s">
         <v>527</v>
       </c>
-      <c r="C4" s="121" t="s">
+      <c r="C8" s="120" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="102" customFormat="1" ht="165">
-      <c r="A5" s="122">
+    <row r="9" spans="1:3" s="102" customFormat="1" ht="150">
+      <c r="A9" s="121">
         <v>42540</v>
       </c>
-      <c r="B5" s="121" t="s">
+      <c r="B9" s="120" t="s">
         <v>529</v>
       </c>
-      <c r="C5" s="121" t="s">
+      <c r="C9" s="120" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="102" customFormat="1" ht="180">
-      <c r="A6" s="122">
+    <row r="10" spans="1:3" s="102" customFormat="1" ht="180">
+      <c r="A10" s="121">
         <v>42539</v>
       </c>
-      <c r="B6" s="121" t="s">
+      <c r="B10" s="120" t="s">
         <v>527</v>
       </c>
-      <c r="C6" s="121" t="s">
+      <c r="C10" s="120" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A7" s="122">
+    <row r="11" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A11" s="121">
         <v>42539</v>
       </c>
-      <c r="B7" s="121" t="s">
+      <c r="B11" s="120" t="s">
         <v>532</v>
       </c>
-      <c r="C7" s="121" t="s">
+      <c r="C11" s="120" t="s">
         <v>533</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A8" s="2">
-        <v>42534</v>
-      </c>
-      <c r="B8" s="119" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="119" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A9" s="2">
-        <v>42517</v>
-      </c>
-      <c r="B9" s="118" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="118" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A10" s="2">
-        <v>42514</v>
-      </c>
-      <c r="B10" s="117" t="s">
-        <v>519</v>
-      </c>
-      <c r="C10" s="117" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A11" s="2">
-        <v>42507</v>
-      </c>
-      <c r="B11" s="116" t="s">
-        <v>519</v>
-      </c>
-      <c r="C11" s="116" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="102" customFormat="1" ht="60">
       <c r="A12" s="2">
+        <v>42534</v>
+      </c>
+      <c r="B12" s="119" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="119" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A13" s="2">
+        <v>42517</v>
+      </c>
+      <c r="B13" s="118" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="118" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A14" s="2">
+        <v>42514</v>
+      </c>
+      <c r="B14" s="117" t="s">
+        <v>519</v>
+      </c>
+      <c r="C14" s="117" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A15" s="2">
+        <v>42507</v>
+      </c>
+      <c r="B15" s="116" t="s">
+        <v>519</v>
+      </c>
+      <c r="C15" s="116" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A16" s="2">
         <v>42502</v>
       </c>
-      <c r="B12" s="115" t="s">
+      <c r="B16" s="115" t="s">
         <v>519</v>
       </c>
-      <c r="C12" s="116" t="s">
+      <c r="C16" s="116" t="s">
         <v>520</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A13" s="2">
-        <v>42485</v>
-      </c>
-      <c r="B13" s="113" t="s">
-        <v>516</v>
-      </c>
-      <c r="C13" s="113" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A14" s="2">
-        <v>42485</v>
-      </c>
-      <c r="B14" s="110" t="s">
-        <v>514</v>
-      </c>
-      <c r="C14" s="110" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="102" customFormat="1" ht="300">
-      <c r="A15" s="2">
-        <v>42485</v>
-      </c>
-      <c r="B15" s="112" t="s">
-        <v>241</v>
-      </c>
-      <c r="C15" s="112" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A16" s="2">
-        <v>42479</v>
-      </c>
-      <c r="B16" s="111" t="s">
-        <v>241</v>
-      </c>
-      <c r="C16" s="111" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="102" customFormat="1" ht="90">
       <c r="A17" s="2">
+        <v>42485</v>
+      </c>
+      <c r="B17" s="113" t="s">
+        <v>516</v>
+      </c>
+      <c r="C17" s="113" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A18" s="2">
+        <v>42485</v>
+      </c>
+      <c r="B18" s="110" t="s">
+        <v>514</v>
+      </c>
+      <c r="C18" s="110" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="102" customFormat="1" ht="300">
+      <c r="A19" s="2">
+        <v>42485</v>
+      </c>
+      <c r="B19" s="112" t="s">
+        <v>241</v>
+      </c>
+      <c r="C19" s="112" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="102" customFormat="1" ht="150">
+      <c r="A20" s="2">
+        <v>42479</v>
+      </c>
+      <c r="B20" s="111" t="s">
+        <v>241</v>
+      </c>
+      <c r="C20" s="111" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="A21" s="2">
         <v>42478</v>
       </c>
-      <c r="B17" s="110" t="s">
+      <c r="B21" s="110" t="s">
         <v>509</v>
       </c>
-      <c r="C17" s="110" t="s">
+      <c r="C21" s="110" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="102" customFormat="1" ht="120">
-      <c r="A18" s="2">
+    <row r="22" spans="1:3" s="102" customFormat="1" ht="120">
+      <c r="A22" s="2">
         <v>42477</v>
       </c>
-      <c r="B18" s="109" t="s">
+      <c r="B22" s="109" t="s">
         <v>509</v>
       </c>
-      <c r="C18" s="109" t="s">
+      <c r="C22" s="109" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A19" s="2">
+    <row r="23" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A23" s="2">
         <v>42477</v>
       </c>
-      <c r="B19" s="108" t="s">
+      <c r="B23" s="108" t="s">
         <v>507</v>
       </c>
-      <c r="C19" s="108" t="s">
+      <c r="C23" s="108" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="102" customFormat="1">
-      <c r="A20" s="2">
+    <row r="24" spans="1:3" s="102" customFormat="1">
+      <c r="A24" s="2">
         <v>42473</v>
       </c>
-      <c r="B20" s="106" t="s">
+      <c r="B24" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="106" t="s">
+      <c r="C24" s="106" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A21" s="2">
+    <row r="25" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A25" s="2">
         <v>42473</v>
       </c>
-      <c r="B21" s="106" t="s">
+      <c r="B25" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="107" t="s">
+      <c r="C25" s="107" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="102" customFormat="1">
-      <c r="A22" s="2">
+    <row r="26" spans="1:3" s="102" customFormat="1">
+      <c r="A26" s="2">
         <v>42469</v>
       </c>
-      <c r="B22" s="105" t="s">
+      <c r="B26" s="105" t="s">
         <v>504</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C26" s="8" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="102" customFormat="1" ht="75">
-      <c r="A23" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B23" s="104" t="s">
-        <v>497</v>
-      </c>
-      <c r="C23" s="104" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A24" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B24" s="104" t="s">
-        <v>499</v>
-      </c>
-      <c r="C24" s="104" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" s="102" customFormat="1">
-      <c r="A25" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B25" s="104" t="s">
-        <v>501</v>
-      </c>
-      <c r="C25" s="104" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A26" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B26" s="100" t="s">
-        <v>493</v>
-      </c>
-      <c r="C26" s="100" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="102" customFormat="1" ht="90">
+    <row r="27" spans="1:3" s="102" customFormat="1" ht="75">
       <c r="A27" s="2">
         <v>42463</v>
       </c>
-      <c r="B27" s="103" t="s">
-        <v>492</v>
-      </c>
-      <c r="C27" s="103" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="B27" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="C27" s="104" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="102" customFormat="1" ht="105">
       <c r="A28" s="2">
         <v>42463</v>
       </c>
-      <c r="B28" s="101" t="s">
-        <v>489</v>
-      </c>
-      <c r="C28" s="101" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="B28" s="104" t="s">
+        <v>499</v>
+      </c>
+      <c r="C28" s="104" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="102" customFormat="1">
       <c r="A29" s="2">
         <v>42463</v>
       </c>
-      <c r="B29" s="101" t="s">
-        <v>488</v>
-      </c>
-      <c r="C29" s="101" t="s">
-        <v>494</v>
+      <c r="B29" s="104" t="s">
+        <v>501</v>
+      </c>
+      <c r="C29" s="104" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="102" customFormat="1" ht="150">
       <c r="A30" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B30" s="100" t="s">
+        <v>493</v>
+      </c>
+      <c r="C30" s="100" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="A31" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B31" s="103" t="s">
+        <v>492</v>
+      </c>
+      <c r="C31" s="103" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A32" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B32" s="101" t="s">
+        <v>489</v>
+      </c>
+      <c r="C32" s="101" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A33" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B33" s="101" t="s">
+        <v>488</v>
+      </c>
+      <c r="C33" s="101" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="102" customFormat="1" ht="150">
+      <c r="A34" s="2">
         <v>42462</v>
       </c>
-      <c r="B30" s="100" t="s">
+      <c r="B34" s="100" t="s">
         <v>486</v>
       </c>
-      <c r="C30" s="100" t="s">
+      <c r="C34" s="100" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="102" customFormat="1" ht="135">
-      <c r="A31" s="2">
+    <row r="35" spans="1:3" s="102" customFormat="1" ht="135">
+      <c r="A35" s="2">
         <v>42462</v>
       </c>
-      <c r="B31" s="100" t="s">
+      <c r="B35" s="100" t="s">
         <v>484</v>
       </c>
-      <c r="C31" s="100" t="s">
+      <c r="C35" s="100" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="102" customFormat="1" ht="240">
-      <c r="A32" s="2">
+    <row r="36" spans="1:3" s="102" customFormat="1" ht="240">
+      <c r="A36" s="2">
         <v>42462</v>
       </c>
-      <c r="B32" s="100" t="s">
+      <c r="B36" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="C32" s="100" t="s">
+      <c r="C36" s="100" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="102" customFormat="1" ht="120">
-      <c r="A33" s="2">
+    <row r="37" spans="1:3" s="102" customFormat="1" ht="120">
+      <c r="A37" s="2">
         <v>42462</v>
       </c>
-      <c r="B33" s="100" t="s">
+      <c r="B37" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="C33" s="100" t="s">
+      <c r="C37" s="100" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="4" customFormat="1" ht="120">
-      <c r="A34" s="2">
+    <row r="38" spans="1:3" s="4" customFormat="1" ht="120">
+      <c r="A38" s="2">
         <v>42460</v>
       </c>
-      <c r="B34" s="99" t="s">
+      <c r="B38" s="99" t="s">
         <v>477</v>
       </c>
-      <c r="C34" s="99" t="s">
+      <c r="C38" s="99" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="4" customFormat="1" ht="30">
-      <c r="A35" s="2">
+    <row r="39" spans="1:3" s="4" customFormat="1" ht="30">
+      <c r="A39" s="2">
         <v>42460</v>
       </c>
-      <c r="B35" s="99" t="s">
+      <c r="B39" s="99" t="s">
         <v>476</v>
       </c>
-      <c r="C35" s="99" t="s">
+      <c r="C39" s="99" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="4" customFormat="1" ht="195">
-      <c r="A36" s="2">
+    <row r="40" spans="1:3" s="4" customFormat="1" ht="180">
+      <c r="A40" s="2">
         <v>42460</v>
       </c>
-      <c r="B36" s="99" t="s">
+      <c r="B40" s="99" t="s">
         <v>475</v>
       </c>
-      <c r="C36" s="99" t="s">
+      <c r="C40" s="99" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="4" customFormat="1" ht="60">
-      <c r="A37" s="2">
+    <row r="41" spans="1:3" s="4" customFormat="1" ht="60">
+      <c r="A41" s="2">
         <v>42460</v>
       </c>
-      <c r="B37" s="99" t="s">
+      <c r="B41" s="99" t="s">
         <v>478</v>
       </c>
-      <c r="C37" s="99" t="s">
+      <c r="C41" s="99" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="4" customFormat="1" ht="105">
-      <c r="A38" s="2">
+    <row r="42" spans="1:3" s="4" customFormat="1" ht="105">
+      <c r="A42" s="2">
         <v>42459</v>
       </c>
-      <c r="B38" s="99" t="s">
+      <c r="B42" s="99" t="s">
         <v>470</v>
       </c>
-      <c r="C38" s="98" t="s">
+      <c r="C42" s="98" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="4" customFormat="1" ht="60">
-      <c r="A39" s="2">
+    <row r="43" spans="1:3" s="4" customFormat="1" ht="60">
+      <c r="A43" s="2">
         <v>42459</v>
       </c>
-      <c r="B39" s="99" t="s">
+      <c r="B43" s="99" t="s">
         <v>241</v>
       </c>
-      <c r="C39" s="99" t="s">
+      <c r="C43" s="99" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="4" customFormat="1">
-      <c r="A40" s="2">
+    <row r="44" spans="1:3" s="4" customFormat="1">
+      <c r="A44" s="2">
         <v>42458</v>
       </c>
-      <c r="B40" s="97" t="s">
+      <c r="B44" s="97" t="s">
         <v>470</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C44" s="8" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="4" customFormat="1" ht="105">
-      <c r="A41" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B41" s="96" t="s">
-        <v>254</v>
-      </c>
-      <c r="C41" s="100" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="60">
-      <c r="A42" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B42" s="96" t="s">
-        <v>462</v>
-      </c>
-      <c r="C42" s="44" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="45">
-      <c r="A43" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B43" s="96" t="s">
-        <v>463</v>
-      </c>
-      <c r="C43" s="44" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="C44" s="44" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="45">
+    <row r="45" spans="1:3" s="4" customFormat="1" ht="105">
       <c r="A45" s="2">
         <v>42456</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="96" t="s">
+        <v>254</v>
+      </c>
+      <c r="C45" s="100" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="60">
+      <c r="A46" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B46" s="96" t="s">
+        <v>462</v>
+      </c>
+      <c r="C46" s="44" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="45">
+      <c r="A47" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B47" s="96" t="s">
+        <v>463</v>
+      </c>
+      <c r="C47" s="44" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C48" s="44" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="45">
+      <c r="A49" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="C45" s="44" t="s">
+      <c r="C49" s="44" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="77.25">
-      <c r="A46" s="79">
+    <row r="50" spans="1:3" ht="77.25">
+      <c r="A50" s="79">
         <v>42453</v>
       </c>
-      <c r="B46" s="78" t="s">
+      <c r="B50" s="78" t="s">
         <v>264</v>
       </c>
-      <c r="C46" s="78" t="s">
+      <c r="C50" s="78" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="26.25">
-      <c r="A47" s="79">
+    <row r="51" spans="1:3" ht="26.25">
+      <c r="A51" s="79">
         <v>42453</v>
       </c>
-      <c r="B47" s="78" t="s">
+      <c r="B51" s="78" t="s">
         <v>262</v>
       </c>
-      <c r="C47" s="78" t="s">
+      <c r="C51" s="78" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="39">
-      <c r="A48" s="79">
+    <row r="52" spans="1:3" ht="39">
+      <c r="A52" s="79">
         <v>42452</v>
       </c>
-      <c r="B48" s="78" t="s">
+      <c r="B52" s="78" t="s">
         <v>260</v>
       </c>
-      <c r="C48" s="78" t="s">
+      <c r="C52" s="78" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="165">
-      <c r="A49" s="75">
+    <row r="53" spans="1:3" ht="165">
+      <c r="A53" s="75">
         <v>42451</v>
       </c>
-      <c r="B49" s="74" t="s">
+      <c r="B53" s="74" t="s">
         <v>247</v>
       </c>
-      <c r="C49" s="100" t="s">
+      <c r="C53" s="100" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="45">
-      <c r="A50" s="2">
+    <row r="54" spans="1:3" ht="45">
+      <c r="A54" s="2">
         <v>42451</v>
       </c>
-      <c r="B50" s="100" t="s">
+      <c r="B54" s="100" t="s">
         <v>249</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="30">
-      <c r="A51" s="2">
+    <row r="55" spans="1:3" ht="30">
+      <c r="A55" s="2">
         <v>42451</v>
       </c>
-      <c r="B51" s="96" t="s">
+      <c r="B55" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="165">
-      <c r="A52" s="2">
+    <row r="56" spans="1:3" ht="165">
+      <c r="A56" s="2">
         <v>42451</v>
       </c>
-      <c r="B52" s="96" t="s">
+      <c r="B56" s="96" t="s">
         <v>253</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="64.5">
-      <c r="A53" s="79">
+    <row r="57" spans="1:3" ht="64.5">
+      <c r="A57" s="79">
         <v>42451</v>
       </c>
-      <c r="B53" s="78" t="s">
+      <c r="B57" s="78" t="s">
         <v>253</v>
       </c>
-      <c r="C53" s="78" t="s">
+      <c r="C57" s="78" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="64.5">
-      <c r="A54" s="79">
+    <row r="58" spans="1:3" ht="64.5">
+      <c r="A58" s="79">
         <v>42447</v>
       </c>
-      <c r="B54" s="78" t="s">
+      <c r="B58" s="78" t="s">
         <v>257</v>
       </c>
-      <c r="C54" s="78" t="s">
+      <c r="C58" s="78" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="2">
+    <row r="59" spans="1:3">
+      <c r="A59" s="2">
         <v>42440</v>
       </c>
-      <c r="B55" s="100" t="s">
+      <c r="B59" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="100" t="s">
+      <c r="C59" s="100" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="75">
-      <c r="A56" s="2">
+    <row r="60" spans="1:3" ht="75">
+      <c r="A60" s="2">
         <v>42436</v>
       </c>
-      <c r="B56" s="96" t="s">
+      <c r="B60" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="39">
-      <c r="A57" s="79">
+    <row r="61" spans="1:3" ht="39">
+      <c r="A61" s="79">
         <v>42431</v>
       </c>
-      <c r="B57" s="78" t="s">
+      <c r="B61" s="78" t="s">
         <v>274</v>
       </c>
-      <c r="C57" s="78" t="s">
+      <c r="C61" s="78" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="26.25">
-      <c r="A58" s="79">
+    <row r="62" spans="1:3" ht="26.25">
+      <c r="A62" s="79">
         <v>42431</v>
       </c>
-      <c r="B58" s="78" t="s">
+      <c r="B62" s="78" t="s">
         <v>272</v>
       </c>
-      <c r="C58" s="78" t="s">
+      <c r="C62" s="78" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="51.75">
-      <c r="A59" s="79">
+    <row r="63" spans="1:3" ht="51.75">
+      <c r="A63" s="79">
         <v>42430</v>
       </c>
-      <c r="B59" s="78" t="s">
+      <c r="B63" s="78" t="s">
         <v>270</v>
       </c>
-      <c r="C59" s="78" t="s">
+      <c r="C63" s="78" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="26.25">
-      <c r="A60" s="79">
+    <row r="64" spans="1:3" ht="26.25">
+      <c r="A64" s="79">
         <v>42428</v>
       </c>
-      <c r="B60" s="78" t="s">
+      <c r="B64" s="78" t="s">
         <v>268</v>
       </c>
-      <c r="C60" s="78" t="s">
+      <c r="C64" s="78" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="30">
-      <c r="A61" s="2">
+    <row r="65" spans="1:3" ht="30">
+      <c r="A65" s="2">
         <v>42426</v>
       </c>
-      <c r="B61" s="100" t="s">
+      <c r="B65" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="C61" s="100" t="s">
+      <c r="C65" s="100" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="77.25">
-      <c r="A62" s="79">
+    <row r="66" spans="1:3" ht="77.25">
+      <c r="A66" s="79">
         <v>42426</v>
       </c>
-      <c r="B62" s="78" t="s">
+      <c r="B66" s="78" t="s">
         <v>266</v>
       </c>
-      <c r="C62" s="78" t="s">
+      <c r="C66" s="78" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="2">
+    <row r="67" spans="1:3">
+      <c r="A67" s="2">
         <v>42425</v>
       </c>
-      <c r="B63" s="100" t="s">
+      <c r="B67" s="100" t="s">
         <v>241</v>
       </c>
-      <c r="C63" s="100" t="s">
+      <c r="C67" s="100" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="30">
-      <c r="A64" s="2">
+    <row r="68" spans="1:3" ht="30">
+      <c r="A68" s="2">
         <v>42425</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="26.25">
-      <c r="A65" s="79">
+    <row r="69" spans="1:3" ht="26.25">
+      <c r="A69" s="79">
         <v>42425</v>
       </c>
-      <c r="B65" s="78" t="s">
+      <c r="B69" s="78" t="s">
         <v>276</v>
       </c>
-      <c r="C65" s="78" t="s">
+      <c r="C69" s="78" t="s">
         <v>275</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="79">
-        <v>42425</v>
-      </c>
-      <c r="B66" s="78" t="s">
-        <v>276</v>
-      </c>
-      <c r="C66" s="78" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="26.25">
-      <c r="A67" s="79">
-        <v>42425</v>
-      </c>
-      <c r="B67" s="78" t="s">
-        <v>279</v>
-      </c>
-      <c r="C67" s="78" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="165">
-      <c r="A68" s="2">
-        <v>42424</v>
-      </c>
-      <c r="B68" s="100" t="s">
-        <v>239</v>
-      </c>
-      <c r="C68" s="114" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="45">
-      <c r="A69" s="2">
-        <v>42423</v>
-      </c>
-      <c r="B69" s="96" t="s">
-        <v>196</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="79">
+        <v>42425</v>
+      </c>
+      <c r="B70" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="C70" s="78" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="26.25">
+      <c r="A71" s="79">
+        <v>42425</v>
+      </c>
+      <c r="B71" s="78" t="s">
+        <v>279</v>
+      </c>
+      <c r="C71" s="78" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="165">
+      <c r="A72" s="2">
+        <v>42424</v>
+      </c>
+      <c r="B72" s="100" t="s">
+        <v>239</v>
+      </c>
+      <c r="C72" s="114" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="45">
+      <c r="A73" s="2">
         <v>42423</v>
       </c>
-      <c r="B70" s="78" t="s">
+      <c r="B73" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="79">
+        <v>42423</v>
+      </c>
+      <c r="B74" s="78" t="s">
         <v>281</v>
       </c>
-      <c r="C70" s="78" t="s">
+      <c r="C74" s="78" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="90">
-      <c r="A71" s="2">
+    <row r="75" spans="1:3" ht="90">
+      <c r="A75" s="2">
         <v>42422</v>
       </c>
-      <c r="B71" s="100" t="s">
+      <c r="B75" s="100" t="s">
         <v>236</v>
       </c>
-      <c r="C71" s="100" t="s">
+      <c r="C75" s="100" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="60">
-      <c r="A72" s="2">
+    <row r="76" spans="1:3" ht="60">
+      <c r="A76" s="2">
         <v>42419</v>
       </c>
-      <c r="B72" s="10" t="s">
+      <c r="B76" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="C72" s="36" t="s">
+      <c r="C76" s="36" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="195">
-      <c r="A73" s="2">
+    <row r="77" spans="1:3" ht="195">
+      <c r="A77" s="2">
         <v>42418</v>
       </c>
-      <c r="B73" s="10" t="s">
+      <c r="B77" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="18" t="s">
+      <c r="C77" s="18" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="45">
-      <c r="A74" s="2">
-        <v>42403</v>
-      </c>
-      <c r="B74" s="96" t="s">
-        <v>229</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="75">
-      <c r="A75" s="2">
-        <v>42403</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="C75" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="90">
-      <c r="A76" s="2">
-        <v>42403</v>
-      </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="90">
-      <c r="A77" s="2">
-        <v>42398</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C77" s="12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="45">
       <c r="A78" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B78" s="96" t="s">
+        <v>229</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="75">
+      <c r="A79" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="90">
+      <c r="A80" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="90">
+      <c r="A81" s="2">
         <v>42398</v>
       </c>
-      <c r="B78" s="12" t="s">
+      <c r="B81" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="45">
+      <c r="A82" s="2">
+        <v>42398</v>
+      </c>
+      <c r="B82" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="C78" s="12" t="s">
+      <c r="C82" s="12" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="2">
+    <row r="83" spans="1:3">
+      <c r="A83" s="2">
         <v>42397</v>
       </c>
-      <c r="B79" s="96" t="s">
+      <c r="B83" s="96" t="s">
         <v>201</v>
       </c>
-      <c r="C79" s="14" t="s">
+      <c r="C83" s="14" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="45">
-      <c r="A80" s="2">
-        <v>42396</v>
-      </c>
-      <c r="B80" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C80" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="30">
-      <c r="A81" s="2">
-        <v>42396</v>
-      </c>
-      <c r="B81" s="96" t="s">
-        <v>39</v>
-      </c>
-      <c r="C81" s="14" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="128.25">
-      <c r="A82" s="79">
-        <v>42386</v>
-      </c>
-      <c r="B82" s="78" t="s">
-        <v>283</v>
-      </c>
-      <c r="C82" s="78" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="64.5">
-      <c r="A83" s="79">
-        <v>42386</v>
-      </c>
-      <c r="B83" s="78" t="s">
-        <v>285</v>
-      </c>
-      <c r="C83" s="78" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="45">
       <c r="A84" s="2">
-        <v>42384</v>
-      </c>
-      <c r="B84" s="100" t="s">
-        <v>220</v>
-      </c>
-      <c r="C84" s="100" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="180">
+        <v>42396</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="30">
       <c r="A85" s="2">
-        <v>42382</v>
-      </c>
-      <c r="B85" s="14" t="s">
-        <v>219</v>
+        <v>42396</v>
+      </c>
+      <c r="B85" s="96" t="s">
+        <v>39</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="64.5">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="128.25">
       <c r="A86" s="79">
-        <v>42382</v>
+        <v>42386</v>
       </c>
       <c r="B86" s="78" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C86" s="78" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="30">
-      <c r="A87" s="2">
-        <v>42381</v>
-      </c>
-      <c r="B87" s="100" t="s">
-        <v>216</v>
-      </c>
-      <c r="C87" s="100" t="s">
-        <v>217</v>
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="64.5">
+      <c r="A87" s="79">
+        <v>42386</v>
+      </c>
+      <c r="B87" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="C87" s="78" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="45">
       <c r="A88" s="2">
+        <v>42384</v>
+      </c>
+      <c r="B88" s="100" t="s">
+        <v>220</v>
+      </c>
+      <c r="C88" s="100" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="180">
+      <c r="A89" s="2">
+        <v>42382</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="64.5">
+      <c r="A90" s="79">
+        <v>42382</v>
+      </c>
+      <c r="B90" s="78" t="s">
+        <v>287</v>
+      </c>
+      <c r="C90" s="78" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="30">
+      <c r="A91" s="2">
+        <v>42381</v>
+      </c>
+      <c r="B91" s="100" t="s">
+        <v>216</v>
+      </c>
+      <c r="C91" s="100" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="45">
+      <c r="A92" s="2">
         <v>42380</v>
       </c>
-      <c r="B88" s="16" t="s">
+      <c r="B92" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C88" s="16" t="s">
+      <c r="C92" s="16" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="75">
-      <c r="A89" s="2">
+    <row r="93" spans="1:3" ht="75">
+      <c r="A93" s="2">
         <v>42380</v>
       </c>
-      <c r="B89" s="50" t="s">
+      <c r="B93" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C89" s="17" t="s">
+      <c r="C93" s="17" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="180">
-      <c r="A90" s="2">
+    <row r="94" spans="1:3" ht="180">
+      <c r="A94" s="2">
         <v>42380</v>
       </c>
-      <c r="B90" s="50" t="s">
+      <c r="B94" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C90" s="18" t="s">
+      <c r="C94" s="18" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="217.5">
-      <c r="A91" s="79">
+    <row r="95" spans="1:3" ht="217.5">
+      <c r="A95" s="79">
         <v>42380</v>
       </c>
-      <c r="B91" s="78" t="s">
+      <c r="B95" s="78" t="s">
         <v>288</v>
       </c>
-      <c r="C91" s="78" t="s">
+      <c r="C95" s="78" t="s">
         <v>289</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="102.75">
-      <c r="A92" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B92" s="78" t="s">
-        <v>291</v>
-      </c>
-      <c r="C92" s="78" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="102.75">
-      <c r="A93" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B93" s="78" t="s">
-        <v>293</v>
-      </c>
-      <c r="C93" s="78" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="141">
-      <c r="A94" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B94" s="78" t="s">
-        <v>297</v>
-      </c>
-      <c r="C94" s="78" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="77.25">
-      <c r="A95" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B95" s="78" t="s">
-        <v>297</v>
-      </c>
-      <c r="C95" s="78" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="102.75">
@@ -4842,1037 +4884,1037 @@
         <v>42378</v>
       </c>
       <c r="B96" s="78" t="s">
+        <v>291</v>
+      </c>
+      <c r="C96" s="78" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="102.75">
+      <c r="A97" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B97" s="78" t="s">
+        <v>293</v>
+      </c>
+      <c r="C97" s="78" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="141">
+      <c r="A98" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B98" s="78" t="s">
+        <v>297</v>
+      </c>
+      <c r="C98" s="78" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="77.25">
+      <c r="A99" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B99" s="78" t="s">
+        <v>297</v>
+      </c>
+      <c r="C99" s="78" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="102.75">
+      <c r="A100" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B100" s="78" t="s">
         <v>295</v>
       </c>
-      <c r="C96" s="78" t="s">
+      <c r="C100" s="78" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="60">
-      <c r="A97" s="2">
+    <row r="101" spans="1:3" ht="60">
+      <c r="A101" s="2">
         <v>42377</v>
       </c>
-      <c r="B97" s="100" t="s">
+      <c r="B101" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="C97" s="100" t="s">
+      <c r="C101" s="100" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="77.25">
-      <c r="A98" s="79">
+    <row r="102" spans="1:3" ht="77.25">
+      <c r="A102" s="79">
         <v>42376</v>
       </c>
-      <c r="B98" s="78" t="s">
+      <c r="B102" s="78" t="s">
         <v>300</v>
       </c>
-      <c r="C98" s="78" t="s">
+      <c r="C102" s="78" t="s">
         <v>299</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="45">
-      <c r="A99" s="2">
-        <v>42375</v>
-      </c>
-      <c r="B99" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C99" s="100" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" s="2">
-        <v>42369</v>
-      </c>
-      <c r="B100" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="C100" s="19" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="195">
-      <c r="A101" s="2">
-        <v>42368</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C101" s="19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="135">
-      <c r="A102" s="2">
-        <v>42368</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C102" s="20" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="45">
       <c r="A103" s="2">
+        <v>42375</v>
+      </c>
+      <c r="B103" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C103" s="100" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="2">
+        <v>42369</v>
+      </c>
+      <c r="B104" s="100" t="s">
+        <v>202</v>
+      </c>
+      <c r="C104" s="19" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="195">
+      <c r="A105" s="2">
         <v>42368</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B105" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C105" s="19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="135">
+      <c r="A106" s="2">
+        <v>42368</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C106" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="45">
+      <c r="A107" s="2">
+        <v>42368</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C103" s="20" t="s">
+      <c r="C107" s="20" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="30">
-      <c r="A104" s="2">
+    <row r="108" spans="1:3" ht="30">
+      <c r="A108" s="2">
         <v>42366</v>
       </c>
-      <c r="B104" s="20" t="s">
+      <c r="B108" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C104" s="20" t="s">
+      <c r="C108" s="20" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="30">
-      <c r="A105" s="2">
-        <v>42366</v>
-      </c>
-      <c r="B105" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C105" s="20" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="150">
-      <c r="A106" s="2">
-        <v>42361</v>
-      </c>
-      <c r="C106" s="20" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="30">
-      <c r="A107" s="2">
-        <v>42361</v>
-      </c>
-      <c r="C107" s="20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="270">
-      <c r="A108" s="2">
-        <v>42361</v>
-      </c>
-      <c r="B108" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C108" s="22" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="30">
       <c r="A109" s="2">
-        <v>42361</v>
-      </c>
-      <c r="B109" s="100" t="s">
-        <v>53</v>
+        <v>42366</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="C109" s="20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="150">
       <c r="A110" s="2">
         <v>42361</v>
       </c>
-      <c r="B110" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C110" s="21" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="225">
+      <c r="C110" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="30">
       <c r="A111" s="2">
         <v>42361</v>
       </c>
-      <c r="B111" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C111" s="22" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="60">
+      <c r="C111" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="270">
       <c r="A112" s="2">
         <v>42361</v>
       </c>
-      <c r="B112" s="100" t="s">
-        <v>49</v>
+      <c r="B112" s="35" t="s">
+        <v>186</v>
       </c>
       <c r="C112" s="22" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="90">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="30">
       <c r="A113" s="2">
         <v>42361</v>
       </c>
-      <c r="B113" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C113" s="22" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="60">
+      <c r="B113" s="100" t="s">
+        <v>53</v>
+      </c>
+      <c r="C113" s="20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" s="2">
         <v>42361</v>
       </c>
-      <c r="B114" s="24" t="s">
+      <c r="B114" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C114" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="225">
+      <c r="A115" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B115" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C115" s="22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="60">
+      <c r="A116" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B116" s="100" t="s">
+        <v>49</v>
+      </c>
+      <c r="C116" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="90">
+      <c r="A117" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C114" s="24" t="s">
+      <c r="C117" s="22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="60">
+      <c r="A118" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B118" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C118" s="24" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
-      <c r="A115" s="40">
+    <row r="119" spans="1:3">
+      <c r="A119" s="40">
         <v>42360</v>
       </c>
-      <c r="B115" s="50" t="s">
+      <c r="B119" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C119" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="40">
+    <row r="120" spans="1:3">
+      <c r="A120" s="40">
         <v>42360</v>
       </c>
-      <c r="B116" s="50" t="s">
+      <c r="B120" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C120" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="102.75">
-      <c r="A117" s="80">
+    <row r="121" spans="1:3" ht="102.75">
+      <c r="A121" s="80">
         <v>42360</v>
       </c>
-      <c r="B117" s="78" t="s">
+      <c r="B121" s="78" t="s">
         <v>302</v>
       </c>
-      <c r="C117" s="78" t="s">
+      <c r="C121" s="78" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="30">
-      <c r="A118" s="2">
+    <row r="122" spans="1:3" ht="30">
+      <c r="A122" s="2">
         <v>42356</v>
       </c>
-      <c r="B118" s="100" t="s">
+      <c r="B122" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="C118" s="100" t="s">
+      <c r="C122" s="100" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B119" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="C119" s="23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B120" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="C120" s="25" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="30">
-      <c r="A121" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B121" s="96"/>
-      <c r="C121" s="25" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="60">
-      <c r="A122" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B122" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="C122" s="26" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B123" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C123" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="150">
+        <v>42356</v>
+      </c>
+      <c r="B123" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="C123" s="23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
       <c r="A124" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B124" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C124" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="120">
+        <v>42356</v>
+      </c>
+      <c r="B124" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C124" s="25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="30">
       <c r="A125" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B125" s="100" t="s">
-        <v>168</v>
-      </c>
-      <c r="C125" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="30">
+        <v>42356</v>
+      </c>
+      <c r="B125" s="96"/>
+      <c r="C125" s="25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="60">
       <c r="A126" s="2">
         <v>42355</v>
       </c>
       <c r="B126" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C126" s="28" t="s">
-        <v>169</v>
+        <v>91</v>
+      </c>
+      <c r="C126" s="26" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="2">
         <v>42355</v>
       </c>
-      <c r="B127" s="29" t="s">
-        <v>171</v>
+      <c r="B127" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="C127" s="29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="75">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="150">
       <c r="A128" s="2">
         <v>42355</v>
       </c>
-      <c r="B128" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C128" s="29" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="135">
+      <c r="B128" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C128" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="120">
       <c r="A129" s="2">
         <v>42355</v>
       </c>
       <c r="B129" s="100" t="s">
-        <v>173</v>
-      </c>
-      <c r="C129" s="29" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="75">
+        <v>168</v>
+      </c>
+      <c r="C129" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="30">
       <c r="A130" s="2">
         <v>42355</v>
       </c>
-      <c r="B130" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C130" s="42" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="30">
+      <c r="B130" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C130" s="28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
       <c r="A131" s="2">
         <v>42355</v>
       </c>
-      <c r="B131" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C131" s="30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
+      <c r="B131" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C131" s="29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="75">
       <c r="A132" s="2">
         <v>42355</v>
       </c>
-      <c r="C132" s="30" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3">
+      <c r="B132" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C132" s="29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="135">
       <c r="A133" s="2">
         <v>42355</v>
       </c>
-      <c r="B133" s="42"/>
-      <c r="C133" s="30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
+      <c r="B133" s="100" t="s">
+        <v>173</v>
+      </c>
+      <c r="C133" s="29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="75">
       <c r="A134" s="2">
         <v>42355</v>
       </c>
-      <c r="B134" s="42"/>
-      <c r="C134" s="30" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="75">
+      <c r="B134" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C134" s="42" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="30">
       <c r="A135" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B135" s="42" t="s">
-        <v>189</v>
+        <v>42355</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="C135" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="30">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
       <c r="A136" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B136" s="26"/>
-      <c r="C136" s="31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="75">
+        <v>42355</v>
+      </c>
+      <c r="C136" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
       <c r="A137" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B137" s="26"/>
-      <c r="C137" s="70" t="s">
-        <v>66</v>
+        <v>42355</v>
+      </c>
+      <c r="B137" s="42"/>
+      <c r="C137" s="30" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B138" s="26"/>
-      <c r="C138" s="32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
+        <v>42355</v>
+      </c>
+      <c r="B138" s="42"/>
+      <c r="C138" s="30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="75">
       <c r="A139" s="2">
         <v>42352</v>
       </c>
-      <c r="B139" s="96"/>
-      <c r="C139" s="33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
+      <c r="B139" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C139" s="30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="30">
       <c r="A140" s="2">
         <v>42352</v>
       </c>
-      <c r="B140" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C140" s="34" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
+      <c r="B140" s="26"/>
+      <c r="C140" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="75">
       <c r="A141" s="2">
         <v>42352</v>
       </c>
-      <c r="B141" s="96"/>
-      <c r="C141" s="34" t="s">
-        <v>73</v>
+      <c r="B141" s="26"/>
+      <c r="C141" s="70" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="2">
         <v>42352</v>
       </c>
-      <c r="B142" s="96"/>
-      <c r="C142" s="37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="30">
+      <c r="B142" s="26"/>
+      <c r="C142" s="32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
       <c r="A143" s="2">
         <v>42352</v>
       </c>
-      <c r="B143" s="37"/>
-      <c r="C143" s="37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="30">
+      <c r="B143" s="96"/>
+      <c r="C143" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
       <c r="A144" s="2">
         <v>42352</v>
       </c>
-      <c r="B144" s="96"/>
-      <c r="C144" s="96" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" ht="45">
+      <c r="B144" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C144" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
       <c r="A145" s="2">
         <v>42352</v>
       </c>
-      <c r="B145" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C145" s="96" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" ht="45">
+      <c r="B145" s="96"/>
+      <c r="C145" s="34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146" s="2">
         <v>42352</v>
       </c>
-      <c r="B146" s="100"/>
-      <c r="C146" s="39" t="s">
-        <v>80</v>
+      <c r="B146" s="96"/>
+      <c r="C146" s="37" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="30">
       <c r="A147" s="2">
         <v>42352</v>
       </c>
-      <c r="B147" s="38"/>
-      <c r="C147" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="F147" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" ht="75">
+      <c r="B147" s="37"/>
+      <c r="C147" s="37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="30">
       <c r="A148" s="2">
         <v>42352</v>
       </c>
-      <c r="B148" s="41"/>
-      <c r="C148" s="41" t="s">
-        <v>82</v>
+      <c r="B148" s="96"/>
+      <c r="C148" s="96" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="45">
       <c r="A149" s="2">
         <v>42352</v>
       </c>
-      <c r="B149" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C149" s="41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" ht="30">
+      <c r="B149" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C149" s="96" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="45">
       <c r="A150" s="2">
         <v>42352</v>
       </c>
-      <c r="B150" s="43"/>
-      <c r="C150" s="43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" ht="45">
+      <c r="B150" s="100"/>
+      <c r="C150" s="39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="30">
       <c r="A151" s="2">
         <v>42352</v>
       </c>
-      <c r="B151" s="44"/>
-      <c r="C151" s="44" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" ht="30">
+      <c r="B151" s="38"/>
+      <c r="C151" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="F151" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="75">
       <c r="A152" s="2">
         <v>42352</v>
       </c>
-      <c r="B152" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="C152" s="46" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" ht="30">
+      <c r="B152" s="41"/>
+      <c r="C152" s="41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="45">
       <c r="A153" s="2">
         <v>42352</v>
       </c>
-      <c r="B153" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C153" s="47" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6">
+      <c r="B153" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C153" s="41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="30">
       <c r="A154" s="2">
         <v>42352</v>
       </c>
-      <c r="B154" s="100" t="s">
-        <v>83</v>
-      </c>
-      <c r="C154" s="48" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" ht="135">
+      <c r="B154" s="43"/>
+      <c r="C154" s="43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="45">
       <c r="A155" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B155" s="49"/>
-      <c r="C155" s="49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="60">
+        <v>42352</v>
+      </c>
+      <c r="B155" s="44"/>
+      <c r="C155" s="44" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="30">
       <c r="A156" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B156" s="51" t="s">
+        <v>42352</v>
+      </c>
+      <c r="B156" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="C156" s="51" t="s">
-        <v>56</v>
+      <c r="C156" s="46" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="30">
       <c r="A157" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B157" s="96"/>
-      <c r="C157" s="53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="120">
+        <v>42352</v>
+      </c>
+      <c r="B157" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C157" s="47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
       <c r="A158" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B158" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C158" s="53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="150">
+        <v>42352</v>
+      </c>
+      <c r="B158" s="100" t="s">
+        <v>83</v>
+      </c>
+      <c r="C158" s="48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="135">
       <c r="A159" s="2">
         <v>42349</v>
       </c>
-      <c r="B159" s="52"/>
-      <c r="C159" s="52" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="30">
+      <c r="B159" s="49"/>
+      <c r="C159" s="49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="60">
       <c r="A160" s="2">
         <v>42349</v>
       </c>
-      <c r="B160" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C160" s="54" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3">
+      <c r="B160" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C160" s="51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="30">
       <c r="A161" s="2">
         <v>42349</v>
       </c>
-      <c r="B161" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C161" s="55" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3">
+      <c r="B161" s="96"/>
+      <c r="C161" s="53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="120">
       <c r="A162" s="2">
         <v>42349</v>
       </c>
-      <c r="B162" s="100"/>
-      <c r="C162" s="57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3">
+      <c r="B162" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C162" s="53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="150">
       <c r="A163" s="2">
         <v>42349</v>
       </c>
-      <c r="B163" s="58"/>
-      <c r="C163" s="58" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3">
+      <c r="B163" s="52"/>
+      <c r="C163" s="52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="30">
       <c r="A164" s="2">
         <v>42349</v>
       </c>
-      <c r="B164" s="59"/>
-      <c r="C164" s="59" t="s">
-        <v>70</v>
+      <c r="B164" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C164" s="54" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="2">
         <v>42349</v>
       </c>
-      <c r="B165" s="60"/>
-      <c r="C165" s="60" t="s">
-        <v>64</v>
+      <c r="B165" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C165" s="55" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="2">
         <v>42349</v>
       </c>
-      <c r="B166" s="61"/>
-      <c r="C166" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="60">
+      <c r="B166" s="100"/>
+      <c r="C166" s="57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
       <c r="A167" s="2">
         <v>42349</v>
       </c>
-      <c r="B167" s="62" t="s">
-        <v>168</v>
-      </c>
-      <c r="C167" s="100" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="90">
+      <c r="B167" s="58"/>
+      <c r="C167" s="58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
       <c r="A168" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B168" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C168" s="62" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="30">
+        <v>42349</v>
+      </c>
+      <c r="B168" s="59"/>
+      <c r="C168" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
       <c r="A169" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C169" s="62" t="s">
-        <v>36</v>
+        <v>42349</v>
+      </c>
+      <c r="B169" s="60"/>
+      <c r="C169" s="60" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B170" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C170" s="63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3">
+        <v>42349</v>
+      </c>
+      <c r="B170" s="61"/>
+      <c r="C170" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="60">
       <c r="A171" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B171" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C171" s="64" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" ht="30">
+        <v>42349</v>
+      </c>
+      <c r="B171" s="62" t="s">
+        <v>168</v>
+      </c>
+      <c r="C171" s="100" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="90">
       <c r="A172" s="2">
         <v>42345</v>
       </c>
-      <c r="B172" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C172" s="65" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="195">
+      <c r="B172" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C172" s="62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="30">
       <c r="A173" s="2">
         <v>42345</v>
       </c>
-      <c r="B173" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C173" s="66" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="150">
+      <c r="B173" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C173" s="62" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
       <c r="A174" s="2">
         <v>42345</v>
       </c>
-      <c r="B174" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="C174" s="67" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" ht="75">
+      <c r="B174" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C174" s="63" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
       <c r="A175" s="2">
         <v>42345</v>
       </c>
-      <c r="B175" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="C175" s="68" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" ht="75">
+      <c r="B175" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C175" s="64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="30">
       <c r="A176" s="2">
         <v>42345</v>
       </c>
-      <c r="B176" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C176" s="69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" ht="30">
+      <c r="B176" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C176" s="65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="195">
       <c r="A177" s="2">
         <v>42345</v>
       </c>
-      <c r="B177" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C177" s="73" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3">
+      <c r="B177" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C177" s="66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="135">
       <c r="A178" s="2">
         <v>42345</v>
       </c>
-      <c r="B178" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="C178" s="73" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3">
+      <c r="B178" s="100" t="s">
+        <v>31</v>
+      </c>
+      <c r="C178" s="67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="75">
       <c r="A179" s="2">
         <v>42345</v>
       </c>
-      <c r="B179" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="C179" s="73" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="60">
+      <c r="B179" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C179" s="68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="75">
       <c r="A180" s="2">
         <v>42345</v>
       </c>
-      <c r="B180" s="96" t="s">
-        <v>39</v>
-      </c>
-      <c r="C180" s="73" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" ht="150">
+      <c r="B180" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C180" s="69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="30">
       <c r="A181" s="2">
         <v>42345</v>
       </c>
-      <c r="B181" s="15" t="s">
-        <v>43</v>
+      <c r="B181" s="100" t="s">
+        <v>12</v>
       </c>
       <c r="C181" s="73" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" ht="45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
       <c r="A182" s="2">
         <v>42345</v>
       </c>
-      <c r="B182" s="100" t="s">
+      <c r="B182" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="C182" s="76" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" ht="60">
+      <c r="C182" s="73" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
       <c r="A183" s="2">
         <v>42345</v>
       </c>
-      <c r="B183" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C183" s="77" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" ht="105">
+      <c r="B183" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C183" s="73" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="60">
       <c r="A184" s="2">
         <v>42345</v>
       </c>
-      <c r="B184" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C184" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
+      <c r="B184" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="C184" s="73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="150">
       <c r="A185" s="2">
         <v>42345</v>
       </c>
-      <c r="B185" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C185" s="96" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3">
+      <c r="B185" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C185" s="73" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="45">
       <c r="A186" s="2">
         <v>42345</v>
       </c>
-      <c r="B186" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C186" s="96" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="75">
+      <c r="B186" s="100" t="s">
+        <v>39</v>
+      </c>
+      <c r="C186" s="76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="60">
       <c r="A187" s="2">
         <v>42345</v>
       </c>
-      <c r="B187" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C187" s="96" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" ht="45">
+      <c r="B187" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C187" s="77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="105">
       <c r="A188" s="2">
         <v>42345</v>
       </c>
-      <c r="B188" s="96" t="s">
+      <c r="B188" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B189" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C189" s="96" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B190" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C190" s="96" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="75">
+      <c r="A191" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B191" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C191" s="96" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="45">
+      <c r="A192" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B192" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C188" s="96" t="s">
+      <c r="C192" s="96" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="141">
-      <c r="A189" s="80">
+    <row r="193" spans="1:3" ht="141">
+      <c r="A193" s="80">
         <v>42345</v>
       </c>
-      <c r="B189" s="78" t="s">
+      <c r="B193" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="C189" s="78" t="s">
+      <c r="C193" s="78" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="105">
-      <c r="A190" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C190" s="100" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" ht="90">
-      <c r="A191" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C191" s="96" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" ht="75">
-      <c r="A192" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C192" s="96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="30">
-      <c r="A193" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B193" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C193" s="96" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="30">
+    <row r="194" spans="1:3" ht="105">
       <c r="A194" s="2">
         <v>42341</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C194" s="96" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="45">
+        <v>12</v>
+      </c>
+      <c r="C194" s="100" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="90">
       <c r="A195" s="2">
         <v>42341</v>
       </c>
@@ -5880,18 +5922,18 @@
         <v>15</v>
       </c>
       <c r="C195" s="96" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" ht="90">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="75">
       <c r="A196" s="2">
         <v>42341</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C196" s="96" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="30">
@@ -5902,10 +5944,10 @@
         <v>15</v>
       </c>
       <c r="C197" s="96" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" ht="150">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="30">
       <c r="A198" s="2">
         <v>42341</v>
       </c>
@@ -5913,10 +5955,10 @@
         <v>15</v>
       </c>
       <c r="C198" s="96" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="45">
       <c r="A199" s="2">
         <v>42341</v>
       </c>
@@ -5924,73 +5966,73 @@
         <v>15</v>
       </c>
       <c r="C199" s="96" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="90">
       <c r="A200" s="2">
         <v>42341</v>
       </c>
-      <c r="B200" s="100" t="s">
-        <v>12</v>
+      <c r="B200" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C200" s="96" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" ht="60">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="30">
       <c r="A201" s="2">
         <v>42341</v>
       </c>
-      <c r="B201" s="96" t="s">
+      <c r="B201" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C201" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="150">
       <c r="A202" s="2">
         <v>42341</v>
       </c>
-      <c r="B202" s="96" t="s">
-        <v>12</v>
+      <c r="B202" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C202" s="96" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="75">
       <c r="A203" s="2">
         <v>42341</v>
       </c>
-      <c r="B203" s="96" t="s">
+      <c r="B203" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C203" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3">
+      <c r="C203" s="96" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="90">
       <c r="A204" s="2">
         <v>42341</v>
       </c>
-      <c r="B204" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C204" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3">
+      <c r="B204" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C204" s="96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="60">
       <c r="A205" s="2">
         <v>42341</v>
       </c>
       <c r="B205" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C205" s="8" t="s">
-        <v>165</v>
+      <c r="C205" s="96" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -5998,309 +6040,353 @@
         <v>42341</v>
       </c>
       <c r="B206" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C206" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" ht="75">
+        <v>12</v>
+      </c>
+      <c r="C206" s="96" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
       <c r="A207" s="2">
         <v>42341</v>
       </c>
       <c r="B207" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C207" s="100" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="60">
+      <c r="C207" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
       <c r="A208" s="2">
         <v>42341</v>
       </c>
       <c r="B208" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C208" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B209" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C209" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B210" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C210" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="75">
+      <c r="A211" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B211" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C211" s="100" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="60">
+      <c r="A212" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B212" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C208" s="96" t="s">
+      <c r="C212" s="96" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="60">
-      <c r="A209" s="2">
+    <row r="213" spans="1:3" ht="60">
+      <c r="A213" s="2">
         <v>42340</v>
       </c>
-      <c r="B209" s="96"/>
-      <c r="C209" s="96" t="s">
+      <c r="B213" s="96"/>
+      <c r="C213" s="96" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="45">
-      <c r="A210" s="2">
+    <row r="214" spans="1:3" ht="45">
+      <c r="A214" s="2">
         <v>42340</v>
       </c>
-      <c r="B210" s="96"/>
-      <c r="C210" s="96" t="s">
+      <c r="B214" s="96"/>
+      <c r="C214" s="96" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="60">
-      <c r="A211" s="2">
+    <row r="215" spans="1:3" ht="60">
+      <c r="A215" s="2">
         <v>42340</v>
       </c>
-      <c r="B211" s="2" t="s">
+      <c r="B215" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C211" s="96" t="s">
+      <c r="C215" s="96" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
-      <c r="A212" s="2">
+    <row r="216" spans="1:3">
+      <c r="A216" s="2">
         <v>42339</v>
       </c>
-      <c r="B212" s="2"/>
-      <c r="C212" s="96" t="s">
+      <c r="B216" s="2"/>
+      <c r="C216" s="96" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:3">
-      <c r="A213" s="2">
+    <row r="217" spans="1:3">
+      <c r="A217" s="2">
         <v>42339</v>
       </c>
-      <c r="B213" s="2"/>
-      <c r="C213" s="96" t="s">
+      <c r="B217" s="2"/>
+      <c r="C217" s="96" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="64.5">
-      <c r="A214" s="80">
+    <row r="218" spans="1:3" ht="64.5">
+      <c r="A218" s="80">
         <v>42334</v>
       </c>
-      <c r="B214" s="78" t="s">
+      <c r="B218" s="78" t="s">
         <v>309</v>
       </c>
-      <c r="C214" s="78" t="s">
+      <c r="C218" s="78" t="s">
         <v>308</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" ht="26.25">
-      <c r="A215" s="80">
-        <v>42334</v>
-      </c>
-      <c r="B215" s="78" t="s">
-        <v>307</v>
-      </c>
-      <c r="C215" s="78" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" ht="39">
-      <c r="A216" s="80">
-        <v>42334</v>
-      </c>
-      <c r="B216" s="78" t="s">
-        <v>272</v>
-      </c>
-      <c r="C216" s="78" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" ht="128.25">
-      <c r="A217" s="80">
-        <v>42333</v>
-      </c>
-      <c r="B217" s="78" t="s">
-        <v>268</v>
-      </c>
-      <c r="C217" s="78" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="51.75">
-      <c r="A218" s="80">
-        <v>42333</v>
-      </c>
-      <c r="B218" s="78" t="s">
-        <v>216</v>
-      </c>
-      <c r="C218" s="78" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="26.25">
       <c r="A219" s="80">
-        <v>42331</v>
+        <v>42334</v>
       </c>
       <c r="B219" s="78" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C219" s="78" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="39">
       <c r="A220" s="80">
+        <v>42334</v>
+      </c>
+      <c r="B220" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="C220" s="78" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" ht="128.25">
+      <c r="A221" s="80">
+        <v>42333</v>
+      </c>
+      <c r="B221" s="78" t="s">
+        <v>268</v>
+      </c>
+      <c r="C221" s="78" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" ht="51.75">
+      <c r="A222" s="80">
+        <v>42333</v>
+      </c>
+      <c r="B222" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="C222" s="78" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" ht="26.25">
+      <c r="A223" s="80">
+        <v>42331</v>
+      </c>
+      <c r="B223" s="78" t="s">
+        <v>313</v>
+      </c>
+      <c r="C223" s="78" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" ht="39">
+      <c r="A224" s="80">
         <v>42329</v>
       </c>
-      <c r="B220" s="78" t="s">
+      <c r="B224" s="78" t="s">
         <v>315</v>
       </c>
-      <c r="C220" s="78" t="s">
+      <c r="C224" s="78" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="39">
-      <c r="A221" s="80">
-        <v>42328</v>
-      </c>
-      <c r="B221" s="78" t="s">
-        <v>324</v>
-      </c>
-      <c r="C221" s="78" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="26.25">
-      <c r="A222" s="80">
-        <v>42328</v>
-      </c>
-      <c r="B222" s="78" t="s">
-        <v>322</v>
-      </c>
-      <c r="C222" s="78" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" ht="115.5">
-      <c r="A223" s="80">
-        <v>42328</v>
-      </c>
-      <c r="B223" s="78" t="s">
-        <v>320</v>
-      </c>
-      <c r="C223" s="78" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" ht="90">
-      <c r="A224" s="80">
-        <v>42328</v>
-      </c>
-      <c r="B224" s="78" t="s">
-        <v>317</v>
-      </c>
-      <c r="C224" s="78" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" ht="166.5">
+    <row r="225" spans="1:3" ht="39">
       <c r="A225" s="80">
         <v>42328</v>
       </c>
       <c r="B225" s="78" t="s">
+        <v>324</v>
+      </c>
+      <c r="C225" s="78" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" ht="26.25">
+      <c r="A226" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B226" s="78" t="s">
+        <v>322</v>
+      </c>
+      <c r="C226" s="78" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" ht="115.5">
+      <c r="A227" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B227" s="78" t="s">
+        <v>320</v>
+      </c>
+      <c r="C227" s="78" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" ht="90">
+      <c r="A228" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B228" s="78" t="s">
         <v>317</v>
       </c>
-      <c r="C225" s="78" t="s">
+      <c r="C228" s="78" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="153.75">
+      <c r="A229" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B229" s="78" t="s">
+        <v>317</v>
+      </c>
+      <c r="C229" s="78" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="226" spans="1:3" ht="102.75">
-      <c r="A226" s="80">
+    <row r="230" spans="1:3" ht="102.75">
+      <c r="A230" s="80">
         <v>42324</v>
       </c>
-      <c r="B226" s="78" t="s">
+      <c r="B230" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="C226" s="78" t="s">
+      <c r="C230" s="78" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="227" spans="1:3" ht="90">
-      <c r="A227" s="80">
+    <row r="231" spans="1:3" ht="90">
+      <c r="A231" s="80">
         <v>42321</v>
       </c>
-      <c r="B227" s="78" t="s">
+      <c r="B231" s="78" t="s">
         <v>327</v>
       </c>
-      <c r="C227" s="78" t="s">
+      <c r="C231" s="78" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="228" spans="1:3" ht="26.25">
-      <c r="A228" s="80">
+    <row r="232" spans="1:3" ht="26.25">
+      <c r="A232" s="80">
         <v>42321</v>
       </c>
-      <c r="B228" s="78" t="s">
+      <c r="B232" s="78" t="s">
         <v>327</v>
       </c>
-      <c r="C228" s="78" t="s">
+      <c r="C232" s="78" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="229" spans="1:3" ht="90">
-      <c r="A229" s="79">
+    <row r="233" spans="1:3" ht="77.25">
+      <c r="A233" s="79">
         <v>42318</v>
       </c>
-      <c r="B229" s="78" t="s">
+      <c r="B233" s="78" t="s">
         <v>330</v>
       </c>
-      <c r="C229" s="78" t="s">
+      <c r="C233" s="78" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="230" spans="1:3" ht="115.5">
-      <c r="A230" s="79">
+    <row r="234" spans="1:3" ht="115.5">
+      <c r="A234" s="79">
         <v>42311</v>
       </c>
-      <c r="B230" s="78" t="s">
+      <c r="B234" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C230" s="78" t="s">
+      <c r="C234" s="78" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="77.25">
-      <c r="A231" s="79">
+    <row r="235" spans="1:3" ht="77.25">
+      <c r="A235" s="79">
         <v>42310</v>
       </c>
-      <c r="B231" s="78" t="s">
+      <c r="B235" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C231" s="78" t="s">
+      <c r="C235" s="78" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="51.75">
-      <c r="A232" s="79">
+    <row r="236" spans="1:3" ht="51.75">
+      <c r="A236" s="79">
         <v>42306</v>
       </c>
-      <c r="B232" s="78" t="s">
+      <c r="B236" s="78" t="s">
         <v>333</v>
       </c>
-      <c r="C232" s="78" t="s">
+      <c r="C236" s="78" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="233" spans="1:3">
-      <c r="A233" s="100"/>
-      <c r="B233" s="100"/>
-      <c r="C233" s="100"/>
+    <row r="237" spans="1:3">
+      <c r="A237" s="100"/>
+      <c r="B237" s="100"/>
+      <c r="C237" s="100"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C233">
+  <autoFilter ref="A1:C237">
     <sortState ref="A2:C201">
       <sortCondition descending="1" ref="A1:A201"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C205" r:id="rId1"/>
-    <hyperlink ref="C166" r:id="rId2"/>
-    <hyperlink ref="C206" r:id="rId3"/>
-    <hyperlink ref="C40" r:id="rId4"/>
-    <hyperlink ref="C25" r:id="rId5"/>
-    <hyperlink ref="C22" r:id="rId6"/>
+    <hyperlink ref="C209" r:id="rId1"/>
+    <hyperlink ref="C170" r:id="rId2"/>
+    <hyperlink ref="C210" r:id="rId3"/>
+    <hyperlink ref="C44" r:id="rId4"/>
+    <hyperlink ref="C29" r:id="rId5"/>
+    <hyperlink ref="C26" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -6320,16 +6406,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="60.75" customHeight="1">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add learning to index fro migration
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -15,14 +15,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'AS400 Version'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$237</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$240</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="546">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -2786,6 +2786,21 @@
     1. Volume(卷): A way to mount a folder to container from host machine(this allows awesome code-environ seperation)
     2. Link(連接): Simulate a LAN within the host machine and containers so that the communication is secured.
     3. Priviledge: Grant priviledge to container to run docker on itself recursively.</t>
+  </si>
+  <si>
+    <t>昨晚看完書中最後一個應用例子, 以Crefits作為支持分布式的平台分別安裝在三台Docker host 上(我的設備也足以做到PI+EPC+ASUS), 然後安裝一處APP_SERVER, 另一處為APP_CLIENT, 該APP_SERVER端以已有的Plugin和Crefits連接, 那就可以享受Crefits提供的分布式服務啦.</t>
+  </si>
+  <si>
+    <t>to be migrate</t>
+  </si>
+  <si>
+    <t>因為我是跨學科的, 我的idea即使在概念上和別人重合, 但implementation 的方式也很不一樣, 導致的質量也更好. 而且我的idea通常比較早於別人.</t>
+  </si>
+  <si>
+    <t>Learning from Car Commission Task Lession:
+1. 寸進精神 (很多時自己都止步在)
+2. 髒法: 一個getleadacc module, ip1, op1, ip1輸入後輸出op1為ip1的Lead acc, 但若ip1為lead acc或非multi ccy acc, op1均會賦上ip1的值然後返回. 當時死腦只想找個方法求是否Lead account, 後發現轉下彎, 若能用ip1&lt;&gt;op1來判定是subacc這第三個可能性, 是能得到確定的定性結果的, 然後可以加以利用.
+3. 圖形化思考方法</t>
   </si>
 </sst>
 </file>
@@ -2980,7 +2995,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3044,6 +3059,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3114,7 +3135,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3475,6 +3496,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3508,13 +3535,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4202207</xdr:colOff>
-      <xdr:row>124</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>593914</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>414618</xdr:colOff>
-      <xdr:row>128</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>257735</xdr:colOff>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>102264</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3831,10 +3858,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F237"/>
+  <dimension ref="A1:F240"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3842,9 +3869,10 @@
     <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
     <col min="3" max="3" width="77" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:4" s="4" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -3855,1072 +3883,1074 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="102" customFormat="1">
+    <row r="2" spans="1:4" s="102" customFormat="1">
       <c r="A2" s="100"/>
       <c r="B2" s="100"/>
       <c r="C2" s="100"/>
     </row>
-    <row r="3" spans="1:3" s="102" customFormat="1" ht="135">
+    <row r="3" spans="1:4" s="102" customFormat="1" ht="30">
       <c r="A3" s="121">
-        <v>42562</v>
-      </c>
-      <c r="B3" s="120" t="s">
-        <v>537</v>
-      </c>
-      <c r="C3" s="120" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="102" customFormat="1" ht="60">
+        <v>42564</v>
+      </c>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122" t="s">
+        <v>544</v>
+      </c>
+      <c r="D3" s="124" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="102" customFormat="1" ht="120">
       <c r="A4" s="121">
-        <v>42562</v>
-      </c>
-      <c r="B4" s="120" t="s">
-        <v>536</v>
-      </c>
-      <c r="C4" s="120" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="102" customFormat="1" ht="75">
+        <v>42564</v>
+      </c>
+      <c r="B4" s="122"/>
+      <c r="C4" s="122" t="s">
+        <v>545</v>
+      </c>
+      <c r="D4" s="124" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="102" customFormat="1" ht="75">
       <c r="A5" s="121">
-        <v>42562</v>
-      </c>
-      <c r="B5" s="120" t="s">
-        <v>535</v>
-      </c>
-      <c r="C5" s="120" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="102" customFormat="1" ht="165">
+        <v>42564</v>
+      </c>
+      <c r="B5" s="122" t="s">
+        <v>534</v>
+      </c>
+      <c r="C5" s="122" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="102" customFormat="1" ht="135">
       <c r="A6" s="121">
         <v>42562</v>
       </c>
       <c r="B6" s="120" t="s">
+        <v>537</v>
+      </c>
+      <c r="C6" s="120" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="102" customFormat="1" ht="60">
+      <c r="A7" s="121">
+        <v>42562</v>
+      </c>
+      <c r="B7" s="120" t="s">
+        <v>536</v>
+      </c>
+      <c r="C7" s="120" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="102" customFormat="1" ht="75">
+      <c r="A8" s="121">
+        <v>42562</v>
+      </c>
+      <c r="B8" s="120" t="s">
+        <v>535</v>
+      </c>
+      <c r="C8" s="120" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="102" customFormat="1" ht="165">
+      <c r="A9" s="121">
+        <v>42562</v>
+      </c>
+      <c r="B9" s="120" t="s">
         <v>534</v>
       </c>
-      <c r="C6" s="120" t="s">
+      <c r="C9" s="120" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A7" s="121">
+    <row r="10" spans="1:4" s="102" customFormat="1" ht="30">
+      <c r="A10" s="121">
         <v>42557</v>
       </c>
-      <c r="B7" s="120" t="s">
+      <c r="B10" s="120" t="s">
         <v>525</v>
       </c>
-      <c r="C7" s="120" t="s">
+      <c r="C10" s="120" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="102" customFormat="1" ht="180">
-      <c r="A8" s="120"/>
-      <c r="B8" s="120" t="s">
+    <row r="11" spans="1:4" s="102" customFormat="1" ht="180">
+      <c r="A11" s="120"/>
+      <c r="B11" s="120" t="s">
         <v>527</v>
       </c>
-      <c r="C8" s="120" t="s">
+      <c r="C11" s="120" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A9" s="121">
+    <row r="12" spans="1:4" s="102" customFormat="1" ht="150">
+      <c r="A12" s="121">
         <v>42540</v>
       </c>
-      <c r="B9" s="120" t="s">
+      <c r="B12" s="120" t="s">
         <v>529</v>
       </c>
-      <c r="C9" s="120" t="s">
+      <c r="C12" s="120" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="102" customFormat="1" ht="180">
-      <c r="A10" s="121">
+    <row r="13" spans="1:4" s="102" customFormat="1" ht="180">
+      <c r="A13" s="121">
         <v>42539</v>
       </c>
-      <c r="B10" s="120" t="s">
+      <c r="B13" s="120" t="s">
         <v>527</v>
       </c>
-      <c r="C10" s="120" t="s">
+      <c r="C13" s="120" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A11" s="121">
+    <row r="14" spans="1:4" s="102" customFormat="1" ht="105">
+      <c r="A14" s="121">
         <v>42539</v>
       </c>
-      <c r="B11" s="120" t="s">
+      <c r="B14" s="120" t="s">
         <v>532</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C14" s="120" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A12" s="2">
+    <row r="15" spans="1:4" s="102" customFormat="1" ht="60">
+      <c r="A15" s="2">
         <v>42534</v>
       </c>
-      <c r="B12" s="119" t="s">
+      <c r="B15" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C15" s="119" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A13" s="2">
+    <row r="16" spans="1:4" s="102" customFormat="1" ht="45">
+      <c r="A16" s="2">
         <v>42517</v>
       </c>
-      <c r="B13" s="118" t="s">
+      <c r="B16" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="118" t="s">
+      <c r="C16" s="118" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A14" s="2">
+    <row r="17" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A17" s="2">
         <v>42514</v>
       </c>
-      <c r="B14" s="117" t="s">
+      <c r="B17" s="117" t="s">
         <v>519</v>
       </c>
-      <c r="C14" s="117" t="s">
+      <c r="C17" s="117" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A15" s="2">
+    <row r="18" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A18" s="2">
         <v>42507</v>
       </c>
-      <c r="B15" s="116" t="s">
+      <c r="B18" s="116" t="s">
         <v>519</v>
       </c>
-      <c r="C15" s="116" t="s">
+      <c r="C18" s="116" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A16" s="2">
+    <row r="19" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A19" s="2">
         <v>42502</v>
       </c>
-      <c r="B16" s="115" t="s">
+      <c r="B19" s="115" t="s">
         <v>519</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="C19" s="116" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A17" s="2">
+    <row r="20" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="A20" s="2">
         <v>42485</v>
       </c>
-      <c r="B17" s="113" t="s">
+      <c r="B20" s="113" t="s">
         <v>516</v>
       </c>
-      <c r="C17" s="113" t="s">
+      <c r="C20" s="113" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A18" s="2">
+    <row r="21" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A21" s="2">
         <v>42485</v>
       </c>
-      <c r="B18" s="110" t="s">
+      <c r="B21" s="110" t="s">
         <v>514</v>
       </c>
-      <c r="C18" s="110" t="s">
+      <c r="C21" s="110" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="102" customFormat="1" ht="300">
-      <c r="A19" s="2">
+    <row r="22" spans="1:3" s="102" customFormat="1" ht="300">
+      <c r="A22" s="2">
         <v>42485</v>
       </c>
-      <c r="B19" s="112" t="s">
+      <c r="B22" s="112" t="s">
         <v>241</v>
       </c>
-      <c r="C19" s="112" t="s">
+      <c r="C22" s="112" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A20" s="2">
+    <row r="23" spans="1:3" s="102" customFormat="1" ht="150">
+      <c r="A23" s="2">
         <v>42479</v>
       </c>
-      <c r="B20" s="111" t="s">
+      <c r="B23" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="C20" s="111" t="s">
+      <c r="C23" s="111" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A21" s="2">
+    <row r="24" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="A24" s="2">
         <v>42478</v>
       </c>
-      <c r="B21" s="110" t="s">
+      <c r="B24" s="110" t="s">
         <v>509</v>
       </c>
-      <c r="C21" s="110" t="s">
+      <c r="C24" s="110" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="102" customFormat="1" ht="120">
-      <c r="A22" s="2">
+    <row r="25" spans="1:3" s="102" customFormat="1" ht="120">
+      <c r="A25" s="2">
         <v>42477</v>
       </c>
-      <c r="B22" s="109" t="s">
+      <c r="B25" s="109" t="s">
         <v>509</v>
       </c>
-      <c r="C22" s="109" t="s">
+      <c r="C25" s="109" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A23" s="2">
+    <row r="26" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A26" s="2">
         <v>42477</v>
       </c>
-      <c r="B23" s="108" t="s">
+      <c r="B26" s="108" t="s">
         <v>507</v>
       </c>
-      <c r="C23" s="108" t="s">
+      <c r="C26" s="108" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="102" customFormat="1">
-      <c r="A24" s="2">
+    <row r="27" spans="1:3" s="102" customFormat="1">
+      <c r="A27" s="2">
         <v>42473</v>
       </c>
-      <c r="B24" s="106" t="s">
+      <c r="B27" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="106" t="s">
+      <c r="C27" s="106" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A25" s="2">
+    <row r="28" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A28" s="2">
         <v>42473</v>
       </c>
-      <c r="B25" s="106" t="s">
+      <c r="B28" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="107" t="s">
+      <c r="C28" s="107" t="s">
         <v>506</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="102" customFormat="1">
-      <c r="A26" s="2">
-        <v>42469</v>
-      </c>
-      <c r="B26" s="105" t="s">
-        <v>504</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="102" customFormat="1" ht="75">
-      <c r="A27" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B27" s="104" t="s">
-        <v>497</v>
-      </c>
-      <c r="C27" s="104" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A28" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B28" s="104" t="s">
-        <v>499</v>
-      </c>
-      <c r="C28" s="104" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="102" customFormat="1">
       <c r="A29" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B29" s="104" t="s">
-        <v>501</v>
-      </c>
-      <c r="C29" s="104" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="102" customFormat="1" ht="150">
+        <v>42469</v>
+      </c>
+      <c r="B29" s="105" t="s">
+        <v>504</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="102" customFormat="1" ht="75">
       <c r="A30" s="2">
         <v>42463</v>
       </c>
-      <c r="B30" s="100" t="s">
-        <v>493</v>
-      </c>
-      <c r="C30" s="100" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="B30" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="C30" s="104" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="102" customFormat="1" ht="105">
       <c r="A31" s="2">
         <v>42463</v>
       </c>
-      <c r="B31" s="103" t="s">
-        <v>492</v>
-      </c>
-      <c r="C31" s="103" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="B31" s="104" t="s">
+        <v>499</v>
+      </c>
+      <c r="C31" s="104" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="102" customFormat="1">
       <c r="A32" s="2">
         <v>42463</v>
       </c>
-      <c r="B32" s="101" t="s">
-        <v>489</v>
-      </c>
-      <c r="C32" s="101" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="B32" s="104" t="s">
+        <v>501</v>
+      </c>
+      <c r="C32" s="104" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="102" customFormat="1" ht="150">
       <c r="A33" s="2">
         <v>42463</v>
       </c>
-      <c r="B33" s="101" t="s">
+      <c r="B33" s="100" t="s">
+        <v>493</v>
+      </c>
+      <c r="C33" s="100" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="A34" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B34" s="103" t="s">
+        <v>492</v>
+      </c>
+      <c r="C34" s="103" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A35" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B35" s="101" t="s">
+        <v>489</v>
+      </c>
+      <c r="C35" s="101" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A36" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B36" s="101" t="s">
         <v>488</v>
       </c>
-      <c r="C33" s="101" t="s">
+      <c r="C36" s="101" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A34" s="2">
-        <v>42462</v>
-      </c>
-      <c r="B34" s="100" t="s">
-        <v>486</v>
-      </c>
-      <c r="C34" s="100" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="102" customFormat="1" ht="135">
-      <c r="A35" s="2">
-        <v>42462</v>
-      </c>
-      <c r="B35" s="100" t="s">
-        <v>484</v>
-      </c>
-      <c r="C35" s="100" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="102" customFormat="1" ht="240">
-      <c r="A36" s="2">
-        <v>42462</v>
-      </c>
-      <c r="B36" s="100" t="s">
-        <v>480</v>
-      </c>
-      <c r="C36" s="100" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" s="102" customFormat="1" ht="120">
+    <row r="37" spans="1:3" s="102" customFormat="1" ht="150">
       <c r="A37" s="2">
         <v>42462</v>
       </c>
       <c r="B37" s="100" t="s">
+        <v>486</v>
+      </c>
+      <c r="C37" s="100" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="102" customFormat="1" ht="135">
+      <c r="A38" s="2">
+        <v>42462</v>
+      </c>
+      <c r="B38" s="100" t="s">
+        <v>484</v>
+      </c>
+      <c r="C38" s="100" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="102" customFormat="1" ht="240">
+      <c r="A39" s="2">
+        <v>42462</v>
+      </c>
+      <c r="B39" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="C37" s="100" t="s">
+      <c r="C39" s="100" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="102" customFormat="1" ht="120">
+      <c r="A40" s="2">
+        <v>42462</v>
+      </c>
+      <c r="B40" s="100" t="s">
+        <v>480</v>
+      </c>
+      <c r="C40" s="100" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="4" customFormat="1" ht="120">
-      <c r="A38" s="2">
-        <v>42460</v>
-      </c>
-      <c r="B38" s="99" t="s">
-        <v>477</v>
-      </c>
-      <c r="C38" s="99" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="4" customFormat="1" ht="30">
-      <c r="A39" s="2">
-        <v>42460</v>
-      </c>
-      <c r="B39" s="99" t="s">
-        <v>476</v>
-      </c>
-      <c r="C39" s="99" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" s="4" customFormat="1" ht="180">
-      <c r="A40" s="2">
-        <v>42460</v>
-      </c>
-      <c r="B40" s="99" t="s">
-        <v>475</v>
-      </c>
-      <c r="C40" s="99" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" s="4" customFormat="1" ht="60">
+    <row r="41" spans="1:3" s="4" customFormat="1" ht="120">
       <c r="A41" s="2">
         <v>42460</v>
       </c>
       <c r="B41" s="99" t="s">
+        <v>477</v>
+      </c>
+      <c r="C41" s="99" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="4" customFormat="1" ht="30">
+      <c r="A42" s="2">
+        <v>42460</v>
+      </c>
+      <c r="B42" s="99" t="s">
+        <v>476</v>
+      </c>
+      <c r="C42" s="99" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="4" customFormat="1" ht="180">
+      <c r="A43" s="2">
+        <v>42460</v>
+      </c>
+      <c r="B43" s="99" t="s">
+        <v>475</v>
+      </c>
+      <c r="C43" s="99" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="4" customFormat="1" ht="60">
+      <c r="A44" s="2">
+        <v>42460</v>
+      </c>
+      <c r="B44" s="99" t="s">
         <v>478</v>
       </c>
-      <c r="C41" s="99" t="s">
+      <c r="C44" s="99" t="s">
         <v>479</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="4" customFormat="1" ht="105">
-      <c r="A42" s="2">
-        <v>42459</v>
-      </c>
-      <c r="B42" s="99" t="s">
-        <v>470</v>
-      </c>
-      <c r="C42" s="98" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="4" customFormat="1" ht="60">
-      <c r="A43" s="2">
-        <v>42459</v>
-      </c>
-      <c r="B43" s="99" t="s">
-        <v>241</v>
-      </c>
-      <c r="C43" s="99" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" s="4" customFormat="1">
-      <c r="A44" s="2">
-        <v>42458</v>
-      </c>
-      <c r="B44" s="97" t="s">
-        <v>470</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="4" customFormat="1" ht="105">
       <c r="A45" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B45" s="96" t="s">
-        <v>254</v>
-      </c>
-      <c r="C45" s="100" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="60">
+        <v>42459</v>
+      </c>
+      <c r="B45" s="99" t="s">
+        <v>470</v>
+      </c>
+      <c r="C45" s="98" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="4" customFormat="1" ht="60">
       <c r="A46" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B46" s="96" t="s">
-        <v>462</v>
-      </c>
-      <c r="C46" s="44" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="45">
+        <v>42459</v>
+      </c>
+      <c r="B46" s="99" t="s">
+        <v>241</v>
+      </c>
+      <c r="C46" s="99" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="4" customFormat="1">
       <c r="A47" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B47" s="96" t="s">
-        <v>463</v>
-      </c>
-      <c r="C47" s="44" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>42458</v>
+      </c>
+      <c r="B47" s="97" t="s">
+        <v>470</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="4" customFormat="1" ht="105">
       <c r="A48" s="2">
         <v>42456</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="C48" s="44" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="45">
+      <c r="B48" s="96" t="s">
+        <v>254</v>
+      </c>
+      <c r="C48" s="100" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="60">
       <c r="A49" s="2">
         <v>42456</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="96" t="s">
+        <v>462</v>
+      </c>
+      <c r="C49" s="44" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="45">
+      <c r="A50" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B50" s="96" t="s">
+        <v>463</v>
+      </c>
+      <c r="C50" s="44" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C51" s="44" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="45">
+      <c r="A52" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="C49" s="44" t="s">
+      <c r="C52" s="44" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="77.25">
-      <c r="A50" s="79">
+    <row r="53" spans="1:3" ht="77.25">
+      <c r="A53" s="79">
         <v>42453</v>
       </c>
-      <c r="B50" s="78" t="s">
+      <c r="B53" s="78" t="s">
         <v>264</v>
       </c>
-      <c r="C50" s="78" t="s">
+      <c r="C53" s="78" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="26.25">
-      <c r="A51" s="79">
+    <row r="54" spans="1:3" ht="26.25">
+      <c r="A54" s="79">
         <v>42453</v>
       </c>
-      <c r="B51" s="78" t="s">
+      <c r="B54" s="78" t="s">
         <v>262</v>
       </c>
-      <c r="C51" s="78" t="s">
+      <c r="C54" s="78" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="39">
-      <c r="A52" s="79">
+    <row r="55" spans="1:3" ht="39">
+      <c r="A55" s="79">
         <v>42452</v>
       </c>
-      <c r="B52" s="78" t="s">
+      <c r="B55" s="78" t="s">
         <v>260</v>
       </c>
-      <c r="C52" s="78" t="s">
+      <c r="C55" s="78" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="165">
-      <c r="A53" s="75">
+    <row r="56" spans="1:3" ht="165">
+      <c r="A56" s="75">
         <v>42451</v>
       </c>
-      <c r="B53" s="74" t="s">
+      <c r="B56" s="74" t="s">
         <v>247</v>
       </c>
-      <c r="C53" s="100" t="s">
+      <c r="C56" s="100" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="45">
-      <c r="A54" s="2">
+    <row r="57" spans="1:3" ht="45">
+      <c r="A57" s="2">
         <v>42451</v>
       </c>
-      <c r="B54" s="100" t="s">
+      <c r="B57" s="100" t="s">
         <v>249</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="30">
-      <c r="A55" s="2">
+    <row r="58" spans="1:3" ht="30">
+      <c r="A58" s="2">
         <v>42451</v>
       </c>
-      <c r="B55" s="96" t="s">
+      <c r="B58" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="165">
-      <c r="A56" s="2">
+    <row r="59" spans="1:3" ht="165">
+      <c r="A59" s="2">
         <v>42451</v>
       </c>
-      <c r="B56" s="96" t="s">
+      <c r="B59" s="96" t="s">
         <v>253</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="64.5">
-      <c r="A57" s="79">
+    <row r="60" spans="1:3" ht="64.5">
+      <c r="A60" s="79">
         <v>42451</v>
       </c>
-      <c r="B57" s="78" t="s">
+      <c r="B60" s="78" t="s">
         <v>253</v>
       </c>
-      <c r="C57" s="78" t="s">
+      <c r="C60" s="78" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="64.5">
-      <c r="A58" s="79">
+    <row r="61" spans="1:3" ht="64.5">
+      <c r="A61" s="79">
         <v>42447</v>
       </c>
-      <c r="B58" s="78" t="s">
+      <c r="B61" s="78" t="s">
         <v>257</v>
       </c>
-      <c r="C58" s="78" t="s">
+      <c r="C61" s="78" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="2">
+    <row r="62" spans="1:3">
+      <c r="A62" s="2">
         <v>42440</v>
       </c>
-      <c r="B59" s="100" t="s">
+      <c r="B62" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="C59" s="100" t="s">
+      <c r="C62" s="100" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="75">
-      <c r="A60" s="2">
+    <row r="63" spans="1:3" ht="75">
+      <c r="A63" s="2">
         <v>42436</v>
       </c>
-      <c r="B60" s="96" t="s">
+      <c r="B63" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="39">
-      <c r="A61" s="79">
+    <row r="64" spans="1:3" ht="39">
+      <c r="A64" s="79">
         <v>42431</v>
       </c>
-      <c r="B61" s="78" t="s">
+      <c r="B64" s="78" t="s">
         <v>274</v>
       </c>
-      <c r="C61" s="78" t="s">
+      <c r="C64" s="78" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="26.25">
-      <c r="A62" s="79">
+    <row r="65" spans="1:3" ht="26.25">
+      <c r="A65" s="79">
         <v>42431</v>
       </c>
-      <c r="B62" s="78" t="s">
+      <c r="B65" s="78" t="s">
         <v>272</v>
       </c>
-      <c r="C62" s="78" t="s">
+      <c r="C65" s="78" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="51.75">
-      <c r="A63" s="79">
+    <row r="66" spans="1:3" ht="51.75">
+      <c r="A66" s="79">
         <v>42430</v>
       </c>
-      <c r="B63" s="78" t="s">
+      <c r="B66" s="78" t="s">
         <v>270</v>
       </c>
-      <c r="C63" s="78" t="s">
+      <c r="C66" s="78" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="26.25">
-      <c r="A64" s="79">
+    <row r="67" spans="1:3" ht="26.25">
+      <c r="A67" s="79">
         <v>42428</v>
       </c>
-      <c r="B64" s="78" t="s">
+      <c r="B67" s="78" t="s">
         <v>268</v>
       </c>
-      <c r="C64" s="78" t="s">
+      <c r="C67" s="78" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="30">
-      <c r="A65" s="2">
-        <v>42426</v>
-      </c>
-      <c r="B65" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="C65" s="100" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="77.25">
-      <c r="A66" s="79">
-        <v>42426</v>
-      </c>
-      <c r="B66" s="78" t="s">
-        <v>266</v>
-      </c>
-      <c r="C66" s="78" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="2">
-        <v>42425</v>
-      </c>
-      <c r="B67" s="100" t="s">
-        <v>241</v>
-      </c>
-      <c r="C67" s="100" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="30">
       <c r="A68" s="2">
+        <v>42426</v>
+      </c>
+      <c r="B68" s="100" t="s">
+        <v>186</v>
+      </c>
+      <c r="C68" s="100" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="77.25">
+      <c r="A69" s="79">
+        <v>42426</v>
+      </c>
+      <c r="B69" s="78" t="s">
+        <v>266</v>
+      </c>
+      <c r="C69" s="78" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="2">
         <v>42425</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B70" s="100" t="s">
+        <v>241</v>
+      </c>
+      <c r="C70" s="100" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="2">
+        <v>42425</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="26.25">
-      <c r="A69" s="79">
+    <row r="72" spans="1:3" ht="26.25">
+      <c r="A72" s="79">
         <v>42425</v>
       </c>
-      <c r="B69" s="78" t="s">
+      <c r="B72" s="78" t="s">
         <v>276</v>
       </c>
-      <c r="C69" s="78" t="s">
+      <c r="C72" s="78" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="79">
+    <row r="73" spans="1:3">
+      <c r="A73" s="79">
         <v>42425</v>
       </c>
-      <c r="B70" s="78" t="s">
+      <c r="B73" s="78" t="s">
         <v>276</v>
       </c>
-      <c r="C70" s="78" t="s">
+      <c r="C73" s="78" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="26.25">
-      <c r="A71" s="79">
+    <row r="74" spans="1:3" ht="26.25">
+      <c r="A74" s="79">
         <v>42425</v>
       </c>
-      <c r="B71" s="78" t="s">
+      <c r="B74" s="78" t="s">
         <v>279</v>
       </c>
-      <c r="C71" s="78" t="s">
+      <c r="C74" s="78" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="165">
-      <c r="A72" s="2">
+    <row r="75" spans="1:3" ht="165">
+      <c r="A75" s="2">
         <v>42424</v>
       </c>
-      <c r="B72" s="100" t="s">
+      <c r="B75" s="100" t="s">
         <v>239</v>
       </c>
-      <c r="C72" s="114" t="s">
+      <c r="C75" s="114" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="45">
-      <c r="A73" s="2">
+    <row r="76" spans="1:3" ht="45">
+      <c r="A76" s="2">
         <v>42423</v>
       </c>
-      <c r="B73" s="96" t="s">
+      <c r="B76" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C76" s="11" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="79">
+    <row r="77" spans="1:3">
+      <c r="A77" s="79">
         <v>42423</v>
       </c>
-      <c r="B74" s="78" t="s">
+      <c r="B77" s="78" t="s">
         <v>281</v>
       </c>
-      <c r="C74" s="78" t="s">
+      <c r="C77" s="78" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="90">
-      <c r="A75" s="2">
+    <row r="78" spans="1:3" ht="90">
+      <c r="A78" s="2">
         <v>42422</v>
       </c>
-      <c r="B75" s="100" t="s">
+      <c r="B78" s="100" t="s">
         <v>236</v>
       </c>
-      <c r="C75" s="100" t="s">
+      <c r="C78" s="100" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="60">
-      <c r="A76" s="2">
+    <row r="79" spans="1:3" ht="60">
+      <c r="A79" s="2">
         <v>42419</v>
       </c>
-      <c r="B76" s="10" t="s">
+      <c r="B79" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="C76" s="36" t="s">
+      <c r="C79" s="36" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="195">
-      <c r="A77" s="2">
+    <row r="80" spans="1:3" ht="195">
+      <c r="A80" s="2">
         <v>42418</v>
       </c>
-      <c r="B77" s="10" t="s">
+      <c r="B80" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C77" s="18" t="s">
+      <c r="C80" s="18" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="45">
-      <c r="A78" s="2">
+    <row r="81" spans="1:3" ht="45">
+      <c r="A81" s="2">
         <v>42403</v>
       </c>
-      <c r="B78" s="96" t="s">
+      <c r="B81" s="96" t="s">
         <v>229</v>
       </c>
-      <c r="C78" s="12" t="s">
+      <c r="C81" s="12" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="75">
-      <c r="A79" s="2">
+    <row r="82" spans="1:3" ht="75">
+      <c r="A82" s="2">
         <v>42403</v>
       </c>
-      <c r="B79" s="12" t="s">
+      <c r="B82" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="C79" s="12" t="s">
+      <c r="C82" s="12" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="90">
-      <c r="A80" s="2">
+    <row r="83" spans="1:3" ht="90">
+      <c r="A83" s="2">
         <v>42403</v>
       </c>
-      <c r="B80" s="12"/>
-      <c r="C80" s="12" t="s">
+      <c r="B83" s="12"/>
+      <c r="C83" s="12" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="90">
-      <c r="A81" s="2">
+    <row r="84" spans="1:3" ht="90">
+      <c r="A84" s="2">
         <v>42398</v>
-      </c>
-      <c r="B81" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C81" s="12" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="45">
-      <c r="A82" s="2">
-        <v>42398</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="C82" s="12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="2">
-        <v>42397</v>
-      </c>
-      <c r="B83" s="96" t="s">
-        <v>201</v>
-      </c>
-      <c r="C83" s="14" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="45">
-      <c r="A84" s="2">
-        <v>42396</v>
       </c>
       <c r="B84" s="12" t="s">
         <v>196</v>
       </c>
       <c r="C84" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="45">
+      <c r="A85" s="2">
+        <v>42398</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="2">
+        <v>42397</v>
+      </c>
+      <c r="B86" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="45">
+      <c r="A87" s="2">
+        <v>42396</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C87" s="12" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="30">
-      <c r="A85" s="2">
+    <row r="88" spans="1:3" ht="30">
+      <c r="A88" s="2">
         <v>42396</v>
       </c>
-      <c r="B85" s="96" t="s">
+      <c r="B88" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="C85" s="14" t="s">
+      <c r="C88" s="14" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="128.25">
-      <c r="A86" s="79">
+    <row r="89" spans="1:3" ht="128.25">
+      <c r="A89" s="79">
         <v>42386</v>
       </c>
-      <c r="B86" s="78" t="s">
+      <c r="B89" s="78" t="s">
         <v>283</v>
       </c>
-      <c r="C86" s="78" t="s">
+      <c r="C89" s="78" t="s">
         <v>282</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="64.5">
-      <c r="A87" s="79">
-        <v>42386</v>
-      </c>
-      <c r="B87" s="78" t="s">
-        <v>285</v>
-      </c>
-      <c r="C87" s="78" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="45">
-      <c r="A88" s="2">
-        <v>42384</v>
-      </c>
-      <c r="B88" s="100" t="s">
-        <v>220</v>
-      </c>
-      <c r="C88" s="100" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="180">
-      <c r="A89" s="2">
-        <v>42382</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="64.5">
       <c r="A90" s="79">
+        <v>42386</v>
+      </c>
+      <c r="B90" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="C90" s="78" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="45">
+      <c r="A91" s="2">
+        <v>42384</v>
+      </c>
+      <c r="B91" s="100" t="s">
+        <v>220</v>
+      </c>
+      <c r="C91" s="100" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="180">
+      <c r="A92" s="2">
         <v>42382</v>
       </c>
-      <c r="B90" s="78" t="s">
+      <c r="B92" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="64.5">
+      <c r="A93" s="79">
+        <v>42382</v>
+      </c>
+      <c r="B93" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="C90" s="78" t="s">
+      <c r="C93" s="78" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="30">
-      <c r="A91" s="2">
+    <row r="94" spans="1:3" ht="30">
+      <c r="A94" s="2">
         <v>42381</v>
       </c>
-      <c r="B91" s="100" t="s">
+      <c r="B94" s="100" t="s">
         <v>216</v>
       </c>
-      <c r="C91" s="100" t="s">
+      <c r="C94" s="100" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="45">
-      <c r="A92" s="2">
+    <row r="95" spans="1:3" ht="45">
+      <c r="A95" s="2">
         <v>42380</v>
       </c>
-      <c r="B92" s="16" t="s">
+      <c r="B95" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C92" s="16" t="s">
+      <c r="C95" s="16" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="75">
-      <c r="A93" s="2">
+    <row r="96" spans="1:3" ht="75">
+      <c r="A96" s="2">
         <v>42380</v>
       </c>
-      <c r="B93" s="50" t="s">
+      <c r="B96" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C93" s="17" t="s">
+      <c r="C96" s="17" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="180">
-      <c r="A94" s="2">
+    <row r="97" spans="1:3" ht="180">
+      <c r="A97" s="2">
         <v>42380</v>
       </c>
-      <c r="B94" s="50" t="s">
+      <c r="B97" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C94" s="18" t="s">
+      <c r="C97" s="18" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="217.5">
-      <c r="A95" s="79">
+    <row r="98" spans="1:3" ht="217.5">
+      <c r="A98" s="79">
         <v>42380</v>
       </c>
-      <c r="B95" s="78" t="s">
+      <c r="B98" s="78" t="s">
         <v>288</v>
       </c>
-      <c r="C95" s="78" t="s">
+      <c r="C98" s="78" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="102.75">
-      <c r="A96" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B96" s="78" t="s">
-        <v>291</v>
-      </c>
-      <c r="C96" s="78" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="102.75">
-      <c r="A97" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B97" s="78" t="s">
-        <v>293</v>
-      </c>
-      <c r="C97" s="78" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="141">
-      <c r="A98" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B98" s="78" t="s">
-        <v>297</v>
-      </c>
-      <c r="C98" s="78" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="77.25">
+    <row r="99" spans="1:3" ht="102.75">
       <c r="A99" s="79">
         <v>42378</v>
       </c>
       <c r="B99" s="78" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C99" s="78" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="102.75">
@@ -4928,161 +4958,161 @@
         <v>42378</v>
       </c>
       <c r="B100" s="78" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C100" s="78" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="60">
-      <c r="A101" s="2">
-        <v>42377</v>
-      </c>
-      <c r="B101" s="100" t="s">
-        <v>202</v>
-      </c>
-      <c r="C101" s="100" t="s">
-        <v>211</v>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="141">
+      <c r="A101" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B101" s="78" t="s">
+        <v>297</v>
+      </c>
+      <c r="C101" s="78" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="77.25">
       <c r="A102" s="79">
-        <v>42376</v>
+        <v>42378</v>
       </c>
       <c r="B102" s="78" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C102" s="78" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="45">
-      <c r="A103" s="2">
-        <v>42375</v>
-      </c>
-      <c r="B103" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C103" s="100" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="102.75">
+      <c r="A103" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B103" s="78" t="s">
+        <v>295</v>
+      </c>
+      <c r="C103" s="78" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="60">
       <c r="A104" s="2">
-        <v>42369</v>
+        <v>42377</v>
       </c>
       <c r="B104" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="C104" s="19" t="s">
+      <c r="C104" s="100" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="77.25">
+      <c r="A105" s="79">
+        <v>42376</v>
+      </c>
+      <c r="B105" s="78" t="s">
+        <v>300</v>
+      </c>
+      <c r="C105" s="78" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="45">
+      <c r="A106" s="2">
+        <v>42375</v>
+      </c>
+      <c r="B106" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C106" s="100" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="2">
+        <v>42369</v>
+      </c>
+      <c r="B107" s="100" t="s">
+        <v>202</v>
+      </c>
+      <c r="C107" s="19" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="195">
-      <c r="A105" s="2">
+    <row r="108" spans="1:3" ht="195">
+      <c r="A108" s="2">
         <v>42368</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C105" s="19" t="s">
+      <c r="C108" s="19" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="135">
-      <c r="A106" s="2">
+    <row r="109" spans="1:3" ht="135">
+      <c r="A109" s="2">
         <v>42368</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C106" s="20" t="s">
+      <c r="C109" s="20" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="45">
-      <c r="A107" s="2">
+    <row r="110" spans="1:3" ht="45">
+      <c r="A110" s="2">
         <v>42368</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B110" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C107" s="20" t="s">
+      <c r="C110" s="20" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="30">
-      <c r="A108" s="2">
-        <v>42366</v>
-      </c>
-      <c r="B108" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C108" s="20" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="30">
-      <c r="A109" s="2">
-        <v>42366</v>
-      </c>
-      <c r="B109" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C109" s="20" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="150">
-      <c r="A110" s="2">
-        <v>42361</v>
-      </c>
-      <c r="C110" s="20" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="30">
       <c r="A111" s="2">
-        <v>42361</v>
+        <v>42366</v>
+      </c>
+      <c r="B111" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="C111" s="20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="270">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="30">
       <c r="A112" s="2">
-        <v>42361</v>
-      </c>
-      <c r="B112" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C112" s="22" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="30">
+        <v>42366</v>
+      </c>
+      <c r="B112" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C112" s="20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="150">
       <c r="A113" s="2">
         <v>42361</v>
       </c>
-      <c r="B113" s="100" t="s">
-        <v>53</v>
-      </c>
       <c r="C113" s="20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="30">
       <c r="A114" s="2">
         <v>42361</v>
       </c>
-      <c r="B114" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C114" s="21" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="225">
+      <c r="C114" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="270">
       <c r="A115" s="2">
         <v>42361</v>
       </c>
@@ -5090,318 +5120,322 @@
         <v>186</v>
       </c>
       <c r="C115" s="22" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="60">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="30">
       <c r="A116" s="2">
         <v>42361</v>
       </c>
       <c r="B116" s="100" t="s">
-        <v>49</v>
-      </c>
-      <c r="C116" s="22" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="90">
+        <v>53</v>
+      </c>
+      <c r="C116" s="20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
       <c r="A117" s="2">
         <v>42361</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C117" s="22" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="60">
+      <c r="B117" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C117" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="225">
       <c r="A118" s="2">
         <v>42361</v>
       </c>
-      <c r="B118" s="24" t="s">
+      <c r="B118" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C118" s="22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="60">
+      <c r="A119" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B119" s="100" t="s">
+        <v>49</v>
+      </c>
+      <c r="C119" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="90">
+      <c r="A120" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C118" s="24" t="s">
+      <c r="C120" s="22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="60">
+      <c r="A121" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B121" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C121" s="24" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
-      <c r="A119" s="40">
+    <row r="122" spans="1:3">
+      <c r="A122" s="40">
         <v>42360</v>
       </c>
-      <c r="B119" s="50" t="s">
+      <c r="B122" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C122" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
-      <c r="A120" s="40">
+    <row r="123" spans="1:3">
+      <c r="A123" s="40">
         <v>42360</v>
       </c>
-      <c r="B120" s="50" t="s">
+      <c r="B123" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C123" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="102.75">
-      <c r="A121" s="80">
+    <row r="124" spans="1:3" ht="102.75">
+      <c r="A124" s="80">
         <v>42360</v>
       </c>
-      <c r="B121" s="78" t="s">
+      <c r="B124" s="78" t="s">
         <v>302</v>
       </c>
-      <c r="C121" s="78" t="s">
+      <c r="C124" s="78" t="s">
         <v>301</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="30">
-      <c r="A122" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B122" s="100" t="s">
-        <v>43</v>
-      </c>
-      <c r="C122" s="100" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B123" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="C123" s="23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B124" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="C124" s="25" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="30">
       <c r="A125" s="2">
         <v>42356</v>
       </c>
-      <c r="B125" s="96"/>
-      <c r="C125" s="25" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="60">
+      <c r="B125" s="100" t="s">
+        <v>43</v>
+      </c>
+      <c r="C125" s="100" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
       <c r="A126" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B126" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="C126" s="26" t="s">
-        <v>92</v>
+        <v>42356</v>
+      </c>
+      <c r="B126" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="C126" s="23" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B127" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C127" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="150">
+        <v>42356</v>
+      </c>
+      <c r="B127" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C127" s="25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="30">
       <c r="A128" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B128" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C128" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="120">
+        <v>42356</v>
+      </c>
+      <c r="B128" s="96"/>
+      <c r="C128" s="25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="60">
       <c r="A129" s="2">
         <v>42355</v>
       </c>
-      <c r="B129" s="100" t="s">
-        <v>168</v>
+      <c r="B129" s="96" t="s">
+        <v>91</v>
       </c>
       <c r="C129" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="30">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
       <c r="A130" s="2">
         <v>42355</v>
       </c>
-      <c r="B130" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C130" s="28" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
+      <c r="B130" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C130" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="150">
       <c r="A131" s="2">
         <v>42355</v>
       </c>
-      <c r="B131" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="C131" s="29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="75">
+      <c r="B131" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C131" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="120">
       <c r="A132" s="2">
         <v>42355</v>
       </c>
-      <c r="B132" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C132" s="29" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="135">
+      <c r="B132" s="100" t="s">
+        <v>168</v>
+      </c>
+      <c r="C132" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="30">
       <c r="A133" s="2">
         <v>42355</v>
       </c>
-      <c r="B133" s="100" t="s">
-        <v>173</v>
-      </c>
-      <c r="C133" s="29" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="75">
+      <c r="B133" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C133" s="28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
       <c r="A134" s="2">
         <v>42355</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C134" s="42" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="30">
+      <c r="B134" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C134" s="29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="75">
       <c r="A135" s="2">
         <v>42355</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C135" s="30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3">
+      <c r="B135" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C135" s="29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="135">
       <c r="A136" s="2">
         <v>42355</v>
       </c>
-      <c r="C136" s="30" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3">
+      <c r="B136" s="100" t="s">
+        <v>173</v>
+      </c>
+      <c r="C136" s="29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="75">
       <c r="A137" s="2">
         <v>42355</v>
       </c>
-      <c r="B137" s="42"/>
-      <c r="C137" s="30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3">
+      <c r="B137" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C137" s="42" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="30">
       <c r="A138" s="2">
         <v>42355</v>
       </c>
-      <c r="B138" s="42"/>
+      <c r="B138" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="C138" s="30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="2">
+        <v>42355</v>
+      </c>
+      <c r="C139" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="2">
+        <v>42355</v>
+      </c>
+      <c r="B140" s="42"/>
+      <c r="C140" s="30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="2">
+        <v>42355</v>
+      </c>
+      <c r="B141" s="42"/>
+      <c r="C141" s="30" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="75">
-      <c r="A139" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B139" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="C139" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="30">
-      <c r="A140" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B140" s="26"/>
-      <c r="C140" s="31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="75">
-      <c r="A141" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B141" s="26"/>
-      <c r="C141" s="70" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" ht="75">
       <c r="A142" s="2">
         <v>42352</v>
       </c>
-      <c r="B142" s="26"/>
-      <c r="C142" s="32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3">
+      <c r="B142" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C142" s="30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="30">
       <c r="A143" s="2">
         <v>42352</v>
       </c>
-      <c r="B143" s="96"/>
-      <c r="C143" s="33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
+      <c r="B143" s="26"/>
+      <c r="C143" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="75">
       <c r="A144" s="2">
         <v>42352</v>
       </c>
-      <c r="B144" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C144" s="34" t="s">
-        <v>72</v>
+      <c r="B144" s="26"/>
+      <c r="C144" s="70" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="145" spans="1:6">
       <c r="A145" s="2">
         <v>42352</v>
       </c>
-      <c r="B145" s="96"/>
-      <c r="C145" s="34" t="s">
-        <v>73</v>
+      <c r="B145" s="26"/>
+      <c r="C145" s="32" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -5409,545 +5443,541 @@
         <v>42352</v>
       </c>
       <c r="B146" s="96"/>
-      <c r="C146" s="37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" ht="30">
+      <c r="C146" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
       <c r="A147" s="2">
         <v>42352</v>
       </c>
-      <c r="B147" s="37"/>
-      <c r="C147" s="37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" ht="30">
+      <c r="B147" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C147" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
       <c r="A148" s="2">
         <v>42352</v>
       </c>
       <c r="B148" s="96"/>
-      <c r="C148" s="96" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" ht="45">
+      <c r="C148" s="34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
       <c r="A149" s="2">
         <v>42352</v>
       </c>
-      <c r="B149" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C149" s="96" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" ht="45">
+      <c r="B149" s="96"/>
+      <c r="C149" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="30">
       <c r="A150" s="2">
         <v>42352</v>
       </c>
-      <c r="B150" s="100"/>
-      <c r="C150" s="39" t="s">
-        <v>80</v>
+      <c r="B150" s="37"/>
+      <c r="C150" s="37" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="30">
       <c r="A151" s="2">
         <v>42352</v>
       </c>
-      <c r="B151" s="38"/>
-      <c r="C151" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="F151" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" ht="75">
+      <c r="B151" s="96"/>
+      <c r="C151" s="96" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="45">
       <c r="A152" s="2">
         <v>42352</v>
       </c>
-      <c r="B152" s="41"/>
-      <c r="C152" s="41" t="s">
-        <v>82</v>
+      <c r="B152" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C152" s="96" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="153" spans="1:6" ht="45">
       <c r="A153" s="2">
         <v>42352</v>
       </c>
-      <c r="B153" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C153" s="41" t="s">
-        <v>90</v>
+      <c r="B153" s="100"/>
+      <c r="C153" s="39" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="154" spans="1:6" ht="30">
       <c r="A154" s="2">
         <v>42352</v>
       </c>
-      <c r="B154" s="43"/>
-      <c r="C154" s="43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" ht="45">
+      <c r="B154" s="38"/>
+      <c r="C154" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="F154" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="75">
       <c r="A155" s="2">
         <v>42352</v>
       </c>
-      <c r="B155" s="44"/>
-      <c r="C155" s="44" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="30">
+      <c r="B155" s="41"/>
+      <c r="C155" s="41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="45">
       <c r="A156" s="2">
         <v>42352</v>
       </c>
-      <c r="B156" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="C156" s="46" t="s">
-        <v>86</v>
+      <c r="B156" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C156" s="41" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="30">
       <c r="A157" s="2">
         <v>42352</v>
       </c>
-      <c r="B157" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C157" s="47" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6">
+      <c r="B157" s="43"/>
+      <c r="C157" s="43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="45">
       <c r="A158" s="2">
         <v>42352</v>
       </c>
-      <c r="B158" s="100" t="s">
+      <c r="B158" s="44"/>
+      <c r="C158" s="44" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="30">
+      <c r="A159" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B159" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C159" s="46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="30">
+      <c r="A160" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B160" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C160" s="47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B161" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="C158" s="48" t="s">
+      <c r="C161" s="48" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="135">
-      <c r="A159" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B159" s="49"/>
-      <c r="C159" s="49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="60">
-      <c r="A160" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B160" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="C160" s="51" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="30">
-      <c r="A161" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B161" s="96"/>
-      <c r="C161" s="53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="120">
+    <row r="162" spans="1:3" ht="135">
       <c r="A162" s="2">
         <v>42349</v>
       </c>
-      <c r="B162" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C162" s="53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="150">
+      <c r="B162" s="49"/>
+      <c r="C162" s="49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="60">
       <c r="A163" s="2">
         <v>42349</v>
       </c>
-      <c r="B163" s="52"/>
-      <c r="C163" s="52" t="s">
-        <v>59</v>
+      <c r="B163" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C163" s="51" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="30">
       <c r="A164" s="2">
         <v>42349</v>
       </c>
-      <c r="B164" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C164" s="54" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3">
+      <c r="B164" s="96"/>
+      <c r="C164" s="53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="120">
       <c r="A165" s="2">
         <v>42349</v>
       </c>
-      <c r="B165" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C165" s="55" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
+      <c r="B165" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C165" s="53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="150">
       <c r="A166" s="2">
         <v>42349</v>
       </c>
-      <c r="B166" s="100"/>
-      <c r="C166" s="57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3">
+      <c r="B166" s="52"/>
+      <c r="C166" s="52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="30">
       <c r="A167" s="2">
         <v>42349</v>
       </c>
-      <c r="B167" s="58"/>
-      <c r="C167" s="58" t="s">
-        <v>62</v>
+      <c r="B167" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C167" s="54" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="2">
         <v>42349</v>
       </c>
-      <c r="B168" s="59"/>
-      <c r="C168" s="59" t="s">
-        <v>70</v>
+      <c r="B168" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C168" s="55" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="2">
         <v>42349</v>
       </c>
-      <c r="B169" s="60"/>
-      <c r="C169" s="60" t="s">
-        <v>64</v>
+      <c r="B169" s="100"/>
+      <c r="C169" s="57" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="2">
         <v>42349</v>
       </c>
-      <c r="B170" s="61"/>
-      <c r="C170" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" ht="60">
+      <c r="B170" s="58"/>
+      <c r="C170" s="58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
       <c r="A171" s="2">
         <v>42349</v>
       </c>
-      <c r="B171" s="62" t="s">
+      <c r="B171" s="59"/>
+      <c r="C171" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" s="2">
+        <v>42349</v>
+      </c>
+      <c r="B172" s="60"/>
+      <c r="C172" s="60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" s="2">
+        <v>42349</v>
+      </c>
+      <c r="B173" s="61"/>
+      <c r="C173" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="60">
+      <c r="A174" s="2">
+        <v>42349</v>
+      </c>
+      <c r="B174" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="C171" s="100" t="s">
+      <c r="C174" s="100" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="90">
-      <c r="A172" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B172" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C172" s="62" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="30">
-      <c r="A173" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C173" s="62" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3">
-      <c r="A174" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B174" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C174" s="63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" ht="90">
       <c r="A175" s="2">
         <v>42345</v>
       </c>
-      <c r="B175" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C175" s="64" t="s">
-        <v>29</v>
+      <c r="B175" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C175" s="62" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="30">
       <c r="A176" s="2">
         <v>42345</v>
       </c>
-      <c r="B176" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C176" s="65" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" ht="195">
+      <c r="B176" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C176" s="62" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
       <c r="A177" s="2">
         <v>42345</v>
       </c>
-      <c r="B177" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C177" s="66" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" ht="135">
+      <c r="B177" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C177" s="63" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
       <c r="A178" s="2">
         <v>42345</v>
       </c>
-      <c r="B178" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="C178" s="67" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="75">
+      <c r="B178" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C178" s="64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="30">
       <c r="A179" s="2">
         <v>42345</v>
       </c>
-      <c r="B179" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="C179" s="68" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="75">
+      <c r="B179" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C179" s="65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="195">
       <c r="A180" s="2">
         <v>42345</v>
       </c>
       <c r="B180" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C180" s="69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" ht="30">
+      <c r="C180" s="66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="135">
       <c r="A181" s="2">
         <v>42345</v>
       </c>
       <c r="B181" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C181" s="73" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3">
+        <v>31</v>
+      </c>
+      <c r="C181" s="67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="75">
       <c r="A182" s="2">
         <v>42345</v>
       </c>
-      <c r="B182" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="C182" s="73" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3">
+      <c r="B182" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C182" s="68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="75">
       <c r="A183" s="2">
         <v>42345</v>
       </c>
-      <c r="B183" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="C183" s="73" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" ht="60">
+      <c r="B183" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C183" s="69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="30">
       <c r="A184" s="2">
         <v>42345</v>
       </c>
-      <c r="B184" s="96" t="s">
-        <v>39</v>
+      <c r="B184" s="100" t="s">
+        <v>12</v>
       </c>
       <c r="C184" s="73" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" ht="150">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
       <c r="A185" s="2">
         <v>42345</v>
       </c>
-      <c r="B185" s="15" t="s">
-        <v>43</v>
+      <c r="B185" s="71" t="s">
+        <v>39</v>
       </c>
       <c r="C185" s="73" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
       <c r="A186" s="2">
         <v>42345</v>
       </c>
-      <c r="B186" s="100" t="s">
+      <c r="B186" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="C186" s="76" t="s">
-        <v>45</v>
+      <c r="C186" s="73" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="60">
       <c r="A187" s="2">
         <v>42345</v>
       </c>
-      <c r="B187" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C187" s="77" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" ht="105">
+      <c r="B187" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="C187" s="73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="150">
       <c r="A188" s="2">
         <v>42345</v>
       </c>
-      <c r="B188" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C188" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3">
+      <c r="B188" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C188" s="73" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="45">
       <c r="A189" s="2">
         <v>42345</v>
       </c>
-      <c r="B189" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C189" s="96" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
+      <c r="B189" s="100" t="s">
+        <v>39</v>
+      </c>
+      <c r="C189" s="76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="60">
       <c r="A190" s="2">
         <v>42345</v>
       </c>
-      <c r="B190" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C190" s="96" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" ht="75">
+      <c r="B190" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C190" s="77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="105">
       <c r="A191" s="2">
         <v>42345</v>
       </c>
-      <c r="B191" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C191" s="96" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" ht="45">
+      <c r="B191" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
       <c r="A192" s="2">
         <v>42345</v>
       </c>
       <c r="B192" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C192" s="96" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B193" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C193" s="96" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" ht="75">
+      <c r="A194" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B194" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C194" s="96" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="45">
+      <c r="A195" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B195" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C192" s="96" t="s">
+      <c r="C195" s="96" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="141">
-      <c r="A193" s="80">
+    <row r="196" spans="1:3" ht="141">
+      <c r="A196" s="80">
         <v>42345</v>
       </c>
-      <c r="B193" s="78" t="s">
+      <c r="B196" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="C193" s="78" t="s">
+      <c r="C196" s="78" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="105">
-      <c r="A194" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C194" s="100" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="90">
-      <c r="A195" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C195" s="96" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" ht="75">
-      <c r="A196" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C196" s="96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" ht="30">
+    <row r="197" spans="1:3" ht="105">
       <c r="A197" s="2">
         <v>42341</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C197" s="96" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" ht="30">
+        <v>12</v>
+      </c>
+      <c r="C197" s="100" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="90">
       <c r="A198" s="2">
         <v>42341</v>
       </c>
@@ -5955,10 +5985,10 @@
         <v>15</v>
       </c>
       <c r="C198" s="96" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="75">
       <c r="A199" s="2">
         <v>42341</v>
       </c>
@@ -5966,18 +5996,18 @@
         <v>15</v>
       </c>
       <c r="C199" s="96" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" ht="90">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="30">
       <c r="A200" s="2">
         <v>42341</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C200" s="96" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="30">
@@ -5988,10 +6018,10 @@
         <v>15</v>
       </c>
       <c r="C201" s="96" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="150">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="45">
       <c r="A202" s="2">
         <v>42341</v>
       </c>
@@ -5999,73 +6029,73 @@
         <v>15</v>
       </c>
       <c r="C202" s="96" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="75">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="90">
       <c r="A203" s="2">
         <v>42341</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C203" s="96" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="90">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="30">
       <c r="A204" s="2">
         <v>42341</v>
       </c>
-      <c r="B204" s="100" t="s">
-        <v>12</v>
+      <c r="B204" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C204" s="96" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" ht="60">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="150">
       <c r="A205" s="2">
         <v>42341</v>
       </c>
-      <c r="B205" s="96" t="s">
+      <c r="B205" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C205" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="75">
       <c r="A206" s="2">
         <v>42341</v>
       </c>
-      <c r="B206" s="96" t="s">
-        <v>12</v>
+      <c r="B206" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C206" s="96" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="90">
       <c r="A207" s="2">
         <v>42341</v>
       </c>
-      <c r="B207" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C207" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3">
+      <c r="B207" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C207" s="96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="60">
       <c r="A208" s="2">
         <v>42341</v>
       </c>
       <c r="B208" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C208" s="7" t="s">
-        <v>166</v>
+      <c r="C208" s="96" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -6073,10 +6103,10 @@
         <v>42341</v>
       </c>
       <c r="B209" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C209" s="8" t="s">
-        <v>165</v>
+        <v>12</v>
+      </c>
+      <c r="C209" s="96" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -6086,307 +6116,340 @@
       <c r="B210" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C210" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" ht="75">
+      <c r="C210" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
       <c r="A211" s="2">
         <v>42341</v>
       </c>
       <c r="B211" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C211" s="100" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" ht="60">
+      <c r="C211" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
       <c r="A212" s="2">
         <v>42341</v>
       </c>
       <c r="B212" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C212" s="96" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" ht="60">
+        <v>15</v>
+      </c>
+      <c r="C212" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
       <c r="A213" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B213" s="96"/>
-      <c r="C213" s="96" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" ht="45">
+        <v>42341</v>
+      </c>
+      <c r="B213" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C213" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" ht="75">
       <c r="A214" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B214" s="96"/>
-      <c r="C214" s="96" t="s">
-        <v>8</v>
+        <v>42341</v>
+      </c>
+      <c r="B214" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C214" s="100" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="60">
       <c r="A215" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B215" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C215" s="96" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="60">
+      <c r="A216" s="2">
         <v>42340</v>
       </c>
-      <c r="B215" s="2" t="s">
+      <c r="B216" s="96"/>
+      <c r="C216" s="96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" ht="45">
+      <c r="A217" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B217" s="96"/>
+      <c r="C217" s="96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="60">
+      <c r="A218" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B218" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C215" s="96" t="s">
+      <c r="C218" s="96" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="1:3">
-      <c r="A216" s="2">
+    <row r="219" spans="1:3">
+      <c r="A219" s="2">
         <v>42339</v>
       </c>
-      <c r="B216" s="2"/>
-      <c r="C216" s="96" t="s">
+      <c r="B219" s="2"/>
+      <c r="C219" s="96" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
-      <c r="A217" s="2">
+    <row r="220" spans="1:3">
+      <c r="A220" s="2">
         <v>42339</v>
       </c>
-      <c r="B217" s="2"/>
-      <c r="C217" s="96" t="s">
+      <c r="B220" s="2"/>
+      <c r="C220" s="96" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="64.5">
-      <c r="A218" s="80">
+    <row r="221" spans="1:3" ht="64.5">
+      <c r="A221" s="80">
         <v>42334</v>
       </c>
-      <c r="B218" s="78" t="s">
+      <c r="B221" s="78" t="s">
         <v>309</v>
       </c>
-      <c r="C218" s="78" t="s">
+      <c r="C221" s="78" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="26.25">
-      <c r="A219" s="80">
+    <row r="222" spans="1:3" ht="26.25">
+      <c r="A222" s="80">
         <v>42334</v>
       </c>
-      <c r="B219" s="78" t="s">
+      <c r="B222" s="78" t="s">
         <v>307</v>
       </c>
-      <c r="C219" s="78" t="s">
+      <c r="C222" s="78" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="39">
-      <c r="A220" s="80">
+    <row r="223" spans="1:3" ht="39">
+      <c r="A223" s="80">
         <v>42334</v>
       </c>
-      <c r="B220" s="78" t="s">
+      <c r="B223" s="78" t="s">
         <v>272</v>
       </c>
-      <c r="C220" s="78" t="s">
+      <c r="C223" s="78" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="128.25">
-      <c r="A221" s="80">
+    <row r="224" spans="1:3" ht="128.25">
+      <c r="A224" s="80">
         <v>42333</v>
       </c>
-      <c r="B221" s="78" t="s">
+      <c r="B224" s="78" t="s">
         <v>268</v>
       </c>
-      <c r="C221" s="78" t="s">
+      <c r="C224" s="78" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="222" spans="1:3" ht="51.75">
-      <c r="A222" s="80">
+    <row r="225" spans="1:3" ht="51.75">
+      <c r="A225" s="80">
         <v>42333</v>
       </c>
-      <c r="B222" s="78" t="s">
+      <c r="B225" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C222" s="78" t="s">
+      <c r="C225" s="78" t="s">
         <v>311</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" ht="26.25">
-      <c r="A223" s="80">
-        <v>42331</v>
-      </c>
-      <c r="B223" s="78" t="s">
-        <v>313</v>
-      </c>
-      <c r="C223" s="78" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" ht="39">
-      <c r="A224" s="80">
-        <v>42329</v>
-      </c>
-      <c r="B224" s="78" t="s">
-        <v>315</v>
-      </c>
-      <c r="C224" s="78" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" ht="39">
-      <c r="A225" s="80">
-        <v>42328</v>
-      </c>
-      <c r="B225" s="78" t="s">
-        <v>324</v>
-      </c>
-      <c r="C225" s="78" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="26.25">
       <c r="A226" s="80">
-        <v>42328</v>
+        <v>42331</v>
       </c>
       <c r="B226" s="78" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="C226" s="78" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" ht="115.5">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" ht="39">
       <c r="A227" s="80">
-        <v>42328</v>
+        <v>42329</v>
       </c>
       <c r="B227" s="78" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C227" s="78" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" ht="90">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" ht="39">
       <c r="A228" s="80">
         <v>42328</v>
       </c>
       <c r="B228" s="78" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="C228" s="78" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" ht="153.75">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="26.25">
       <c r="A229" s="80">
         <v>42328</v>
       </c>
       <c r="B229" s="78" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="C229" s="78" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" ht="102.75">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" ht="115.5">
       <c r="A230" s="80">
-        <v>42324</v>
+        <v>42328</v>
       </c>
       <c r="B230" s="78" t="s">
-        <v>49</v>
+        <v>320</v>
       </c>
       <c r="C230" s="78" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="90">
       <c r="A231" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B231" s="78" t="s">
+        <v>317</v>
+      </c>
+      <c r="C231" s="78" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" ht="153.75">
+      <c r="A232" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B232" s="78" t="s">
+        <v>317</v>
+      </c>
+      <c r="C232" s="78" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" ht="102.75">
+      <c r="A233" s="80">
+        <v>42324</v>
+      </c>
+      <c r="B233" s="78" t="s">
+        <v>49</v>
+      </c>
+      <c r="C233" s="78" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="90">
+      <c r="A234" s="80">
         <v>42321</v>
       </c>
-      <c r="B231" s="78" t="s">
+      <c r="B234" s="78" t="s">
         <v>327</v>
       </c>
-      <c r="C231" s="78" t="s">
+      <c r="C234" s="78" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="26.25">
-      <c r="A232" s="80">
+    <row r="235" spans="1:3" ht="26.25">
+      <c r="A235" s="80">
         <v>42321</v>
       </c>
-      <c r="B232" s="78" t="s">
+      <c r="B235" s="78" t="s">
         <v>327</v>
       </c>
-      <c r="C232" s="78" t="s">
+      <c r="C235" s="78" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="77.25">
-      <c r="A233" s="79">
+    <row r="236" spans="1:3" ht="77.25">
+      <c r="A236" s="79">
         <v>42318</v>
       </c>
-      <c r="B233" s="78" t="s">
+      <c r="B236" s="78" t="s">
         <v>330</v>
       </c>
-      <c r="C233" s="78" t="s">
+      <c r="C236" s="78" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="115.5">
-      <c r="A234" s="79">
+    <row r="237" spans="1:3" ht="115.5">
+      <c r="A237" s="79">
         <v>42311</v>
       </c>
-      <c r="B234" s="78" t="s">
+      <c r="B237" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C234" s="78" t="s">
+      <c r="C237" s="78" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="235" spans="1:3" ht="77.25">
-      <c r="A235" s="79">
+    <row r="238" spans="1:3" ht="77.25">
+      <c r="A238" s="79">
         <v>42310</v>
       </c>
-      <c r="B235" s="78" t="s">
+      <c r="B238" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C235" s="78" t="s">
+      <c r="C238" s="78" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="51.75">
-      <c r="A236" s="79">
+    <row r="239" spans="1:3" ht="51.75">
+      <c r="A239" s="79">
         <v>42306</v>
       </c>
-      <c r="B236" s="78" t="s">
+      <c r="B239" s="78" t="s">
         <v>333</v>
       </c>
-      <c r="C236" s="78" t="s">
+      <c r="C239" s="78" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="237" spans="1:3">
-      <c r="A237" s="100"/>
-      <c r="B237" s="100"/>
-      <c r="C237" s="100"/>
+    <row r="240" spans="1:3">
+      <c r="A240" s="100"/>
+      <c r="B240" s="100"/>
+      <c r="C240" s="100"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C237">
+  <autoFilter ref="A1:C240">
     <sortState ref="A2:C201">
       <sortCondition descending="1" ref="A1:A201"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C209" r:id="rId1"/>
-    <hyperlink ref="C170" r:id="rId2"/>
-    <hyperlink ref="C210" r:id="rId3"/>
-    <hyperlink ref="C44" r:id="rId4"/>
-    <hyperlink ref="C29" r:id="rId5"/>
-    <hyperlink ref="C26" r:id="rId6"/>
+    <hyperlink ref="C212" r:id="rId1"/>
+    <hyperlink ref="C173" r:id="rId2"/>
+    <hyperlink ref="C213" r:id="rId3"/>
+    <hyperlink ref="C47" r:id="rId4"/>
+    <hyperlink ref="C32" r:id="rId5"/>
+    <hyperlink ref="C29" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -6406,16 +6469,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="60.75" customHeight="1">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add 2048 source and Fragement Sample source
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -15,14 +15,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'AS400 Version'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$240</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$241</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="548">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -2801,6 +2801,14 @@
 1. 寸進精神 (很多時自己都止步在)
 2. 髒法: 一個getleadacc module, ip1, op1, ip1輸入後輸出op1為ip1的Lead acc, 但若ip1為lead acc或非multi ccy acc, op1均會賦上ip1的值然後返回. 當時死腦只想找個方法求是否Lead account, 後發現轉下彎, 若能用ip1&lt;&gt;op1來判定是subacc這第三個可能性, 是能得到確定的定性結果的, 然後可以加以利用.
 3. 圖形化思考方法</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>To learn android application development, open-source app is the best way to go:
+1. On android developer official website page, there are lots of sample
+2. On wikipedia search Open-source Android App, there would be a list and those projects can be found on github.</t>
   </si>
 </sst>
 </file>
@@ -3135,7 +3143,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3502,6 +3510,9 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3535,13 +3546,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4202207</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>593914</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>257735</xdr:colOff>
-      <xdr:row>131</xdr:row>
+      <xdr:row>132</xdr:row>
       <xdr:rowOff>102264</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3858,10 +3869,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F240"/>
+  <dimension ref="A1:F241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3888,414 +3899,414 @@
       <c r="B2" s="100"/>
       <c r="C2" s="100"/>
     </row>
-    <row r="3" spans="1:4" s="102" customFormat="1" ht="30">
+    <row r="3" spans="1:4" s="102" customFormat="1" ht="60">
       <c r="A3" s="121">
-        <v>42564</v>
-      </c>
-      <c r="B3" s="122"/>
-      <c r="C3" s="122" t="s">
-        <v>544</v>
-      </c>
-      <c r="D3" s="124" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="102" customFormat="1" ht="120">
+        <v>42565</v>
+      </c>
+      <c r="B3" s="123" t="s">
+        <v>546</v>
+      </c>
+      <c r="C3" s="123" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="102" customFormat="1" ht="30">
       <c r="A4" s="121">
         <v>42564</v>
       </c>
       <c r="B4" s="122"/>
       <c r="C4" s="122" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D4" s="124" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="102" customFormat="1" ht="75">
+    <row r="5" spans="1:4" s="102" customFormat="1" ht="120">
       <c r="A5" s="121">
         <v>42564</v>
       </c>
-      <c r="B5" s="122" t="s">
+      <c r="B5" s="122"/>
+      <c r="C5" s="122" t="s">
+        <v>545</v>
+      </c>
+      <c r="D5" s="124" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="102" customFormat="1" ht="75">
+      <c r="A6" s="121">
+        <v>42564</v>
+      </c>
+      <c r="B6" s="122" t="s">
         <v>534</v>
       </c>
-      <c r="C5" s="122" t="s">
+      <c r="C6" s="122" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="102" customFormat="1" ht="135">
-      <c r="A6" s="121">
-        <v>42562</v>
-      </c>
-      <c r="B6" s="120" t="s">
-        <v>537</v>
-      </c>
-      <c r="C6" s="120" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="102" customFormat="1" ht="60">
+    <row r="7" spans="1:4" s="102" customFormat="1" ht="135">
       <c r="A7" s="121">
         <v>42562</v>
       </c>
       <c r="B7" s="120" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C7" s="120" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="102" customFormat="1" ht="75">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="102" customFormat="1" ht="60">
       <c r="A8" s="121">
         <v>42562</v>
       </c>
       <c r="B8" s="120" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C8" s="120" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="102" customFormat="1" ht="165">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="102" customFormat="1" ht="75">
       <c r="A9" s="121">
         <v>42562</v>
       </c>
       <c r="B9" s="120" t="s">
+        <v>535</v>
+      </c>
+      <c r="C9" s="120" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="102" customFormat="1" ht="165">
+      <c r="A10" s="121">
+        <v>42562</v>
+      </c>
+      <c r="B10" s="120" t="s">
         <v>534</v>
       </c>
-      <c r="C9" s="120" t="s">
+      <c r="C10" s="120" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="102" customFormat="1" ht="30">
-      <c r="A10" s="121">
+    <row r="11" spans="1:4" s="102" customFormat="1" ht="30">
+      <c r="A11" s="121">
         <v>42557</v>
       </c>
-      <c r="B10" s="120" t="s">
+      <c r="B11" s="120" t="s">
         <v>525</v>
       </c>
-      <c r="C10" s="120" t="s">
+      <c r="C11" s="120" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="102" customFormat="1" ht="180">
-      <c r="A11" s="120"/>
-      <c r="B11" s="120" t="s">
+    <row r="12" spans="1:4" s="102" customFormat="1" ht="180">
+      <c r="A12" s="120"/>
+      <c r="B12" s="120" t="s">
         <v>527</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C12" s="120" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="102" customFormat="1" ht="150">
-      <c r="A12" s="121">
+    <row r="13" spans="1:4" s="102" customFormat="1" ht="150">
+      <c r="A13" s="121">
         <v>42540</v>
       </c>
-      <c r="B12" s="120" t="s">
+      <c r="B13" s="120" t="s">
         <v>529</v>
       </c>
-      <c r="C12" s="120" t="s">
+      <c r="C13" s="120" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="102" customFormat="1" ht="180">
-      <c r="A13" s="121">
-        <v>42539</v>
-      </c>
-      <c r="B13" s="120" t="s">
-        <v>527</v>
-      </c>
-      <c r="C13" s="120" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="102" customFormat="1" ht="105">
+    <row r="14" spans="1:4" s="102" customFormat="1" ht="180">
       <c r="A14" s="121">
         <v>42539</v>
       </c>
       <c r="B14" s="120" t="s">
+        <v>527</v>
+      </c>
+      <c r="C14" s="120" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="102" customFormat="1" ht="105">
+      <c r="A15" s="121">
+        <v>42539</v>
+      </c>
+      <c r="B15" s="120" t="s">
         <v>532</v>
       </c>
-      <c r="C14" s="120" t="s">
+      <c r="C15" s="120" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="102" customFormat="1" ht="60">
-      <c r="A15" s="2">
+    <row r="16" spans="1:4" s="102" customFormat="1" ht="60">
+      <c r="A16" s="2">
         <v>42534</v>
       </c>
-      <c r="B15" s="119" t="s">
+      <c r="B16" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="119" t="s">
+      <c r="C16" s="119" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="102" customFormat="1" ht="45">
-      <c r="A16" s="2">
+    <row r="17" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A17" s="2">
         <v>42517</v>
       </c>
-      <c r="B16" s="118" t="s">
+      <c r="B17" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="118" t="s">
+      <c r="C17" s="118" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A17" s="2">
+    <row r="18" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A18" s="2">
         <v>42514</v>
       </c>
-      <c r="B17" s="117" t="s">
+      <c r="B18" s="117" t="s">
         <v>519</v>
       </c>
-      <c r="C17" s="117" t="s">
+      <c r="C18" s="117" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A18" s="2">
+    <row r="19" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A19" s="2">
         <v>42507</v>
       </c>
-      <c r="B18" s="116" t="s">
+      <c r="B19" s="116" t="s">
         <v>519</v>
       </c>
-      <c r="C18" s="116" t="s">
+      <c r="C19" s="116" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A19" s="2">
+    <row r="20" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A20" s="2">
         <v>42502</v>
       </c>
-      <c r="B19" s="115" t="s">
+      <c r="B20" s="115" t="s">
         <v>519</v>
       </c>
-      <c r="C19" s="116" t="s">
+      <c r="C20" s="116" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A20" s="2">
-        <v>42485</v>
-      </c>
-      <c r="B20" s="113" t="s">
-        <v>516</v>
-      </c>
-      <c r="C20" s="113" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="102" customFormat="1" ht="30">
+    <row r="21" spans="1:3" s="102" customFormat="1" ht="90">
       <c r="A21" s="2">
         <v>42485</v>
       </c>
-      <c r="B21" s="110" t="s">
-        <v>514</v>
-      </c>
-      <c r="C21" s="110" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="102" customFormat="1" ht="300">
+      <c r="B21" s="113" t="s">
+        <v>516</v>
+      </c>
+      <c r="C21" s="113" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="102" customFormat="1" ht="30">
       <c r="A22" s="2">
         <v>42485</v>
       </c>
-      <c r="B22" s="112" t="s">
+      <c r="B22" s="110" t="s">
+        <v>514</v>
+      </c>
+      <c r="C22" s="110" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="102" customFormat="1" ht="300">
+      <c r="A23" s="2">
+        <v>42485</v>
+      </c>
+      <c r="B23" s="112" t="s">
         <v>241</v>
       </c>
-      <c r="C22" s="112" t="s">
+      <c r="C23" s="112" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A23" s="2">
+    <row r="24" spans="1:3" s="102" customFormat="1" ht="150">
+      <c r="A24" s="2">
         <v>42479</v>
       </c>
-      <c r="B23" s="111" t="s">
+      <c r="B24" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="C23" s="111" t="s">
+      <c r="C24" s="111" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A24" s="2">
+    <row r="25" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="A25" s="2">
         <v>42478</v>
       </c>
-      <c r="B24" s="110" t="s">
+      <c r="B25" s="110" t="s">
         <v>509</v>
       </c>
-      <c r="C24" s="110" t="s">
+      <c r="C25" s="110" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="102" customFormat="1" ht="120">
-      <c r="A25" s="2">
-        <v>42477</v>
-      </c>
-      <c r="B25" s="109" t="s">
-        <v>509</v>
-      </c>
-      <c r="C25" s="109" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="102" customFormat="1" ht="30">
+    <row r="26" spans="1:3" s="102" customFormat="1" ht="120">
       <c r="A26" s="2">
         <v>42477</v>
       </c>
-      <c r="B26" s="108" t="s">
+      <c r="B26" s="109" t="s">
+        <v>509</v>
+      </c>
+      <c r="C26" s="109" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A27" s="2">
+        <v>42477</v>
+      </c>
+      <c r="B27" s="108" t="s">
         <v>507</v>
       </c>
-      <c r="C26" s="108" t="s">
+      <c r="C27" s="108" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="102" customFormat="1">
-      <c r="A27" s="2">
-        <v>42473</v>
-      </c>
-      <c r="B27" s="106" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="106" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="102" customFormat="1" ht="45">
+    <row r="28" spans="1:3" s="102" customFormat="1">
       <c r="A28" s="2">
         <v>42473</v>
       </c>
       <c r="B28" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="107" t="s">
+      <c r="C28" s="106" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A29" s="2">
+        <v>42473</v>
+      </c>
+      <c r="B29" s="106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="107" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="102" customFormat="1">
-      <c r="A29" s="2">
+    <row r="30" spans="1:3" s="102" customFormat="1">
+      <c r="A30" s="2">
         <v>42469</v>
       </c>
-      <c r="B29" s="105" t="s">
+      <c r="B30" s="105" t="s">
         <v>504</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="102" customFormat="1" ht="75">
-      <c r="A30" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B30" s="104" t="s">
-        <v>497</v>
-      </c>
-      <c r="C30" s="104" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="102" customFormat="1" ht="105">
+    <row r="31" spans="1:3" s="102" customFormat="1" ht="75">
       <c r="A31" s="2">
         <v>42463</v>
       </c>
       <c r="B31" s="104" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C31" s="104" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="102" customFormat="1">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="102" customFormat="1" ht="105">
       <c r="A32" s="2">
         <v>42463</v>
       </c>
       <c r="B32" s="104" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C32" s="104" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="102" customFormat="1" ht="150">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="102" customFormat="1">
       <c r="A33" s="2">
         <v>42463</v>
       </c>
-      <c r="B33" s="100" t="s">
-        <v>493</v>
-      </c>
-      <c r="C33" s="100" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="B33" s="104" t="s">
+        <v>501</v>
+      </c>
+      <c r="C33" s="104" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="102" customFormat="1" ht="150">
       <c r="A34" s="2">
         <v>42463</v>
       </c>
-      <c r="B34" s="103" t="s">
-        <v>492</v>
-      </c>
-      <c r="C34" s="103" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="B34" s="100" t="s">
+        <v>493</v>
+      </c>
+      <c r="C34" s="100" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="102" customFormat="1" ht="90">
       <c r="A35" s="2">
         <v>42463</v>
       </c>
-      <c r="B35" s="101" t="s">
-        <v>489</v>
-      </c>
-      <c r="C35" s="101" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="B35" s="103" t="s">
+        <v>492</v>
+      </c>
+      <c r="C35" s="103" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="102" customFormat="1" ht="30">
       <c r="A36" s="2">
         <v>42463</v>
       </c>
       <c r="B36" s="101" t="s">
+        <v>489</v>
+      </c>
+      <c r="C36" s="101" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A37" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B37" s="101" t="s">
         <v>488</v>
       </c>
-      <c r="C36" s="101" t="s">
+      <c r="C37" s="101" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A37" s="2">
-        <v>42462</v>
-      </c>
-      <c r="B37" s="100" t="s">
-        <v>486</v>
-      </c>
-      <c r="C37" s="100" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="102" customFormat="1" ht="135">
+    <row r="38" spans="1:3" s="102" customFormat="1" ht="150">
       <c r="A38" s="2">
         <v>42462</v>
       </c>
       <c r="B38" s="100" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C38" s="100" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="102" customFormat="1" ht="240">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="102" customFormat="1" ht="135">
       <c r="A39" s="2">
         <v>42462</v>
       </c>
       <c r="B39" s="100" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="C39" s="100" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" s="102" customFormat="1" ht="120">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="102" customFormat="1" ht="240">
       <c r="A40" s="2">
         <v>42462</v>
       </c>
@@ -4303,362 +4314,362 @@
         <v>480</v>
       </c>
       <c r="C40" s="100" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="102" customFormat="1" ht="120">
+      <c r="A41" s="2">
+        <v>42462</v>
+      </c>
+      <c r="B41" s="100" t="s">
+        <v>480</v>
+      </c>
+      <c r="C41" s="100" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="4" customFormat="1" ht="120">
-      <c r="A41" s="2">
-        <v>42460</v>
-      </c>
-      <c r="B41" s="99" t="s">
-        <v>477</v>
-      </c>
-      <c r="C41" s="99" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="4" customFormat="1" ht="30">
+    <row r="42" spans="1:3" s="4" customFormat="1" ht="120">
       <c r="A42" s="2">
         <v>42460</v>
       </c>
       <c r="B42" s="99" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C42" s="99" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="4" customFormat="1" ht="180">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="4" customFormat="1" ht="30">
       <c r="A43" s="2">
         <v>42460</v>
       </c>
       <c r="B43" s="99" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C43" s="99" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" s="4" customFormat="1" ht="60">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="4" customFormat="1" ht="180">
       <c r="A44" s="2">
         <v>42460</v>
       </c>
       <c r="B44" s="99" t="s">
+        <v>475</v>
+      </c>
+      <c r="C44" s="99" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="4" customFormat="1" ht="60">
+      <c r="A45" s="2">
+        <v>42460</v>
+      </c>
+      <c r="B45" s="99" t="s">
         <v>478</v>
       </c>
-      <c r="C44" s="99" t="s">
+      <c r="C45" s="99" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="4" customFormat="1" ht="105">
-      <c r="A45" s="2">
-        <v>42459</v>
-      </c>
-      <c r="B45" s="99" t="s">
-        <v>470</v>
-      </c>
-      <c r="C45" s="98" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" s="4" customFormat="1" ht="60">
+    <row r="46" spans="1:3" s="4" customFormat="1" ht="105">
       <c r="A46" s="2">
         <v>42459</v>
       </c>
       <c r="B46" s="99" t="s">
+        <v>470</v>
+      </c>
+      <c r="C46" s="98" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="4" customFormat="1" ht="60">
+      <c r="A47" s="2">
+        <v>42459</v>
+      </c>
+      <c r="B47" s="99" t="s">
         <v>241</v>
       </c>
-      <c r="C46" s="99" t="s">
+      <c r="C47" s="99" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="4" customFormat="1">
-      <c r="A47" s="2">
+    <row r="48" spans="1:3" s="4" customFormat="1">
+      <c r="A48" s="2">
         <v>42458</v>
       </c>
-      <c r="B47" s="97" t="s">
+      <c r="B48" s="97" t="s">
         <v>470</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C48" s="8" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="4" customFormat="1" ht="105">
-      <c r="A48" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B48" s="96" t="s">
-        <v>254</v>
-      </c>
-      <c r="C48" s="100" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="60">
+    <row r="49" spans="1:3" s="4" customFormat="1" ht="105">
       <c r="A49" s="2">
         <v>42456</v>
       </c>
       <c r="B49" s="96" t="s">
-        <v>462</v>
-      </c>
-      <c r="C49" s="44" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="45">
+        <v>254</v>
+      </c>
+      <c r="C49" s="100" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="60">
       <c r="A50" s="2">
         <v>42456</v>
       </c>
       <c r="B50" s="96" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="45">
       <c r="A51" s="2">
         <v>42456</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>466</v>
+      <c r="B51" s="96" t="s">
+        <v>463</v>
       </c>
       <c r="C51" s="44" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="45">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="2">
         <v>42456</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C52" s="44" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="45">
+      <c r="A53" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="C52" s="44" t="s">
+      <c r="C53" s="44" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="77.25">
-      <c r="A53" s="79">
-        <v>42453</v>
-      </c>
-      <c r="B53" s="78" t="s">
-        <v>264</v>
-      </c>
-      <c r="C53" s="78" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="26.25">
+    <row r="54" spans="1:3" ht="77.25">
       <c r="A54" s="79">
         <v>42453</v>
       </c>
       <c r="B54" s="78" t="s">
+        <v>264</v>
+      </c>
+      <c r="C54" s="78" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="26.25">
+      <c r="A55" s="79">
+        <v>42453</v>
+      </c>
+      <c r="B55" s="78" t="s">
         <v>262</v>
       </c>
-      <c r="C54" s="78" t="s">
+      <c r="C55" s="78" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="39">
-      <c r="A55" s="79">
+    <row r="56" spans="1:3" ht="39">
+      <c r="A56" s="79">
         <v>42452</v>
       </c>
-      <c r="B55" s="78" t="s">
+      <c r="B56" s="78" t="s">
         <v>260</v>
       </c>
-      <c r="C55" s="78" t="s">
+      <c r="C56" s="78" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="165">
-      <c r="A56" s="75">
+    <row r="57" spans="1:3" ht="165">
+      <c r="A57" s="75">
         <v>42451</v>
       </c>
-      <c r="B56" s="74" t="s">
+      <c r="B57" s="74" t="s">
         <v>247</v>
       </c>
-      <c r="C56" s="100" t="s">
+      <c r="C57" s="100" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="45">
-      <c r="A57" s="2">
-        <v>42451</v>
-      </c>
-      <c r="B57" s="100" t="s">
-        <v>249</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="30">
+    <row r="58" spans="1:3" ht="45">
       <c r="A58" s="2">
         <v>42451</v>
       </c>
-      <c r="B58" s="96" t="s">
-        <v>196</v>
+      <c r="B58" s="100" t="s">
+        <v>249</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="165">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="30">
       <c r="A59" s="2">
         <v>42451</v>
       </c>
       <c r="B59" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="165">
+      <c r="A60" s="2">
+        <v>42451</v>
+      </c>
+      <c r="B60" s="96" t="s">
         <v>253</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="64.5">
-      <c r="A60" s="79">
-        <v>42451</v>
-      </c>
-      <c r="B60" s="78" t="s">
-        <v>253</v>
-      </c>
-      <c r="C60" s="78" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="64.5">
       <c r="A61" s="79">
+        <v>42451</v>
+      </c>
+      <c r="B61" s="78" t="s">
+        <v>253</v>
+      </c>
+      <c r="C61" s="78" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="64.5">
+      <c r="A62" s="79">
         <v>42447</v>
       </c>
-      <c r="B61" s="78" t="s">
+      <c r="B62" s="78" t="s">
         <v>257</v>
       </c>
-      <c r="C61" s="78" t="s">
+      <c r="C62" s="78" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="2">
+    <row r="63" spans="1:3">
+      <c r="A63" s="2">
         <v>42440</v>
       </c>
-      <c r="B62" s="100" t="s">
+      <c r="B63" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="100" t="s">
+      <c r="C63" s="100" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="75">
-      <c r="A63" s="2">
+    <row r="64" spans="1:3" ht="75">
+      <c r="A64" s="2">
         <v>42436</v>
       </c>
-      <c r="B63" s="96" t="s">
+      <c r="B64" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="39">
-      <c r="A64" s="79">
-        <v>42431</v>
-      </c>
-      <c r="B64" s="78" t="s">
-        <v>274</v>
-      </c>
-      <c r="C64" s="78" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="26.25">
+    <row r="65" spans="1:3" ht="39">
       <c r="A65" s="79">
         <v>42431</v>
       </c>
       <c r="B65" s="78" t="s">
+        <v>274</v>
+      </c>
+      <c r="C65" s="78" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="26.25">
+      <c r="A66" s="79">
+        <v>42431</v>
+      </c>
+      <c r="B66" s="78" t="s">
         <v>272</v>
       </c>
-      <c r="C65" s="78" t="s">
+      <c r="C66" s="78" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="51.75">
-      <c r="A66" s="79">
+    <row r="67" spans="1:3" ht="51.75">
+      <c r="A67" s="79">
         <v>42430</v>
       </c>
-      <c r="B66" s="78" t="s">
+      <c r="B67" s="78" t="s">
         <v>270</v>
       </c>
-      <c r="C66" s="78" t="s">
+      <c r="C67" s="78" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="26.25">
-      <c r="A67" s="79">
+    <row r="68" spans="1:3" ht="26.25">
+      <c r="A68" s="79">
         <v>42428</v>
       </c>
-      <c r="B67" s="78" t="s">
+      <c r="B68" s="78" t="s">
         <v>268</v>
       </c>
-      <c r="C67" s="78" t="s">
+      <c r="C68" s="78" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="30">
-      <c r="A68" s="2">
+    <row r="69" spans="1:3" ht="30">
+      <c r="A69" s="2">
         <v>42426</v>
       </c>
-      <c r="B68" s="100" t="s">
+      <c r="B69" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="C68" s="100" t="s">
+      <c r="C69" s="100" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="77.25">
-      <c r="A69" s="79">
+    <row r="70" spans="1:3" ht="77.25">
+      <c r="A70" s="79">
         <v>42426</v>
       </c>
-      <c r="B69" s="78" t="s">
+      <c r="B70" s="78" t="s">
         <v>266</v>
       </c>
-      <c r="C69" s="78" t="s">
+      <c r="C70" s="78" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="2">
-        <v>42425</v>
-      </c>
-      <c r="B70" s="100" t="s">
-        <v>241</v>
-      </c>
-      <c r="C70" s="100" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="2">
         <v>42425</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="100" t="s">
+        <v>241</v>
+      </c>
+      <c r="C71" s="100" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="2">
+        <v>42425</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="26.25">
-      <c r="A72" s="79">
-        <v>42425</v>
-      </c>
-      <c r="B72" s="78" t="s">
-        <v>276</v>
-      </c>
-      <c r="C72" s="78" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" ht="26.25">
       <c r="A73" s="79">
         <v>42425</v>
       </c>
@@ -4666,291 +4677,291 @@
         <v>276</v>
       </c>
       <c r="C73" s="78" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="26.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="79">
         <v>42425</v>
       </c>
       <c r="B74" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="C74" s="78" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="26.25">
+      <c r="A75" s="79">
+        <v>42425</v>
+      </c>
+      <c r="B75" s="78" t="s">
         <v>279</v>
       </c>
-      <c r="C74" s="78" t="s">
+      <c r="C75" s="78" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="165">
-      <c r="A75" s="2">
+    <row r="76" spans="1:3" ht="165">
+      <c r="A76" s="2">
         <v>42424</v>
       </c>
-      <c r="B75" s="100" t="s">
+      <c r="B76" s="100" t="s">
         <v>239</v>
       </c>
-      <c r="C75" s="114" t="s">
+      <c r="C76" s="114" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="45">
-      <c r="A76" s="2">
+    <row r="77" spans="1:3" ht="45">
+      <c r="A77" s="2">
         <v>42423</v>
       </c>
-      <c r="B76" s="96" t="s">
+      <c r="B77" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="C77" s="11" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="79">
+    <row r="78" spans="1:3">
+      <c r="A78" s="79">
         <v>42423</v>
       </c>
-      <c r="B77" s="78" t="s">
+      <c r="B78" s="78" t="s">
         <v>281</v>
       </c>
-      <c r="C77" s="78" t="s">
+      <c r="C78" s="78" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="90">
-      <c r="A78" s="2">
+    <row r="79" spans="1:3" ht="90">
+      <c r="A79" s="2">
         <v>42422</v>
       </c>
-      <c r="B78" s="100" t="s">
+      <c r="B79" s="100" t="s">
         <v>236</v>
       </c>
-      <c r="C78" s="100" t="s">
+      <c r="C79" s="100" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="60">
-      <c r="A79" s="2">
+    <row r="80" spans="1:3" ht="60">
+      <c r="A80" s="2">
         <v>42419</v>
       </c>
-      <c r="B79" s="10" t="s">
+      <c r="B80" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="C79" s="36" t="s">
+      <c r="C80" s="36" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="195">
-      <c r="A80" s="2">
+    <row r="81" spans="1:3" ht="195">
+      <c r="A81" s="2">
         <v>42418</v>
       </c>
-      <c r="B80" s="10" t="s">
+      <c r="B81" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C80" s="18" t="s">
+      <c r="C81" s="18" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="45">
-      <c r="A81" s="2">
-        <v>42403</v>
-      </c>
-      <c r="B81" s="96" t="s">
-        <v>229</v>
-      </c>
-      <c r="C81" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="75">
+    <row r="82" spans="1:3" ht="45">
       <c r="A82" s="2">
         <v>42403</v>
       </c>
-      <c r="B82" s="12" t="s">
-        <v>230</v>
+      <c r="B82" s="96" t="s">
+        <v>229</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="90">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="75">
       <c r="A83" s="2">
         <v>42403</v>
       </c>
-      <c r="B83" s="12"/>
+      <c r="B83" s="12" t="s">
+        <v>230</v>
+      </c>
       <c r="C83" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="90">
       <c r="A84" s="2">
-        <v>42398</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>196</v>
-      </c>
+        <v>42403</v>
+      </c>
+      <c r="B84" s="12"/>
       <c r="C84" s="12" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="45">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="90">
       <c r="A85" s="2">
         <v>42398</v>
       </c>
       <c r="B85" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="45">
+      <c r="A86" s="2">
+        <v>42398</v>
+      </c>
+      <c r="B86" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="C85" s="12" t="s">
+      <c r="C86" s="12" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="2">
+    <row r="87" spans="1:3">
+      <c r="A87" s="2">
         <v>42397</v>
       </c>
-      <c r="B86" s="96" t="s">
+      <c r="B87" s="96" t="s">
         <v>201</v>
       </c>
-      <c r="C86" s="14" t="s">
+      <c r="C87" s="14" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="45">
-      <c r="A87" s="2">
-        <v>42396</v>
-      </c>
-      <c r="B87" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C87" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="30">
+    <row r="88" spans="1:3" ht="45">
       <c r="A88" s="2">
         <v>42396</v>
       </c>
-      <c r="B88" s="96" t="s">
+      <c r="B88" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C88" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="30">
+      <c r="A89" s="2">
+        <v>42396</v>
+      </c>
+      <c r="B89" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="C88" s="14" t="s">
+      <c r="C89" s="14" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="128.25">
-      <c r="A89" s="79">
-        <v>42386</v>
-      </c>
-      <c r="B89" s="78" t="s">
-        <v>283</v>
-      </c>
-      <c r="C89" s="78" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="64.5">
+    <row r="90" spans="1:3" ht="128.25">
       <c r="A90" s="79">
         <v>42386</v>
       </c>
       <c r="B90" s="78" t="s">
+        <v>283</v>
+      </c>
+      <c r="C90" s="78" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="64.5">
+      <c r="A91" s="79">
+        <v>42386</v>
+      </c>
+      <c r="B91" s="78" t="s">
         <v>285</v>
       </c>
-      <c r="C90" s="78" t="s">
+      <c r="C91" s="78" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="45">
-      <c r="A91" s="2">
+    <row r="92" spans="1:3" ht="45">
+      <c r="A92" s="2">
         <v>42384</v>
       </c>
-      <c r="B91" s="100" t="s">
+      <c r="B92" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="C91" s="100" t="s">
+      <c r="C92" s="100" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="180">
-      <c r="A92" s="2">
+    <row r="93" spans="1:3" ht="180">
+      <c r="A93" s="2">
         <v>42382</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B93" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="C92" s="14" t="s">
+      <c r="C93" s="14" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="64.5">
-      <c r="A93" s="79">
+    <row r="94" spans="1:3" ht="64.5">
+      <c r="A94" s="79">
         <v>42382</v>
       </c>
-      <c r="B93" s="78" t="s">
+      <c r="B94" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="C93" s="78" t="s">
+      <c r="C94" s="78" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="30">
-      <c r="A94" s="2">
+    <row r="95" spans="1:3" ht="30">
+      <c r="A95" s="2">
         <v>42381</v>
       </c>
-      <c r="B94" s="100" t="s">
+      <c r="B95" s="100" t="s">
         <v>216</v>
       </c>
-      <c r="C94" s="100" t="s">
+      <c r="C95" s="100" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="45">
-      <c r="A95" s="2">
-        <v>42380</v>
-      </c>
-      <c r="B95" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C95" s="16" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="75">
+    <row r="96" spans="1:3" ht="45">
       <c r="A96" s="2">
         <v>42380</v>
       </c>
-      <c r="B96" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="C96" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="180">
+      <c r="B96" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C96" s="16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="75">
       <c r="A97" s="2">
         <v>42380</v>
       </c>
       <c r="B97" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C97" s="18" t="s">
+      <c r="C97" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="180">
+      <c r="A98" s="2">
+        <v>42380</v>
+      </c>
+      <c r="B98" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="C98" s="18" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="217.5">
-      <c r="A98" s="79">
+    <row r="99" spans="1:3" ht="217.5">
+      <c r="A99" s="79">
         <v>42380</v>
       </c>
-      <c r="B98" s="78" t="s">
+      <c r="B99" s="78" t="s">
         <v>288</v>
       </c>
-      <c r="C98" s="78" t="s">
+      <c r="C99" s="78" t="s">
         <v>289</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="102.75">
-      <c r="A99" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B99" s="78" t="s">
-        <v>291</v>
-      </c>
-      <c r="C99" s="78" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="102.75">
@@ -4958,24 +4969,24 @@
         <v>42378</v>
       </c>
       <c r="B100" s="78" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C100" s="78" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="141">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="102.75">
       <c r="A101" s="79">
         <v>42378</v>
       </c>
       <c r="B101" s="78" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C101" s="78" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="77.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="141">
       <c r="A102" s="79">
         <v>42378</v>
       </c>
@@ -4983,106 +4994,106 @@
         <v>297</v>
       </c>
       <c r="C102" s="78" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="102.75">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="77.25">
       <c r="A103" s="79">
         <v>42378</v>
       </c>
       <c r="B103" s="78" t="s">
+        <v>297</v>
+      </c>
+      <c r="C103" s="78" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="102.75">
+      <c r="A104" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B104" s="78" t="s">
         <v>295</v>
       </c>
-      <c r="C103" s="78" t="s">
+      <c r="C104" s="78" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="60">
-      <c r="A104" s="2">
+    <row r="105" spans="1:3" ht="60">
+      <c r="A105" s="2">
         <v>42377</v>
       </c>
-      <c r="B104" s="100" t="s">
+      <c r="B105" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="C104" s="100" t="s">
+      <c r="C105" s="100" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="77.25">
-      <c r="A105" s="79">
+    <row r="106" spans="1:3" ht="77.25">
+      <c r="A106" s="79">
         <v>42376</v>
       </c>
-      <c r="B105" s="78" t="s">
+      <c r="B106" s="78" t="s">
         <v>300</v>
       </c>
-      <c r="C105" s="78" t="s">
+      <c r="C106" s="78" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="45">
-      <c r="A106" s="2">
+    <row r="107" spans="1:3" ht="45">
+      <c r="A107" s="2">
         <v>42375</v>
       </c>
-      <c r="B106" s="15" t="s">
+      <c r="B107" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C106" s="100" t="s">
+      <c r="C107" s="100" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="2">
+    <row r="108" spans="1:3">
+      <c r="A108" s="2">
         <v>42369</v>
       </c>
-      <c r="B107" s="100" t="s">
+      <c r="B108" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="C107" s="19" t="s">
+      <c r="C108" s="19" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="195">
-      <c r="A108" s="2">
-        <v>42368</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C108" s="19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="135">
+    <row r="109" spans="1:3" ht="195">
       <c r="A109" s="2">
         <v>42368</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C109" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="45">
+        <v>196</v>
+      </c>
+      <c r="C109" s="19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="135">
       <c r="A110" s="2">
         <v>42368</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C110" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="45">
+      <c r="A111" s="2">
+        <v>42368</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C110" s="20" t="s">
+      <c r="C111" s="20" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="30">
-      <c r="A111" s="2">
-        <v>42366</v>
-      </c>
-      <c r="B111" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C111" s="20" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="30">
@@ -5093,111 +5104,111 @@
         <v>49</v>
       </c>
       <c r="C112" s="20" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="30">
+      <c r="A113" s="2">
+        <v>42366</v>
+      </c>
+      <c r="B113" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C113" s="20" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="150">
-      <c r="A113" s="2">
-        <v>42361</v>
-      </c>
-      <c r="C113" s="20" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="30">
+    <row r="114" spans="1:3" ht="150">
       <c r="A114" s="2">
         <v>42361</v>
       </c>
       <c r="C114" s="20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="270">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="30">
       <c r="A115" s="2">
         <v>42361</v>
       </c>
-      <c r="B115" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C115" s="22" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="30">
+      <c r="C115" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="270">
       <c r="A116" s="2">
         <v>42361</v>
       </c>
-      <c r="B116" s="100" t="s">
-        <v>53</v>
-      </c>
-      <c r="C116" s="20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
+      <c r="B116" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C116" s="22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="30">
       <c r="A117" s="2">
         <v>42361</v>
       </c>
-      <c r="B117" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C117" s="21" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="225">
+      <c r="B117" s="100" t="s">
+        <v>53</v>
+      </c>
+      <c r="C117" s="20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
       <c r="A118" s="2">
         <v>42361</v>
       </c>
       <c r="B118" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="C118" s="22" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="60">
+      <c r="C118" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="225">
       <c r="A119" s="2">
         <v>42361</v>
       </c>
-      <c r="B119" s="100" t="s">
-        <v>49</v>
+      <c r="B119" s="35" t="s">
+        <v>186</v>
       </c>
       <c r="C119" s="22" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="90">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="60">
       <c r="A120" s="2">
         <v>42361</v>
       </c>
-      <c r="B120" s="1" t="s">
-        <v>196</v>
+      <c r="B120" s="100" t="s">
+        <v>49</v>
       </c>
       <c r="C120" s="22" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="60">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="90">
       <c r="A121" s="2">
         <v>42361</v>
       </c>
-      <c r="B121" s="24" t="s">
+      <c r="B121" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C121" s="24" t="s">
+      <c r="C121" s="22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="60">
+      <c r="A122" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B122" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C122" s="24" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" s="40">
-        <v>42360</v>
-      </c>
-      <c r="B122" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="C122" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -5208,187 +5219,189 @@
         <v>195</v>
       </c>
       <c r="C123" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="40">
+        <v>42360</v>
+      </c>
+      <c r="B124" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="C124" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="102.75">
-      <c r="A124" s="80">
+    <row r="125" spans="1:3" ht="102.75">
+      <c r="A125" s="80">
         <v>42360</v>
       </c>
-      <c r="B124" s="78" t="s">
+      <c r="B125" s="78" t="s">
         <v>302</v>
       </c>
-      <c r="C124" s="78" t="s">
+      <c r="C125" s="78" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="30">
-      <c r="A125" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B125" s="100" t="s">
-        <v>43</v>
-      </c>
-      <c r="C125" s="100" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" ht="30">
       <c r="A126" s="2">
         <v>42356</v>
       </c>
-      <c r="B126" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="C126" s="23" t="s">
-        <v>181</v>
+      <c r="B126" s="100" t="s">
+        <v>43</v>
+      </c>
+      <c r="C126" s="100" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="2">
         <v>42356</v>
       </c>
-      <c r="B127" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="C127" s="25" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="30">
+      <c r="B127" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="C127" s="23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
       <c r="A128" s="2">
         <v>42356</v>
       </c>
-      <c r="B128" s="96"/>
+      <c r="B128" s="25" t="s">
+        <v>201</v>
+      </c>
       <c r="C128" s="25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="30">
+      <c r="A129" s="2">
+        <v>42356</v>
+      </c>
+      <c r="B129" s="96"/>
+      <c r="C129" s="25" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="60">
-      <c r="A129" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B129" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="C129" s="26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" ht="60">
       <c r="A130" s="2">
         <v>42355</v>
       </c>
-      <c r="B130" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C130" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="150">
+      <c r="B130" s="96" t="s">
+        <v>91</v>
+      </c>
+      <c r="C130" s="26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
       <c r="A131" s="2">
         <v>42355</v>
       </c>
       <c r="B131" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C131" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="120">
+      <c r="C131" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="150">
       <c r="A132" s="2">
         <v>42355</v>
       </c>
-      <c r="B132" s="100" t="s">
-        <v>168</v>
+      <c r="B132" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="C132" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="30">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="120">
       <c r="A133" s="2">
         <v>42355</v>
       </c>
-      <c r="B133" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C133" s="28" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
+      <c r="B133" s="100" t="s">
+        <v>168</v>
+      </c>
+      <c r="C133" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="30">
       <c r="A134" s="2">
         <v>42355</v>
       </c>
-      <c r="B134" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="C134" s="29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="75">
+      <c r="B134" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C134" s="28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
       <c r="A135" s="2">
         <v>42355</v>
       </c>
-      <c r="B135" s="15" t="s">
-        <v>43</v>
+      <c r="B135" s="29" t="s">
+        <v>171</v>
       </c>
       <c r="C135" s="29" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="135">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="75">
       <c r="A136" s="2">
         <v>42355</v>
       </c>
-      <c r="B136" s="100" t="s">
-        <v>173</v>
+      <c r="B136" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="C136" s="29" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="75">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="135">
       <c r="A137" s="2">
         <v>42355</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" s="100" t="s">
         <v>173</v>
       </c>
-      <c r="C137" s="42" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="30">
+      <c r="C137" s="29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="75">
       <c r="A138" s="2">
         <v>42355</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C138" s="30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
+      <c r="C138" s="42" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="30">
       <c r="A139" s="2">
         <v>42355</v>
       </c>
+      <c r="B139" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="C139" s="30" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="2">
         <v>42355</v>
       </c>
-      <c r="B140" s="42"/>
       <c r="C140" s="30" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -5397,74 +5410,74 @@
       </c>
       <c r="B141" s="42"/>
       <c r="C141" s="30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="2">
+        <v>42355</v>
+      </c>
+      <c r="B142" s="42"/>
+      <c r="C142" s="30" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="75">
-      <c r="A142" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B142" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="C142" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="30">
+    <row r="143" spans="1:3" ht="75">
       <c r="A143" s="2">
         <v>42352</v>
       </c>
-      <c r="B143" s="26"/>
-      <c r="C143" s="31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="75">
+      <c r="B143" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C143" s="30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="30">
       <c r="A144" s="2">
         <v>42352</v>
       </c>
       <c r="B144" s="26"/>
-      <c r="C144" s="70" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6">
+      <c r="C144" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="75">
       <c r="A145" s="2">
         <v>42352</v>
       </c>
       <c r="B145" s="26"/>
-      <c r="C145" s="32" t="s">
-        <v>69</v>
+      <c r="C145" s="70" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" s="2">
         <v>42352</v>
       </c>
-      <c r="B146" s="96"/>
-      <c r="C146" s="33" t="s">
-        <v>75</v>
+      <c r="B146" s="26"/>
+      <c r="C146" s="32" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="147" spans="1:6">
       <c r="A147" s="2">
         <v>42352</v>
       </c>
-      <c r="B147" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C147" s="34" t="s">
-        <v>72</v>
+      <c r="B147" s="96"/>
+      <c r="C147" s="33" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="148" spans="1:6">
       <c r="A148" s="2">
         <v>42352</v>
       </c>
-      <c r="B148" s="96"/>
+      <c r="B148" s="34" t="s">
+        <v>71</v>
+      </c>
       <c r="C148" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -5472,289 +5485,287 @@
         <v>42352</v>
       </c>
       <c r="B149" s="96"/>
-      <c r="C149" s="37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" ht="30">
+      <c r="C149" s="34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
       <c r="A150" s="2">
         <v>42352</v>
       </c>
-      <c r="B150" s="37"/>
+      <c r="B150" s="96"/>
       <c r="C150" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="30">
       <c r="A151" s="2">
         <v>42352</v>
       </c>
-      <c r="B151" s="96"/>
-      <c r="C151" s="96" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" ht="45">
+      <c r="B151" s="37"/>
+      <c r="C151" s="37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="30">
       <c r="A152" s="2">
         <v>42352</v>
       </c>
-      <c r="B152" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="B152" s="96"/>
       <c r="C152" s="96" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="153" spans="1:6" ht="45">
       <c r="A153" s="2">
         <v>42352</v>
       </c>
-      <c r="B153" s="100"/>
-      <c r="C153" s="39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" ht="30">
+      <c r="B153" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C153" s="96" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="45">
       <c r="A154" s="2">
         <v>42352</v>
       </c>
-      <c r="B154" s="38"/>
-      <c r="C154" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="F154" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" ht="75">
+      <c r="B154" s="100"/>
+      <c r="C154" s="39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="30">
       <c r="A155" s="2">
         <v>42352</v>
       </c>
-      <c r="B155" s="41"/>
-      <c r="C155" s="41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="45">
+      <c r="B155" s="38"/>
+      <c r="C155" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="F155" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="75">
       <c r="A156" s="2">
         <v>42352</v>
       </c>
-      <c r="B156" s="41" t="s">
-        <v>89</v>
-      </c>
+      <c r="B156" s="41"/>
       <c r="C156" s="41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" ht="30">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="45">
       <c r="A157" s="2">
         <v>42352</v>
       </c>
-      <c r="B157" s="43"/>
-      <c r="C157" s="43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="45">
+      <c r="B157" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C157" s="41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="30">
       <c r="A158" s="2">
         <v>42352</v>
       </c>
-      <c r="B158" s="44"/>
-      <c r="C158" s="44" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="30">
+      <c r="B158" s="43"/>
+      <c r="C158" s="43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="45">
       <c r="A159" s="2">
         <v>42352</v>
       </c>
-      <c r="B159" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="C159" s="46" t="s">
-        <v>86</v>
+      <c r="B159" s="44"/>
+      <c r="C159" s="44" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="30">
       <c r="A160" s="2">
         <v>42352</v>
       </c>
-      <c r="B160" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C160" s="47" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3">
+      <c r="B160" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C160" s="46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="30">
       <c r="A161" s="2">
         <v>42352</v>
       </c>
-      <c r="B161" s="100" t="s">
+      <c r="B161" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C161" s="47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B162" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="C161" s="48" t="s">
+      <c r="C162" s="48" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="135">
-      <c r="A162" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B162" s="49"/>
-      <c r="C162" s="49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="60">
+    <row r="163" spans="1:3" ht="135">
       <c r="A163" s="2">
         <v>42349</v>
       </c>
-      <c r="B163" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="C163" s="51" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="30">
+      <c r="B163" s="49"/>
+      <c r="C163" s="49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="60">
       <c r="A164" s="2">
         <v>42349</v>
       </c>
-      <c r="B164" s="96"/>
-      <c r="C164" s="53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="120">
+      <c r="B164" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C164" s="51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="30">
       <c r="A165" s="2">
         <v>42349</v>
       </c>
-      <c r="B165" s="96" t="s">
-        <v>12</v>
-      </c>
+      <c r="B165" s="96"/>
       <c r="C165" s="53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="150">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="120">
       <c r="A166" s="2">
         <v>42349</v>
       </c>
-      <c r="B166" s="52"/>
-      <c r="C166" s="52" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="30">
+      <c r="B166" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C166" s="53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="150">
       <c r="A167" s="2">
         <v>42349</v>
       </c>
-      <c r="B167" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C167" s="54" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3">
+      <c r="B167" s="52"/>
+      <c r="C167" s="52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="30">
       <c r="A168" s="2">
         <v>42349</v>
       </c>
       <c r="B168" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C168" s="55" t="s">
-        <v>61</v>
+      <c r="C168" s="54" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="2">
         <v>42349</v>
       </c>
-      <c r="B169" s="100"/>
-      <c r="C169" s="57" t="s">
-        <v>78</v>
+      <c r="B169" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C169" s="55" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="2">
         <v>42349</v>
       </c>
-      <c r="B170" s="58"/>
-      <c r="C170" s="58" t="s">
-        <v>62</v>
+      <c r="B170" s="100"/>
+      <c r="C170" s="57" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="2">
         <v>42349</v>
       </c>
-      <c r="B171" s="59"/>
-      <c r="C171" s="59" t="s">
-        <v>70</v>
+      <c r="B171" s="58"/>
+      <c r="C171" s="58" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="2">
         <v>42349</v>
       </c>
-      <c r="B172" s="60"/>
-      <c r="C172" s="60" t="s">
-        <v>64</v>
+      <c r="B172" s="59"/>
+      <c r="C172" s="59" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="2">
         <v>42349</v>
       </c>
-      <c r="B173" s="61"/>
-      <c r="C173" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="60">
+      <c r="B173" s="60"/>
+      <c r="C173" s="60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
       <c r="A174" s="2">
         <v>42349</v>
       </c>
-      <c r="B174" s="62" t="s">
+      <c r="B174" s="61"/>
+      <c r="C174" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="60">
+      <c r="A175" s="2">
+        <v>42349</v>
+      </c>
+      <c r="B175" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="C174" s="100" t="s">
+      <c r="C175" s="100" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="90">
-      <c r="A175" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B175" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C175" s="62" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" ht="30">
+    <row r="176" spans="1:3" ht="90">
       <c r="A176" s="2">
         <v>42345</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="B176" s="62" t="s">
         <v>12</v>
       </c>
       <c r="C176" s="62" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="30">
       <c r="A177" s="2">
         <v>42345</v>
       </c>
-      <c r="B177" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C177" s="63" t="s">
-        <v>28</v>
+      <c r="B177" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C177" s="62" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -5764,162 +5775,162 @@
       <c r="B178" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C178" s="64" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="30">
+      <c r="C178" s="63" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
       <c r="A179" s="2">
         <v>42345</v>
       </c>
       <c r="B179" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C179" s="65" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="195">
+      <c r="C179" s="64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="30">
       <c r="A180" s="2">
         <v>42345</v>
       </c>
-      <c r="B180" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C180" s="66" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" ht="135">
+      <c r="B180" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C180" s="65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="195">
       <c r="A181" s="2">
         <v>42345</v>
       </c>
-      <c r="B181" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="C181" s="67" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" ht="75">
+      <c r="B181" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C181" s="66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="135">
       <c r="A182" s="2">
         <v>42345</v>
       </c>
-      <c r="B182" s="69" t="s">
+      <c r="B182" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C182" s="68" t="s">
-        <v>32</v>
+      <c r="C182" s="67" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="75">
       <c r="A183" s="2">
         <v>42345</v>
       </c>
-      <c r="B183" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C183" s="69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" ht="30">
+      <c r="B183" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C183" s="68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="75">
       <c r="A184" s="2">
         <v>42345</v>
       </c>
-      <c r="B184" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C184" s="73" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
+      <c r="B184" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C184" s="69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="30">
       <c r="A185" s="2">
         <v>42345</v>
       </c>
-      <c r="B185" s="71" t="s">
-        <v>39</v>
+      <c r="B185" s="100" t="s">
+        <v>12</v>
       </c>
       <c r="C185" s="73" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="2">
         <v>42345</v>
       </c>
-      <c r="B186" s="72" t="s">
+      <c r="B186" s="71" t="s">
         <v>39</v>
       </c>
       <c r="C186" s="73" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="60">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
       <c r="A187" s="2">
         <v>42345</v>
       </c>
-      <c r="B187" s="96" t="s">
+      <c r="B187" s="72" t="s">
         <v>39</v>
       </c>
       <c r="C187" s="73" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" ht="150">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="60">
       <c r="A188" s="2">
         <v>42345</v>
       </c>
-      <c r="B188" s="15" t="s">
-        <v>43</v>
+      <c r="B188" s="96" t="s">
+        <v>39</v>
       </c>
       <c r="C188" s="73" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" ht="45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="150">
       <c r="A189" s="2">
         <v>42345</v>
       </c>
-      <c r="B189" s="100" t="s">
-        <v>39</v>
-      </c>
-      <c r="C189" s="76" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" ht="60">
+      <c r="B189" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C189" s="73" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="45">
       <c r="A190" s="2">
         <v>42345</v>
       </c>
-      <c r="B190" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C190" s="77" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" ht="105">
+      <c r="B190" s="100" t="s">
+        <v>39</v>
+      </c>
+      <c r="C190" s="76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="60">
       <c r="A191" s="2">
         <v>42345</v>
       </c>
-      <c r="B191" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C191" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3">
+      <c r="B191" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C191" s="77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="105">
       <c r="A192" s="2">
         <v>42345</v>
       </c>
-      <c r="B192" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C192" s="96" t="s">
-        <v>50</v>
+      <c r="B192" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -5930,10 +5941,10 @@
         <v>49</v>
       </c>
       <c r="C193" s="96" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="75">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
       <c r="A194" s="2">
         <v>42345</v>
       </c>
@@ -5941,54 +5952,54 @@
         <v>49</v>
       </c>
       <c r="C194" s="96" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="75">
       <c r="A195" s="2">
         <v>42345</v>
       </c>
       <c r="B195" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C195" s="96" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="45">
+      <c r="A196" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B196" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C195" s="96" t="s">
+      <c r="C196" s="96" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="141">
-      <c r="A196" s="80">
+    <row r="197" spans="1:3" ht="141">
+      <c r="A197" s="80">
         <v>42345</v>
       </c>
-      <c r="B196" s="78" t="s">
+      <c r="B197" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="C196" s="78" t="s">
+      <c r="C197" s="78" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="105">
-      <c r="A197" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C197" s="100" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" ht="90">
+    <row r="198" spans="1:3" ht="105">
       <c r="A198" s="2">
         <v>42341</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C198" s="96" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="75">
+        <v>12</v>
+      </c>
+      <c r="C198" s="100" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="90">
       <c r="A199" s="2">
         <v>42341</v>
       </c>
@@ -5996,10 +6007,10 @@
         <v>15</v>
       </c>
       <c r="C199" s="96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="75">
       <c r="A200" s="2">
         <v>42341</v>
       </c>
@@ -6007,7 +6018,7 @@
         <v>15</v>
       </c>
       <c r="C200" s="96" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="30">
@@ -6018,10 +6029,10 @@
         <v>15</v>
       </c>
       <c r="C201" s="96" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="30">
       <c r="A202" s="2">
         <v>42341</v>
       </c>
@@ -6029,32 +6040,32 @@
         <v>15</v>
       </c>
       <c r="C202" s="96" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="90">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="45">
       <c r="A203" s="2">
         <v>42341</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C203" s="96" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="90">
       <c r="A204" s="2">
         <v>42341</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C204" s="96" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" ht="150">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="30">
       <c r="A205" s="2">
         <v>42341</v>
       </c>
@@ -6062,10 +6073,10 @@
         <v>15</v>
       </c>
       <c r="C205" s="96" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" ht="75">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="150">
       <c r="A206" s="2">
         <v>42341</v>
       </c>
@@ -6073,40 +6084,40 @@
         <v>15</v>
       </c>
       <c r="C206" s="96" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" ht="90">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="75">
       <c r="A207" s="2">
         <v>42341</v>
       </c>
-      <c r="B207" s="100" t="s">
-        <v>12</v>
+      <c r="B207" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C207" s="96" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="90">
       <c r="A208" s="2">
         <v>42341</v>
       </c>
-      <c r="B208" s="96" t="s">
-        <v>15</v>
+      <c r="B208" s="100" t="s">
+        <v>12</v>
       </c>
       <c r="C208" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="60">
       <c r="A209" s="2">
         <v>42341</v>
       </c>
       <c r="B209" s="96" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C209" s="96" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -6114,10 +6125,10 @@
         <v>42341</v>
       </c>
       <c r="B210" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C210" s="7" t="s">
-        <v>34</v>
+        <v>12</v>
+      </c>
+      <c r="C210" s="96" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -6128,7 +6139,7 @@
         <v>15</v>
       </c>
       <c r="C211" s="7" t="s">
-        <v>166</v>
+        <v>34</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -6138,8 +6149,8 @@
       <c r="B212" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C212" s="8" t="s">
-        <v>165</v>
+      <c r="C212" s="7" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -6150,67 +6161,69 @@
         <v>15</v>
       </c>
       <c r="C213" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" ht="75">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
       <c r="A214" s="2">
         <v>42341</v>
       </c>
       <c r="B214" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C214" s="100" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" ht="60">
+      <c r="C214" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" ht="75">
       <c r="A215" s="2">
         <v>42341</v>
       </c>
       <c r="B215" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C215" s="96" t="s">
-        <v>26</v>
+        <v>15</v>
+      </c>
+      <c r="C215" s="100" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="60">
       <c r="A216" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B216" s="96"/>
+        <v>42341</v>
+      </c>
+      <c r="B216" s="96" t="s">
+        <v>12</v>
+      </c>
       <c r="C216" s="96" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" ht="45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" ht="60">
       <c r="A217" s="2">
         <v>42340</v>
       </c>
       <c r="B217" s="96"/>
       <c r="C217" s="96" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="45">
       <c r="A218" s="2">
         <v>42340</v>
       </c>
-      <c r="B218" s="2" t="s">
+      <c r="B218" s="96"/>
+      <c r="C218" s="96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="60">
+      <c r="A219" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B219" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C218" s="96" t="s">
+      <c r="C219" s="96" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3">
-      <c r="A219" s="2">
-        <v>42339</v>
-      </c>
-      <c r="B219" s="2"/>
-      <c r="C219" s="96" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -6219,131 +6232,129 @@
       </c>
       <c r="B220" s="2"/>
       <c r="C220" s="96" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" s="2">
+        <v>42339</v>
+      </c>
+      <c r="B221" s="2"/>
+      <c r="C221" s="96" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="64.5">
-      <c r="A221" s="80">
-        <v>42334</v>
-      </c>
-      <c r="B221" s="78" t="s">
-        <v>309</v>
-      </c>
-      <c r="C221" s="78" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="26.25">
+    <row r="222" spans="1:3" ht="64.5">
       <c r="A222" s="80">
         <v>42334</v>
       </c>
       <c r="B222" s="78" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C222" s="78" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" ht="39">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" ht="26.25">
       <c r="A223" s="80">
         <v>42334</v>
       </c>
       <c r="B223" s="78" t="s">
+        <v>307</v>
+      </c>
+      <c r="C223" s="78" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" ht="39">
+      <c r="A224" s="80">
+        <v>42334</v>
+      </c>
+      <c r="B224" s="78" t="s">
         <v>272</v>
       </c>
-      <c r="C223" s="78" t="s">
+      <c r="C224" s="78" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="128.25">
-      <c r="A224" s="80">
-        <v>42333</v>
-      </c>
-      <c r="B224" s="78" t="s">
-        <v>268</v>
-      </c>
-      <c r="C224" s="78" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" ht="51.75">
+    <row r="225" spans="1:3" ht="128.25">
       <c r="A225" s="80">
         <v>42333</v>
       </c>
       <c r="B225" s="78" t="s">
+        <v>268</v>
+      </c>
+      <c r="C225" s="78" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" ht="51.75">
+      <c r="A226" s="80">
+        <v>42333</v>
+      </c>
+      <c r="B226" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C225" s="78" t="s">
+      <c r="C226" s="78" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="226" spans="1:3" ht="26.25">
-      <c r="A226" s="80">
+    <row r="227" spans="1:3" ht="26.25">
+      <c r="A227" s="80">
         <v>42331</v>
       </c>
-      <c r="B226" s="78" t="s">
+      <c r="B227" s="78" t="s">
         <v>313</v>
       </c>
-      <c r="C226" s="78" t="s">
+      <c r="C227" s="78" t="s">
         <v>312</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" ht="39">
-      <c r="A227" s="80">
-        <v>42329</v>
-      </c>
-      <c r="B227" s="78" t="s">
-        <v>315</v>
-      </c>
-      <c r="C227" s="78" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="39">
       <c r="A228" s="80">
-        <v>42328</v>
+        <v>42329</v>
       </c>
       <c r="B228" s="78" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="C228" s="78" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" ht="26.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="39">
       <c r="A229" s="80">
         <v>42328</v>
       </c>
       <c r="B229" s="78" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C229" s="78" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" ht="115.5">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" ht="26.25">
       <c r="A230" s="80">
         <v>42328</v>
       </c>
       <c r="B230" s="78" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C230" s="78" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" ht="90">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" ht="115.5">
       <c r="A231" s="80">
         <v>42328</v>
       </c>
       <c r="B231" s="78" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C231" s="78" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" ht="153.75">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" ht="90">
       <c r="A232" s="80">
         <v>42328</v>
       </c>
@@ -6351,32 +6362,32 @@
         <v>317</v>
       </c>
       <c r="C232" s="78" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" ht="153.75">
+      <c r="A233" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B233" s="78" t="s">
+        <v>317</v>
+      </c>
+      <c r="C233" s="78" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="102.75">
-      <c r="A233" s="80">
+    <row r="234" spans="1:3" ht="102.75">
+      <c r="A234" s="80">
         <v>42324</v>
       </c>
-      <c r="B233" s="78" t="s">
+      <c r="B234" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="C233" s="78" t="s">
+      <c r="C234" s="78" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="90">
-      <c r="A234" s="80">
-        <v>42321</v>
-      </c>
-      <c r="B234" s="78" t="s">
-        <v>327</v>
-      </c>
-      <c r="C234" s="78" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" ht="26.25">
+    <row r="235" spans="1:3" ht="90">
       <c r="A235" s="80">
         <v>42321</v>
       </c>
@@ -6384,72 +6395,83 @@
         <v>327</v>
       </c>
       <c r="C235" s="78" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" ht="26.25">
+      <c r="A236" s="80">
+        <v>42321</v>
+      </c>
+      <c r="B236" s="78" t="s">
+        <v>327</v>
+      </c>
+      <c r="C236" s="78" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="77.25">
-      <c r="A236" s="79">
+    <row r="237" spans="1:3" ht="77.25">
+      <c r="A237" s="79">
         <v>42318</v>
       </c>
-      <c r="B236" s="78" t="s">
+      <c r="B237" s="78" t="s">
         <v>330</v>
       </c>
-      <c r="C236" s="78" t="s">
+      <c r="C237" s="78" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="237" spans="1:3" ht="115.5">
-      <c r="A237" s="79">
+    <row r="238" spans="1:3" ht="115.5">
+      <c r="A238" s="79">
         <v>42311</v>
-      </c>
-      <c r="B237" s="78" t="s">
-        <v>216</v>
-      </c>
-      <c r="C237" s="78" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" ht="77.25">
-      <c r="A238" s="79">
-        <v>42310</v>
       </c>
       <c r="B238" s="78" t="s">
         <v>216</v>
       </c>
       <c r="C238" s="78" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" ht="77.25">
+      <c r="A239" s="79">
+        <v>42310</v>
+      </c>
+      <c r="B239" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="C239" s="78" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="51.75">
-      <c r="A239" s="79">
+    <row r="240" spans="1:3" ht="51.75">
+      <c r="A240" s="79">
         <v>42306</v>
       </c>
-      <c r="B239" s="78" t="s">
+      <c r="B240" s="78" t="s">
         <v>333</v>
       </c>
-      <c r="C239" s="78" t="s">
+      <c r="C240" s="78" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="240" spans="1:3">
-      <c r="A240" s="100"/>
-      <c r="B240" s="100"/>
-      <c r="C240" s="100"/>
+    <row r="241" spans="1:3">
+      <c r="A241" s="100"/>
+      <c r="B241" s="100"/>
+      <c r="C241" s="100"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C240">
+  <autoFilter ref="A1:C241">
     <sortState ref="A2:C201">
       <sortCondition descending="1" ref="A1:A201"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C212" r:id="rId1"/>
-    <hyperlink ref="C173" r:id="rId2"/>
-    <hyperlink ref="C213" r:id="rId3"/>
-    <hyperlink ref="C47" r:id="rId4"/>
-    <hyperlink ref="C32" r:id="rId5"/>
-    <hyperlink ref="C29" r:id="rId6"/>
+    <hyperlink ref="C213" r:id="rId1"/>
+    <hyperlink ref="C174" r:id="rId2"/>
+    <hyperlink ref="C214" r:id="rId3"/>
+    <hyperlink ref="C48" r:id="rId4"/>
+    <hyperlink ref="C33" r:id="rId5"/>
+    <hyperlink ref="C30" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -6469,16 +6491,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="60.75" customHeight="1">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add vmware and network 4 pc entry
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -15,14 +15,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'AS400 Version'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$239</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$241</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="549">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -2797,6 +2797,23 @@
     <t>To learn android application development, open-source app is the best way to go:
 1. On android developer official website page, there are lots of sample
 2. On wikipedia search Open-source Android App, there would be a list and those projects can be found on github.</t>
+  </si>
+  <si>
+    <t>Vmware在上網時遇到的問題: 環境Host Win10+VM player 4-6, Client Kali Linux(base on Debian)都有Ping不到gateway的問題, 原來是要extract其VM的安裝檔在其中找尋小工具vmnetcfg.exe來添加virtual NIC(Vm的三種連接方式分別對應三張virtual nic- bridge:enet0;nat:enat1;?:enet8)
+此問題到vmware workstation player 12解決.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Network for PC</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>對於個人電腦, 幾個變量設好就可以上網了: IP, SUBNETMASK, GATEWAY, DNSNAMESERVER, 而在Linux下, 設定文件大多在etc里, 而Network interface card的運行進程則在/etc/init.d/network</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vmware</t>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3125,7 +3142,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3482,6 +3499,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3530,13 +3550,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4202207</xdr:colOff>
-      <xdr:row>126</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>593914</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>257735</xdr:colOff>
-      <xdr:row>130</xdr:row>
+      <xdr:row>132</xdr:row>
       <xdr:rowOff>102263</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3855,15 +3875,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F239"/>
+  <dimension ref="A1:F241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
     <col min="3" max="3" width="77" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.625" customWidth="1"/>
@@ -3885,772 +3905,772 @@
       <c r="B2" s="100"/>
       <c r="C2" s="100"/>
     </row>
-    <row r="3" spans="1:3" s="102" customFormat="1" ht="60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="102" customFormat="1" ht="75" x14ac:dyDescent="0.3">
       <c r="A3" s="121">
+        <v>42567</v>
+      </c>
+      <c r="B3" s="124" t="s">
+        <v>548</v>
+      </c>
+      <c r="C3" s="124" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="102" customFormat="1" ht="45" x14ac:dyDescent="0.3">
+      <c r="A4" s="121">
+        <v>42567</v>
+      </c>
+      <c r="B4" s="124" t="s">
+        <v>546</v>
+      </c>
+      <c r="C4" s="124" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="102" customFormat="1" ht="60" x14ac:dyDescent="0.3">
+      <c r="A5" s="121">
         <v>42565</v>
       </c>
-      <c r="B3" s="123" t="s">
+      <c r="B5" s="123" t="s">
         <v>543</v>
       </c>
-      <c r="C3" s="123" t="s">
+      <c r="C5" s="123" t="s">
         <v>544</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="102" customFormat="1" ht="60" x14ac:dyDescent="0.3">
-      <c r="A4" s="121">
-        <v>42564</v>
-      </c>
-      <c r="B4" s="122" t="s">
-        <v>534</v>
-      </c>
-      <c r="C4" s="122" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="102" customFormat="1" ht="135" x14ac:dyDescent="0.3">
-      <c r="A5" s="121">
-        <v>42562</v>
-      </c>
-      <c r="B5" s="120" t="s">
-        <v>537</v>
-      </c>
-      <c r="C5" s="120" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="102" customFormat="1" ht="60" x14ac:dyDescent="0.3">
       <c r="A6" s="121">
-        <v>42562</v>
-      </c>
-      <c r="B6" s="120" t="s">
-        <v>536</v>
-      </c>
-      <c r="C6" s="120" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="102" customFormat="1" ht="75" x14ac:dyDescent="0.3">
+        <v>42564</v>
+      </c>
+      <c r="B6" s="122" t="s">
+        <v>534</v>
+      </c>
+      <c r="C6" s="122" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="102" customFormat="1" ht="135" x14ac:dyDescent="0.3">
       <c r="A7" s="121">
         <v>42562</v>
       </c>
       <c r="B7" s="120" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C7" s="120" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="102" customFormat="1" ht="165" x14ac:dyDescent="0.3">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="102" customFormat="1" ht="60" x14ac:dyDescent="0.3">
       <c r="A8" s="121">
         <v>42562</v>
       </c>
       <c r="B8" s="120" t="s">
+        <v>536</v>
+      </c>
+      <c r="C8" s="120" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="102" customFormat="1" ht="75" x14ac:dyDescent="0.3">
+      <c r="A9" s="121">
+        <v>42562</v>
+      </c>
+      <c r="B9" s="120" t="s">
+        <v>535</v>
+      </c>
+      <c r="C9" s="120" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="102" customFormat="1" ht="165" x14ac:dyDescent="0.3">
+      <c r="A10" s="121">
+        <v>42562</v>
+      </c>
+      <c r="B10" s="120" t="s">
         <v>534</v>
       </c>
-      <c r="C8" s="120" t="s">
+      <c r="C10" s="120" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="102" customFormat="1" ht="30" x14ac:dyDescent="0.3">
-      <c r="A9" s="121">
+    <row r="11" spans="1:3" s="102" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A11" s="121">
         <v>42557</v>
       </c>
-      <c r="B9" s="120" t="s">
+      <c r="B11" s="120" t="s">
         <v>525</v>
       </c>
-      <c r="C9" s="120" t="s">
+      <c r="C11" s="120" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="102" customFormat="1" ht="180" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
-      <c r="B10" s="120" t="s">
-        <v>527</v>
-      </c>
-      <c r="C10" s="120" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="102" customFormat="1" ht="135" x14ac:dyDescent="0.3">
-      <c r="A11" s="121">
-        <v>42540</v>
-      </c>
-      <c r="B11" s="120" t="s">
-        <v>529</v>
-      </c>
-      <c r="C11" s="120" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="102" customFormat="1" ht="165" x14ac:dyDescent="0.3">
-      <c r="A12" s="121">
-        <v>42539</v>
-      </c>
+    <row r="12" spans="1:3" s="102" customFormat="1" ht="180" x14ac:dyDescent="0.3">
+      <c r="A12" s="120"/>
       <c r="B12" s="120" t="s">
         <v>527</v>
       </c>
       <c r="C12" s="120" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="102" customFormat="1" ht="135" x14ac:dyDescent="0.3">
+      <c r="A13" s="121">
+        <v>42540</v>
+      </c>
+      <c r="B13" s="120" t="s">
+        <v>529</v>
+      </c>
+      <c r="C13" s="120" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="102" customFormat="1" ht="165" x14ac:dyDescent="0.3">
+      <c r="A14" s="121">
+        <v>42539</v>
+      </c>
+      <c r="B14" s="120" t="s">
+        <v>527</v>
+      </c>
+      <c r="C14" s="120" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="102" customFormat="1" ht="90" x14ac:dyDescent="0.3">
-      <c r="A13" s="121">
+    <row r="15" spans="1:3" s="102" customFormat="1" ht="90" x14ac:dyDescent="0.3">
+      <c r="A15" s="121">
         <v>42539</v>
       </c>
-      <c r="B13" s="120" t="s">
+      <c r="B15" s="120" t="s">
         <v>532</v>
       </c>
-      <c r="C13" s="120" t="s">
+      <c r="C15" s="120" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="102" customFormat="1" ht="60" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+    <row r="16" spans="1:3" s="102" customFormat="1" ht="60" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>42534</v>
       </c>
-      <c r="B14" s="119" t="s">
+      <c r="B16" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="119" t="s">
+      <c r="C16" s="119" t="s">
         <v>524</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="102" customFormat="1" ht="45" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>42517</v>
-      </c>
-      <c r="B15" s="118" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="118" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="102" customFormat="1" ht="105" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>42514</v>
-      </c>
-      <c r="B16" s="117" t="s">
-        <v>519</v>
-      </c>
-      <c r="C16" s="117" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="102" customFormat="1" ht="45" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
+        <v>42517</v>
+      </c>
+      <c r="B17" s="118" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="118" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="102" customFormat="1" ht="105" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>42514</v>
+      </c>
+      <c r="B18" s="117" t="s">
+        <v>519</v>
+      </c>
+      <c r="C18" s="117" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="102" customFormat="1" ht="45" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
         <v>42507</v>
       </c>
-      <c r="B17" s="116" t="s">
+      <c r="B19" s="116" t="s">
         <v>519</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C19" s="116" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="102" customFormat="1" ht="60" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+    <row r="20" spans="1:3" s="102" customFormat="1" ht="60" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
         <v>42502</v>
       </c>
-      <c r="B18" s="115" t="s">
+      <c r="B20" s="115" t="s">
         <v>519</v>
       </c>
-      <c r="C18" s="116" t="s">
+      <c r="C20" s="116" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="102" customFormat="1" ht="75" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>42485</v>
-      </c>
-      <c r="B19" s="113" t="s">
-        <v>516</v>
-      </c>
-      <c r="C19" s="113" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="102" customFormat="1" ht="30" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>42485</v>
-      </c>
-      <c r="B20" s="110" t="s">
-        <v>514</v>
-      </c>
-      <c r="C20" s="110" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="102" customFormat="1" ht="300" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" s="102" customFormat="1" ht="75" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>42485</v>
       </c>
-      <c r="B21" s="112" t="s">
+      <c r="B21" s="113" t="s">
+        <v>516</v>
+      </c>
+      <c r="C21" s="113" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="102" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>42485</v>
+      </c>
+      <c r="B22" s="110" t="s">
+        <v>514</v>
+      </c>
+      <c r="C22" s="110" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="102" customFormat="1" ht="300" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>42485</v>
+      </c>
+      <c r="B23" s="112" t="s">
         <v>241</v>
       </c>
-      <c r="C21" s="112" t="s">
+      <c r="C23" s="112" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="102" customFormat="1" ht="135" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+    <row r="24" spans="1:3" s="102" customFormat="1" ht="135" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
         <v>42479</v>
       </c>
-      <c r="B22" s="111" t="s">
+      <c r="B24" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="C22" s="111" t="s">
+      <c r="C24" s="111" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="102" customFormat="1" ht="90" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+    <row r="25" spans="1:3" s="102" customFormat="1" ht="90" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
         <v>42478</v>
       </c>
-      <c r="B23" s="110" t="s">
+      <c r="B25" s="110" t="s">
         <v>509</v>
       </c>
-      <c r="C23" s="110" t="s">
+      <c r="C25" s="110" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="102" customFormat="1" ht="120" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+    <row r="26" spans="1:3" s="102" customFormat="1" ht="120" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
         <v>42477</v>
       </c>
-      <c r="B24" s="109" t="s">
+      <c r="B26" s="109" t="s">
         <v>509</v>
       </c>
-      <c r="C24" s="109" t="s">
+      <c r="C26" s="109" t="s">
         <v>510</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" s="102" customFormat="1" ht="30" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>42477</v>
-      </c>
-      <c r="B25" s="108" t="s">
-        <v>507</v>
-      </c>
-      <c r="C25" s="108" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>42473</v>
-      </c>
-      <c r="B26" s="106" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="106" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="102" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <v>42473</v>
-      </c>
-      <c r="B27" s="106" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="107" t="s">
-        <v>506</v>
+        <v>42477</v>
+      </c>
+      <c r="B27" s="108" t="s">
+        <v>507</v>
+      </c>
+      <c r="C27" s="108" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
+        <v>42473</v>
+      </c>
+      <c r="B28" s="106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="106" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="102" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>42473</v>
+      </c>
+      <c r="B29" s="106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="107" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
         <v>42469</v>
       </c>
-      <c r="B28" s="105" t="s">
+      <c r="B30" s="105" t="s">
         <v>504</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="102" customFormat="1" ht="60" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B29" s="104" t="s">
-        <v>497</v>
-      </c>
-      <c r="C29" s="104" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="102" customFormat="1" ht="75" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B30" s="104" t="s">
-        <v>499</v>
-      </c>
-      <c r="C30" s="104" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" s="102" customFormat="1" ht="60" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>42463</v>
       </c>
       <c r="B31" s="104" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C31" s="104" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="102" customFormat="1" ht="135" x14ac:dyDescent="0.3">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="102" customFormat="1" ht="75" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>42463</v>
       </c>
-      <c r="B32" s="100" t="s">
-        <v>493</v>
-      </c>
-      <c r="C32" s="100" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="102" customFormat="1" ht="90" x14ac:dyDescent="0.3">
+      <c r="B32" s="104" t="s">
+        <v>499</v>
+      </c>
+      <c r="C32" s="104" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="102" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>42463</v>
       </c>
-      <c r="B33" s="103" t="s">
-        <v>492</v>
-      </c>
-      <c r="C33" s="103" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="102" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="B33" s="104" t="s">
+        <v>501</v>
+      </c>
+      <c r="C33" s="104" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="102" customFormat="1" ht="135" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>42463</v>
       </c>
-      <c r="B34" s="101" t="s">
-        <v>489</v>
-      </c>
-      <c r="C34" s="101" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="102" customFormat="1" ht="105" x14ac:dyDescent="0.3">
+      <c r="B34" s="100" t="s">
+        <v>493</v>
+      </c>
+      <c r="C34" s="100" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="102" customFormat="1" ht="90" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>42463</v>
       </c>
-      <c r="B35" s="101" t="s">
+      <c r="B35" s="103" t="s">
+        <v>492</v>
+      </c>
+      <c r="C35" s="103" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="102" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B36" s="101" t="s">
+        <v>489</v>
+      </c>
+      <c r="C36" s="101" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="102" customFormat="1" ht="105" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B37" s="101" t="s">
         <v>488</v>
       </c>
-      <c r="C35" s="101" t="s">
+      <c r="C37" s="101" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="102" customFormat="1" ht="150" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <v>42462</v>
-      </c>
-      <c r="B36" s="100" t="s">
-        <v>486</v>
-      </c>
-      <c r="C36" s="100" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" s="102" customFormat="1" ht="135" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <v>42462</v>
-      </c>
-      <c r="B37" s="100" t="s">
-        <v>484</v>
-      </c>
-      <c r="C37" s="100" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="102" customFormat="1" ht="240" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" s="102" customFormat="1" ht="150" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>42462</v>
       </c>
       <c r="B38" s="100" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="C38" s="100" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="102" customFormat="1" ht="120" x14ac:dyDescent="0.3">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="102" customFormat="1" ht="135" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>42462</v>
       </c>
       <c r="B39" s="100" t="s">
+        <v>484</v>
+      </c>
+      <c r="C39" s="100" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="102" customFormat="1" ht="240" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>42462</v>
+      </c>
+      <c r="B40" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="C39" s="100" t="s">
+      <c r="C40" s="100" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="102" customFormat="1" ht="120" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>42462</v>
+      </c>
+      <c r="B41" s="100" t="s">
+        <v>480</v>
+      </c>
+      <c r="C41" s="100" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
-        <v>42460</v>
-      </c>
-      <c r="B40" s="99" t="s">
-        <v>477</v>
-      </c>
-      <c r="C40" s="99" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <v>42460</v>
-      </c>
-      <c r="B41" s="99" t="s">
-        <v>476</v>
-      </c>
-      <c r="C41" s="99" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>42460</v>
       </c>
       <c r="B42" s="99" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C42" s="99" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.3">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42460</v>
       </c>
       <c r="B43" s="99" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C43" s="99" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.3">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>42459</v>
+        <v>42460</v>
       </c>
       <c r="B44" s="99" t="s">
-        <v>470</v>
-      </c>
-      <c r="C44" s="98" t="s">
-        <v>473</v>
+        <v>475</v>
+      </c>
+      <c r="C44" s="99" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
+        <v>42460</v>
+      </c>
+      <c r="B45" s="99" t="s">
+        <v>478</v>
+      </c>
+      <c r="C45" s="99" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
         <v>42459</v>
       </c>
-      <c r="B45" s="99" t="s">
+      <c r="B46" s="99" t="s">
+        <v>470</v>
+      </c>
+      <c r="C46" s="98" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>42459</v>
+      </c>
+      <c r="B47" s="99" t="s">
         <v>241</v>
       </c>
-      <c r="C45" s="99" t="s">
+      <c r="C47" s="99" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
+    <row r="48" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
         <v>42458</v>
       </c>
-      <c r="B46" s="97" t="s">
+      <c r="B48" s="97" t="s">
         <v>470</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C48" s="8" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B47" s="96" t="s">
-        <v>254</v>
-      </c>
-      <c r="C47" s="100" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="60" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B48" s="96" t="s">
-        <v>462</v>
-      </c>
-      <c r="C48" s="44" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>42456</v>
       </c>
       <c r="B49" s="96" t="s">
-        <v>463</v>
-      </c>
-      <c r="C49" s="44" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+      <c r="C49" s="100" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>42456</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>466</v>
+      <c r="B50" s="96" t="s">
+        <v>462</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>42456</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="96" t="s">
+        <v>463</v>
+      </c>
+      <c r="C51" s="44" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C52" s="44" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="C51" s="44" t="s">
+      <c r="C53" s="44" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="66.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A52" s="79">
+    <row r="54" spans="1:3" ht="66.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A54" s="79">
         <v>42453</v>
       </c>
-      <c r="B52" s="78" t="s">
+      <c r="B54" s="78" t="s">
         <v>264</v>
       </c>
-      <c r="C52" s="78" t="s">
+      <c r="C54" s="78" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A53" s="79">
+    <row r="55" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+      <c r="A55" s="79">
         <v>42453</v>
       </c>
-      <c r="B53" s="78" t="s">
+      <c r="B55" s="78" t="s">
         <v>262</v>
       </c>
-      <c r="C53" s="78" t="s">
+      <c r="C55" s="78" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A54" s="79">
+    <row r="56" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+      <c r="A56" s="79">
         <v>42452</v>
       </c>
-      <c r="B54" s="78" t="s">
+      <c r="B56" s="78" t="s">
         <v>260</v>
       </c>
-      <c r="C54" s="78" t="s">
+      <c r="C56" s="78" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="165" x14ac:dyDescent="0.3">
-      <c r="A55" s="75">
+    <row r="57" spans="1:3" ht="165" x14ac:dyDescent="0.3">
+      <c r="A57" s="75">
         <v>42451</v>
       </c>
-      <c r="B55" s="74" t="s">
+      <c r="B57" s="74" t="s">
         <v>247</v>
       </c>
-      <c r="C55" s="100" t="s">
+      <c r="C57" s="100" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
-        <v>42451</v>
-      </c>
-      <c r="B56" s="100" t="s">
-        <v>249</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A57" s="2">
-        <v>42451</v>
-      </c>
-      <c r="B57" s="96" t="s">
-        <v>196</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="135" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>42451</v>
       </c>
-      <c r="B58" s="96" t="s">
+      <c r="B58" s="100" t="s">
+        <v>249</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>42451</v>
+      </c>
+      <c r="B59" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="135" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>42451</v>
+      </c>
+      <c r="B60" s="96" t="s">
         <v>253</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
-      <c r="A59" s="79">
+    <row r="61" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A61" s="79">
         <v>42451</v>
       </c>
-      <c r="B59" s="78" t="s">
+      <c r="B61" s="78" t="s">
         <v>253</v>
       </c>
-      <c r="C59" s="78" t="s">
+      <c r="C61" s="78" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="79.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="79">
+    <row r="62" spans="1:3" ht="79.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="79">
         <v>42447</v>
       </c>
-      <c r="B60" s="78" t="s">
+      <c r="B62" s="78" t="s">
         <v>257</v>
       </c>
-      <c r="C60" s="78" t="s">
+      <c r="C62" s="78" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
         <v>42440</v>
       </c>
-      <c r="B61" s="100" t="s">
+      <c r="B63" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="C61" s="100" t="s">
+      <c r="C63" s="100" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="75" x14ac:dyDescent="0.3">
-      <c r="A62" s="2">
+    <row r="64" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
         <v>42436</v>
       </c>
-      <c r="B62" s="96" t="s">
+      <c r="B64" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>245</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
-      <c r="A63" s="79">
-        <v>42431</v>
-      </c>
-      <c r="B63" s="78" t="s">
-        <v>274</v>
-      </c>
-      <c r="C63" s="78" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A64" s="79">
-        <v>42431</v>
-      </c>
-      <c r="B64" s="78" t="s">
-        <v>272</v>
-      </c>
-      <c r="C64" s="78" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A65" s="79">
-        <v>42430</v>
+        <v>42431</v>
       </c>
       <c r="B65" s="78" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C65" s="78" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A66" s="79">
+        <v>42431</v>
+      </c>
+      <c r="B66" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="C66" s="78" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A67" s="79">
+        <v>42430</v>
+      </c>
+      <c r="B67" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="C67" s="78" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+      <c r="A68" s="79">
         <v>42428</v>
       </c>
-      <c r="B66" s="78" t="s">
+      <c r="B68" s="78" t="s">
         <v>268</v>
       </c>
-      <c r="C66" s="78" t="s">
+      <c r="C68" s="78" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
-        <v>42426</v>
-      </c>
-      <c r="B67" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="C67" s="100" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="79.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="79">
-        <v>42426</v>
-      </c>
-      <c r="B68" s="78" t="s">
-        <v>266</v>
-      </c>
-      <c r="C68" s="78" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
+        <v>42426</v>
+      </c>
+      <c r="B69" s="100" t="s">
+        <v>186</v>
+      </c>
+      <c r="C69" s="100" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="79.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="79">
+        <v>42426</v>
+      </c>
+      <c r="B70" s="78" t="s">
+        <v>266</v>
+      </c>
+      <c r="C70" s="78" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
         <v>42425</v>
       </c>
-      <c r="B69" s="100" t="s">
+      <c r="B71" s="100" t="s">
         <v>241</v>
       </c>
-      <c r="C69" s="100" t="s">
+      <c r="C71" s="100" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
         <v>42425</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A71" s="79">
-        <v>42425</v>
-      </c>
-      <c r="B71" s="78" t="s">
-        <v>276</v>
-      </c>
-      <c r="C71" s="78" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A72" s="79">
-        <v>42425</v>
-      </c>
-      <c r="B72" s="78" t="s">
-        <v>276</v>
-      </c>
-      <c r="C72" s="78" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="27" x14ac:dyDescent="0.3">
@@ -4658,788 +4678,790 @@
         <v>42425</v>
       </c>
       <c r="B73" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="C73" s="78" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+      <c r="A74" s="79">
+        <v>42425</v>
+      </c>
+      <c r="B74" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="C74" s="78" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+      <c r="A75" s="79">
+        <v>42425</v>
+      </c>
+      <c r="B75" s="78" t="s">
         <v>279</v>
       </c>
-      <c r="C73" s="78" t="s">
+      <c r="C75" s="78" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="180" x14ac:dyDescent="0.3">
-      <c r="A74" s="2">
+    <row r="76" spans="1:3" ht="180" x14ac:dyDescent="0.3">
+      <c r="A76" s="2">
         <v>42424</v>
       </c>
-      <c r="B74" s="100" t="s">
+      <c r="B76" s="100" t="s">
         <v>239</v>
       </c>
-      <c r="C74" s="114" t="s">
+      <c r="C76" s="114" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A75" s="2">
+    <row r="77" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A77" s="2">
         <v>42423</v>
       </c>
-      <c r="B75" s="96" t="s">
+      <c r="B77" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="C77" s="11" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="79">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="79">
         <v>42423</v>
       </c>
-      <c r="B76" s="78" t="s">
+      <c r="B78" s="78" t="s">
         <v>281</v>
       </c>
-      <c r="C76" s="78" t="s">
+      <c r="C78" s="78" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="90" x14ac:dyDescent="0.3">
-      <c r="A77" s="2">
+    <row r="79" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+      <c r="A79" s="2">
         <v>42422</v>
       </c>
-      <c r="B77" s="100" t="s">
+      <c r="B79" s="100" t="s">
         <v>236</v>
       </c>
-      <c r="C77" s="100" t="s">
+      <c r="C79" s="100" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="60" x14ac:dyDescent="0.3">
-      <c r="A78" s="2">
+    <row r="80" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="A80" s="2">
         <v>42419</v>
       </c>
-      <c r="B78" s="10" t="s">
+      <c r="B80" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="C78" s="36" t="s">
+      <c r="C80" s="36" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="180" x14ac:dyDescent="0.3">
-      <c r="A79" s="2">
+    <row r="81" spans="1:3" ht="180" x14ac:dyDescent="0.3">
+      <c r="A81" s="2">
         <v>42418</v>
       </c>
-      <c r="B79" s="10" t="s">
+      <c r="B81" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C79" s="18" t="s">
+      <c r="C81" s="18" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A80" s="2">
-        <v>42403</v>
-      </c>
-      <c r="B80" s="96" t="s">
-        <v>229</v>
-      </c>
-      <c r="C80" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="75" x14ac:dyDescent="0.3">
-      <c r="A81" s="2">
-        <v>42403</v>
-      </c>
-      <c r="B81" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="C81" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>42403</v>
       </c>
-      <c r="B82" s="12"/>
+      <c r="B82" s="96" t="s">
+        <v>229</v>
+      </c>
       <c r="C82" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A83" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+      <c r="A84" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B84" s="12"/>
+      <c r="C84" s="12" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="90" x14ac:dyDescent="0.3">
-      <c r="A83" s="2">
+    <row r="85" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+      <c r="A85" s="2">
         <v>42398</v>
       </c>
-      <c r="B83" s="12" t="s">
+      <c r="B85" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C83" s="12" t="s">
+      <c r="C85" s="12" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A84" s="2">
-        <v>42398</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="C84" s="12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="2">
-        <v>42397</v>
-      </c>
-      <c r="B85" s="96" t="s">
-        <v>201</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
+        <v>42398</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="2">
+        <v>42397</v>
+      </c>
+      <c r="B87" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A88" s="2">
         <v>42396</v>
       </c>
-      <c r="B86" s="12" t="s">
+      <c r="B88" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C86" s="12" t="s">
+      <c r="C88" s="12" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A87" s="2">
+    <row r="89" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A89" s="2">
         <v>42396</v>
       </c>
-      <c r="B87" s="96" t="s">
+      <c r="B89" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="C87" s="14" t="s">
+      <c r="C89" s="14" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="132.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="79">
+    <row r="90" spans="1:3" ht="132.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="79">
         <v>42386</v>
       </c>
-      <c r="B88" s="78" t="s">
+      <c r="B90" s="78" t="s">
         <v>283</v>
       </c>
-      <c r="C88" s="78" t="s">
+      <c r="C90" s="78" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="66.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A89" s="79">
+    <row r="91" spans="1:3" ht="66.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A91" s="79">
         <v>42386</v>
       </c>
-      <c r="B89" s="78" t="s">
+      <c r="B91" s="78" t="s">
         <v>285</v>
       </c>
-      <c r="C89" s="78" t="s">
+      <c r="C91" s="78" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A90" s="2">
+    <row r="92" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A92" s="2">
         <v>42384</v>
       </c>
-      <c r="B90" s="100" t="s">
+      <c r="B92" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="C90" s="100" t="s">
+      <c r="C92" s="100" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="180" x14ac:dyDescent="0.3">
-      <c r="A91" s="2">
+    <row r="93" spans="1:3" ht="180" x14ac:dyDescent="0.3">
+      <c r="A93" s="2">
         <v>42382</v>
       </c>
-      <c r="B91" s="14" t="s">
+      <c r="B93" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="C91" s="14" t="s">
+      <c r="C93" s="14" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="66.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A92" s="79">
+    <row r="94" spans="1:3" ht="66.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A94" s="79">
         <v>42382</v>
       </c>
-      <c r="B92" s="78" t="s">
+      <c r="B94" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="C92" s="78" t="s">
+      <c r="C94" s="78" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A93" s="2">
+    <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A95" s="2">
         <v>42381</v>
       </c>
-      <c r="B93" s="100" t="s">
+      <c r="B95" s="100" t="s">
         <v>216</v>
       </c>
-      <c r="C93" s="100" t="s">
+      <c r="C95" s="100" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A94" s="2">
-        <v>42380</v>
-      </c>
-      <c r="B94" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C94" s="16" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="60" x14ac:dyDescent="0.3">
-      <c r="A95" s="2">
-        <v>42380</v>
-      </c>
-      <c r="B95" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="C95" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="180" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>42380</v>
       </c>
-      <c r="B96" s="50" t="s">
+      <c r="B96" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C96" s="16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="A97" s="2">
+        <v>42380</v>
+      </c>
+      <c r="B97" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C96" s="18" t="s">
+      <c r="C97" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="180" x14ac:dyDescent="0.3">
+      <c r="A98" s="2">
+        <v>42380</v>
+      </c>
+      <c r="B98" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="C98" s="18" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="277.8" x14ac:dyDescent="0.3">
-      <c r="A97" s="79">
+    <row r="99" spans="1:3" ht="277.8" x14ac:dyDescent="0.3">
+      <c r="A99" s="79">
         <v>42380</v>
       </c>
-      <c r="B97" s="78" t="s">
+      <c r="B99" s="78" t="s">
         <v>288</v>
       </c>
-      <c r="C97" s="78" t="s">
+      <c r="C99" s="78" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="106.2" x14ac:dyDescent="0.3">
-      <c r="A98" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B98" s="78" t="s">
-        <v>291</v>
-      </c>
-      <c r="C98" s="78" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="106.2" x14ac:dyDescent="0.3">
-      <c r="A99" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B99" s="78" t="s">
-        <v>293</v>
-      </c>
-      <c r="C99" s="78" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="145.80000000000001" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A100" s="79">
         <v>42378</v>
       </c>
       <c r="B100" s="78" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C100" s="78" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="79.8" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="106.2" x14ac:dyDescent="0.3">
       <c r="A101" s="79">
         <v>42378</v>
       </c>
       <c r="B101" s="78" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C101" s="78" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="106.2" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A102" s="79">
         <v>42378</v>
       </c>
       <c r="B102" s="78" t="s">
+        <v>297</v>
+      </c>
+      <c r="C102" s="78" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="79.8" x14ac:dyDescent="0.3">
+      <c r="A103" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B103" s="78" t="s">
+        <v>297</v>
+      </c>
+      <c r="C103" s="78" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="106.2" x14ac:dyDescent="0.3">
+      <c r="A104" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B104" s="78" t="s">
         <v>295</v>
       </c>
-      <c r="C102" s="78" t="s">
+      <c r="C104" s="78" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="60" x14ac:dyDescent="0.3">
-      <c r="A103" s="2">
+    <row r="105" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="A105" s="2">
         <v>42377</v>
       </c>
-      <c r="B103" s="100" t="s">
+      <c r="B105" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="C103" s="100" t="s">
+      <c r="C105" s="100" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="93" x14ac:dyDescent="0.3">
-      <c r="A104" s="79">
+    <row r="106" spans="1:3" ht="93" x14ac:dyDescent="0.3">
+      <c r="A106" s="79">
         <v>42376</v>
       </c>
-      <c r="B104" s="78" t="s">
+      <c r="B106" s="78" t="s">
         <v>300</v>
       </c>
-      <c r="C104" s="78" t="s">
+      <c r="C106" s="78" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A105" s="2">
+    <row r="107" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A107" s="2">
         <v>42375</v>
       </c>
-      <c r="B105" s="15" t="s">
+      <c r="B107" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C105" s="100" t="s">
+      <c r="C107" s="100" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="2">
         <v>42369</v>
       </c>
-      <c r="B106" s="100" t="s">
+      <c r="B108" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="C106" s="19" t="s">
+      <c r="C108" s="19" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="180" x14ac:dyDescent="0.3">
-      <c r="A107" s="2">
-        <v>42368</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C107" s="19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="135" x14ac:dyDescent="0.3">
-      <c r="A108" s="2">
-        <v>42368</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C108" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="180" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>42368</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C109" s="19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="135" x14ac:dyDescent="0.3">
+      <c r="A110" s="2">
+        <v>42368</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C110" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A111" s="2">
+        <v>42368</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C109" s="20" t="s">
+      <c r="C111" s="20" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A110" s="2">
+    <row r="112" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A112" s="2">
         <v>42366</v>
       </c>
-      <c r="B110" s="20" t="s">
+      <c r="B112" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C110" s="20" t="s">
+      <c r="C112" s="20" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A111" s="2">
-        <v>42366</v>
-      </c>
-      <c r="B111" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C111" s="20" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="150" x14ac:dyDescent="0.3">
-      <c r="A112" s="2">
-        <v>42361</v>
-      </c>
-      <c r="C112" s="20" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
-        <v>42361</v>
+        <v>42366</v>
+      </c>
+      <c r="B113" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="C113" s="20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="270" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="150" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>42361</v>
       </c>
-      <c r="B114" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C114" s="22" t="s">
-        <v>187</v>
+      <c r="C114" s="20" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>42361</v>
       </c>
-      <c r="B115" s="100" t="s">
-        <v>53</v>
-      </c>
       <c r="C115" s="20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="270" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>42361</v>
       </c>
       <c r="B116" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="C116" s="21" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="225" x14ac:dyDescent="0.3">
+      <c r="C116" s="22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>42361</v>
       </c>
-      <c r="B117" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C117" s="22" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="B117" s="100" t="s">
+        <v>53</v>
+      </c>
+      <c r="C117" s="20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>42361</v>
       </c>
-      <c r="B118" s="100" t="s">
-        <v>49</v>
-      </c>
-      <c r="C118" s="22" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+      <c r="B118" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C118" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="225" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>42361</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>196</v>
+      <c r="B119" s="35" t="s">
+        <v>186</v>
       </c>
       <c r="C119" s="22" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>42361</v>
       </c>
-      <c r="B120" s="24" t="s">
+      <c r="B120" s="100" t="s">
+        <v>49</v>
+      </c>
+      <c r="C120" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+      <c r="A121" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C120" s="24" t="s">
+      <c r="C121" s="22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="A122" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B122" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C122" s="24" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" s="40">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="40">
         <v>42360</v>
       </c>
-      <c r="B121" s="50" t="s">
+      <c r="B123" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C123" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" s="40">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="40">
         <v>42360</v>
       </c>
-      <c r="B122" s="50" t="s">
+      <c r="B124" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C124" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="106.2" x14ac:dyDescent="0.3">
-      <c r="A123" s="80">
+    <row r="125" spans="1:3" ht="106.2" x14ac:dyDescent="0.3">
+      <c r="A125" s="80">
         <v>42360</v>
       </c>
-      <c r="B123" s="78" t="s">
+      <c r="B125" s="78" t="s">
         <v>302</v>
       </c>
-      <c r="C123" s="78" t="s">
+      <c r="C125" s="78" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A124" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B124" s="100" t="s">
-        <v>43</v>
-      </c>
-      <c r="C124" s="100" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B125" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="C125" s="23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>42356</v>
       </c>
-      <c r="B126" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="C126" s="25" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="B126" s="100" t="s">
+        <v>43</v>
+      </c>
+      <c r="C126" s="100" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <v>42356</v>
       </c>
-      <c r="B127" s="96"/>
-      <c r="C127" s="25" t="s">
+      <c r="B127" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="C127" s="23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="2">
+        <v>42356</v>
+      </c>
+      <c r="B128" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C128" s="25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A129" s="2">
+        <v>42356</v>
+      </c>
+      <c r="B129" s="96"/>
+      <c r="C129" s="25" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A128" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B128" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="C128" s="26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B129" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C129" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="150" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>42355</v>
       </c>
-      <c r="B130" s="13" t="s">
-        <v>33</v>
+      <c r="B130" s="96" t="s">
+        <v>91</v>
       </c>
       <c r="C130" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <v>42355</v>
       </c>
-      <c r="B131" s="100" t="s">
-        <v>168</v>
-      </c>
-      <c r="C131" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="B131" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C131" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="150" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>42355</v>
       </c>
-      <c r="B132" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C132" s="28" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B132" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C132" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <v>42355</v>
       </c>
-      <c r="B133" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="C133" s="29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="B133" s="100" t="s">
+        <v>168</v>
+      </c>
+      <c r="C133" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <v>42355</v>
       </c>
-      <c r="B134" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C134" s="29" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="135" x14ac:dyDescent="0.3">
+      <c r="B134" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C134" s="28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
         <v>42355</v>
       </c>
-      <c r="B135" s="100" t="s">
-        <v>173</v>
+      <c r="B135" s="29" t="s">
+        <v>171</v>
       </c>
       <c r="C135" s="29" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <v>42355</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C136" s="42" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="B136" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C136" s="29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="135" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
         <v>42355</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" s="100" t="s">
         <v>173</v>
       </c>
-      <c r="C137" s="30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C137" s="29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="75" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>42355</v>
       </c>
-      <c r="C138" s="30" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B138" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C138" s="42" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
         <v>42355</v>
       </c>
-      <c r="B139" s="42"/>
+      <c r="B139" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="C139" s="30" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
         <v>42355</v>
       </c>
-      <c r="B140" s="42"/>
       <c r="C140" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" s="2">
+        <v>42355</v>
+      </c>
+      <c r="B141" s="42"/>
+      <c r="C141" s="30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" s="2">
+        <v>42355</v>
+      </c>
+      <c r="B142" s="42"/>
+      <c r="C142" s="30" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="60" x14ac:dyDescent="0.3">
-      <c r="A141" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B141" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="C141" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A142" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B142" s="26"/>
-      <c r="C142" s="31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <v>42352</v>
       </c>
-      <c r="B143" s="26"/>
-      <c r="C143" s="70" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B143" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C143" s="30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
         <v>42352</v>
       </c>
       <c r="B144" s="26"/>
-      <c r="C144" s="32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C144" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="75" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <v>42352</v>
       </c>
-      <c r="B145" s="96"/>
-      <c r="C145" s="33" t="s">
-        <v>75</v>
+      <c r="B145" s="26"/>
+      <c r="C145" s="70" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
         <v>42352</v>
       </c>
-      <c r="B146" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C146" s="34" t="s">
-        <v>72</v>
+      <c r="B146" s="26"/>
+      <c r="C146" s="32" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -5447,477 +5469,475 @@
         <v>42352</v>
       </c>
       <c r="B147" s="96"/>
-      <c r="C147" s="34" t="s">
-        <v>73</v>
+      <c r="C147" s="33" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
         <v>42352</v>
       </c>
-      <c r="B148" s="96"/>
-      <c r="C148" s="37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" ht="45" x14ac:dyDescent="0.3">
+      <c r="B148" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C148" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
         <v>42352</v>
       </c>
-      <c r="B149" s="37"/>
-      <c r="C149" s="37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+      <c r="B149" s="96"/>
+      <c r="C149" s="34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="2">
         <v>42352</v>
       </c>
       <c r="B150" s="96"/>
-      <c r="C150" s="96" t="s">
-        <v>77</v>
+      <c r="C150" s="37" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <v>42352</v>
       </c>
-      <c r="B151" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C151" s="96" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" ht="45" x14ac:dyDescent="0.3">
+      <c r="B151" s="37"/>
+      <c r="C151" s="37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
         <v>42352</v>
       </c>
-      <c r="B152" s="100"/>
-      <c r="C152" s="39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+      <c r="B152" s="96"/>
+      <c r="C152" s="96" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
         <v>42352</v>
       </c>
-      <c r="B153" s="38"/>
-      <c r="C153" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="F153" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" ht="75" x14ac:dyDescent="0.3">
+      <c r="B153" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C153" s="96" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
         <v>42352</v>
       </c>
-      <c r="B154" s="41"/>
-      <c r="C154" s="41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" ht="45" x14ac:dyDescent="0.3">
+      <c r="B154" s="100"/>
+      <c r="C154" s="39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A155" s="2">
         <v>42352</v>
       </c>
-      <c r="B155" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C155" s="41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+      <c r="B155" s="38"/>
+      <c r="C155" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="F155" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="75" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
         <v>42352</v>
       </c>
-      <c r="B156" s="43"/>
-      <c r="C156" s="43" t="s">
-        <v>84</v>
+      <c r="B156" s="41"/>
+      <c r="C156" s="41" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A157" s="2">
         <v>42352</v>
       </c>
-      <c r="B157" s="44"/>
-      <c r="C157" s="44" t="s">
-        <v>177</v>
+      <c r="B157" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C157" s="41" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
         <v>42352</v>
       </c>
-      <c r="B158" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="C158" s="46" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+      <c r="B158" s="43"/>
+      <c r="C158" s="43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A159" s="2">
         <v>42352</v>
       </c>
-      <c r="B159" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C159" s="47" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B159" s="44"/>
+      <c r="C159" s="44" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
         <v>42352</v>
       </c>
-      <c r="B160" s="100" t="s">
+      <c r="B160" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C160" s="46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A161" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B161" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C161" s="47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B162" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="C160" s="48" t="s">
+      <c r="C162" s="48" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="135" x14ac:dyDescent="0.3">
-      <c r="A161" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B161" s="49"/>
-      <c r="C161" s="49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="60" x14ac:dyDescent="0.3">
-      <c r="A162" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B162" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="C162" s="51" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" ht="135" x14ac:dyDescent="0.3">
       <c r="A163" s="2">
         <v>42349</v>
       </c>
-      <c r="B163" s="96"/>
-      <c r="C163" s="53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="120" x14ac:dyDescent="0.3">
+      <c r="B163" s="49"/>
+      <c r="C163" s="49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A164" s="2">
         <v>42349</v>
       </c>
-      <c r="B164" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C164" s="53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="150" x14ac:dyDescent="0.3">
+      <c r="B164" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C164" s="51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A165" s="2">
         <v>42349</v>
       </c>
-      <c r="B165" s="52"/>
-      <c r="C165" s="52" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="B165" s="96"/>
+      <c r="C165" s="53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="120" x14ac:dyDescent="0.3">
       <c r="A166" s="2">
         <v>42349</v>
       </c>
-      <c r="B166" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C166" s="54" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B166" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C166" s="53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="150" x14ac:dyDescent="0.3">
       <c r="A167" s="2">
         <v>42349</v>
       </c>
-      <c r="B167" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C167" s="55" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B167" s="52"/>
+      <c r="C167" s="52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A168" s="2">
         <v>42349</v>
       </c>
-      <c r="B168" s="100"/>
-      <c r="C168" s="57" t="s">
-        <v>78</v>
+      <c r="B168" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C168" s="54" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="2">
         <v>42349</v>
       </c>
-      <c r="B169" s="58"/>
-      <c r="C169" s="58" t="s">
-        <v>62</v>
+      <c r="B169" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C169" s="55" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="2">
         <v>42349</v>
       </c>
-      <c r="B170" s="59"/>
-      <c r="C170" s="59" t="s">
-        <v>70</v>
+      <c r="B170" s="100"/>
+      <c r="C170" s="57" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="2">
         <v>42349</v>
       </c>
-      <c r="B171" s="60"/>
-      <c r="C171" s="60" t="s">
-        <v>64</v>
+      <c r="B171" s="58"/>
+      <c r="C171" s="58" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="2">
         <v>42349</v>
       </c>
-      <c r="B172" s="61"/>
-      <c r="C172" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="B172" s="59"/>
+      <c r="C172" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="2">
         <v>42349</v>
       </c>
-      <c r="B173" s="62" t="s">
+      <c r="B173" s="60"/>
+      <c r="C173" s="60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" s="2">
+        <v>42349</v>
+      </c>
+      <c r="B174" s="61"/>
+      <c r="C174" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="A175" s="2">
+        <v>42349</v>
+      </c>
+      <c r="B175" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="C173" s="100" t="s">
+      <c r="C175" s="100" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="90" x14ac:dyDescent="0.3">
-      <c r="A174" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B174" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C174" s="62" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A175" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C175" s="62" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" ht="90" x14ac:dyDescent="0.3">
       <c r="A176" s="2">
         <v>42345</v>
       </c>
-      <c r="B176" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C176" s="63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B176" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C176" s="62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A177" s="2">
         <v>42345</v>
       </c>
-      <c r="B177" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C177" s="64" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="B177" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C177" s="62" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="2">
         <v>42345</v>
       </c>
       <c r="B178" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C178" s="65" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="195" x14ac:dyDescent="0.3">
+      <c r="C178" s="63" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="2">
         <v>42345</v>
       </c>
-      <c r="B179" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C179" s="66" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="135" x14ac:dyDescent="0.3">
+      <c r="B179" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C179" s="64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A180" s="2">
         <v>42345</v>
       </c>
-      <c r="B180" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="C180" s="67" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="B180" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C180" s="65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="195" x14ac:dyDescent="0.3">
       <c r="A181" s="2">
         <v>42345</v>
       </c>
-      <c r="B181" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="C181" s="68" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="B181" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C181" s="66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="135" x14ac:dyDescent="0.3">
       <c r="A182" s="2">
         <v>42345</v>
       </c>
-      <c r="B182" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C182" s="69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="B182" s="100" t="s">
+        <v>31</v>
+      </c>
+      <c r="C182" s="67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="75" x14ac:dyDescent="0.3">
       <c r="A183" s="2">
         <v>42345</v>
       </c>
-      <c r="B183" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C183" s="73" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B183" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C183" s="68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="75" x14ac:dyDescent="0.3">
       <c r="A184" s="2">
         <v>42345</v>
       </c>
-      <c r="B184" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="C184" s="73" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B184" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C184" s="69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A185" s="2">
         <v>42345</v>
       </c>
-      <c r="B185" s="72" t="s">
-        <v>39</v>
+      <c r="B185" s="100" t="s">
+        <v>12</v>
       </c>
       <c r="C185" s="73" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="2">
         <v>42345</v>
       </c>
-      <c r="B186" s="96" t="s">
+      <c r="B186" s="71" t="s">
         <v>39</v>
       </c>
       <c r="C186" s="73" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="150" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="2">
         <v>42345</v>
       </c>
-      <c r="B187" s="15" t="s">
-        <v>43</v>
+      <c r="B187" s="72" t="s">
+        <v>39</v>
       </c>
       <c r="C187" s="73" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A188" s="2">
         <v>42345</v>
       </c>
-      <c r="B188" s="100" t="s">
+      <c r="B188" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="C188" s="76" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="C188" s="73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="150" x14ac:dyDescent="0.3">
       <c r="A189" s="2">
         <v>42345</v>
       </c>
       <c r="B189" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C189" s="77" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+      <c r="C189" s="73" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A190" s="2">
         <v>42345</v>
       </c>
       <c r="B190" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C190" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="C190" s="76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A191" s="2">
         <v>42345</v>
       </c>
-      <c r="B191" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C191" s="96" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B191" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C191" s="77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A192" s="2">
         <v>42345</v>
       </c>
-      <c r="B192" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C192" s="96" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="B192" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="2">
         <v>42345</v>
       </c>
@@ -5925,65 +5945,65 @@
         <v>49</v>
       </c>
       <c r="C193" s="96" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="2">
         <v>42345</v>
       </c>
       <c r="B194" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C194" s="96" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A195" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B195" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C195" s="96" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A196" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B196" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C194" s="96" t="s">
+      <c r="C196" s="96" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="159" x14ac:dyDescent="0.3">
-      <c r="A195" s="80">
+    <row r="197" spans="1:3" ht="159" x14ac:dyDescent="0.3">
+      <c r="A197" s="80">
         <v>42345</v>
       </c>
-      <c r="B195" s="78" t="s">
+      <c r="B197" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="C195" s="78" t="s">
+      <c r="C197" s="78" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="105" x14ac:dyDescent="0.3">
-      <c r="A196" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C196" s="100" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" ht="90" x14ac:dyDescent="0.3">
-      <c r="A197" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C197" s="96" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A198" s="2">
         <v>42341</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C198" s="96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="C198" s="100" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="90" x14ac:dyDescent="0.3">
       <c r="A199" s="2">
         <v>42341</v>
       </c>
@@ -5991,10 +6011,10 @@
         <v>15</v>
       </c>
       <c r="C199" s="96" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="75" x14ac:dyDescent="0.3">
       <c r="A200" s="2">
         <v>42341</v>
       </c>
@@ -6002,10 +6022,10 @@
         <v>15</v>
       </c>
       <c r="C200" s="96" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A201" s="2">
         <v>42341</v>
       </c>
@@ -6013,21 +6033,21 @@
         <v>15</v>
       </c>
       <c r="C201" s="96" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A202" s="2">
         <v>42341</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C202" s="96" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A203" s="2">
         <v>42341</v>
       </c>
@@ -6035,21 +6055,21 @@
         <v>15</v>
       </c>
       <c r="C203" s="96" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="150" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="90" x14ac:dyDescent="0.3">
       <c r="A204" s="2">
         <v>42341</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C204" s="96" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A205" s="2">
         <v>42341</v>
       </c>
@@ -6057,51 +6077,51 @@
         <v>15</v>
       </c>
       <c r="C205" s="96" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="150" x14ac:dyDescent="0.3">
       <c r="A206" s="2">
         <v>42341</v>
       </c>
-      <c r="B206" s="100" t="s">
-        <v>12</v>
+      <c r="B206" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C206" s="96" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="75" x14ac:dyDescent="0.3">
       <c r="A207" s="2">
         <v>42341</v>
       </c>
-      <c r="B207" s="96" t="s">
+      <c r="B207" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C207" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="90" x14ac:dyDescent="0.3">
       <c r="A208" s="2">
         <v>42341</v>
       </c>
-      <c r="B208" s="96" t="s">
+      <c r="B208" s="100" t="s">
         <v>12</v>
       </c>
       <c r="C208" s="96" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A209" s="2">
         <v>42341</v>
       </c>
       <c r="B209" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C209" s="7" t="s">
-        <v>34</v>
+      <c r="C209" s="96" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
@@ -6109,10 +6129,10 @@
         <v>42341</v>
       </c>
       <c r="B210" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C210" s="7" t="s">
-        <v>166</v>
+        <v>12</v>
+      </c>
+      <c r="C210" s="96" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
@@ -6122,8 +6142,8 @@
       <c r="B211" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C211" s="8" t="s">
-        <v>165</v>
+      <c r="C211" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
@@ -6133,307 +6153,329 @@
       <c r="B212" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C212" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="C212" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="2">
         <v>42341</v>
       </c>
       <c r="B213" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C213" s="100" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="C213" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="2">
         <v>42341</v>
       </c>
       <c r="B214" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C214" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+      <c r="A215" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B215" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C215" s="100" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="A216" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B216" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C214" s="96" t="s">
+      <c r="C216" s="96" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" ht="60" x14ac:dyDescent="0.3">
-      <c r="A215" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B215" s="96"/>
-      <c r="C215" s="96" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A216" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B216" s="96"/>
-      <c r="C216" s="96" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A217" s="2">
         <v>42340</v>
       </c>
-      <c r="B217" s="2" t="s">
+      <c r="B217" s="96"/>
+      <c r="C217" s="96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A218" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B218" s="96"/>
+      <c r="C218" s="96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+      <c r="A219" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B219" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C217" s="96" t="s">
+      <c r="C219" s="96" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A218" s="2">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A220" s="2">
         <v>42339</v>
       </c>
-      <c r="B218" s="2"/>
-      <c r="C218" s="96" t="s">
+      <c r="B220" s="2"/>
+      <c r="C220" s="96" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A219" s="2">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A221" s="2">
         <v>42339</v>
       </c>
-      <c r="B219" s="2"/>
-      <c r="C219" s="96" t="s">
+      <c r="B221" s="2"/>
+      <c r="C221" s="96" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="66.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A220" s="80">
-        <v>42334</v>
-      </c>
-      <c r="B220" s="78" t="s">
-        <v>309</v>
-      </c>
-      <c r="C220" s="78" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A221" s="80">
-        <v>42334</v>
-      </c>
-      <c r="B221" s="78" t="s">
-        <v>307</v>
-      </c>
-      <c r="C221" s="78" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A222" s="80">
         <v>42334</v>
       </c>
       <c r="B222" s="78" t="s">
-        <v>272</v>
+        <v>309</v>
       </c>
       <c r="C222" s="78" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" ht="132.6" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A223" s="80">
-        <v>42333</v>
+        <v>42334</v>
       </c>
       <c r="B223" s="78" t="s">
-        <v>268</v>
+        <v>307</v>
       </c>
       <c r="C223" s="78" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A224" s="80">
+        <v>42334</v>
+      </c>
+      <c r="B224" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="C224" s="78" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" ht="132.6" x14ac:dyDescent="0.3">
+      <c r="A225" s="80">
         <v>42333</v>
       </c>
-      <c r="B224" s="78" t="s">
+      <c r="B225" s="78" t="s">
+        <v>268</v>
+      </c>
+      <c r="C225" s="78" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A226" s="80">
+        <v>42333</v>
+      </c>
+      <c r="B226" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C224" s="78" t="s">
+      <c r="C226" s="78" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A225" s="80">
+    <row r="227" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+      <c r="A227" s="80">
         <v>42331</v>
       </c>
-      <c r="B225" s="78" t="s">
+      <c r="B227" s="78" t="s">
         <v>313</v>
       </c>
-      <c r="C225" s="78" t="s">
+      <c r="C227" s="78" t="s">
         <v>312</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A226" s="80">
-        <v>42329</v>
-      </c>
-      <c r="B226" s="78" t="s">
-        <v>315</v>
-      </c>
-      <c r="C226" s="78" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A227" s="80">
-        <v>42328</v>
-      </c>
-      <c r="B227" s="78" t="s">
-        <v>324</v>
-      </c>
-      <c r="C227" s="78" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A228" s="80">
-        <v>42328</v>
+        <v>42329</v>
       </c>
       <c r="B228" s="78" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C228" s="78" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" ht="119.4" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A229" s="80">
         <v>42328</v>
       </c>
       <c r="B229" s="78" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="C229" s="78" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" ht="106.2" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A230" s="80">
         <v>42328</v>
       </c>
       <c r="B230" s="78" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="C230" s="78" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" ht="172.2" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" ht="119.4" x14ac:dyDescent="0.3">
       <c r="A231" s="80">
         <v>42328</v>
       </c>
       <c r="B231" s="78" t="s">
+        <v>320</v>
+      </c>
+      <c r="C231" s="78" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" ht="106.2" x14ac:dyDescent="0.3">
+      <c r="A232" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B232" s="78" t="s">
         <v>317</v>
       </c>
-      <c r="C231" s="78" t="s">
+      <c r="C232" s="78" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" ht="172.2" x14ac:dyDescent="0.3">
+      <c r="A233" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B233" s="78" t="s">
+        <v>317</v>
+      </c>
+      <c r="C233" s="78" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="119.4" x14ac:dyDescent="0.3">
-      <c r="A232" s="80">
+    <row r="234" spans="1:3" ht="119.4" x14ac:dyDescent="0.3">
+      <c r="A234" s="80">
         <v>42324</v>
       </c>
-      <c r="B232" s="78" t="s">
+      <c r="B234" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="C232" s="78" t="s">
+      <c r="C234" s="78" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="93" x14ac:dyDescent="0.3">
-      <c r="A233" s="80">
+    <row r="235" spans="1:3" ht="93" x14ac:dyDescent="0.3">
+      <c r="A235" s="80">
         <v>42321</v>
       </c>
-      <c r="B233" s="78" t="s">
+      <c r="B235" s="78" t="s">
         <v>327</v>
       </c>
-      <c r="C233" s="78" t="s">
+      <c r="C235" s="78" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A234" s="80">
+    <row r="236" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+      <c r="A236" s="80">
         <v>42321</v>
       </c>
-      <c r="B234" s="78" t="s">
+      <c r="B236" s="78" t="s">
         <v>327</v>
       </c>
-      <c r="C234" s="78" t="s">
+      <c r="C236" s="78" t="s">
         <v>326</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" ht="93" x14ac:dyDescent="0.3">
-      <c r="A235" s="79">
-        <v>42318</v>
-      </c>
-      <c r="B235" s="78" t="s">
-        <v>330</v>
-      </c>
-      <c r="C235" s="78" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" ht="132.6" x14ac:dyDescent="0.3">
-      <c r="A236" s="79">
-        <v>42311</v>
-      </c>
-      <c r="B236" s="78" t="s">
-        <v>216</v>
-      </c>
-      <c r="C236" s="78" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="237" spans="1:3" ht="93" x14ac:dyDescent="0.3">
       <c r="A237" s="79">
+        <v>42318</v>
+      </c>
+      <c r="B237" s="78" t="s">
+        <v>330</v>
+      </c>
+      <c r="C237" s="78" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" ht="132.6" x14ac:dyDescent="0.3">
+      <c r="A238" s="79">
+        <v>42311</v>
+      </c>
+      <c r="B238" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="C238" s="78" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" ht="93" x14ac:dyDescent="0.3">
+      <c r="A239" s="79">
         <v>42310</v>
       </c>
-      <c r="B237" s="78" t="s">
+      <c r="B239" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C237" s="78" t="s">
+      <c r="C239" s="78" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="238" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
-      <c r="A238" s="79">
+    <row r="240" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A240" s="79">
         <v>42306</v>
       </c>
-      <c r="B238" s="78" t="s">
+      <c r="B240" s="78" t="s">
         <v>333</v>
       </c>
-      <c r="C238" s="78" t="s">
+      <c r="C240" s="78" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A239" s="100"/>
-      <c r="B239" s="100"/>
-      <c r="C239" s="100"/>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A241" s="100"/>
+      <c r="B241" s="100"/>
+      <c r="C241" s="100"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C239">
+  <autoFilter ref="A1:C241">
     <sortState ref="A2:C201">
       <sortCondition descending="1" ref="A1:A201"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C211" r:id="rId1"/>
-    <hyperlink ref="C172" r:id="rId2"/>
-    <hyperlink ref="C212" r:id="rId3"/>
-    <hyperlink ref="C46" r:id="rId4"/>
-    <hyperlink ref="C31" r:id="rId5"/>
-    <hyperlink ref="C28" r:id="rId6"/>
+    <hyperlink ref="C213" r:id="rId1"/>
+    <hyperlink ref="C174" r:id="rId2"/>
+    <hyperlink ref="C214" r:id="rId3"/>
+    <hyperlink ref="C48" r:id="rId4"/>
+    <hyperlink ref="C33" r:id="rId5"/>
+    <hyperlink ref="C30" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -6453,16 +6495,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
index entry and netcat cheatsheet
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -15,14 +15,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'AS400 Version'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$245</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$247</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="560">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -2825,9 +2825,6 @@
     <t>Interface的抽象意義</t>
   </si>
   <si>
-    <t>Interface是一種機制, 他相當於是兩個不同世界的類的溝通橋樑, 比如A不知道B的類名和祖先, 所以不能在A里CALL B, 這時只能通過接口來調用B的資源/特殊能力. 這是解耦的一個方法. 他的再一層抽象就是Keying 鑰匙, 願意交流的人打造鑰匙孔鎖, 其他知道此匙的人可以開鎖.</t>
-  </si>
-  <si>
     <t>Decorator 這些有趣的Design pattern好像DNA的樣子, 也和DNA(病毒)很像(在抽象的意義上). 有個網站介紹不錯: https://sourcemaking.com/design_patterns/factory_method</t>
   </si>
   <si>
@@ -2838,6 +2835,19 @@
   </si>
   <si>
     <t>Kernel 在kernel.org上是開源的, Linus Torvalds把i386的硬件仿照MINUX(UNIX的一個開源衍生版)開發的內核, 包含各種manager, 這就是linux的核心.</t>
+  </si>
+  <si>
+    <t>Interface是一種機制, 他相當於是兩個不同世界的類的溝通橋樑, 比如A不知道B的類名和祖先, 所以不能在A里CALL B, 這時只能通過接口來調用B的資源/特殊能力. 這是解耦的一個方法. 他的再一層抽象就是Keying 鑰匙, 有人制作了一把KEY, 願意交流的人根據KEY打造鑰匙孔鎖, 其他只要知道此匙的外型(其存在)的人可以均開鎖.</t>
+  </si>
+  <si>
+    <t>前面提到interface的進一步抽象表述可以是這麼一把KEY和根据KEY打造的門鎖s. 這個比喻通俗, 但信息量和抽象可塑性較低, 若把Interface比喻為病毒, class為生命體. 接入interface相當於是感染病毒, Inherit相當於是把病毒代代相傳, 知道這個病毒結構的, 即可以在活體中依靠特徵來追蹤到病毒本身.</t>
+  </si>
+  <si>
+    <t>callback的理解</t>
+  </si>
+  <si>
+    <t>Callback是A叫B做事, B在做的過程中或做完了都要通知回A, 若B非A的從屬機構, 則用一個兩者地位對等的方法Callback返A, 相當於打電話回電A一樣.
+所以Callback號碼/地址會存在於受託人那里, 而委託人也會有相應的接聽Callback的機制.</t>
   </si>
 </sst>
 </file>
@@ -3166,7 +3176,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3523,6 +3533,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3580,13 +3599,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4202207</xdr:colOff>
-      <xdr:row>132</xdr:row>
+      <xdr:row>134</xdr:row>
       <xdr:rowOff>593914</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>257735</xdr:colOff>
-      <xdr:row>136</xdr:row>
+      <xdr:row>138</xdr:row>
       <xdr:rowOff>102263</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3903,10 +3922,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F245"/>
+  <dimension ref="A1:F247"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3933,838 +3952,838 @@
       <c r="B2" s="100"/>
       <c r="C2" s="100"/>
     </row>
-    <row r="3" spans="1:3" s="102" customFormat="1" ht="45">
+    <row r="3" spans="1:3" s="102" customFormat="1" ht="75">
       <c r="A3" s="121">
-        <v>42569</v>
-      </c>
-      <c r="B3" s="126" t="s">
-        <v>555</v>
-      </c>
-      <c r="C3" s="126" t="s">
-        <v>556</v>
+        <v>42570</v>
+      </c>
+      <c r="B3" s="128" t="s">
+        <v>558</v>
+      </c>
+      <c r="C3" s="129" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="102" customFormat="1" ht="75">
       <c r="A4" s="121">
-        <v>42569</v>
-      </c>
-      <c r="B4" s="125" t="s">
+        <v>42570</v>
+      </c>
+      <c r="B4" s="127" t="s">
         <v>551</v>
       </c>
-      <c r="C4" s="125" t="s">
-        <v>552</v>
+      <c r="C4" s="127" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="102" customFormat="1" ht="45">
       <c r="A5" s="121">
         <v>42569</v>
       </c>
-      <c r="B5" s="125" t="s">
-        <v>550</v>
-      </c>
-      <c r="C5" s="125" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="B5" s="126" t="s">
+        <v>554</v>
+      </c>
+      <c r="C5" s="126" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="102" customFormat="1" ht="90">
       <c r="A6" s="121">
         <v>42569</v>
       </c>
       <c r="B6" s="125" t="s">
+        <v>551</v>
+      </c>
+      <c r="C6" s="127" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A7" s="121">
+        <v>42569</v>
+      </c>
+      <c r="B7" s="125" t="s">
+        <v>550</v>
+      </c>
+      <c r="C7" s="125" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A8" s="121">
+        <v>42569</v>
+      </c>
+      <c r="B8" s="125" t="s">
         <v>549</v>
       </c>
-      <c r="C6" s="125" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A7" s="121">
+      <c r="C8" s="125" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="A9" s="121">
         <v>42567</v>
       </c>
-      <c r="B7" s="124" t="s">
+      <c r="B9" s="124" t="s">
         <v>548</v>
       </c>
-      <c r="C7" s="124" t="s">
+      <c r="C9" s="124" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A8" s="121">
+    <row r="10" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A10" s="121">
         <v>42567</v>
       </c>
-      <c r="B8" s="124" t="s">
+      <c r="B10" s="124" t="s">
         <v>546</v>
       </c>
-      <c r="C8" s="124" t="s">
+      <c r="C10" s="124" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A9" s="121">
+    <row r="11" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A11" s="121">
         <v>42565</v>
       </c>
-      <c r="B9" s="123" t="s">
+      <c r="B11" s="123" t="s">
         <v>543</v>
       </c>
-      <c r="C9" s="123" t="s">
+      <c r="C11" s="123" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="102" customFormat="1" ht="75">
-      <c r="A10" s="121">
+    <row r="12" spans="1:3" s="102" customFormat="1" ht="75">
+      <c r="A12" s="121">
         <v>42564</v>
       </c>
-      <c r="B10" s="122" t="s">
+      <c r="B12" s="122" t="s">
         <v>534</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C12" s="122" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="102" customFormat="1" ht="135">
-      <c r="A11" s="121">
-        <v>42562</v>
-      </c>
-      <c r="B11" s="120" t="s">
-        <v>537</v>
-      </c>
-      <c r="C11" s="120" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A12" s="121">
-        <v>42562</v>
-      </c>
-      <c r="B12" s="120" t="s">
-        <v>536</v>
-      </c>
-      <c r="C12" s="120" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="102" customFormat="1" ht="75">
+    <row r="13" spans="1:3" s="102" customFormat="1" ht="135">
       <c r="A13" s="121">
         <v>42562</v>
       </c>
       <c r="B13" s="120" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C13" s="120" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="102" customFormat="1" ht="165">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="102" customFormat="1" ht="60">
       <c r="A14" s="121">
         <v>42562</v>
       </c>
       <c r="B14" s="120" t="s">
+        <v>536</v>
+      </c>
+      <c r="C14" s="120" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="102" customFormat="1" ht="75">
+      <c r="A15" s="121">
+        <v>42562</v>
+      </c>
+      <c r="B15" s="120" t="s">
+        <v>535</v>
+      </c>
+      <c r="C15" s="120" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="102" customFormat="1" ht="165">
+      <c r="A16" s="121">
+        <v>42562</v>
+      </c>
+      <c r="B16" s="120" t="s">
         <v>534</v>
       </c>
-      <c r="C14" s="120" t="s">
+      <c r="C16" s="120" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A15" s="121">
+    <row r="17" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A17" s="121">
         <v>42557</v>
       </c>
-      <c r="B15" s="120" t="s">
+      <c r="B17" s="120" t="s">
         <v>525</v>
       </c>
-      <c r="C15" s="120" t="s">
+      <c r="C17" s="120" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="102" customFormat="1" ht="180">
-      <c r="A16" s="120"/>
-      <c r="B16" s="120" t="s">
-        <v>527</v>
-      </c>
-      <c r="C16" s="120" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A17" s="121">
-        <v>42540</v>
-      </c>
-      <c r="B17" s="120" t="s">
-        <v>529</v>
-      </c>
-      <c r="C17" s="120" t="s">
-        <v>530</v>
-      </c>
-    </row>
     <row r="18" spans="1:3" s="102" customFormat="1" ht="180">
-      <c r="A18" s="121">
-        <v>42539</v>
-      </c>
+      <c r="A18" s="120"/>
       <c r="B18" s="120" t="s">
         <v>527</v>
       </c>
       <c r="C18" s="120" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="102" customFormat="1" ht="150">
+      <c r="A19" s="121">
+        <v>42540</v>
+      </c>
+      <c r="B19" s="120" t="s">
+        <v>529</v>
+      </c>
+      <c r="C19" s="120" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="102" customFormat="1" ht="180">
+      <c r="A20" s="121">
+        <v>42539</v>
+      </c>
+      <c r="B20" s="120" t="s">
+        <v>527</v>
+      </c>
+      <c r="C20" s="120" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A19" s="121">
+    <row r="21" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A21" s="121">
         <v>42539</v>
       </c>
-      <c r="B19" s="120" t="s">
+      <c r="B21" s="120" t="s">
         <v>532</v>
       </c>
-      <c r="C19" s="120" t="s">
+      <c r="C21" s="120" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A20" s="2">
+    <row r="22" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A22" s="2">
         <v>42534</v>
       </c>
-      <c r="B20" s="119" t="s">
+      <c r="B22" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="119" t="s">
+      <c r="C22" s="119" t="s">
         <v>524</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A21" s="2">
-        <v>42517</v>
-      </c>
-      <c r="B21" s="118" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="118" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A22" s="2">
-        <v>42514</v>
-      </c>
-      <c r="B22" s="117" t="s">
-        <v>519</v>
-      </c>
-      <c r="C22" s="117" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="102" customFormat="1" ht="45">
       <c r="A23" s="2">
+        <v>42517</v>
+      </c>
+      <c r="B23" s="118" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="118" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A24" s="2">
+        <v>42514</v>
+      </c>
+      <c r="B24" s="117" t="s">
+        <v>519</v>
+      </c>
+      <c r="C24" s="117" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A25" s="2">
         <v>42507</v>
       </c>
-      <c r="B23" s="116" t="s">
+      <c r="B25" s="116" t="s">
         <v>519</v>
       </c>
-      <c r="C23" s="116" t="s">
+      <c r="C25" s="116" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A24" s="2">
+    <row r="26" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A26" s="2">
         <v>42502</v>
       </c>
-      <c r="B24" s="115" t="s">
+      <c r="B26" s="115" t="s">
         <v>519</v>
       </c>
-      <c r="C24" s="116" t="s">
+      <c r="C26" s="116" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A25" s="2">
-        <v>42485</v>
-      </c>
-      <c r="B25" s="113" t="s">
-        <v>516</v>
-      </c>
-      <c r="C25" s="113" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A26" s="2">
-        <v>42485</v>
-      </c>
-      <c r="B26" s="110" t="s">
-        <v>514</v>
-      </c>
-      <c r="C26" s="110" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="102" customFormat="1" ht="300">
+    <row r="27" spans="1:3" s="102" customFormat="1" ht="90">
       <c r="A27" s="2">
         <v>42485</v>
       </c>
-      <c r="B27" s="112" t="s">
+      <c r="B27" s="113" t="s">
+        <v>516</v>
+      </c>
+      <c r="C27" s="113" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A28" s="2">
+        <v>42485</v>
+      </c>
+      <c r="B28" s="110" t="s">
+        <v>514</v>
+      </c>
+      <c r="C28" s="110" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="102" customFormat="1" ht="300">
+      <c r="A29" s="2">
+        <v>42485</v>
+      </c>
+      <c r="B29" s="112" t="s">
         <v>241</v>
       </c>
-      <c r="C27" s="112" t="s">
+      <c r="C29" s="112" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A28" s="2">
+    <row r="30" spans="1:3" s="102" customFormat="1" ht="150">
+      <c r="A30" s="2">
         <v>42479</v>
       </c>
-      <c r="B28" s="111" t="s">
+      <c r="B30" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="C28" s="111" t="s">
+      <c r="C30" s="111" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A29" s="2">
+    <row r="31" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="A31" s="2">
         <v>42478</v>
       </c>
-      <c r="B29" s="110" t="s">
+      <c r="B31" s="110" t="s">
         <v>509</v>
       </c>
-      <c r="C29" s="110" t="s">
+      <c r="C31" s="110" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="102" customFormat="1" ht="120">
-      <c r="A30" s="2">
+    <row r="32" spans="1:3" s="102" customFormat="1" ht="120">
+      <c r="A32" s="2">
         <v>42477</v>
       </c>
-      <c r="B30" s="109" t="s">
+      <c r="B32" s="109" t="s">
         <v>509</v>
       </c>
-      <c r="C30" s="109" t="s">
+      <c r="C32" s="109" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A31" s="2">
+    <row r="33" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A33" s="2">
         <v>42477</v>
       </c>
-      <c r="B31" s="108" t="s">
+      <c r="B33" s="108" t="s">
         <v>507</v>
       </c>
-      <c r="C31" s="108" t="s">
+      <c r="C33" s="108" t="s">
         <v>508</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="102" customFormat="1">
-      <c r="A32" s="2">
-        <v>42473</v>
-      </c>
-      <c r="B32" s="106" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="106" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A33" s="2">
-        <v>42473</v>
-      </c>
-      <c r="B33" s="106" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="107" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="102" customFormat="1">
       <c r="A34" s="2">
+        <v>42473</v>
+      </c>
+      <c r="B34" s="106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="106" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A35" s="2">
+        <v>42473</v>
+      </c>
+      <c r="B35" s="106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="107" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="102" customFormat="1">
+      <c r="A36" s="2">
         <v>42469</v>
       </c>
-      <c r="B34" s="105" t="s">
+      <c r="B36" s="105" t="s">
         <v>504</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C36" s="8" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="102" customFormat="1" ht="75">
-      <c r="A35" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B35" s="104" t="s">
-        <v>497</v>
-      </c>
-      <c r="C35" s="104" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A36" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B36" s="104" t="s">
-        <v>499</v>
-      </c>
-      <c r="C36" s="104" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" s="102" customFormat="1">
+    <row r="37" spans="1:3" s="102" customFormat="1" ht="75">
       <c r="A37" s="2">
         <v>42463</v>
       </c>
       <c r="B37" s="104" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C37" s="104" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="102" customFormat="1" ht="150">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="102" customFormat="1" ht="105">
       <c r="A38" s="2">
         <v>42463</v>
       </c>
-      <c r="B38" s="100" t="s">
-        <v>493</v>
-      </c>
-      <c r="C38" s="100" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="B38" s="104" t="s">
+        <v>499</v>
+      </c>
+      <c r="C38" s="104" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="102" customFormat="1">
       <c r="A39" s="2">
         <v>42463</v>
       </c>
-      <c r="B39" s="103" t="s">
-        <v>492</v>
-      </c>
-      <c r="C39" s="103" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="B39" s="104" t="s">
+        <v>501</v>
+      </c>
+      <c r="C39" s="104" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="102" customFormat="1" ht="150">
       <c r="A40" s="2">
         <v>42463</v>
       </c>
-      <c r="B40" s="101" t="s">
-        <v>489</v>
-      </c>
-      <c r="C40" s="101" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="B40" s="100" t="s">
+        <v>493</v>
+      </c>
+      <c r="C40" s="100" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="102" customFormat="1" ht="90">
       <c r="A41" s="2">
         <v>42463</v>
       </c>
-      <c r="B41" s="101" t="s">
+      <c r="B41" s="103" t="s">
+        <v>492</v>
+      </c>
+      <c r="C41" s="103" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A42" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B42" s="101" t="s">
+        <v>489</v>
+      </c>
+      <c r="C42" s="101" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A43" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B43" s="101" t="s">
         <v>488</v>
       </c>
-      <c r="C41" s="101" t="s">
+      <c r="C43" s="101" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A42" s="2">
-        <v>42462</v>
-      </c>
-      <c r="B42" s="100" t="s">
-        <v>486</v>
-      </c>
-      <c r="C42" s="100" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="102" customFormat="1" ht="135">
-      <c r="A43" s="2">
-        <v>42462</v>
-      </c>
-      <c r="B43" s="100" t="s">
-        <v>484</v>
-      </c>
-      <c r="C43" s="100" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" s="102" customFormat="1" ht="240">
+    <row r="44" spans="1:3" s="102" customFormat="1" ht="150">
       <c r="A44" s="2">
         <v>42462</v>
       </c>
       <c r="B44" s="100" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="C44" s="100" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" s="102" customFormat="1" ht="120">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="102" customFormat="1" ht="135">
       <c r="A45" s="2">
         <v>42462</v>
       </c>
       <c r="B45" s="100" t="s">
+        <v>484</v>
+      </c>
+      <c r="C45" s="100" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="102" customFormat="1" ht="240">
+      <c r="A46" s="2">
+        <v>42462</v>
+      </c>
+      <c r="B46" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="C45" s="100" t="s">
+      <c r="C46" s="100" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="102" customFormat="1" ht="120">
+      <c r="A47" s="2">
+        <v>42462</v>
+      </c>
+      <c r="B47" s="100" t="s">
+        <v>480</v>
+      </c>
+      <c r="C47" s="100" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="4" customFormat="1" ht="120">
-      <c r="A46" s="2">
-        <v>42460</v>
-      </c>
-      <c r="B46" s="99" t="s">
-        <v>477</v>
-      </c>
-      <c r="C46" s="99" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" s="4" customFormat="1" ht="30">
-      <c r="A47" s="2">
-        <v>42460</v>
-      </c>
-      <c r="B47" s="99" t="s">
-        <v>476</v>
-      </c>
-      <c r="C47" s="99" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" s="4" customFormat="1" ht="180">
+    <row r="48" spans="1:3" s="4" customFormat="1" ht="120">
       <c r="A48" s="2">
         <v>42460</v>
       </c>
       <c r="B48" s="99" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C48" s="99" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="4" customFormat="1" ht="60">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="4" customFormat="1" ht="30">
       <c r="A49" s="2">
         <v>42460</v>
       </c>
       <c r="B49" s="99" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C49" s="99" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" s="4" customFormat="1" ht="105">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="4" customFormat="1" ht="180">
       <c r="A50" s="2">
-        <v>42459</v>
+        <v>42460</v>
       </c>
       <c r="B50" s="99" t="s">
-        <v>470</v>
-      </c>
-      <c r="C50" s="98" t="s">
-        <v>473</v>
+        <v>475</v>
+      </c>
+      <c r="C50" s="99" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="4" customFormat="1" ht="60">
       <c r="A51" s="2">
+        <v>42460</v>
+      </c>
+      <c r="B51" s="99" t="s">
+        <v>478</v>
+      </c>
+      <c r="C51" s="99" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" s="4" customFormat="1" ht="105">
+      <c r="A52" s="2">
         <v>42459</v>
       </c>
-      <c r="B51" s="99" t="s">
+      <c r="B52" s="99" t="s">
+        <v>470</v>
+      </c>
+      <c r="C52" s="98" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="4" customFormat="1" ht="60">
+      <c r="A53" s="2">
+        <v>42459</v>
+      </c>
+      <c r="B53" s="99" t="s">
         <v>241</v>
       </c>
-      <c r="C51" s="99" t="s">
+      <c r="C53" s="99" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="4" customFormat="1">
-      <c r="A52" s="2">
+    <row r="54" spans="1:3" s="4" customFormat="1">
+      <c r="A54" s="2">
         <v>42458</v>
       </c>
-      <c r="B52" s="97" t="s">
+      <c r="B54" s="97" t="s">
         <v>470</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C54" s="8" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="4" customFormat="1" ht="105">
-      <c r="A53" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B53" s="96" t="s">
-        <v>254</v>
-      </c>
-      <c r="C53" s="100" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="60">
-      <c r="A54" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B54" s="96" t="s">
-        <v>462</v>
-      </c>
-      <c r="C54" s="44" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="45">
+    <row r="55" spans="1:3" s="4" customFormat="1" ht="105">
       <c r="A55" s="2">
         <v>42456</v>
       </c>
       <c r="B55" s="96" t="s">
-        <v>463</v>
-      </c>
-      <c r="C55" s="44" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>254</v>
+      </c>
+      <c r="C55" s="100" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="60">
       <c r="A56" s="2">
         <v>42456</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>466</v>
+      <c r="B56" s="96" t="s">
+        <v>462</v>
       </c>
       <c r="C56" s="44" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="45">
       <c r="A57" s="2">
         <v>42456</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="96" t="s">
+        <v>463</v>
+      </c>
+      <c r="C57" s="44" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C58" s="44" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="45">
+      <c r="A59" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="C57" s="44" t="s">
+      <c r="C59" s="44" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="77.25">
-      <c r="A58" s="79">
+    <row r="60" spans="1:3" ht="77.25">
+      <c r="A60" s="79">
         <v>42453</v>
       </c>
-      <c r="B58" s="78" t="s">
+      <c r="B60" s="78" t="s">
         <v>264</v>
       </c>
-      <c r="C58" s="78" t="s">
+      <c r="C60" s="78" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="26.25">
-      <c r="A59" s="79">
+    <row r="61" spans="1:3" ht="26.25">
+      <c r="A61" s="79">
         <v>42453</v>
       </c>
-      <c r="B59" s="78" t="s">
+      <c r="B61" s="78" t="s">
         <v>262</v>
       </c>
-      <c r="C59" s="78" t="s">
+      <c r="C61" s="78" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="39">
-      <c r="A60" s="79">
+    <row r="62" spans="1:3" ht="39">
+      <c r="A62" s="79">
         <v>42452</v>
       </c>
-      <c r="B60" s="78" t="s">
+      <c r="B62" s="78" t="s">
         <v>260</v>
       </c>
-      <c r="C60" s="78" t="s">
+      <c r="C62" s="78" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="165">
-      <c r="A61" s="75">
+    <row r="63" spans="1:3" ht="165">
+      <c r="A63" s="75">
         <v>42451</v>
       </c>
-      <c r="B61" s="74" t="s">
+      <c r="B63" s="74" t="s">
         <v>247</v>
       </c>
-      <c r="C61" s="100" t="s">
+      <c r="C63" s="100" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="45">
-      <c r="A62" s="2">
-        <v>42451</v>
-      </c>
-      <c r="B62" s="100" t="s">
-        <v>249</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="30">
-      <c r="A63" s="2">
-        <v>42451</v>
-      </c>
-      <c r="B63" s="96" t="s">
-        <v>196</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="165">
+    <row r="64" spans="1:3" ht="45">
       <c r="A64" s="2">
         <v>42451</v>
       </c>
-      <c r="B64" s="96" t="s">
+      <c r="B64" s="100" t="s">
+        <v>249</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="30">
+      <c r="A65" s="2">
+        <v>42451</v>
+      </c>
+      <c r="B65" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="165">
+      <c r="A66" s="2">
+        <v>42451</v>
+      </c>
+      <c r="B66" s="96" t="s">
         <v>253</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="64.5">
-      <c r="A65" s="79">
+    <row r="67" spans="1:3" ht="64.5">
+      <c r="A67" s="79">
         <v>42451</v>
       </c>
-      <c r="B65" s="78" t="s">
+      <c r="B67" s="78" t="s">
         <v>253</v>
       </c>
-      <c r="C65" s="78" t="s">
+      <c r="C67" s="78" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="64.5">
-      <c r="A66" s="79">
+    <row r="68" spans="1:3" ht="64.5">
+      <c r="A68" s="79">
         <v>42447</v>
       </c>
-      <c r="B66" s="78" t="s">
+      <c r="B68" s="78" t="s">
         <v>257</v>
       </c>
-      <c r="C66" s="78" t="s">
+      <c r="C68" s="78" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="2">
+    <row r="69" spans="1:3">
+      <c r="A69" s="2">
         <v>42440</v>
       </c>
-      <c r="B67" s="100" t="s">
+      <c r="B69" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="C67" s="100" t="s">
+      <c r="C69" s="100" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="75">
-      <c r="A68" s="2">
+    <row r="70" spans="1:3" ht="75">
+      <c r="A70" s="2">
         <v>42436</v>
       </c>
-      <c r="B68" s="96" t="s">
+      <c r="B70" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="39">
-      <c r="A69" s="79">
+    <row r="71" spans="1:3" ht="39">
+      <c r="A71" s="79">
         <v>42431</v>
       </c>
-      <c r="B69" s="78" t="s">
+      <c r="B71" s="78" t="s">
         <v>274</v>
       </c>
-      <c r="C69" s="78" t="s">
+      <c r="C71" s="78" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="26.25">
-      <c r="A70" s="79">
-        <v>42431</v>
-      </c>
-      <c r="B70" s="78" t="s">
-        <v>272</v>
-      </c>
-      <c r="C70" s="78" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="51.75">
-      <c r="A71" s="79">
-        <v>42430</v>
-      </c>
-      <c r="B71" s="78" t="s">
-        <v>270</v>
-      </c>
-      <c r="C71" s="78" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="26.25">
       <c r="A72" s="79">
+        <v>42431</v>
+      </c>
+      <c r="B72" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="C72" s="78" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="51.75">
+      <c r="A73" s="79">
+        <v>42430</v>
+      </c>
+      <c r="B73" s="78" t="s">
+        <v>270</v>
+      </c>
+      <c r="C73" s="78" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="26.25">
+      <c r="A74" s="79">
         <v>42428</v>
       </c>
-      <c r="B72" s="78" t="s">
+      <c r="B74" s="78" t="s">
         <v>268</v>
       </c>
-      <c r="C72" s="78" t="s">
+      <c r="C74" s="78" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="30">
-      <c r="A73" s="2">
+    <row r="75" spans="1:3" ht="30">
+      <c r="A75" s="2">
         <v>42426</v>
       </c>
-      <c r="B73" s="100" t="s">
+      <c r="B75" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="C73" s="100" t="s">
+      <c r="C75" s="100" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="77.25">
-      <c r="A74" s="79">
+    <row r="76" spans="1:3" ht="77.25">
+      <c r="A76" s="79">
         <v>42426</v>
       </c>
-      <c r="B74" s="78" t="s">
+      <c r="B76" s="78" t="s">
         <v>266</v>
       </c>
-      <c r="C74" s="78" t="s">
+      <c r="C76" s="78" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="2">
+    <row r="77" spans="1:3">
+      <c r="A77" s="2">
         <v>42425</v>
       </c>
-      <c r="B75" s="100" t="s">
+      <c r="B77" s="100" t="s">
         <v>241</v>
       </c>
-      <c r="C75" s="100" t="s">
+      <c r="C77" s="100" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="2">
+    <row r="78" spans="1:3">
+      <c r="A78" s="2">
         <v>42425</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="26.25">
-      <c r="A77" s="79">
-        <v>42425</v>
-      </c>
-      <c r="B77" s="78" t="s">
-        <v>276</v>
-      </c>
-      <c r="C77" s="78" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="79">
-        <v>42425</v>
-      </c>
-      <c r="B78" s="78" t="s">
-        <v>276</v>
-      </c>
-      <c r="C78" s="78" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="26.25">
@@ -4772,1266 +4791,1266 @@
         <v>42425</v>
       </c>
       <c r="B79" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="C79" s="78" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="79">
+        <v>42425</v>
+      </c>
+      <c r="B80" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="C80" s="78" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="26.25">
+      <c r="A81" s="79">
+        <v>42425</v>
+      </c>
+      <c r="B81" s="78" t="s">
         <v>279</v>
       </c>
-      <c r="C79" s="78" t="s">
+      <c r="C81" s="78" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="165">
-      <c r="A80" s="2">
+    <row r="82" spans="1:3" ht="165">
+      <c r="A82" s="2">
         <v>42424</v>
       </c>
-      <c r="B80" s="100" t="s">
+      <c r="B82" s="100" t="s">
         <v>239</v>
       </c>
-      <c r="C80" s="114" t="s">
+      <c r="C82" s="114" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="45">
-      <c r="A81" s="2">
+    <row r="83" spans="1:3" ht="45">
+      <c r="A83" s="2">
         <v>42423</v>
       </c>
-      <c r="B81" s="96" t="s">
+      <c r="B83" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="C83" s="11" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="79">
+    <row r="84" spans="1:3">
+      <c r="A84" s="79">
         <v>42423</v>
       </c>
-      <c r="B82" s="78" t="s">
+      <c r="B84" s="78" t="s">
         <v>281</v>
       </c>
-      <c r="C82" s="78" t="s">
+      <c r="C84" s="78" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="90">
-      <c r="A83" s="2">
+    <row r="85" spans="1:3" ht="90">
+      <c r="A85" s="2">
         <v>42422</v>
       </c>
-      <c r="B83" s="100" t="s">
+      <c r="B85" s="100" t="s">
         <v>236</v>
       </c>
-      <c r="C83" s="100" t="s">
+      <c r="C85" s="100" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="60">
-      <c r="A84" s="2">
+    <row r="86" spans="1:3" ht="60">
+      <c r="A86" s="2">
         <v>42419</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="B86" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="C84" s="36" t="s">
+      <c r="C86" s="36" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="195">
-      <c r="A85" s="2">
+    <row r="87" spans="1:3" ht="195">
+      <c r="A87" s="2">
         <v>42418</v>
       </c>
-      <c r="B85" s="10" t="s">
+      <c r="B87" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C85" s="18" t="s">
+      <c r="C87" s="18" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="45">
-      <c r="A86" s="2">
-        <v>42403</v>
-      </c>
-      <c r="B86" s="96" t="s">
-        <v>229</v>
-      </c>
-      <c r="C86" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="75">
-      <c r="A87" s="2">
-        <v>42403</v>
-      </c>
-      <c r="B87" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="C87" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="90">
+    <row r="88" spans="1:3" ht="45">
       <c r="A88" s="2">
         <v>42403</v>
       </c>
-      <c r="B88" s="12"/>
+      <c r="B88" s="96" t="s">
+        <v>229</v>
+      </c>
       <c r="C88" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="75">
+      <c r="A89" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="C89" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="90">
+      <c r="A90" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="90">
-      <c r="A89" s="2">
+    <row r="91" spans="1:3" ht="90">
+      <c r="A91" s="2">
         <v>42398</v>
       </c>
-      <c r="B89" s="12" t="s">
+      <c r="B91" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C89" s="12" t="s">
+      <c r="C91" s="12" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="45">
-      <c r="A90" s="2">
-        <v>42398</v>
-      </c>
-      <c r="B90" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="C90" s="12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="2">
-        <v>42397</v>
-      </c>
-      <c r="B91" s="96" t="s">
-        <v>201</v>
-      </c>
-      <c r="C91" s="14" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="45">
       <c r="A92" s="2">
+        <v>42398</v>
+      </c>
+      <c r="B92" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="2">
+        <v>42397</v>
+      </c>
+      <c r="B93" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="45">
+      <c r="A94" s="2">
         <v>42396</v>
       </c>
-      <c r="B92" s="12" t="s">
+      <c r="B94" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C92" s="12" t="s">
+      <c r="C94" s="12" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="30">
-      <c r="A93" s="2">
+    <row r="95" spans="1:3" ht="30">
+      <c r="A95" s="2">
         <v>42396</v>
       </c>
-      <c r="B93" s="96" t="s">
+      <c r="B95" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="C93" s="14" t="s">
+      <c r="C95" s="14" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="128.25">
-      <c r="A94" s="79">
+    <row r="96" spans="1:3" ht="128.25">
+      <c r="A96" s="79">
         <v>42386</v>
       </c>
-      <c r="B94" s="78" t="s">
+      <c r="B96" s="78" t="s">
         <v>283</v>
       </c>
-      <c r="C94" s="78" t="s">
+      <c r="C96" s="78" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="64.5">
-      <c r="A95" s="79">
+    <row r="97" spans="1:3" ht="64.5">
+      <c r="A97" s="79">
         <v>42386</v>
       </c>
-      <c r="B95" s="78" t="s">
+      <c r="B97" s="78" t="s">
         <v>285</v>
       </c>
-      <c r="C95" s="78" t="s">
+      <c r="C97" s="78" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="45">
-      <c r="A96" s="2">
+    <row r="98" spans="1:3" ht="45">
+      <c r="A98" s="2">
         <v>42384</v>
       </c>
-      <c r="B96" s="100" t="s">
+      <c r="B98" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="C96" s="100" t="s">
+      <c r="C98" s="100" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="180">
-      <c r="A97" s="2">
+    <row r="99" spans="1:3" ht="180">
+      <c r="A99" s="2">
         <v>42382</v>
       </c>
-      <c r="B97" s="14" t="s">
+      <c r="B99" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="C97" s="14" t="s">
+      <c r="C99" s="14" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="64.5">
-      <c r="A98" s="79">
+    <row r="100" spans="1:3" ht="64.5">
+      <c r="A100" s="79">
         <v>42382</v>
       </c>
-      <c r="B98" s="78" t="s">
+      <c r="B100" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="C98" s="78" t="s">
+      <c r="C100" s="78" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="30">
-      <c r="A99" s="2">
+    <row r="101" spans="1:3" ht="30">
+      <c r="A101" s="2">
         <v>42381</v>
       </c>
-      <c r="B99" s="100" t="s">
+      <c r="B101" s="100" t="s">
         <v>216</v>
       </c>
-      <c r="C99" s="100" t="s">
+      <c r="C101" s="100" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="45">
-      <c r="A100" s="2">
-        <v>42380</v>
-      </c>
-      <c r="B100" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C100" s="16" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="75">
-      <c r="A101" s="2">
-        <v>42380</v>
-      </c>
-      <c r="B101" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="C101" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="180">
+    <row r="102" spans="1:3" ht="45">
       <c r="A102" s="2">
         <v>42380</v>
       </c>
-      <c r="B102" s="50" t="s">
+      <c r="B102" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C102" s="16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="75">
+      <c r="A103" s="2">
+        <v>42380</v>
+      </c>
+      <c r="B103" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C102" s="18" t="s">
+      <c r="C103" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="180">
+      <c r="A104" s="2">
+        <v>42380</v>
+      </c>
+      <c r="B104" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="C104" s="18" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="217.5">
-      <c r="A103" s="79">
+    <row r="105" spans="1:3" ht="217.5">
+      <c r="A105" s="79">
         <v>42380</v>
       </c>
-      <c r="B103" s="78" t="s">
+      <c r="B105" s="78" t="s">
         <v>288</v>
       </c>
-      <c r="C103" s="78" t="s">
+      <c r="C105" s="78" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="102.75">
-      <c r="A104" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B104" s="78" t="s">
-        <v>291</v>
-      </c>
-      <c r="C104" s="78" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="102.75">
-      <c r="A105" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B105" s="78" t="s">
-        <v>293</v>
-      </c>
-      <c r="C105" s="78" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="141">
+    <row r="106" spans="1:3" ht="102.75">
       <c r="A106" s="79">
         <v>42378</v>
       </c>
       <c r="B106" s="78" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C106" s="78" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="77.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="102.75">
       <c r="A107" s="79">
         <v>42378</v>
       </c>
       <c r="B107" s="78" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C107" s="78" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="102.75">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="141">
       <c r="A108" s="79">
         <v>42378</v>
       </c>
       <c r="B108" s="78" t="s">
+        <v>297</v>
+      </c>
+      <c r="C108" s="78" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="77.25">
+      <c r="A109" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B109" s="78" t="s">
+        <v>297</v>
+      </c>
+      <c r="C109" s="78" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="102.75">
+      <c r="A110" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B110" s="78" t="s">
         <v>295</v>
       </c>
-      <c r="C108" s="78" t="s">
+      <c r="C110" s="78" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="60">
-      <c r="A109" s="2">
+    <row r="111" spans="1:3" ht="60">
+      <c r="A111" s="2">
         <v>42377</v>
       </c>
-      <c r="B109" s="100" t="s">
+      <c r="B111" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="C109" s="100" t="s">
+      <c r="C111" s="100" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="77.25">
-      <c r="A110" s="79">
+    <row r="112" spans="1:3" ht="77.25">
+      <c r="A112" s="79">
         <v>42376</v>
       </c>
-      <c r="B110" s="78" t="s">
+      <c r="B112" s="78" t="s">
         <v>300</v>
       </c>
-      <c r="C110" s="78" t="s">
+      <c r="C112" s="78" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="45">
-      <c r="A111" s="2">
+    <row r="113" spans="1:3" ht="45">
+      <c r="A113" s="2">
         <v>42375</v>
       </c>
-      <c r="B111" s="15" t="s">
+      <c r="B113" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C111" s="100" t="s">
+      <c r="C113" s="100" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
-      <c r="A112" s="2">
+    <row r="114" spans="1:3">
+      <c r="A114" s="2">
         <v>42369</v>
       </c>
-      <c r="B112" s="100" t="s">
+      <c r="B114" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="C112" s="19" t="s">
+      <c r="C114" s="19" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="195">
-      <c r="A113" s="2">
-        <v>42368</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C113" s="19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="135">
-      <c r="A114" s="2">
-        <v>42368</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C114" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="45">
+    <row r="115" spans="1:3" ht="195">
       <c r="A115" s="2">
         <v>42368</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C115" s="19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="135">
+      <c r="A116" s="2">
+        <v>42368</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C116" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="45">
+      <c r="A117" s="2">
+        <v>42368</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C115" s="20" t="s">
+      <c r="C117" s="20" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="30">
-      <c r="A116" s="2">
+    <row r="118" spans="1:3" ht="30">
+      <c r="A118" s="2">
         <v>42366</v>
       </c>
-      <c r="B116" s="20" t="s">
+      <c r="B118" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C116" s="20" t="s">
+      <c r="C118" s="20" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="30">
-      <c r="A117" s="2">
-        <v>42366</v>
-      </c>
-      <c r="B117" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C117" s="20" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="150">
-      <c r="A118" s="2">
-        <v>42361</v>
-      </c>
-      <c r="C118" s="20" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="30">
       <c r="A119" s="2">
-        <v>42361</v>
+        <v>42366</v>
+      </c>
+      <c r="B119" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="C119" s="20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="270">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="150">
       <c r="A120" s="2">
         <v>42361</v>
       </c>
-      <c r="B120" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C120" s="22" t="s">
-        <v>187</v>
+      <c r="C120" s="20" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="30">
       <c r="A121" s="2">
         <v>42361</v>
       </c>
-      <c r="B121" s="100" t="s">
-        <v>53</v>
-      </c>
       <c r="C121" s="20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="270">
       <c r="A122" s="2">
         <v>42361</v>
       </c>
       <c r="B122" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="C122" s="21" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="225">
+      <c r="C122" s="22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="30">
       <c r="A123" s="2">
         <v>42361</v>
       </c>
-      <c r="B123" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C123" s="22" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="60">
+      <c r="B123" s="100" t="s">
+        <v>53</v>
+      </c>
+      <c r="C123" s="20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
       <c r="A124" s="2">
         <v>42361</v>
       </c>
-      <c r="B124" s="100" t="s">
-        <v>49</v>
-      </c>
-      <c r="C124" s="22" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="90">
+      <c r="B124" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C124" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="225">
       <c r="A125" s="2">
         <v>42361</v>
       </c>
-      <c r="B125" s="1" t="s">
-        <v>196</v>
+      <c r="B125" s="35" t="s">
+        <v>186</v>
       </c>
       <c r="C125" s="22" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="60">
       <c r="A126" s="2">
         <v>42361</v>
       </c>
-      <c r="B126" s="24" t="s">
+      <c r="B126" s="100" t="s">
+        <v>49</v>
+      </c>
+      <c r="C126" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="90">
+      <c r="A127" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C126" s="24" t="s">
+      <c r="C127" s="22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="60">
+      <c r="A128" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B128" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C128" s="24" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
-      <c r="A127" s="40">
+    <row r="129" spans="1:3">
+      <c r="A129" s="40">
         <v>42360</v>
       </c>
-      <c r="B127" s="50" t="s">
+      <c r="B129" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C129" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
-      <c r="A128" s="40">
+    <row r="130" spans="1:3">
+      <c r="A130" s="40">
         <v>42360</v>
       </c>
-      <c r="B128" s="50" t="s">
+      <c r="B130" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C130" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="102.75">
-      <c r="A129" s="80">
+    <row r="131" spans="1:3" ht="102.75">
+      <c r="A131" s="80">
         <v>42360</v>
       </c>
-      <c r="B129" s="78" t="s">
+      <c r="B131" s="78" t="s">
         <v>302</v>
       </c>
-      <c r="C129" s="78" t="s">
+      <c r="C131" s="78" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="30">
-      <c r="A130" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B130" s="100" t="s">
-        <v>43</v>
-      </c>
-      <c r="C130" s="100" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
-      <c r="A131" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B131" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="C131" s="23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" ht="30">
       <c r="A132" s="2">
         <v>42356</v>
       </c>
-      <c r="B132" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="C132" s="25" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="30">
+      <c r="B132" s="100" t="s">
+        <v>43</v>
+      </c>
+      <c r="C132" s="100" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
       <c r="A133" s="2">
         <v>42356</v>
       </c>
-      <c r="B133" s="96"/>
-      <c r="C133" s="25" t="s">
+      <c r="B133" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="C133" s="23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="2">
+        <v>42356</v>
+      </c>
+      <c r="B134" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C134" s="25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="30">
+      <c r="A135" s="2">
+        <v>42356</v>
+      </c>
+      <c r="B135" s="96"/>
+      <c r="C135" s="25" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="60">
-      <c r="A134" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B134" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="C134" s="26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
-      <c r="A135" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B135" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C135" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="150">
+    <row r="136" spans="1:3" ht="60">
       <c r="A136" s="2">
         <v>42355</v>
       </c>
-      <c r="B136" s="13" t="s">
-        <v>33</v>
+      <c r="B136" s="96" t="s">
+        <v>91</v>
       </c>
       <c r="C136" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="120">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
       <c r="A137" s="2">
         <v>42355</v>
       </c>
-      <c r="B137" s="100" t="s">
-        <v>168</v>
-      </c>
-      <c r="C137" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="30">
+      <c r="B137" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C137" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="150">
       <c r="A138" s="2">
         <v>42355</v>
       </c>
-      <c r="B138" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C138" s="28" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
+      <c r="B138" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C138" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="120">
       <c r="A139" s="2">
         <v>42355</v>
       </c>
-      <c r="B139" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="C139" s="29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="75">
+      <c r="B139" s="100" t="s">
+        <v>168</v>
+      </c>
+      <c r="C139" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="30">
       <c r="A140" s="2">
         <v>42355</v>
       </c>
-      <c r="B140" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C140" s="29" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="135">
+      <c r="B140" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C140" s="28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
       <c r="A141" s="2">
         <v>42355</v>
       </c>
-      <c r="B141" s="100" t="s">
-        <v>173</v>
+      <c r="B141" s="29" t="s">
+        <v>171</v>
       </c>
       <c r="C141" s="29" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="75">
       <c r="A142" s="2">
         <v>42355</v>
       </c>
-      <c r="B142" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C142" s="42" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="30">
+      <c r="B142" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C142" s="29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="135">
       <c r="A143" s="2">
         <v>42355</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B143" s="100" t="s">
         <v>173</v>
       </c>
-      <c r="C143" s="30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
+      <c r="C143" s="29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="75">
       <c r="A144" s="2">
         <v>42355</v>
       </c>
-      <c r="C144" s="30" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6">
+      <c r="B144" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C144" s="42" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="30">
       <c r="A145" s="2">
         <v>42355</v>
       </c>
-      <c r="B145" s="42"/>
+      <c r="B145" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="C145" s="30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
       <c r="A146" s="2">
         <v>42355</v>
       </c>
-      <c r="B146" s="42"/>
       <c r="C146" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="2">
+        <v>42355</v>
+      </c>
+      <c r="B147" s="42"/>
+      <c r="C147" s="30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="2">
+        <v>42355</v>
+      </c>
+      <c r="B148" s="42"/>
+      <c r="C148" s="30" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="75">
-      <c r="A147" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B147" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="C147" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" ht="30">
-      <c r="A148" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B148" s="26"/>
-      <c r="C148" s="31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" ht="75">
+    <row r="149" spans="1:3" ht="75">
       <c r="A149" s="2">
         <v>42352</v>
       </c>
-      <c r="B149" s="26"/>
-      <c r="C149" s="70" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6">
+      <c r="B149" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C149" s="30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="30">
       <c r="A150" s="2">
         <v>42352</v>
       </c>
       <c r="B150" s="26"/>
-      <c r="C150" s="32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6">
+      <c r="C150" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="75">
       <c r="A151" s="2">
         <v>42352</v>
       </c>
-      <c r="B151" s="96"/>
-      <c r="C151" s="33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6">
+      <c r="B151" s="26"/>
+      <c r="C151" s="70" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
       <c r="A152" s="2">
         <v>42352</v>
       </c>
-      <c r="B152" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C152" s="34" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6">
+      <c r="B152" s="26"/>
+      <c r="C152" s="32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
       <c r="A153" s="2">
         <v>42352</v>
       </c>
       <c r="B153" s="96"/>
-      <c r="C153" s="34" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6">
+      <c r="C153" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
       <c r="A154" s="2">
         <v>42352</v>
       </c>
-      <c r="B154" s="96"/>
-      <c r="C154" s="37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" ht="30">
+      <c r="B154" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C154" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
       <c r="A155" s="2">
         <v>42352</v>
       </c>
-      <c r="B155" s="37"/>
-      <c r="C155" s="37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="30">
+      <c r="B155" s="96"/>
+      <c r="C155" s="34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
       <c r="A156" s="2">
         <v>42352</v>
       </c>
       <c r="B156" s="96"/>
-      <c r="C156" s="96" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" ht="45">
+      <c r="C156" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="30">
       <c r="A157" s="2">
         <v>42352</v>
       </c>
-      <c r="B157" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C157" s="96" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="45">
+      <c r="B157" s="37"/>
+      <c r="C157" s="37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="30">
       <c r="A158" s="2">
         <v>42352</v>
       </c>
-      <c r="B158" s="100"/>
-      <c r="C158" s="39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="30">
+      <c r="B158" s="96"/>
+      <c r="C158" s="96" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="45">
       <c r="A159" s="2">
         <v>42352</v>
       </c>
-      <c r="B159" s="38"/>
-      <c r="C159" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="F159" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="75">
+      <c r="B159" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C159" s="96" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="45">
       <c r="A160" s="2">
         <v>42352</v>
       </c>
-      <c r="B160" s="41"/>
-      <c r="C160" s="41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="45">
+      <c r="B160" s="100"/>
+      <c r="C160" s="39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="30">
       <c r="A161" s="2">
         <v>42352</v>
       </c>
-      <c r="B161" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C161" s="41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="30">
+      <c r="B161" s="38"/>
+      <c r="C161" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="F161" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="75">
       <c r="A162" s="2">
         <v>42352</v>
       </c>
-      <c r="B162" s="43"/>
-      <c r="C162" s="43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="45">
+      <c r="B162" s="41"/>
+      <c r="C162" s="41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" ht="45">
       <c r="A163" s="2">
         <v>42352</v>
       </c>
-      <c r="B163" s="44"/>
-      <c r="C163" s="44" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="30">
+      <c r="B163" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C163" s="41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="30">
       <c r="A164" s="2">
         <v>42352</v>
       </c>
-      <c r="B164" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="C164" s="46" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="30">
+      <c r="B164" s="43"/>
+      <c r="C164" s="43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="45">
       <c r="A165" s="2">
         <v>42352</v>
       </c>
-      <c r="B165" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C165" s="47" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
+      <c r="B165" s="44"/>
+      <c r="C165" s="44" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="30">
       <c r="A166" s="2">
         <v>42352</v>
       </c>
-      <c r="B166" s="100" t="s">
+      <c r="B166" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C166" s="46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="30">
+      <c r="A167" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B167" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C167" s="47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B168" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="C166" s="48" t="s">
+      <c r="C168" s="48" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="135">
-      <c r="A167" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B167" s="49"/>
-      <c r="C167" s="49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="60">
-      <c r="A168" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B168" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="C168" s="51" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="30">
+    <row r="169" spans="1:6" ht="135">
       <c r="A169" s="2">
         <v>42349</v>
       </c>
-      <c r="B169" s="96"/>
-      <c r="C169" s="53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" ht="120">
+      <c r="B169" s="49"/>
+      <c r="C169" s="49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="60">
       <c r="A170" s="2">
         <v>42349</v>
       </c>
-      <c r="B170" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C170" s="53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" ht="150">
+      <c r="B170" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C170" s="51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="30">
       <c r="A171" s="2">
         <v>42349</v>
       </c>
-      <c r="B171" s="52"/>
-      <c r="C171" s="52" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" ht="30">
+      <c r="B171" s="96"/>
+      <c r="C171" s="53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="120">
       <c r="A172" s="2">
         <v>42349</v>
       </c>
-      <c r="B172" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C172" s="54" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3">
+      <c r="B172" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C172" s="53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="150">
       <c r="A173" s="2">
         <v>42349</v>
       </c>
-      <c r="B173" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C173" s="55" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3">
+      <c r="B173" s="52"/>
+      <c r="C173" s="52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="30">
       <c r="A174" s="2">
         <v>42349</v>
       </c>
-      <c r="B174" s="100"/>
-      <c r="C174" s="57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
+      <c r="B174" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C174" s="54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
       <c r="A175" s="2">
         <v>42349</v>
       </c>
-      <c r="B175" s="58"/>
-      <c r="C175" s="58" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3">
+      <c r="B175" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C175" s="55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
       <c r="A176" s="2">
         <v>42349</v>
       </c>
-      <c r="B176" s="59"/>
-      <c r="C176" s="59" t="s">
-        <v>70</v>
+      <c r="B176" s="100"/>
+      <c r="C176" s="57" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="2">
         <v>42349</v>
       </c>
-      <c r="B177" s="60"/>
-      <c r="C177" s="60" t="s">
-        <v>64</v>
+      <c r="B177" s="58"/>
+      <c r="C177" s="58" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="2">
         <v>42349</v>
       </c>
-      <c r="B178" s="61"/>
-      <c r="C178" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="60">
+      <c r="B178" s="59"/>
+      <c r="C178" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
       <c r="A179" s="2">
         <v>42349</v>
       </c>
-      <c r="B179" s="62" t="s">
+      <c r="B179" s="60"/>
+      <c r="C179" s="60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" s="2">
+        <v>42349</v>
+      </c>
+      <c r="B180" s="61"/>
+      <c r="C180" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="60">
+      <c r="A181" s="2">
+        <v>42349</v>
+      </c>
+      <c r="B181" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="C179" s="100" t="s">
+      <c r="C181" s="100" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="90">
-      <c r="A180" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B180" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C180" s="62" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" ht="30">
-      <c r="A181" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C181" s="62" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" ht="90">
       <c r="A182" s="2">
         <v>42345</v>
       </c>
-      <c r="B182" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C182" s="63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3">
+      <c r="B182" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C182" s="62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="30">
       <c r="A183" s="2">
         <v>42345</v>
       </c>
-      <c r="B183" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C183" s="64" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" ht="30">
+      <c r="B183" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C183" s="62" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
       <c r="A184" s="2">
         <v>42345</v>
       </c>
       <c r="B184" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C184" s="65" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" ht="195">
+      <c r="C184" s="63" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
       <c r="A185" s="2">
         <v>42345</v>
       </c>
-      <c r="B185" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C185" s="66" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="135">
+      <c r="B185" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C185" s="64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="30">
       <c r="A186" s="2">
         <v>42345</v>
       </c>
-      <c r="B186" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="C186" s="67" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="75">
+      <c r="B186" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C186" s="65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="195">
       <c r="A187" s="2">
         <v>42345</v>
       </c>
-      <c r="B187" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="C187" s="68" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" ht="75">
+      <c r="B187" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C187" s="66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="135">
       <c r="A188" s="2">
         <v>42345</v>
       </c>
-      <c r="B188" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C188" s="69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" ht="30">
+      <c r="B188" s="100" t="s">
+        <v>31</v>
+      </c>
+      <c r="C188" s="67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="75">
       <c r="A189" s="2">
         <v>42345</v>
       </c>
-      <c r="B189" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C189" s="73" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
+      <c r="B189" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C189" s="68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="75">
       <c r="A190" s="2">
         <v>42345</v>
       </c>
-      <c r="B190" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="C190" s="73" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3">
+      <c r="B190" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C190" s="69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="30">
       <c r="A191" s="2">
         <v>42345</v>
       </c>
-      <c r="B191" s="72" t="s">
-        <v>39</v>
+      <c r="B191" s="100" t="s">
+        <v>12</v>
       </c>
       <c r="C191" s="73" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" ht="60">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
       <c r="A192" s="2">
         <v>42345</v>
       </c>
-      <c r="B192" s="96" t="s">
+      <c r="B192" s="71" t="s">
         <v>39</v>
       </c>
       <c r="C192" s="73" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="150">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
       <c r="A193" s="2">
         <v>42345</v>
       </c>
-      <c r="B193" s="15" t="s">
-        <v>43</v>
+      <c r="B193" s="72" t="s">
+        <v>39</v>
       </c>
       <c r="C193" s="73" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" ht="60">
       <c r="A194" s="2">
         <v>42345</v>
       </c>
-      <c r="B194" s="100" t="s">
+      <c r="B194" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="C194" s="76" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="60">
+      <c r="C194" s="73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="150">
       <c r="A195" s="2">
         <v>42345</v>
       </c>
       <c r="B195" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C195" s="77" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" ht="105">
+      <c r="C195" s="73" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="45">
       <c r="A196" s="2">
         <v>42345</v>
       </c>
       <c r="B196" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C196" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3">
+        <v>39</v>
+      </c>
+      <c r="C196" s="76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="60">
       <c r="A197" s="2">
         <v>42345</v>
       </c>
-      <c r="B197" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C197" s="96" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3">
+      <c r="B197" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C197" s="77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="105">
       <c r="A198" s="2">
         <v>42345</v>
       </c>
-      <c r="B198" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C198" s="96" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="75">
+      <c r="B198" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
       <c r="A199" s="2">
         <v>42345</v>
       </c>
@@ -6039,65 +6058,65 @@
         <v>49</v>
       </c>
       <c r="C199" s="96" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" ht="45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
       <c r="A200" s="2">
         <v>42345</v>
       </c>
       <c r="B200" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C200" s="96" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="75">
+      <c r="A201" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B201" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C201" s="96" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="45">
+      <c r="A202" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B202" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C200" s="96" t="s">
+      <c r="C202" s="96" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="141">
-      <c r="A201" s="80">
+    <row r="203" spans="1:3" ht="141">
+      <c r="A203" s="80">
         <v>42345</v>
       </c>
-      <c r="B201" s="78" t="s">
+      <c r="B203" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="C201" s="78" t="s">
+      <c r="C203" s="78" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="105">
-      <c r="A202" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B202" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C202" s="100" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="90">
-      <c r="A203" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B203" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C203" s="96" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="75">
+    <row r="204" spans="1:3" ht="105">
       <c r="A204" s="2">
         <v>42341</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C204" s="96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" ht="30">
+        <v>12</v>
+      </c>
+      <c r="C204" s="100" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="90">
       <c r="A205" s="2">
         <v>42341</v>
       </c>
@@ -6105,10 +6124,10 @@
         <v>15</v>
       </c>
       <c r="C205" s="96" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="75">
       <c r="A206" s="2">
         <v>42341</v>
       </c>
@@ -6116,10 +6135,10 @@
         <v>15</v>
       </c>
       <c r="C206" s="96" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" ht="45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="30">
       <c r="A207" s="2">
         <v>42341</v>
       </c>
@@ -6127,21 +6146,21 @@
         <v>15</v>
       </c>
       <c r="C207" s="96" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="90">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="30">
       <c r="A208" s="2">
         <v>42341</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C208" s="96" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="45">
       <c r="A209" s="2">
         <v>42341</v>
       </c>
@@ -6149,21 +6168,21 @@
         <v>15</v>
       </c>
       <c r="C209" s="96" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" ht="150">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" ht="90">
       <c r="A210" s="2">
         <v>42341</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C210" s="96" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" ht="75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="30">
       <c r="A211" s="2">
         <v>42341</v>
       </c>
@@ -6171,51 +6190,51 @@
         <v>15</v>
       </c>
       <c r="C211" s="96" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" ht="90">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="150">
       <c r="A212" s="2">
         <v>42341</v>
       </c>
-      <c r="B212" s="100" t="s">
-        <v>12</v>
+      <c r="B212" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C212" s="96" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" ht="60">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="75">
       <c r="A213" s="2">
         <v>42341</v>
       </c>
-      <c r="B213" s="96" t="s">
+      <c r="B213" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C213" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" ht="90">
       <c r="A214" s="2">
         <v>42341</v>
       </c>
-      <c r="B214" s="96" t="s">
+      <c r="B214" s="100" t="s">
         <v>12</v>
       </c>
       <c r="C214" s="96" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" ht="60">
       <c r="A215" s="2">
         <v>42341</v>
       </c>
       <c r="B215" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C215" s="7" t="s">
-        <v>34</v>
+      <c r="C215" s="96" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -6223,10 +6242,10 @@
         <v>42341</v>
       </c>
       <c r="B216" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C216" s="7" t="s">
-        <v>166</v>
+        <v>12</v>
+      </c>
+      <c r="C216" s="96" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -6236,8 +6255,8 @@
       <c r="B217" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C217" s="8" t="s">
-        <v>165</v>
+      <c r="C217" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -6247,307 +6266,329 @@
       <c r="B218" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C218" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" ht="75">
+      <c r="C218" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
       <c r="A219" s="2">
         <v>42341</v>
       </c>
       <c r="B219" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C219" s="100" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" ht="60">
+      <c r="C219" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
       <c r="A220" s="2">
         <v>42341</v>
       </c>
       <c r="B220" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C220" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" ht="75">
+      <c r="A221" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B221" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C221" s="100" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" ht="60">
+      <c r="A222" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B222" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C220" s="96" t="s">
+      <c r="C222" s="96" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" ht="60">
-      <c r="A221" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B221" s="96"/>
-      <c r="C221" s="96" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="45">
-      <c r="A222" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B222" s="96"/>
-      <c r="C222" s="96" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="60">
       <c r="A223" s="2">
         <v>42340</v>
       </c>
-      <c r="B223" s="2" t="s">
+      <c r="B223" s="96"/>
+      <c r="C223" s="96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" ht="45">
+      <c r="A224" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B224" s="96"/>
+      <c r="C224" s="96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" ht="60">
+      <c r="A225" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B225" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C223" s="96" t="s">
+      <c r="C225" s="96" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:3">
-      <c r="A224" s="2">
+    <row r="226" spans="1:3">
+      <c r="A226" s="2">
         <v>42339</v>
       </c>
-      <c r="B224" s="2"/>
-      <c r="C224" s="96" t="s">
+      <c r="B226" s="2"/>
+      <c r="C226" s="96" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:3">
-      <c r="A225" s="2">
+    <row r="227" spans="1:3">
+      <c r="A227" s="2">
         <v>42339</v>
       </c>
-      <c r="B225" s="2"/>
-      <c r="C225" s="96" t="s">
+      <c r="B227" s="2"/>
+      <c r="C227" s="96" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:3" ht="64.5">
-      <c r="A226" s="80">
-        <v>42334</v>
-      </c>
-      <c r="B226" s="78" t="s">
-        <v>309</v>
-      </c>
-      <c r="C226" s="78" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" ht="26.25">
-      <c r="A227" s="80">
-        <v>42334</v>
-      </c>
-      <c r="B227" s="78" t="s">
-        <v>307</v>
-      </c>
-      <c r="C227" s="78" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" ht="39">
+    <row r="228" spans="1:3" ht="64.5">
       <c r="A228" s="80">
         <v>42334</v>
       </c>
       <c r="B228" s="78" t="s">
+        <v>309</v>
+      </c>
+      <c r="C228" s="78" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="26.25">
+      <c r="A229" s="80">
+        <v>42334</v>
+      </c>
+      <c r="B229" s="78" t="s">
+        <v>307</v>
+      </c>
+      <c r="C229" s="78" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" ht="39">
+      <c r="A230" s="80">
+        <v>42334</v>
+      </c>
+      <c r="B230" s="78" t="s">
         <v>272</v>
       </c>
-      <c r="C228" s="78" t="s">
+      <c r="C230" s="78" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="229" spans="1:3" ht="128.25">
-      <c r="A229" s="80">
+    <row r="231" spans="1:3" ht="128.25">
+      <c r="A231" s="80">
         <v>42333</v>
       </c>
-      <c r="B229" s="78" t="s">
+      <c r="B231" s="78" t="s">
         <v>268</v>
       </c>
-      <c r="C229" s="78" t="s">
+      <c r="C231" s="78" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="230" spans="1:3" ht="51.75">
-      <c r="A230" s="80">
+    <row r="232" spans="1:3" ht="51.75">
+      <c r="A232" s="80">
         <v>42333</v>
       </c>
-      <c r="B230" s="78" t="s">
+      <c r="B232" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C230" s="78" t="s">
+      <c r="C232" s="78" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="26.25">
-      <c r="A231" s="80">
+    <row r="233" spans="1:3" ht="26.25">
+      <c r="A233" s="80">
         <v>42331</v>
       </c>
-      <c r="B231" s="78" t="s">
+      <c r="B233" s="78" t="s">
         <v>313</v>
       </c>
-      <c r="C231" s="78" t="s">
+      <c r="C233" s="78" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="39">
-      <c r="A232" s="80">
+    <row r="234" spans="1:3" ht="39">
+      <c r="A234" s="80">
         <v>42329</v>
       </c>
-      <c r="B232" s="78" t="s">
+      <c r="B234" s="78" t="s">
         <v>315</v>
       </c>
-      <c r="C232" s="78" t="s">
+      <c r="C234" s="78" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="39">
-      <c r="A233" s="80">
-        <v>42328</v>
-      </c>
-      <c r="B233" s="78" t="s">
-        <v>324</v>
-      </c>
-      <c r="C233" s="78" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" ht="26.25">
-      <c r="A234" s="80">
-        <v>42328</v>
-      </c>
-      <c r="B234" s="78" t="s">
-        <v>322</v>
-      </c>
-      <c r="C234" s="78" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" ht="115.5">
+    <row r="235" spans="1:3" ht="39">
       <c r="A235" s="80">
         <v>42328</v>
       </c>
       <c r="B235" s="78" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="C235" s="78" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" ht="90">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" ht="26.25">
       <c r="A236" s="80">
         <v>42328</v>
       </c>
       <c r="B236" s="78" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="C236" s="78" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" ht="153.75">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" ht="115.5">
       <c r="A237" s="80">
         <v>42328</v>
       </c>
       <c r="B237" s="78" t="s">
+        <v>320</v>
+      </c>
+      <c r="C237" s="78" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" ht="90">
+      <c r="A238" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B238" s="78" t="s">
         <v>317</v>
       </c>
-      <c r="C237" s="78" t="s">
+      <c r="C238" s="78" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" ht="153.75">
+      <c r="A239" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B239" s="78" t="s">
+        <v>317</v>
+      </c>
+      <c r="C239" s="78" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="238" spans="1:3" ht="102.75">
-      <c r="A238" s="80">
+    <row r="240" spans="1:3" ht="102.75">
+      <c r="A240" s="80">
         <v>42324</v>
       </c>
-      <c r="B238" s="78" t="s">
+      <c r="B240" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="C238" s="78" t="s">
+      <c r="C240" s="78" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="90">
-      <c r="A239" s="80">
+    <row r="241" spans="1:3" ht="90">
+      <c r="A241" s="80">
         <v>42321</v>
       </c>
-      <c r="B239" s="78" t="s">
+      <c r="B241" s="78" t="s">
         <v>327</v>
       </c>
-      <c r="C239" s="78" t="s">
+      <c r="C241" s="78" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="26.25">
-      <c r="A240" s="80">
+    <row r="242" spans="1:3" ht="26.25">
+      <c r="A242" s="80">
         <v>42321</v>
       </c>
-      <c r="B240" s="78" t="s">
+      <c r="B242" s="78" t="s">
         <v>327</v>
       </c>
-      <c r="C240" s="78" t="s">
+      <c r="C242" s="78" t="s">
         <v>326</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" ht="77.25">
-      <c r="A241" s="79">
-        <v>42318</v>
-      </c>
-      <c r="B241" s="78" t="s">
-        <v>330</v>
-      </c>
-      <c r="C241" s="78" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" ht="115.5">
-      <c r="A242" s="79">
-        <v>42311</v>
-      </c>
-      <c r="B242" s="78" t="s">
-        <v>216</v>
-      </c>
-      <c r="C242" s="78" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="243" spans="1:3" ht="77.25">
       <c r="A243" s="79">
+        <v>42318</v>
+      </c>
+      <c r="B243" s="78" t="s">
+        <v>330</v>
+      </c>
+      <c r="C243" s="78" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" ht="115.5">
+      <c r="A244" s="79">
+        <v>42311</v>
+      </c>
+      <c r="B244" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="C244" s="78" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" ht="77.25">
+      <c r="A245" s="79">
         <v>42310</v>
       </c>
-      <c r="B243" s="78" t="s">
+      <c r="B245" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C243" s="78" t="s">
+      <c r="C245" s="78" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="51.75">
-      <c r="A244" s="79">
+    <row r="246" spans="1:3" ht="51.75">
+      <c r="A246" s="79">
         <v>42306</v>
       </c>
-      <c r="B244" s="78" t="s">
+      <c r="B246" s="78" t="s">
         <v>333</v>
       </c>
-      <c r="C244" s="78" t="s">
+      <c r="C246" s="78" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
-      <c r="A245" s="100"/>
-      <c r="B245" s="100"/>
-      <c r="C245" s="100"/>
+    <row r="247" spans="1:3">
+      <c r="A247" s="100"/>
+      <c r="B247" s="100"/>
+      <c r="C247" s="100"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C245">
+  <autoFilter ref="A1:C247">
     <sortState ref="A2:C201">
       <sortCondition descending="1" ref="A1:A201"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C217" r:id="rId1"/>
-    <hyperlink ref="C178" r:id="rId2"/>
-    <hyperlink ref="C218" r:id="rId3"/>
-    <hyperlink ref="C52" r:id="rId4"/>
-    <hyperlink ref="C37" r:id="rId5"/>
-    <hyperlink ref="C34" r:id="rId6"/>
+    <hyperlink ref="C219" r:id="rId1"/>
+    <hyperlink ref="C180" r:id="rId2"/>
+    <hyperlink ref="C220" r:id="rId3"/>
+    <hyperlink ref="C54" r:id="rId4"/>
+    <hyperlink ref="C39" r:id="rId5"/>
+    <hyperlink ref="C36" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -6567,16 +6608,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="60.75" customHeight="1">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add an awesome java code sample source library
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -15,14 +15,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'AS400 Version'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$254</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$255</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="575">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -2901,12 +2901,42 @@
     <t>這兩天在重構寫好的ECSDAPP, 一開始的方向是沿著美的角度, 比如將流動結構和MODULE有效區域和命名等規則定靚定死. 但再看CODE, 發覺很複雜. 
 今天早上改變方向, 從目標"Easy &amp; quick to add-new/ change feature" 出發, 是一個更好的思路, 由此發散出的規定(LAW)也更貼近現實. 下午繼續改卻發現還是有點離地, 因此再將LAW簡化, 且對AS400 RPG PGMMING原有的特性進行量身訂做, 並OUTPUT了一些LAW, 感覺這就是我需要的東西.</t>
   </si>
+  <si>
+    <t>BANG!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When I am searching for jt400 programcall class example, I come across this AWESOME website:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF152BFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>http://www.programcreek.com/java-api-examples/index.php</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+This is mind-blowing. Awesome!</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3093,8 +3123,15 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF152BFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3167,6 +3204,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -3234,7 +3277,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3630,6 +3673,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3655,6 +3704,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF152BFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3669,13 +3723,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4202207</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>142</xdr:row>
       <xdr:rowOff>593914</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>257735</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>146</xdr:row>
       <xdr:rowOff>102263</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3992,10 +4046,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F254"/>
+  <dimension ref="A1:F255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4027,558 +4081,558 @@
       <c r="B3" s="131"/>
       <c r="C3" s="131"/>
     </row>
-    <row r="4" spans="1:4" s="102" customFormat="1" ht="120">
+    <row r="4" spans="1:4" s="102" customFormat="1" ht="60">
       <c r="A4" s="121">
-        <v>42614</v>
-      </c>
-      <c r="B4" s="133" t="s">
-        <v>571</v>
-      </c>
-      <c r="C4" s="133" t="s">
-        <v>572</v>
+        <v>42642</v>
+      </c>
+      <c r="B4" s="136" t="s">
+        <v>573</v>
+      </c>
+      <c r="C4" s="134" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="102" customFormat="1" ht="120">
       <c r="A5" s="121">
-        <v>42613</v>
-      </c>
-      <c r="B5" s="131" t="s">
-        <v>569</v>
-      </c>
-      <c r="C5" s="131" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="102" customFormat="1" ht="30">
+        <v>42614</v>
+      </c>
+      <c r="B5" s="133" t="s">
+        <v>571</v>
+      </c>
+      <c r="C5" s="133" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="102" customFormat="1" ht="120">
       <c r="A6" s="121">
         <v>42613</v>
       </c>
       <c r="B6" s="131" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="C6" s="131" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="102" customFormat="1" ht="75">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="102" customFormat="1" ht="30">
       <c r="A7" s="121">
         <v>42613</v>
       </c>
       <c r="B7" s="131" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C7" s="131" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="121" customFormat="1" ht="45">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="102" customFormat="1" ht="75">
       <c r="A8" s="121">
         <v>42613</v>
       </c>
-      <c r="B8" s="121" t="s">
+      <c r="B8" s="131" t="s">
+        <v>565</v>
+      </c>
+      <c r="C8" s="131" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="121" customFormat="1" ht="45">
+      <c r="A9" s="121">
+        <v>42613</v>
+      </c>
+      <c r="B9" s="121" t="s">
         <v>567</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C9" s="131" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="102" customFormat="1" ht="30">
-      <c r="A9" s="121">
+    <row r="10" spans="1:4" s="102" customFormat="1" ht="30">
+      <c r="A10" s="121">
         <v>42571</v>
       </c>
-      <c r="B9" s="131" t="s">
+      <c r="B10" s="131" t="s">
         <v>562</v>
       </c>
-      <c r="C9" s="130" t="s">
+      <c r="C10" s="130" t="s">
         <v>561</v>
       </c>
-      <c r="D9" s="132" t="s">
+      <c r="D10" s="132" t="s">
         <v>560</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="102" customFormat="1" ht="75">
-      <c r="A10" s="121">
-        <v>42570</v>
-      </c>
-      <c r="B10" s="128" t="s">
-        <v>558</v>
-      </c>
-      <c r="C10" s="129" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="102" customFormat="1" ht="75">
       <c r="A11" s="121">
         <v>42570</v>
       </c>
-      <c r="B11" s="127" t="s">
+      <c r="B11" s="128" t="s">
+        <v>558</v>
+      </c>
+      <c r="C11" s="129" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="102" customFormat="1" ht="75">
+      <c r="A12" s="121">
+        <v>42570</v>
+      </c>
+      <c r="B12" s="127" t="s">
         <v>551</v>
       </c>
-      <c r="C11" s="127" t="s">
+      <c r="C12" s="127" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="102" customFormat="1" ht="45">
-      <c r="A12" s="121">
-        <v>42569</v>
-      </c>
-      <c r="B12" s="126" t="s">
-        <v>554</v>
-      </c>
-      <c r="C12" s="126" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="102" customFormat="1" ht="90">
+    <row r="13" spans="1:4" s="102" customFormat="1" ht="45">
       <c r="A13" s="121">
         <v>42569</v>
       </c>
-      <c r="B13" s="125" t="s">
-        <v>551</v>
-      </c>
-      <c r="C13" s="127" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="102" customFormat="1" ht="45">
+      <c r="B13" s="126" t="s">
+        <v>554</v>
+      </c>
+      <c r="C13" s="126" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="102" customFormat="1" ht="90">
       <c r="A14" s="121">
         <v>42569</v>
       </c>
       <c r="B14" s="125" t="s">
-        <v>550</v>
-      </c>
-      <c r="C14" s="125" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="102" customFormat="1" ht="30">
+        <v>551</v>
+      </c>
+      <c r="C14" s="127" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="102" customFormat="1" ht="45">
       <c r="A15" s="121">
         <v>42569</v>
       </c>
       <c r="B15" s="125" t="s">
+        <v>550</v>
+      </c>
+      <c r="C15" s="125" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="102" customFormat="1" ht="30">
+      <c r="A16" s="121">
+        <v>42569</v>
+      </c>
+      <c r="B16" s="125" t="s">
         <v>549</v>
       </c>
-      <c r="C15" s="125" t="s">
+      <c r="C16" s="125" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="102" customFormat="1" ht="90">
-      <c r="A16" s="121">
-        <v>42567</v>
-      </c>
-      <c r="B16" s="124" t="s">
-        <v>548</v>
-      </c>
-      <c r="C16" s="124" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="102" customFormat="1" ht="45">
+    <row r="17" spans="1:3" s="102" customFormat="1" ht="90">
       <c r="A17" s="121">
         <v>42567</v>
       </c>
       <c r="B17" s="124" t="s">
+        <v>548</v>
+      </c>
+      <c r="C17" s="124" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A18" s="121">
+        <v>42567</v>
+      </c>
+      <c r="B18" s="124" t="s">
         <v>546</v>
       </c>
-      <c r="C17" s="124" t="s">
+      <c r="C18" s="124" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A18" s="121">
+    <row r="19" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A19" s="121">
         <v>42565</v>
       </c>
-      <c r="B18" s="123" t="s">
+      <c r="B19" s="123" t="s">
         <v>543</v>
       </c>
-      <c r="C18" s="123" t="s">
+      <c r="C19" s="123" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="102" customFormat="1" ht="75">
-      <c r="A19" s="121">
+    <row r="20" spans="1:3" s="102" customFormat="1" ht="75">
+      <c r="A20" s="121">
         <v>42564</v>
       </c>
-      <c r="B19" s="122" t="s">
+      <c r="B20" s="122" t="s">
         <v>534</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C20" s="122" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="102" customFormat="1" ht="135">
-      <c r="A20" s="121">
-        <v>42562</v>
-      </c>
-      <c r="B20" s="120" t="s">
-        <v>537</v>
-      </c>
-      <c r="C20" s="120" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="102" customFormat="1" ht="60">
+    <row r="21" spans="1:3" s="102" customFormat="1" ht="135">
       <c r="A21" s="121">
         <v>42562</v>
       </c>
       <c r="B21" s="120" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C21" s="120" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="102" customFormat="1" ht="75">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="102" customFormat="1" ht="60">
       <c r="A22" s="121">
         <v>42562</v>
       </c>
       <c r="B22" s="120" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C22" s="120" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="102" customFormat="1" ht="165">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="102" customFormat="1" ht="75">
       <c r="A23" s="121">
         <v>42562</v>
       </c>
       <c r="B23" s="120" t="s">
+        <v>535</v>
+      </c>
+      <c r="C23" s="120" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="102" customFormat="1" ht="165">
+      <c r="A24" s="121">
+        <v>42562</v>
+      </c>
+      <c r="B24" s="120" t="s">
         <v>534</v>
       </c>
-      <c r="C23" s="120" t="s">
+      <c r="C24" s="120" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A24" s="121">
+    <row r="25" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A25" s="121">
         <v>42557</v>
       </c>
-      <c r="B24" s="120" t="s">
+      <c r="B25" s="120" t="s">
         <v>525</v>
       </c>
-      <c r="C24" s="120" t="s">
+      <c r="C25" s="120" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="102" customFormat="1" ht="180">
-      <c r="A25" s="120"/>
-      <c r="B25" s="120" t="s">
+    <row r="26" spans="1:3" s="102" customFormat="1" ht="180">
+      <c r="A26" s="120"/>
+      <c r="B26" s="120" t="s">
         <v>527</v>
       </c>
-      <c r="C25" s="120" t="s">
+      <c r="C26" s="120" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A26" s="121">
+    <row r="27" spans="1:3" s="102" customFormat="1" ht="150">
+      <c r="A27" s="121">
         <v>42540</v>
       </c>
-      <c r="B26" s="120" t="s">
+      <c r="B27" s="120" t="s">
         <v>529</v>
       </c>
-      <c r="C26" s="120" t="s">
+      <c r="C27" s="120" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="102" customFormat="1" ht="180">
-      <c r="A27" s="121">
-        <v>42539</v>
-      </c>
-      <c r="B27" s="120" t="s">
-        <v>527</v>
-      </c>
-      <c r="C27" s="120" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="102" customFormat="1" ht="105">
+    <row r="28" spans="1:3" s="102" customFormat="1" ht="180">
       <c r="A28" s="121">
         <v>42539</v>
       </c>
       <c r="B28" s="120" t="s">
+        <v>527</v>
+      </c>
+      <c r="C28" s="120" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A29" s="121">
+        <v>42539</v>
+      </c>
+      <c r="B29" s="120" t="s">
         <v>532</v>
       </c>
-      <c r="C28" s="120" t="s">
+      <c r="C29" s="120" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A29" s="2">
+    <row r="30" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A30" s="2">
         <v>42534</v>
       </c>
-      <c r="B29" s="119" t="s">
+      <c r="B30" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="119" t="s">
+      <c r="C30" s="119" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A30" s="2">
+    <row r="31" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A31" s="2">
         <v>42517</v>
       </c>
-      <c r="B30" s="118" t="s">
+      <c r="B31" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="118" t="s">
+      <c r="C31" s="118" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A31" s="2">
+    <row r="32" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A32" s="2">
         <v>42514</v>
       </c>
-      <c r="B31" s="117" t="s">
+      <c r="B32" s="117" t="s">
         <v>519</v>
       </c>
-      <c r="C31" s="117" t="s">
+      <c r="C32" s="117" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A32" s="2">
+    <row r="33" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A33" s="2">
         <v>42507</v>
       </c>
-      <c r="B32" s="116" t="s">
+      <c r="B33" s="116" t="s">
         <v>519</v>
       </c>
-      <c r="C32" s="116" t="s">
+      <c r="C33" s="116" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A33" s="2">
+    <row r="34" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A34" s="2">
         <v>42502</v>
       </c>
-      <c r="B33" s="115" t="s">
+      <c r="B34" s="115" t="s">
         <v>519</v>
       </c>
-      <c r="C33" s="116" t="s">
+      <c r="C34" s="116" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A34" s="2">
-        <v>42485</v>
-      </c>
-      <c r="B34" s="113" t="s">
-        <v>516</v>
-      </c>
-      <c r="C34" s="113" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="102" customFormat="1" ht="30">
+    <row r="35" spans="1:3" s="102" customFormat="1" ht="90">
       <c r="A35" s="2">
         <v>42485</v>
       </c>
-      <c r="B35" s="110" t="s">
-        <v>514</v>
-      </c>
-      <c r="C35" s="110" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="102" customFormat="1" ht="300">
+      <c r="B35" s="113" t="s">
+        <v>516</v>
+      </c>
+      <c r="C35" s="113" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="102" customFormat="1" ht="30">
       <c r="A36" s="2">
         <v>42485</v>
       </c>
-      <c r="B36" s="112" t="s">
+      <c r="B36" s="110" t="s">
+        <v>514</v>
+      </c>
+      <c r="C36" s="110" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="102" customFormat="1" ht="300">
+      <c r="A37" s="2">
+        <v>42485</v>
+      </c>
+      <c r="B37" s="112" t="s">
         <v>241</v>
       </c>
-      <c r="C36" s="112" t="s">
+      <c r="C37" s="112" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A37" s="2">
+    <row r="38" spans="1:3" s="102" customFormat="1" ht="150">
+      <c r="A38" s="2">
         <v>42479</v>
       </c>
-      <c r="B37" s="111" t="s">
+      <c r="B38" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="C37" s="111" t="s">
+      <c r="C38" s="111" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A38" s="2">
+    <row r="39" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="A39" s="2">
         <v>42478</v>
       </c>
-      <c r="B38" s="110" t="s">
+      <c r="B39" s="110" t="s">
         <v>509</v>
       </c>
-      <c r="C38" s="110" t="s">
+      <c r="C39" s="110" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="102" customFormat="1" ht="120">
-      <c r="A39" s="2">
-        <v>42477</v>
-      </c>
-      <c r="B39" s="109" t="s">
-        <v>509</v>
-      </c>
-      <c r="C39" s="109" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" s="102" customFormat="1" ht="30">
+    <row r="40" spans="1:3" s="102" customFormat="1" ht="120">
       <c r="A40" s="2">
         <v>42477</v>
       </c>
-      <c r="B40" s="108" t="s">
+      <c r="B40" s="109" t="s">
+        <v>509</v>
+      </c>
+      <c r="C40" s="109" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A41" s="2">
+        <v>42477</v>
+      </c>
+      <c r="B41" s="108" t="s">
         <v>507</v>
       </c>
-      <c r="C40" s="108" t="s">
+      <c r="C41" s="108" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="102" customFormat="1">
-      <c r="A41" s="2">
-        <v>42473</v>
-      </c>
-      <c r="B41" s="106" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="106" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="102" customFormat="1" ht="45">
+    <row r="42" spans="1:3" s="102" customFormat="1">
       <c r="A42" s="2">
         <v>42473</v>
       </c>
       <c r="B42" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="107" t="s">
+      <c r="C42" s="106" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A43" s="2">
+        <v>42473</v>
+      </c>
+      <c r="B43" s="106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="107" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="102" customFormat="1">
-      <c r="A43" s="2">
+    <row r="44" spans="1:3" s="102" customFormat="1">
+      <c r="A44" s="2">
         <v>42469</v>
       </c>
-      <c r="B43" s="105" t="s">
+      <c r="B44" s="105" t="s">
         <v>504</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C44" s="8" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="102" customFormat="1" ht="75">
-      <c r="A44" s="2">
-        <v>42463</v>
-      </c>
-      <c r="B44" s="104" t="s">
-        <v>497</v>
-      </c>
-      <c r="C44" s="104" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" s="102" customFormat="1" ht="105">
+    <row r="45" spans="1:3" s="102" customFormat="1" ht="75">
       <c r="A45" s="2">
         <v>42463</v>
       </c>
       <c r="B45" s="104" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C45" s="104" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" s="102" customFormat="1">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="102" customFormat="1" ht="105">
       <c r="A46" s="2">
         <v>42463</v>
       </c>
       <c r="B46" s="104" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C46" s="104" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" s="102" customFormat="1" ht="150">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="102" customFormat="1">
       <c r="A47" s="2">
         <v>42463</v>
       </c>
-      <c r="B47" s="100" t="s">
-        <v>493</v>
-      </c>
-      <c r="C47" s="100" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="B47" s="104" t="s">
+        <v>501</v>
+      </c>
+      <c r="C47" s="104" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="102" customFormat="1" ht="150">
       <c r="A48" s="2">
         <v>42463</v>
       </c>
-      <c r="B48" s="103" t="s">
-        <v>492</v>
-      </c>
-      <c r="C48" s="103" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="B48" s="100" t="s">
+        <v>493</v>
+      </c>
+      <c r="C48" s="100" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="102" customFormat="1" ht="90">
       <c r="A49" s="2">
         <v>42463</v>
       </c>
-      <c r="B49" s="101" t="s">
-        <v>489</v>
-      </c>
-      <c r="C49" s="101" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="B49" s="103" t="s">
+        <v>492</v>
+      </c>
+      <c r="C49" s="103" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="102" customFormat="1" ht="30">
       <c r="A50" s="2">
         <v>42463</v>
       </c>
       <c r="B50" s="101" t="s">
+        <v>489</v>
+      </c>
+      <c r="C50" s="101" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A51" s="2">
+        <v>42463</v>
+      </c>
+      <c r="B51" s="101" t="s">
         <v>488</v>
       </c>
-      <c r="C50" s="101" t="s">
+      <c r="C51" s="101" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A51" s="2">
-        <v>42462</v>
-      </c>
-      <c r="B51" s="100" t="s">
-        <v>486</v>
-      </c>
-      <c r="C51" s="100" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" s="4" customFormat="1" ht="135">
+    <row r="52" spans="1:3" s="102" customFormat="1" ht="150">
       <c r="A52" s="2">
         <v>42462</v>
       </c>
       <c r="B52" s="100" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C52" s="100" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" s="4" customFormat="1" ht="240">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="4" customFormat="1" ht="135">
       <c r="A53" s="2">
         <v>42462</v>
       </c>
       <c r="B53" s="100" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="C53" s="100" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" s="4" customFormat="1" ht="120">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="4" customFormat="1" ht="240">
       <c r="A54" s="2">
         <v>42462</v>
       </c>
@@ -4586,362 +4640,362 @@
         <v>480</v>
       </c>
       <c r="C54" s="100" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="4" customFormat="1" ht="120">
       <c r="A55" s="2">
-        <v>42460</v>
-      </c>
-      <c r="B55" s="99" t="s">
-        <v>477</v>
-      </c>
-      <c r="C55" s="99" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" s="4" customFormat="1" ht="30">
+        <v>42462</v>
+      </c>
+      <c r="B55" s="100" t="s">
+        <v>480</v>
+      </c>
+      <c r="C55" s="100" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="4" customFormat="1" ht="120">
       <c r="A56" s="2">
         <v>42460</v>
       </c>
       <c r="B56" s="99" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C56" s="99" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" s="4" customFormat="1" ht="180">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="4" customFormat="1" ht="30">
       <c r="A57" s="2">
         <v>42460</v>
       </c>
       <c r="B57" s="99" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C57" s="99" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" s="4" customFormat="1" ht="60">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="4" customFormat="1" ht="180">
       <c r="A58" s="2">
         <v>42460</v>
       </c>
       <c r="B58" s="99" t="s">
+        <v>475</v>
+      </c>
+      <c r="C58" s="99" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="4" customFormat="1" ht="60">
+      <c r="A59" s="2">
+        <v>42460</v>
+      </c>
+      <c r="B59" s="99" t="s">
         <v>478</v>
       </c>
-      <c r="C58" s="99" t="s">
+      <c r="C59" s="99" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="4" customFormat="1" ht="105">
-      <c r="A59" s="2">
-        <v>42459</v>
-      </c>
-      <c r="B59" s="99" t="s">
-        <v>470</v>
-      </c>
-      <c r="C59" s="98" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="60">
+    <row r="60" spans="1:3" s="4" customFormat="1" ht="105">
       <c r="A60" s="2">
         <v>42459</v>
       </c>
       <c r="B60" s="99" t="s">
+        <v>470</v>
+      </c>
+      <c r="C60" s="98" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="60">
+      <c r="A61" s="2">
+        <v>42459</v>
+      </c>
+      <c r="B61" s="99" t="s">
         <v>241</v>
       </c>
-      <c r="C60" s="99" t="s">
+      <c r="C61" s="99" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="2">
+    <row r="62" spans="1:3">
+      <c r="A62" s="2">
         <v>42458</v>
       </c>
-      <c r="B61" s="97" t="s">
+      <c r="B62" s="97" t="s">
         <v>470</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C62" s="8" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="105">
-      <c r="A62" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B62" s="96" t="s">
-        <v>254</v>
-      </c>
-      <c r="C62" s="100" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="60">
+    <row r="63" spans="1:3" ht="105">
       <c r="A63" s="2">
         <v>42456</v>
       </c>
       <c r="B63" s="96" t="s">
-        <v>462</v>
-      </c>
-      <c r="C63" s="44" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="45">
+        <v>254</v>
+      </c>
+      <c r="C63" s="100" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="60">
       <c r="A64" s="2">
         <v>42456</v>
       </c>
       <c r="B64" s="96" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C64" s="44" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="45">
       <c r="A65" s="2">
         <v>42456</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>466</v>
+      <c r="B65" s="96" t="s">
+        <v>463</v>
       </c>
       <c r="C65" s="44" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="45">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="2">
         <v>42456</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C66" s="44" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="45">
+      <c r="A67" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="C66" s="44" t="s">
+      <c r="C67" s="44" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="77.25">
-      <c r="A67" s="79">
-        <v>42453</v>
-      </c>
-      <c r="B67" s="78" t="s">
-        <v>264</v>
-      </c>
-      <c r="C67" s="78" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="26.25">
+    <row r="68" spans="1:3" ht="77.25">
       <c r="A68" s="79">
         <v>42453</v>
       </c>
       <c r="B68" s="78" t="s">
+        <v>264</v>
+      </c>
+      <c r="C68" s="78" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="26.25">
+      <c r="A69" s="79">
+        <v>42453</v>
+      </c>
+      <c r="B69" s="78" t="s">
         <v>262</v>
       </c>
-      <c r="C68" s="78" t="s">
+      <c r="C69" s="78" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="39">
-      <c r="A69" s="79">
+    <row r="70" spans="1:3" ht="39">
+      <c r="A70" s="79">
         <v>42452</v>
       </c>
-      <c r="B69" s="78" t="s">
+      <c r="B70" s="78" t="s">
         <v>260</v>
       </c>
-      <c r="C69" s="78" t="s">
+      <c r="C70" s="78" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="165">
-      <c r="A70" s="75">
+    <row r="71" spans="1:3" ht="165">
+      <c r="A71" s="75">
         <v>42451</v>
       </c>
-      <c r="B70" s="74" t="s">
+      <c r="B71" s="74" t="s">
         <v>247</v>
       </c>
-      <c r="C70" s="100" t="s">
+      <c r="C71" s="100" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="45">
-      <c r="A71" s="2">
-        <v>42451</v>
-      </c>
-      <c r="B71" s="100" t="s">
-        <v>249</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="30">
+    <row r="72" spans="1:3" ht="45">
       <c r="A72" s="2">
         <v>42451</v>
       </c>
-      <c r="B72" s="96" t="s">
-        <v>196</v>
+      <c r="B72" s="100" t="s">
+        <v>249</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="165">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="30">
       <c r="A73" s="2">
         <v>42451</v>
       </c>
       <c r="B73" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="165">
+      <c r="A74" s="2">
+        <v>42451</v>
+      </c>
+      <c r="B74" s="96" t="s">
         <v>253</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="64.5">
-      <c r="A74" s="79">
-        <v>42451</v>
-      </c>
-      <c r="B74" s="78" t="s">
-        <v>253</v>
-      </c>
-      <c r="C74" s="78" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="64.5">
       <c r="A75" s="79">
+        <v>42451</v>
+      </c>
+      <c r="B75" s="78" t="s">
+        <v>253</v>
+      </c>
+      <c r="C75" s="78" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="64.5">
+      <c r="A76" s="79">
         <v>42447</v>
       </c>
-      <c r="B75" s="78" t="s">
+      <c r="B76" s="78" t="s">
         <v>257</v>
       </c>
-      <c r="C75" s="78" t="s">
+      <c r="C76" s="78" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="2">
+    <row r="77" spans="1:3">
+      <c r="A77" s="2">
         <v>42440</v>
       </c>
-      <c r="B76" s="100" t="s">
+      <c r="B77" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="C76" s="100" t="s">
+      <c r="C77" s="100" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="75">
-      <c r="A77" s="2">
+    <row r="78" spans="1:3" ht="75">
+      <c r="A78" s="2">
         <v>42436</v>
       </c>
-      <c r="B77" s="96" t="s">
+      <c r="B78" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="39">
-      <c r="A78" s="79">
-        <v>42431</v>
-      </c>
-      <c r="B78" s="78" t="s">
-        <v>274</v>
-      </c>
-      <c r="C78" s="78" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="26.25">
+    <row r="79" spans="1:3" ht="39">
       <c r="A79" s="79">
         <v>42431</v>
       </c>
       <c r="B79" s="78" t="s">
+        <v>274</v>
+      </c>
+      <c r="C79" s="78" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="26.25">
+      <c r="A80" s="79">
+        <v>42431</v>
+      </c>
+      <c r="B80" s="78" t="s">
         <v>272</v>
       </c>
-      <c r="C79" s="78" t="s">
+      <c r="C80" s="78" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="51.75">
-      <c r="A80" s="79">
+    <row r="81" spans="1:3" ht="51.75">
+      <c r="A81" s="79">
         <v>42430</v>
       </c>
-      <c r="B80" s="78" t="s">
+      <c r="B81" s="78" t="s">
         <v>270</v>
       </c>
-      <c r="C80" s="78" t="s">
+      <c r="C81" s="78" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="26.25">
-      <c r="A81" s="79">
+    <row r="82" spans="1:3" ht="26.25">
+      <c r="A82" s="79">
         <v>42428</v>
       </c>
-      <c r="B81" s="78" t="s">
+      <c r="B82" s="78" t="s">
         <v>268</v>
       </c>
-      <c r="C81" s="78" t="s">
+      <c r="C82" s="78" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="30">
-      <c r="A82" s="2">
+    <row r="83" spans="1:3" ht="30">
+      <c r="A83" s="2">
         <v>42426</v>
       </c>
-      <c r="B82" s="100" t="s">
+      <c r="B83" s="100" t="s">
         <v>186</v>
       </c>
-      <c r="C82" s="100" t="s">
+      <c r="C83" s="100" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="77.25">
-      <c r="A83" s="79">
+    <row r="84" spans="1:3" ht="77.25">
+      <c r="A84" s="79">
         <v>42426</v>
       </c>
-      <c r="B83" s="78" t="s">
+      <c r="B84" s="78" t="s">
         <v>266</v>
       </c>
-      <c r="C83" s="78" t="s">
+      <c r="C84" s="78" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="2">
-        <v>42425</v>
-      </c>
-      <c r="B84" s="100" t="s">
-        <v>241</v>
-      </c>
-      <c r="C84" s="100" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="2">
         <v>42425</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="100" t="s">
+        <v>241</v>
+      </c>
+      <c r="C85" s="100" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="2">
+        <v>42425</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="26.25">
-      <c r="A86" s="79">
-        <v>42425</v>
-      </c>
-      <c r="B86" s="78" t="s">
-        <v>276</v>
-      </c>
-      <c r="C86" s="78" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" ht="26.25">
       <c r="A87" s="79">
         <v>42425</v>
       </c>
@@ -4949,291 +5003,291 @@
         <v>276</v>
       </c>
       <c r="C87" s="78" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="26.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88" s="79">
         <v>42425</v>
       </c>
       <c r="B88" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="C88" s="78" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="26.25">
+      <c r="A89" s="79">
+        <v>42425</v>
+      </c>
+      <c r="B89" s="78" t="s">
         <v>279</v>
       </c>
-      <c r="C88" s="78" t="s">
+      <c r="C89" s="78" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="165">
-      <c r="A89" s="2">
+    <row r="90" spans="1:3" ht="165">
+      <c r="A90" s="2">
         <v>42424</v>
       </c>
-      <c r="B89" s="100" t="s">
+      <c r="B90" s="100" t="s">
         <v>239</v>
       </c>
-      <c r="C89" s="114" t="s">
+      <c r="C90" s="114" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="45">
-      <c r="A90" s="2">
+    <row r="91" spans="1:3" ht="45">
+      <c r="A91" s="2">
         <v>42423</v>
       </c>
-      <c r="B90" s="96" t="s">
+      <c r="B91" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="C90" s="11" t="s">
+      <c r="C91" s="11" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="79">
+    <row r="92" spans="1:3">
+      <c r="A92" s="79">
         <v>42423</v>
       </c>
-      <c r="B91" s="78" t="s">
+      <c r="B92" s="78" t="s">
         <v>281</v>
       </c>
-      <c r="C91" s="78" t="s">
+      <c r="C92" s="78" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="90">
-      <c r="A92" s="2">
+    <row r="93" spans="1:3" ht="90">
+      <c r="A93" s="2">
         <v>42422</v>
       </c>
-      <c r="B92" s="100" t="s">
+      <c r="B93" s="100" t="s">
         <v>236</v>
       </c>
-      <c r="C92" s="100" t="s">
+      <c r="C93" s="100" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="60">
-      <c r="A93" s="2">
+    <row r="94" spans="1:3" ht="60">
+      <c r="A94" s="2">
         <v>42419</v>
       </c>
-      <c r="B93" s="10" t="s">
+      <c r="B94" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="C93" s="36" t="s">
+      <c r="C94" s="36" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="195">
-      <c r="A94" s="2">
+    <row r="95" spans="1:3" ht="195">
+      <c r="A95" s="2">
         <v>42418</v>
       </c>
-      <c r="B94" s="10" t="s">
+      <c r="B95" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C94" s="18" t="s">
+      <c r="C95" s="18" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="45">
-      <c r="A95" s="2">
-        <v>42403</v>
-      </c>
-      <c r="B95" s="96" t="s">
-        <v>229</v>
-      </c>
-      <c r="C95" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="75">
+    <row r="96" spans="1:3" ht="45">
       <c r="A96" s="2">
         <v>42403</v>
       </c>
-      <c r="B96" s="12" t="s">
-        <v>230</v>
+      <c r="B96" s="96" t="s">
+        <v>229</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="90">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="75">
       <c r="A97" s="2">
         <v>42403</v>
       </c>
-      <c r="B97" s="12"/>
+      <c r="B97" s="12" t="s">
+        <v>230</v>
+      </c>
       <c r="C97" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="90">
       <c r="A98" s="2">
-        <v>42398</v>
-      </c>
-      <c r="B98" s="12" t="s">
-        <v>196</v>
-      </c>
+        <v>42403</v>
+      </c>
+      <c r="B98" s="12"/>
       <c r="C98" s="12" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="45">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="90">
       <c r="A99" s="2">
         <v>42398</v>
       </c>
       <c r="B99" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C99" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="45">
+      <c r="A100" s="2">
+        <v>42398</v>
+      </c>
+      <c r="B100" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="C99" s="12" t="s">
+      <c r="C100" s="12" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
-      <c r="A100" s="2">
+    <row r="101" spans="1:3">
+      <c r="A101" s="2">
         <v>42397</v>
       </c>
-      <c r="B100" s="96" t="s">
+      <c r="B101" s="96" t="s">
         <v>201</v>
       </c>
-      <c r="C100" s="14" t="s">
+      <c r="C101" s="14" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="45">
-      <c r="A101" s="2">
-        <v>42396</v>
-      </c>
-      <c r="B101" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C101" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="30">
+    <row r="102" spans="1:3" ht="45">
       <c r="A102" s="2">
         <v>42396</v>
       </c>
-      <c r="B102" s="96" t="s">
+      <c r="B102" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="30">
+      <c r="A103" s="2">
+        <v>42396</v>
+      </c>
+      <c r="B103" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="C102" s="14" t="s">
+      <c r="C103" s="14" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="128.25">
-      <c r="A103" s="79">
-        <v>42386</v>
-      </c>
-      <c r="B103" s="78" t="s">
-        <v>283</v>
-      </c>
-      <c r="C103" s="78" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="64.5">
+    <row r="104" spans="1:3" ht="128.25">
       <c r="A104" s="79">
         <v>42386</v>
       </c>
       <c r="B104" s="78" t="s">
+        <v>283</v>
+      </c>
+      <c r="C104" s="78" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="64.5">
+      <c r="A105" s="79">
+        <v>42386</v>
+      </c>
+      <c r="B105" s="78" t="s">
         <v>285</v>
       </c>
-      <c r="C104" s="78" t="s">
+      <c r="C105" s="78" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="45">
-      <c r="A105" s="2">
+    <row r="106" spans="1:3" ht="45">
+      <c r="A106" s="2">
         <v>42384</v>
       </c>
-      <c r="B105" s="100" t="s">
+      <c r="B106" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="C105" s="100" t="s">
+      <c r="C106" s="100" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="180">
-      <c r="A106" s="2">
+    <row r="107" spans="1:3" ht="180">
+      <c r="A107" s="2">
         <v>42382</v>
       </c>
-      <c r="B106" s="14" t="s">
+      <c r="B107" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="C106" s="14" t="s">
+      <c r="C107" s="14" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="64.5">
-      <c r="A107" s="79">
+    <row r="108" spans="1:3" ht="64.5">
+      <c r="A108" s="79">
         <v>42382</v>
       </c>
-      <c r="B107" s="78" t="s">
+      <c r="B108" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="C107" s="78" t="s">
+      <c r="C108" s="78" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="30">
-      <c r="A108" s="2">
+    <row r="109" spans="1:3" ht="30">
+      <c r="A109" s="2">
         <v>42381</v>
       </c>
-      <c r="B108" s="100" t="s">
+      <c r="B109" s="100" t="s">
         <v>216</v>
       </c>
-      <c r="C108" s="100" t="s">
+      <c r="C109" s="100" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="45">
-      <c r="A109" s="2">
-        <v>42380</v>
-      </c>
-      <c r="B109" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C109" s="16" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="75">
+    <row r="110" spans="1:3" ht="45">
       <c r="A110" s="2">
         <v>42380</v>
       </c>
-      <c r="B110" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="C110" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="180">
+      <c r="B110" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C110" s="16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="75">
       <c r="A111" s="2">
         <v>42380</v>
       </c>
       <c r="B111" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C111" s="18" t="s">
+      <c r="C111" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="180">
+      <c r="A112" s="2">
+        <v>42380</v>
+      </c>
+      <c r="B112" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="C112" s="18" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="217.5">
-      <c r="A112" s="79">
+    <row r="113" spans="1:3" ht="217.5">
+      <c r="A113" s="79">
         <v>42380</v>
       </c>
-      <c r="B112" s="78" t="s">
+      <c r="B113" s="78" t="s">
         <v>288</v>
       </c>
-      <c r="C112" s="78" t="s">
+      <c r="C113" s="78" t="s">
         <v>289</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="102.75">
-      <c r="A113" s="79">
-        <v>42378</v>
-      </c>
-      <c r="B113" s="78" t="s">
-        <v>291</v>
-      </c>
-      <c r="C113" s="78" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="102.75">
@@ -5241,24 +5295,24 @@
         <v>42378</v>
       </c>
       <c r="B114" s="78" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C114" s="78" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="141">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="102.75">
       <c r="A115" s="79">
         <v>42378</v>
       </c>
       <c r="B115" s="78" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C115" s="78" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="77.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="141">
       <c r="A116" s="79">
         <v>42378</v>
       </c>
@@ -5266,106 +5320,106 @@
         <v>297</v>
       </c>
       <c r="C116" s="78" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="102.75">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="77.25">
       <c r="A117" s="79">
         <v>42378</v>
       </c>
       <c r="B117" s="78" t="s">
+        <v>297</v>
+      </c>
+      <c r="C117" s="78" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="102.75">
+      <c r="A118" s="79">
+        <v>42378</v>
+      </c>
+      <c r="B118" s="78" t="s">
         <v>295</v>
       </c>
-      <c r="C117" s="78" t="s">
+      <c r="C118" s="78" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="60">
-      <c r="A118" s="2">
+    <row r="119" spans="1:3" ht="60">
+      <c r="A119" s="2">
         <v>42377</v>
       </c>
-      <c r="B118" s="100" t="s">
+      <c r="B119" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="C118" s="100" t="s">
+      <c r="C119" s="100" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="77.25">
-      <c r="A119" s="79">
+    <row r="120" spans="1:3" ht="77.25">
+      <c r="A120" s="79">
         <v>42376</v>
       </c>
-      <c r="B119" s="78" t="s">
+      <c r="B120" s="78" t="s">
         <v>300</v>
       </c>
-      <c r="C119" s="78" t="s">
+      <c r="C120" s="78" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="45">
-      <c r="A120" s="2">
+    <row r="121" spans="1:3" ht="45">
+      <c r="A121" s="2">
         <v>42375</v>
       </c>
-      <c r="B120" s="15" t="s">
+      <c r="B121" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C120" s="100" t="s">
+      <c r="C121" s="100" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
-      <c r="A121" s="2">
+    <row r="122" spans="1:3">
+      <c r="A122" s="2">
         <v>42369</v>
       </c>
-      <c r="B121" s="100" t="s">
+      <c r="B122" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="C121" s="19" t="s">
+      <c r="C122" s="19" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="195">
-      <c r="A122" s="2">
-        <v>42368</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C122" s="19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="135">
+    <row r="123" spans="1:3" ht="195">
       <c r="A123" s="2">
         <v>42368</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C123" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="45">
+        <v>196</v>
+      </c>
+      <c r="C123" s="19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="135">
       <c r="A124" s="2">
         <v>42368</v>
       </c>
       <c r="B124" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C124" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="45">
+      <c r="A125" s="2">
+        <v>42368</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C124" s="20" t="s">
+      <c r="C125" s="20" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="30">
-      <c r="A125" s="2">
-        <v>42366</v>
-      </c>
-      <c r="B125" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C125" s="20" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="30">
@@ -5376,111 +5430,111 @@
         <v>49</v>
       </c>
       <c r="C126" s="20" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="30">
+      <c r="A127" s="2">
+        <v>42366</v>
+      </c>
+      <c r="B127" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C127" s="20" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="150">
-      <c r="A127" s="2">
-        <v>42361</v>
-      </c>
-      <c r="C127" s="20" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="30">
+    <row r="128" spans="1:3" ht="150">
       <c r="A128" s="2">
         <v>42361</v>
       </c>
       <c r="C128" s="20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="270">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="30">
       <c r="A129" s="2">
         <v>42361</v>
       </c>
-      <c r="B129" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C129" s="22" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="30">
+      <c r="C129" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="270">
       <c r="A130" s="2">
         <v>42361</v>
       </c>
-      <c r="B130" s="100" t="s">
-        <v>53</v>
-      </c>
-      <c r="C130" s="20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
+      <c r="B130" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C130" s="22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="30">
       <c r="A131" s="2">
         <v>42361</v>
       </c>
-      <c r="B131" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C131" s="21" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="225">
+      <c r="B131" s="100" t="s">
+        <v>53</v>
+      </c>
+      <c r="C131" s="20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
       <c r="A132" s="2">
         <v>42361</v>
       </c>
       <c r="B132" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="C132" s="22" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="60">
+      <c r="C132" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="225">
       <c r="A133" s="2">
         <v>42361</v>
       </c>
-      <c r="B133" s="100" t="s">
-        <v>49</v>
+      <c r="B133" s="35" t="s">
+        <v>186</v>
       </c>
       <c r="C133" s="22" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="90">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="60">
       <c r="A134" s="2">
         <v>42361</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>196</v>
+      <c r="B134" s="100" t="s">
+        <v>49</v>
       </c>
       <c r="C134" s="22" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="60">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="90">
       <c r="A135" s="2">
         <v>42361</v>
       </c>
-      <c r="B135" s="24" t="s">
+      <c r="B135" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C135" s="24" t="s">
+      <c r="C135" s="22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="60">
+      <c r="A136" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B136" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C136" s="24" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3">
-      <c r="A136" s="40">
-        <v>42360</v>
-      </c>
-      <c r="B136" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="C136" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -5491,187 +5545,189 @@
         <v>195</v>
       </c>
       <c r="C137" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="40">
+        <v>42360</v>
+      </c>
+      <c r="B138" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="C138" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="102.75">
-      <c r="A138" s="80">
+    <row r="139" spans="1:3" ht="102.75">
+      <c r="A139" s="80">
         <v>42360</v>
       </c>
-      <c r="B138" s="78" t="s">
+      <c r="B139" s="78" t="s">
         <v>302</v>
       </c>
-      <c r="C138" s="78" t="s">
+      <c r="C139" s="78" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="30">
-      <c r="A139" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B139" s="100" t="s">
-        <v>43</v>
-      </c>
-      <c r="C139" s="100" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" ht="30">
       <c r="A140" s="2">
         <v>42356</v>
       </c>
-      <c r="B140" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="C140" s="23" t="s">
-        <v>181</v>
+      <c r="B140" s="100" t="s">
+        <v>43</v>
+      </c>
+      <c r="C140" s="100" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="2">
         <v>42356</v>
       </c>
-      <c r="B141" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="C141" s="25" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" ht="30">
+      <c r="B141" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="C141" s="23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
       <c r="A142" s="2">
         <v>42356</v>
       </c>
-      <c r="B142" s="96"/>
+      <c r="B142" s="25" t="s">
+        <v>201</v>
+      </c>
       <c r="C142" s="25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="30">
+      <c r="A143" s="2">
+        <v>42356</v>
+      </c>
+      <c r="B143" s="96"/>
+      <c r="C143" s="25" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="60">
-      <c r="A143" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B143" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="C143" s="26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" ht="60">
       <c r="A144" s="2">
         <v>42355</v>
       </c>
-      <c r="B144" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C144" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="150">
+      <c r="B144" s="96" t="s">
+        <v>91</v>
+      </c>
+      <c r="C144" s="26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
       <c r="A145" s="2">
         <v>42355</v>
       </c>
       <c r="B145" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C145" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="120">
+      <c r="C145" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="150">
       <c r="A146" s="2">
         <v>42355</v>
       </c>
-      <c r="B146" s="100" t="s">
-        <v>168</v>
+      <c r="B146" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="C146" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" ht="30">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="120">
       <c r="A147" s="2">
         <v>42355</v>
       </c>
-      <c r="B147" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C147" s="28" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3">
+      <c r="B147" s="100" t="s">
+        <v>168</v>
+      </c>
+      <c r="C147" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="30">
       <c r="A148" s="2">
         <v>42355</v>
       </c>
-      <c r="B148" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="C148" s="29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" ht="75">
+      <c r="B148" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C148" s="28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
       <c r="A149" s="2">
         <v>42355</v>
       </c>
-      <c r="B149" s="15" t="s">
-        <v>43</v>
+      <c r="B149" s="29" t="s">
+        <v>171</v>
       </c>
       <c r="C149" s="29" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" ht="135">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="75">
       <c r="A150" s="2">
         <v>42355</v>
       </c>
-      <c r="B150" s="100" t="s">
-        <v>173</v>
+      <c r="B150" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="C150" s="29" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="75">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="135">
       <c r="A151" s="2">
         <v>42355</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B151" s="100" t="s">
         <v>173</v>
       </c>
-      <c r="C151" s="42" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="30">
+      <c r="C151" s="29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="75">
       <c r="A152" s="2">
         <v>42355</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C152" s="30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3">
+      <c r="C152" s="42" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="30">
       <c r="A153" s="2">
         <v>42355</v>
       </c>
+      <c r="B153" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="C153" s="30" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="2">
         <v>42355</v>
       </c>
-      <c r="B154" s="42"/>
       <c r="C154" s="30" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -5680,74 +5736,74 @@
       </c>
       <c r="B155" s="42"/>
       <c r="C155" s="30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="2">
+        <v>42355</v>
+      </c>
+      <c r="B156" s="42"/>
+      <c r="C156" s="30" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="75">
-      <c r="A156" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B156" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="C156" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" ht="30">
+    <row r="157" spans="1:3" ht="75">
       <c r="A157" s="2">
         <v>42352</v>
       </c>
-      <c r="B157" s="26"/>
-      <c r="C157" s="31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="75">
+      <c r="B157" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C157" s="30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="30">
       <c r="A158" s="2">
         <v>42352</v>
       </c>
       <c r="B158" s="26"/>
-      <c r="C158" s="70" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3">
+      <c r="C158" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="75">
       <c r="A159" s="2">
         <v>42352</v>
       </c>
       <c r="B159" s="26"/>
-      <c r="C159" s="32" t="s">
-        <v>69</v>
+      <c r="C159" s="70" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="2">
         <v>42352</v>
       </c>
-      <c r="B160" s="96"/>
-      <c r="C160" s="33" t="s">
-        <v>75</v>
+      <c r="B160" s="26"/>
+      <c r="C160" s="32" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="161" spans="1:6">
       <c r="A161" s="2">
         <v>42352</v>
       </c>
-      <c r="B161" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C161" s="34" t="s">
-        <v>72</v>
+      <c r="B161" s="96"/>
+      <c r="C161" s="33" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="162" spans="1:6">
       <c r="A162" s="2">
         <v>42352</v>
       </c>
-      <c r="B162" s="96"/>
+      <c r="B162" s="34" t="s">
+        <v>71</v>
+      </c>
       <c r="C162" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -5755,289 +5811,287 @@
         <v>42352</v>
       </c>
       <c r="B163" s="96"/>
-      <c r="C163" s="37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" ht="30">
+      <c r="C163" s="34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
       <c r="A164" s="2">
         <v>42352</v>
       </c>
-      <c r="B164" s="37"/>
+      <c r="B164" s="96"/>
       <c r="C164" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="30">
       <c r="A165" s="2">
         <v>42352</v>
       </c>
-      <c r="B165" s="96"/>
-      <c r="C165" s="96" t="s">
-        <v>77</v>
-      </c>
-      <c r="F165" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="45">
+      <c r="B165" s="37"/>
+      <c r="C165" s="37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="30">
       <c r="A166" s="2">
         <v>42352</v>
       </c>
-      <c r="B166" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="B166" s="96"/>
       <c r="C166" s="96" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="F166" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="45">
       <c r="A167" s="2">
         <v>42352</v>
       </c>
-      <c r="B167" s="100"/>
-      <c r="C167" s="39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="30">
+      <c r="B167" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C167" s="96" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="45">
       <c r="A168" s="2">
         <v>42352</v>
       </c>
-      <c r="B168" s="38"/>
-      <c r="C168" s="56" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="75">
+      <c r="B168" s="100"/>
+      <c r="C168" s="39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="30">
       <c r="A169" s="2">
         <v>42352</v>
       </c>
-      <c r="B169" s="41"/>
-      <c r="C169" s="41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" ht="45">
+      <c r="B169" s="38"/>
+      <c r="C169" s="56" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="75">
       <c r="A170" s="2">
         <v>42352</v>
       </c>
-      <c r="B170" s="41" t="s">
-        <v>89</v>
-      </c>
+      <c r="B170" s="41"/>
       <c r="C170" s="41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" ht="30">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="45">
       <c r="A171" s="2">
         <v>42352</v>
       </c>
-      <c r="B171" s="43"/>
-      <c r="C171" s="43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" ht="45">
+      <c r="B171" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C171" s="41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="30">
       <c r="A172" s="2">
         <v>42352</v>
       </c>
-      <c r="B172" s="44"/>
-      <c r="C172" s="44" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" ht="30">
+      <c r="B172" s="43"/>
+      <c r="C172" s="43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="45">
       <c r="A173" s="2">
         <v>42352</v>
       </c>
-      <c r="B173" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="C173" s="46" t="s">
-        <v>86</v>
+      <c r="B173" s="44"/>
+      <c r="C173" s="44" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="30">
       <c r="A174" s="2">
         <v>42352</v>
       </c>
-      <c r="B174" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C174" s="47" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6">
+      <c r="B174" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C174" s="46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" ht="30">
       <c r="A175" s="2">
         <v>42352</v>
       </c>
-      <c r="B175" s="100" t="s">
+      <c r="B175" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C175" s="47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B176" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="C175" s="48" t="s">
+      <c r="C176" s="48" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="135">
-      <c r="A176" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B176" s="49"/>
-      <c r="C176" s="49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" ht="60">
+    <row r="177" spans="1:3" ht="135">
       <c r="A177" s="2">
         <v>42349</v>
       </c>
-      <c r="B177" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="C177" s="51" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" ht="30">
+      <c r="B177" s="49"/>
+      <c r="C177" s="49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="60">
       <c r="A178" s="2">
         <v>42349</v>
       </c>
-      <c r="B178" s="96"/>
-      <c r="C178" s="53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="120">
+      <c r="B178" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C178" s="51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="30">
       <c r="A179" s="2">
         <v>42349</v>
       </c>
-      <c r="B179" s="96" t="s">
-        <v>12</v>
-      </c>
+      <c r="B179" s="96"/>
       <c r="C179" s="53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="150">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="120">
       <c r="A180" s="2">
         <v>42349</v>
       </c>
-      <c r="B180" s="52"/>
-      <c r="C180" s="52" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" ht="30">
+      <c r="B180" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C180" s="53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="150">
       <c r="A181" s="2">
         <v>42349</v>
       </c>
-      <c r="B181" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C181" s="54" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3">
+      <c r="B181" s="52"/>
+      <c r="C181" s="52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="30">
       <c r="A182" s="2">
         <v>42349</v>
       </c>
       <c r="B182" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C182" s="55" t="s">
-        <v>61</v>
+      <c r="C182" s="54" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="2">
         <v>42349</v>
       </c>
-      <c r="B183" s="100"/>
-      <c r="C183" s="57" t="s">
-        <v>78</v>
+      <c r="B183" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C183" s="55" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="2">
         <v>42349</v>
       </c>
-      <c r="B184" s="58"/>
-      <c r="C184" s="58" t="s">
-        <v>62</v>
+      <c r="B184" s="100"/>
+      <c r="C184" s="57" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="2">
         <v>42349</v>
       </c>
-      <c r="B185" s="59"/>
-      <c r="C185" s="59" t="s">
-        <v>70</v>
+      <c r="B185" s="58"/>
+      <c r="C185" s="58" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="2">
         <v>42349</v>
       </c>
-      <c r="B186" s="60"/>
-      <c r="C186" s="60" t="s">
-        <v>64</v>
+      <c r="B186" s="59"/>
+      <c r="C186" s="59" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="2">
         <v>42349</v>
       </c>
-      <c r="B187" s="61"/>
-      <c r="C187" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" ht="60">
+      <c r="B187" s="60"/>
+      <c r="C187" s="60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
       <c r="A188" s="2">
         <v>42349</v>
       </c>
-      <c r="B188" s="62" t="s">
+      <c r="B188" s="61"/>
+      <c r="C188" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="60">
+      <c r="A189" s="2">
+        <v>42349</v>
+      </c>
+      <c r="B189" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="C188" s="100" t="s">
+      <c r="C189" s="100" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="90">
-      <c r="A189" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B189" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C189" s="62" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" ht="30">
+    <row r="190" spans="1:3" ht="90">
       <c r="A190" s="2">
         <v>42345</v>
       </c>
-      <c r="B190" s="1" t="s">
+      <c r="B190" s="62" t="s">
         <v>12</v>
       </c>
       <c r="C190" s="62" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="30">
       <c r="A191" s="2">
         <v>42345</v>
       </c>
-      <c r="B191" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C191" s="63" t="s">
-        <v>28</v>
+      <c r="B191" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C191" s="62" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -6047,162 +6101,162 @@
       <c r="B192" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C192" s="64" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="30">
+      <c r="C192" s="63" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
       <c r="A193" s="2">
         <v>42345</v>
       </c>
       <c r="B193" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C193" s="65" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="195">
+      <c r="C193" s="64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" ht="30">
       <c r="A194" s="2">
         <v>42345</v>
       </c>
-      <c r="B194" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C194" s="66" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="135">
+      <c r="B194" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C194" s="65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="195">
       <c r="A195" s="2">
         <v>42345</v>
       </c>
-      <c r="B195" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="C195" s="67" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" ht="75">
+      <c r="B195" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C195" s="66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="135">
       <c r="A196" s="2">
         <v>42345</v>
       </c>
-      <c r="B196" s="69" t="s">
+      <c r="B196" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="C196" s="68" t="s">
-        <v>32</v>
+      <c r="C196" s="67" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="75">
       <c r="A197" s="2">
         <v>42345</v>
       </c>
-      <c r="B197" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C197" s="69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" ht="30">
+      <c r="B197" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C197" s="68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="75">
       <c r="A198" s="2">
         <v>42345</v>
       </c>
-      <c r="B198" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C198" s="73" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3">
+      <c r="B198" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C198" s="69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="30">
       <c r="A199" s="2">
         <v>42345</v>
       </c>
-      <c r="B199" s="71" t="s">
-        <v>39</v>
+      <c r="B199" s="100" t="s">
+        <v>12</v>
       </c>
       <c r="C199" s="73" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="2">
         <v>42345</v>
       </c>
-      <c r="B200" s="72" t="s">
+      <c r="B200" s="71" t="s">
         <v>39</v>
       </c>
       <c r="C200" s="73" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" ht="60">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
       <c r="A201" s="2">
         <v>42345</v>
       </c>
-      <c r="B201" s="96" t="s">
+      <c r="B201" s="72" t="s">
         <v>39</v>
       </c>
       <c r="C201" s="73" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="150">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="60">
       <c r="A202" s="2">
         <v>42345</v>
       </c>
-      <c r="B202" s="15" t="s">
-        <v>43</v>
+      <c r="B202" s="96" t="s">
+        <v>39</v>
       </c>
       <c r="C202" s="73" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="150">
       <c r="A203" s="2">
         <v>42345</v>
       </c>
-      <c r="B203" s="100" t="s">
-        <v>39</v>
-      </c>
-      <c r="C203" s="76" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="60">
+      <c r="B203" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C203" s="73" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="45">
       <c r="A204" s="2">
         <v>42345</v>
       </c>
-      <c r="B204" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C204" s="77" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" ht="105">
+      <c r="B204" s="100" t="s">
+        <v>39</v>
+      </c>
+      <c r="C204" s="76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="60">
       <c r="A205" s="2">
         <v>42345</v>
       </c>
-      <c r="B205" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3">
+      <c r="B205" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C205" s="77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="105">
       <c r="A206" s="2">
         <v>42345</v>
       </c>
-      <c r="B206" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C206" s="96" t="s">
-        <v>50</v>
+      <c r="B206" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -6213,10 +6267,10 @@
         <v>49</v>
       </c>
       <c r="C207" s="96" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="75">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
       <c r="A208" s="2">
         <v>42345</v>
       </c>
@@ -6224,54 +6278,54 @@
         <v>49</v>
       </c>
       <c r="C208" s="96" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="75">
       <c r="A209" s="2">
         <v>42345</v>
       </c>
       <c r="B209" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C209" s="96" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" ht="45">
+      <c r="A210" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B210" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C209" s="96" t="s">
+      <c r="C210" s="96" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="141">
-      <c r="A210" s="80">
+    <row r="211" spans="1:3" ht="141">
+      <c r="A211" s="80">
         <v>42345</v>
       </c>
-      <c r="B210" s="78" t="s">
+      <c r="B211" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="C210" s="78" t="s">
+      <c r="C211" s="78" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="105">
-      <c r="A211" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B211" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C211" s="100" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" ht="90">
+    <row r="212" spans="1:3" ht="105">
       <c r="A212" s="2">
         <v>42341</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C212" s="96" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" ht="75">
+        <v>12</v>
+      </c>
+      <c r="C212" s="100" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="90">
       <c r="A213" s="2">
         <v>42341</v>
       </c>
@@ -6279,10 +6333,10 @@
         <v>15</v>
       </c>
       <c r="C213" s="96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" ht="75">
       <c r="A214" s="2">
         <v>42341</v>
       </c>
@@ -6290,7 +6344,7 @@
         <v>15</v>
       </c>
       <c r="C214" s="96" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="30">
@@ -6301,10 +6355,10 @@
         <v>15</v>
       </c>
       <c r="C215" s="96" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" ht="45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="30">
       <c r="A216" s="2">
         <v>42341</v>
       </c>
@@ -6312,32 +6366,32 @@
         <v>15</v>
       </c>
       <c r="C216" s="96" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" ht="90">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" ht="45">
       <c r="A217" s="2">
         <v>42341</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C217" s="96" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="90">
       <c r="A218" s="2">
         <v>42341</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C218" s="96" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" ht="150">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="30">
       <c r="A219" s="2">
         <v>42341</v>
       </c>
@@ -6345,10 +6399,10 @@
         <v>15</v>
       </c>
       <c r="C219" s="96" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" ht="75">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" ht="150">
       <c r="A220" s="2">
         <v>42341</v>
       </c>
@@ -6356,40 +6410,40 @@
         <v>15</v>
       </c>
       <c r="C220" s="96" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" ht="90">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" ht="75">
       <c r="A221" s="2">
         <v>42341</v>
       </c>
-      <c r="B221" s="100" t="s">
-        <v>12</v>
+      <c r="B221" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C221" s="96" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" ht="90">
       <c r="A222" s="2">
         <v>42341</v>
       </c>
-      <c r="B222" s="96" t="s">
-        <v>15</v>
+      <c r="B222" s="100" t="s">
+        <v>12</v>
       </c>
       <c r="C222" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" ht="60">
       <c r="A223" s="2">
         <v>42341</v>
       </c>
       <c r="B223" s="96" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C223" s="96" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -6397,10 +6451,10 @@
         <v>42341</v>
       </c>
       <c r="B224" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C224" s="7" t="s">
-        <v>34</v>
+        <v>12</v>
+      </c>
+      <c r="C224" s="96" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -6411,7 +6465,7 @@
         <v>15</v>
       </c>
       <c r="C225" s="7" t="s">
-        <v>166</v>
+        <v>34</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -6421,8 +6475,8 @@
       <c r="B226" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C226" s="8" t="s">
-        <v>165</v>
+      <c r="C226" s="7" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -6433,67 +6487,69 @@
         <v>15</v>
       </c>
       <c r="C227" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" ht="75">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
       <c r="A228" s="2">
         <v>42341</v>
       </c>
       <c r="B228" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C228" s="100" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" ht="60">
+      <c r="C228" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="75">
       <c r="A229" s="2">
         <v>42341</v>
       </c>
       <c r="B229" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C229" s="96" t="s">
-        <v>26</v>
+        <v>15</v>
+      </c>
+      <c r="C229" s="100" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="60">
       <c r="A230" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B230" s="96"/>
+        <v>42341</v>
+      </c>
+      <c r="B230" s="96" t="s">
+        <v>12</v>
+      </c>
       <c r="C230" s="96" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" ht="45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" ht="60">
       <c r="A231" s="2">
         <v>42340</v>
       </c>
       <c r="B231" s="96"/>
       <c r="C231" s="96" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" ht="60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" ht="45">
       <c r="A232" s="2">
         <v>42340</v>
       </c>
-      <c r="B232" s="2" t="s">
+      <c r="B232" s="96"/>
+      <c r="C232" s="96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" ht="60">
+      <c r="A233" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B233" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C232" s="96" t="s">
+      <c r="C233" s="96" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3">
-      <c r="A233" s="2">
-        <v>42339</v>
-      </c>
-      <c r="B233" s="2"/>
-      <c r="C233" s="96" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -6502,131 +6558,129 @@
       </c>
       <c r="B234" s="2"/>
       <c r="C234" s="96" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" s="2">
+        <v>42339</v>
+      </c>
+      <c r="B235" s="2"/>
+      <c r="C235" s="96" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:3" ht="64.5">
-      <c r="A235" s="80">
-        <v>42334</v>
-      </c>
-      <c r="B235" s="78" t="s">
-        <v>309</v>
-      </c>
-      <c r="C235" s="78" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" ht="26.25">
+    <row r="236" spans="1:3" ht="64.5">
       <c r="A236" s="80">
         <v>42334</v>
       </c>
       <c r="B236" s="78" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C236" s="78" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" ht="39">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" ht="26.25">
       <c r="A237" s="80">
         <v>42334</v>
       </c>
       <c r="B237" s="78" t="s">
+        <v>307</v>
+      </c>
+      <c r="C237" s="78" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" ht="39">
+      <c r="A238" s="80">
+        <v>42334</v>
+      </c>
+      <c r="B238" s="78" t="s">
         <v>272</v>
       </c>
-      <c r="C237" s="78" t="s">
+      <c r="C238" s="78" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="238" spans="1:3" ht="128.25">
-      <c r="A238" s="80">
-        <v>42333</v>
-      </c>
-      <c r="B238" s="78" t="s">
-        <v>268</v>
-      </c>
-      <c r="C238" s="78" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" ht="51.75">
+    <row r="239" spans="1:3" ht="128.25">
       <c r="A239" s="80">
         <v>42333</v>
       </c>
       <c r="B239" s="78" t="s">
+        <v>268</v>
+      </c>
+      <c r="C239" s="78" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" ht="51.75">
+      <c r="A240" s="80">
+        <v>42333</v>
+      </c>
+      <c r="B240" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C239" s="78" t="s">
+      <c r="C240" s="78" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="26.25">
-      <c r="A240" s="80">
+    <row r="241" spans="1:3" ht="26.25">
+      <c r="A241" s="80">
         <v>42331</v>
       </c>
-      <c r="B240" s="78" t="s">
+      <c r="B241" s="78" t="s">
         <v>313</v>
       </c>
-      <c r="C240" s="78" t="s">
+      <c r="C241" s="78" t="s">
         <v>312</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" ht="39">
-      <c r="A241" s="80">
-        <v>42329</v>
-      </c>
-      <c r="B241" s="78" t="s">
-        <v>315</v>
-      </c>
-      <c r="C241" s="78" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="242" spans="1:3" ht="39">
       <c r="A242" s="80">
-        <v>42328</v>
+        <v>42329</v>
       </c>
       <c r="B242" s="78" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="C242" s="78" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" ht="26.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" ht="39">
       <c r="A243" s="80">
         <v>42328</v>
       </c>
       <c r="B243" s="78" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C243" s="78" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" ht="115.5">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" ht="26.25">
       <c r="A244" s="80">
         <v>42328</v>
       </c>
       <c r="B244" s="78" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C244" s="78" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" ht="90">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" ht="115.5">
       <c r="A245" s="80">
         <v>42328</v>
       </c>
       <c r="B245" s="78" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C245" s="78" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" ht="153.75">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" ht="90">
       <c r="A246" s="80">
         <v>42328</v>
       </c>
@@ -6634,32 +6688,32 @@
         <v>317</v>
       </c>
       <c r="C246" s="78" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" ht="153.75">
+      <c r="A247" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B247" s="78" t="s">
+        <v>317</v>
+      </c>
+      <c r="C247" s="78" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="102.75">
-      <c r="A247" s="80">
+    <row r="248" spans="1:3" ht="102.75">
+      <c r="A248" s="80">
         <v>42324</v>
       </c>
-      <c r="B247" s="78" t="s">
+      <c r="B248" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="C247" s="78" t="s">
+      <c r="C248" s="78" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="90">
-      <c r="A248" s="80">
-        <v>42321</v>
-      </c>
-      <c r="B248" s="78" t="s">
-        <v>327</v>
-      </c>
-      <c r="C248" s="78" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" ht="26.25">
+    <row r="249" spans="1:3" ht="90">
       <c r="A249" s="80">
         <v>42321</v>
       </c>
@@ -6667,72 +6721,83 @@
         <v>327</v>
       </c>
       <c r="C249" s="78" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" ht="26.25">
+      <c r="A250" s="80">
+        <v>42321</v>
+      </c>
+      <c r="B250" s="78" t="s">
+        <v>327</v>
+      </c>
+      <c r="C250" s="78" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="77.25">
-      <c r="A250" s="79">
+    <row r="251" spans="1:3" ht="77.25">
+      <c r="A251" s="79">
         <v>42318</v>
       </c>
-      <c r="B250" s="78" t="s">
+      <c r="B251" s="78" t="s">
         <v>330</v>
       </c>
-      <c r="C250" s="78" t="s">
+      <c r="C251" s="78" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="115.5">
-      <c r="A251" s="79">
+    <row r="252" spans="1:3" ht="115.5">
+      <c r="A252" s="79">
         <v>42311</v>
-      </c>
-      <c r="B251" s="78" t="s">
-        <v>216</v>
-      </c>
-      <c r="C251" s="78" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" ht="77.25">
-      <c r="A252" s="79">
-        <v>42310</v>
       </c>
       <c r="B252" s="78" t="s">
         <v>216</v>
       </c>
       <c r="C252" s="78" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" ht="77.25">
+      <c r="A253" s="79">
+        <v>42310</v>
+      </c>
+      <c r="B253" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="C253" s="78" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="253" spans="1:3" ht="51.75">
-      <c r="A253" s="79">
+    <row r="254" spans="1:3" ht="51.75">
+      <c r="A254" s="79">
         <v>42306</v>
       </c>
-      <c r="B253" s="78" t="s">
+      <c r="B254" s="78" t="s">
         <v>333</v>
       </c>
-      <c r="C253" s="78" t="s">
+      <c r="C254" s="78" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="254" spans="1:3">
-      <c r="A254" s="100"/>
-      <c r="B254" s="100"/>
-      <c r="C254" s="100"/>
+    <row r="255" spans="1:3">
+      <c r="A255" s="100"/>
+      <c r="B255" s="100"/>
+      <c r="C255" s="100"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C254">
+  <autoFilter ref="A1:C255">
     <sortState ref="A2:C201">
       <sortCondition descending="1" ref="A1:A201"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C226" r:id="rId1"/>
-    <hyperlink ref="C187" r:id="rId2"/>
-    <hyperlink ref="C227" r:id="rId3"/>
-    <hyperlink ref="C61" r:id="rId4"/>
-    <hyperlink ref="C46" r:id="rId5"/>
-    <hyperlink ref="C43" r:id="rId6"/>
+    <hyperlink ref="C227" r:id="rId1"/>
+    <hyperlink ref="C188" r:id="rId2"/>
+    <hyperlink ref="C228" r:id="rId3"/>
+    <hyperlink ref="C62" r:id="rId4"/>
+    <hyperlink ref="C47" r:id="rId5"/>
+    <hyperlink ref="C44" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -6752,16 +6817,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="60.75" customHeight="1">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="135" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add new entries to index:
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -15,14 +15,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'AS400 Version'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$255</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$C$262</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="591">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -2902,9 +2902,6 @@
 今天早上改變方向, 從目標"Easy &amp; quick to add-new/ change feature" 出發, 是一個更好的思路, 由此發散出的規定(LAW)也更貼近現實. 下午繼續改卻發現還是有點離地, 因此再將LAW簡化, 且對AS400 RPG PGMMING原有的特性進行量身訂做, 並OUTPUT了一些LAW, 感覺這就是我需要的東西.</t>
   </si>
   <si>
-    <t>BANG!</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">When I am searching for jt400 programcall class example, I come across this AWESOME website:
 </t>
@@ -2930,6 +2927,76 @@
       <t xml:space="preserve">
 This is mind-blowing. Awesome!</t>
     </r>
+  </si>
+  <si>
+    <t>Java API example</t>
+  </si>
+  <si>
+    <t>Thinking about Framework</t>
+  </si>
+  <si>
+    <t>IBM Watsons</t>
+  </si>
+  <si>
+    <t>IBM Bluemix</t>
+  </si>
+  <si>
+    <t>Google VR</t>
+  </si>
+  <si>
+    <t>Google Firebase</t>
+  </si>
+  <si>
+    <t>Bluemix is a cloud platform for developer to run their application. The application can be webapp, mobile backend, web-service etc. Bluemix is more automated and dominated than VPS(virtual private server) so that it can provide its unique characteristic to users.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBM Watson is the lab that provides </t>
+  </si>
+  <si>
+    <t>Framework is the basic model of governence? Framework must have a manager(or equivalent role)?</t>
+  </si>
+  <si>
+    <t>A demo/example of google vr sdk is Treasure Hurt(can visit on github). The manifest xml should add intent-filter, landscape mandation etc. And MainActivity should inherit GVRActivity and implement StereoRenderer so that developer use ability gained from GVRActivity to fulfill StereoRenderer's abstract method to define application behavior (onDrawEye method and etc).</t>
+  </si>
+  <si>
+    <t>面向對像的內核是:
+* 實現臣服於邏輯 (缺點是不務實, 優點是可以最大限度重用)</t>
+  </si>
+  <si>
+    <t>Object Oriented</t>
+  </si>
+  <si>
+    <t>Firebase is a cloud platform that provide different aspect of functionality including:
+* Mobile-app testing tool: help developer to mock different machine version of user to the app
+* Online-database: allow developer to get/set value to the database easily
+* Firebase Cloud Messaging (FCM): listen on the state change of a certain value from the database so that when it changed
+* AdMob: advertisement for mobile</t>
+  </si>
+  <si>
+    <t>Android Transition Framework</t>
+  </si>
+  <si>
+    <t>Google Codelabs</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Google Codelabs provides different tutorials for google products like Android, Web, Firebase, Wear and many others.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF152BFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://codelabs.developers.google.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>2016年最值得學習的五大Android開源項目- 項目1:
+Easy to use, action and presentation seperated design, manager handle the implementation.</t>
   </si>
 </sst>
 </file>
@@ -3131,7 +3198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3204,12 +3271,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -3277,7 +3338,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3678,7 +3739,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3723,13 +3793,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4202207</xdr:colOff>
-      <xdr:row>142</xdr:row>
+      <xdr:row>149</xdr:row>
       <xdr:rowOff>593914</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>257735</xdr:colOff>
-      <xdr:row>146</xdr:row>
+      <xdr:row>153</xdr:row>
       <xdr:rowOff>102263</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4046,10 +4116,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F255"/>
+  <dimension ref="A1:F262"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4060,7 +4130,7 @@
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1">
+    <row r="1" spans="1:3" s="4" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -4071,2338 +4141,2344 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="102" customFormat="1">
+    <row r="2" spans="1:3" s="102" customFormat="1">
       <c r="A2" s="100"/>
       <c r="B2" s="100"/>
       <c r="C2" s="100"/>
     </row>
-    <row r="3" spans="1:4" s="102" customFormat="1">
-      <c r="A3" s="131"/>
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
-    </row>
-    <row r="4" spans="1:4" s="102" customFormat="1" ht="60">
+    <row r="3" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A3" s="121">
+        <v>42682</v>
+      </c>
+      <c r="B3" s="138" t="s">
+        <v>588</v>
+      </c>
+      <c r="C3" s="138" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="102" customFormat="1" ht="45">
       <c r="A4" s="121">
+        <v>42682</v>
+      </c>
+      <c r="B4" s="138" t="s">
+        <v>587</v>
+      </c>
+      <c r="C4" s="138" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A5" s="121">
+        <v>42682</v>
+      </c>
+      <c r="B5" s="136" t="s">
+        <v>585</v>
+      </c>
+      <c r="C5" s="136" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A6" s="121">
+        <v>42681</v>
+      </c>
+      <c r="B6" s="136" t="s">
+        <v>579</v>
+      </c>
+      <c r="C6" s="138" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="102" customFormat="1" ht="75">
+      <c r="A7" s="121">
+        <v>42681</v>
+      </c>
+      <c r="B7" s="135" t="s">
+        <v>578</v>
+      </c>
+      <c r="C7" s="135" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="102" customFormat="1">
+      <c r="A8" s="121">
+        <v>42681</v>
+      </c>
+      <c r="B8" s="135" t="s">
+        <v>576</v>
+      </c>
+      <c r="C8" s="135" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A9" s="121">
+        <v>42681</v>
+      </c>
+      <c r="B9" s="135" t="s">
+        <v>577</v>
+      </c>
+      <c r="C9" s="135" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A10" s="121">
+        <v>42681</v>
+      </c>
+      <c r="B10" s="135" t="s">
+        <v>575</v>
+      </c>
+      <c r="C10" s="136" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A11" s="121">
         <v>42642</v>
       </c>
-      <c r="B4" s="136" t="s">
+      <c r="B11" s="137" t="s">
+        <v>574</v>
+      </c>
+      <c r="C11" s="134" t="s">
         <v>573</v>
       </c>
-      <c r="C4" s="134" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="102" customFormat="1" ht="120">
-      <c r="A5" s="121">
+    </row>
+    <row r="12" spans="1:3" s="102" customFormat="1" ht="120">
+      <c r="A12" s="121">
         <v>42614</v>
       </c>
-      <c r="B5" s="133" t="s">
+      <c r="B12" s="133" t="s">
         <v>571</v>
       </c>
-      <c r="C5" s="133" t="s">
+      <c r="C12" s="136" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="102" customFormat="1" ht="120">
-      <c r="A6" s="121">
+    <row r="13" spans="1:3" s="102" customFormat="1" ht="120">
+      <c r="A13" s="121">
         <v>42613</v>
       </c>
-      <c r="B6" s="131" t="s">
+      <c r="B13" s="131" t="s">
         <v>569</v>
       </c>
-      <c r="C6" s="131" t="s">
+      <c r="C13" s="131" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="102" customFormat="1" ht="30">
-      <c r="A7" s="121">
+    <row r="14" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A14" s="121">
         <v>42613</v>
       </c>
-      <c r="B7" s="131" t="s">
+      <c r="B14" s="131" t="s">
         <v>563</v>
       </c>
-      <c r="C7" s="131" t="s">
+      <c r="C14" s="131" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="102" customFormat="1" ht="75">
-      <c r="A8" s="121">
+    <row r="15" spans="1:3" s="102" customFormat="1" ht="75">
+      <c r="A15" s="121">
         <v>42613</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B15" s="131" t="s">
         <v>565</v>
       </c>
-      <c r="C8" s="131" t="s">
+      <c r="C15" s="131" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="121" customFormat="1" ht="45">
-      <c r="A9" s="121">
+    <row r="16" spans="1:3" s="121" customFormat="1" ht="45">
+      <c r="A16" s="121">
         <v>42613</v>
       </c>
-      <c r="B9" s="121" t="s">
+      <c r="B16" s="121" t="s">
         <v>567</v>
       </c>
-      <c r="C9" s="131" t="s">
+      <c r="C16" s="131" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="102" customFormat="1" ht="30">
-      <c r="A10" s="121">
+    <row r="17" spans="1:4" s="102" customFormat="1" ht="30">
+      <c r="A17" s="121">
         <v>42571</v>
       </c>
-      <c r="B10" s="131" t="s">
+      <c r="B17" s="131" t="s">
         <v>562</v>
       </c>
-      <c r="C10" s="130" t="s">
+      <c r="C17" s="130" t="s">
         <v>561</v>
       </c>
-      <c r="D10" s="132" t="s">
+      <c r="D17" s="132" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="102" customFormat="1" ht="75">
-      <c r="A11" s="121">
+    <row r="18" spans="1:4" s="102" customFormat="1" ht="75">
+      <c r="A18" s="121">
         <v>42570</v>
       </c>
-      <c r="B11" s="128" t="s">
+      <c r="B18" s="128" t="s">
         <v>558</v>
       </c>
-      <c r="C11" s="129" t="s">
+      <c r="C18" s="129" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="102" customFormat="1" ht="75">
-      <c r="A12" s="121">
+    <row r="19" spans="1:4" s="102" customFormat="1" ht="75">
+      <c r="A19" s="121">
         <v>42570</v>
       </c>
-      <c r="B12" s="127" t="s">
+      <c r="B19" s="127" t="s">
         <v>551</v>
       </c>
-      <c r="C12" s="127" t="s">
+      <c r="C19" s="127" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="102" customFormat="1" ht="45">
-      <c r="A13" s="121">
+    <row r="20" spans="1:4" s="102" customFormat="1" ht="45">
+      <c r="A20" s="121">
         <v>42569</v>
       </c>
-      <c r="B13" s="126" t="s">
+      <c r="B20" s="126" t="s">
         <v>554</v>
       </c>
-      <c r="C13" s="126" t="s">
+      <c r="C20" s="126" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="102" customFormat="1" ht="90">
-      <c r="A14" s="121">
+    <row r="21" spans="1:4" s="102" customFormat="1" ht="90">
+      <c r="A21" s="121">
         <v>42569</v>
       </c>
-      <c r="B14" s="125" t="s">
+      <c r="B21" s="125" t="s">
         <v>551</v>
       </c>
-      <c r="C14" s="127" t="s">
+      <c r="C21" s="127" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="102" customFormat="1" ht="45">
-      <c r="A15" s="121">
+    <row r="22" spans="1:4" s="102" customFormat="1" ht="45">
+      <c r="A22" s="121">
         <v>42569</v>
       </c>
-      <c r="B15" s="125" t="s">
+      <c r="B22" s="125" t="s">
         <v>550</v>
       </c>
-      <c r="C15" s="125" t="s">
+      <c r="C22" s="125" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="102" customFormat="1" ht="30">
-      <c r="A16" s="121">
+    <row r="23" spans="1:4" s="102" customFormat="1" ht="30">
+      <c r="A23" s="121">
         <v>42569</v>
       </c>
-      <c r="B16" s="125" t="s">
+      <c r="B23" s="125" t="s">
         <v>549</v>
       </c>
-      <c r="C16" s="125" t="s">
+      <c r="C23" s="125" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A17" s="121">
+    <row r="24" spans="1:4" s="102" customFormat="1" ht="90">
+      <c r="A24" s="121">
         <v>42567</v>
       </c>
-      <c r="B17" s="124" t="s">
+      <c r="B24" s="124" t="s">
         <v>548</v>
       </c>
-      <c r="C17" s="124" t="s">
+      <c r="C24" s="124" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A18" s="121">
+    <row r="25" spans="1:4" s="102" customFormat="1" ht="45">
+      <c r="A25" s="121">
         <v>42567</v>
       </c>
-      <c r="B18" s="124" t="s">
+      <c r="B25" s="124" t="s">
         <v>546</v>
       </c>
-      <c r="C18" s="124" t="s">
+      <c r="C25" s="124" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A19" s="121">
+    <row r="26" spans="1:4" s="102" customFormat="1" ht="60">
+      <c r="A26" s="121">
         <v>42565</v>
       </c>
-      <c r="B19" s="123" t="s">
+      <c r="B26" s="123" t="s">
         <v>543</v>
       </c>
-      <c r="C19" s="123" t="s">
+      <c r="C26" s="123" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="102" customFormat="1" ht="75">
-      <c r="A20" s="121">
+    <row r="27" spans="1:4" s="102" customFormat="1" ht="75">
+      <c r="A27" s="121">
         <v>42564</v>
       </c>
-      <c r="B20" s="122" t="s">
+      <c r="B27" s="122" t="s">
         <v>534</v>
       </c>
-      <c r="C20" s="122" t="s">
+      <c r="C27" s="122" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="102" customFormat="1" ht="135">
-      <c r="A21" s="121">
+    <row r="28" spans="1:4" s="102" customFormat="1" ht="135">
+      <c r="A28" s="121">
         <v>42562</v>
       </c>
-      <c r="B21" s="120" t="s">
+      <c r="B28" s="120" t="s">
         <v>537</v>
       </c>
-      <c r="C21" s="120" t="s">
+      <c r="C28" s="120" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A22" s="121">
+    <row r="29" spans="1:4" s="102" customFormat="1" ht="60">
+      <c r="A29" s="121">
         <v>42562</v>
       </c>
-      <c r="B22" s="120" t="s">
+      <c r="B29" s="120" t="s">
         <v>536</v>
       </c>
-      <c r="C22" s="120" t="s">
+      <c r="C29" s="120" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="102" customFormat="1" ht="75">
-      <c r="A23" s="121">
+    <row r="30" spans="1:4" s="102" customFormat="1" ht="75">
+      <c r="A30" s="121">
         <v>42562</v>
       </c>
-      <c r="B23" s="120" t="s">
+      <c r="B30" s="120" t="s">
         <v>535</v>
       </c>
-      <c r="C23" s="120" t="s">
+      <c r="C30" s="120" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="102" customFormat="1" ht="165">
-      <c r="A24" s="121">
+    <row r="31" spans="1:4" s="102" customFormat="1" ht="165">
+      <c r="A31" s="121">
         <v>42562</v>
       </c>
-      <c r="B24" s="120" t="s">
+      <c r="B31" s="120" t="s">
         <v>534</v>
       </c>
-      <c r="C24" s="120" t="s">
+      <c r="C31" s="120" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A25" s="121">
+    <row r="32" spans="1:4" s="102" customFormat="1" ht="30">
+      <c r="A32" s="121">
         <v>42557</v>
       </c>
-      <c r="B25" s="120" t="s">
+      <c r="B32" s="120" t="s">
         <v>525</v>
       </c>
-      <c r="C25" s="120" t="s">
+      <c r="C32" s="120" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="102" customFormat="1" ht="180">
-      <c r="A26" s="120"/>
-      <c r="B26" s="120" t="s">
+    <row r="33" spans="1:3" s="102" customFormat="1" ht="180">
+      <c r="A33" s="120"/>
+      <c r="B33" s="120" t="s">
         <v>527</v>
       </c>
-      <c r="C26" s="120" t="s">
+      <c r="C33" s="120" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A27" s="121">
+    <row r="34" spans="1:3" s="102" customFormat="1" ht="150">
+      <c r="A34" s="121">
         <v>42540</v>
       </c>
-      <c r="B27" s="120" t="s">
+      <c r="B34" s="120" t="s">
         <v>529</v>
       </c>
-      <c r="C27" s="120" t="s">
+      <c r="C34" s="120" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="102" customFormat="1" ht="180">
-      <c r="A28" s="121">
+    <row r="35" spans="1:3" s="102" customFormat="1" ht="180">
+      <c r="A35" s="121">
         <v>42539</v>
       </c>
-      <c r="B28" s="120" t="s">
+      <c r="B35" s="120" t="s">
         <v>527</v>
       </c>
-      <c r="C28" s="120" t="s">
+      <c r="C35" s="120" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A29" s="121">
+    <row r="36" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A36" s="121">
         <v>42539</v>
       </c>
-      <c r="B29" s="120" t="s">
+      <c r="B36" s="120" t="s">
         <v>532</v>
       </c>
-      <c r="C29" s="120" t="s">
+      <c r="C36" s="120" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A30" s="2">
+    <row r="37" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A37" s="2">
         <v>42534</v>
       </c>
-      <c r="B30" s="119" t="s">
+      <c r="B37" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="119" t="s">
+      <c r="C37" s="119" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A31" s="2">
+    <row r="38" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A38" s="2">
         <v>42517</v>
       </c>
-      <c r="B31" s="118" t="s">
+      <c r="B38" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="118" t="s">
+      <c r="C38" s="118" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A32" s="2">
+    <row r="39" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A39" s="2">
         <v>42514</v>
       </c>
-      <c r="B32" s="117" t="s">
+      <c r="B39" s="117" t="s">
         <v>519</v>
       </c>
-      <c r="C32" s="117" t="s">
+      <c r="C39" s="117" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A33" s="2">
+    <row r="40" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A40" s="2">
         <v>42507</v>
       </c>
-      <c r="B33" s="116" t="s">
+      <c r="B40" s="116" t="s">
         <v>519</v>
       </c>
-      <c r="C33" s="116" t="s">
+      <c r="C40" s="116" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="102" customFormat="1" ht="60">
-      <c r="A34" s="2">
+    <row r="41" spans="1:3" s="102" customFormat="1" ht="60">
+      <c r="A41" s="2">
         <v>42502</v>
       </c>
-      <c r="B34" s="115" t="s">
+      <c r="B41" s="115" t="s">
         <v>519</v>
       </c>
-      <c r="C34" s="116" t="s">
+      <c r="C41" s="116" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A35" s="2">
+    <row r="42" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="A42" s="2">
         <v>42485</v>
       </c>
-      <c r="B35" s="113" t="s">
+      <c r="B42" s="113" t="s">
         <v>516</v>
       </c>
-      <c r="C35" s="113" t="s">
+      <c r="C42" s="113" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A36" s="2">
+    <row r="43" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A43" s="2">
         <v>42485</v>
       </c>
-      <c r="B36" s="110" t="s">
+      <c r="B43" s="110" t="s">
         <v>514</v>
       </c>
-      <c r="C36" s="110" t="s">
+      <c r="C43" s="110" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="102" customFormat="1" ht="300">
-      <c r="A37" s="2">
+    <row r="44" spans="1:3" s="102" customFormat="1" ht="300">
+      <c r="A44" s="2">
         <v>42485</v>
       </c>
-      <c r="B37" s="112" t="s">
+      <c r="B44" s="112" t="s">
         <v>241</v>
       </c>
-      <c r="C37" s="112" t="s">
+      <c r="C44" s="112" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A38" s="2">
+    <row r="45" spans="1:3" s="102" customFormat="1" ht="150">
+      <c r="A45" s="2">
         <v>42479</v>
       </c>
-      <c r="B38" s="111" t="s">
+      <c r="B45" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="C38" s="111" t="s">
+      <c r="C45" s="111" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A39" s="2">
+    <row r="46" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="A46" s="2">
         <v>42478</v>
       </c>
-      <c r="B39" s="110" t="s">
+      <c r="B46" s="110" t="s">
         <v>509</v>
       </c>
-      <c r="C39" s="110" t="s">
+      <c r="C46" s="110" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="102" customFormat="1" ht="120">
-      <c r="A40" s="2">
+    <row r="47" spans="1:3" s="102" customFormat="1" ht="120">
+      <c r="A47" s="2">
         <v>42477</v>
       </c>
-      <c r="B40" s="109" t="s">
+      <c r="B47" s="109" t="s">
         <v>509</v>
       </c>
-      <c r="C40" s="109" t="s">
+      <c r="C47" s="109" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A41" s="2">
+    <row r="48" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A48" s="2">
         <v>42477</v>
       </c>
-      <c r="B41" s="108" t="s">
+      <c r="B48" s="108" t="s">
         <v>507</v>
       </c>
-      <c r="C41" s="108" t="s">
+      <c r="C48" s="108" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="102" customFormat="1">
-      <c r="A42" s="2">
+    <row r="49" spans="1:3" s="102" customFormat="1">
+      <c r="A49" s="2">
         <v>42473</v>
       </c>
-      <c r="B42" s="106" t="s">
+      <c r="B49" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="106" t="s">
+      <c r="C49" s="106" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="102" customFormat="1" ht="45">
-      <c r="A43" s="2">
+    <row r="50" spans="1:3" s="102" customFormat="1" ht="45">
+      <c r="A50" s="2">
         <v>42473</v>
       </c>
-      <c r="B43" s="106" t="s">
+      <c r="B50" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="107" t="s">
+      <c r="C50" s="107" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="102" customFormat="1">
-      <c r="A44" s="2">
+    <row r="51" spans="1:3" s="102" customFormat="1">
+      <c r="A51" s="2">
         <v>42469</v>
       </c>
-      <c r="B44" s="105" t="s">
+      <c r="B51" s="105" t="s">
         <v>504</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C51" s="8" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="102" customFormat="1" ht="75">
-      <c r="A45" s="2">
+    <row r="52" spans="1:3" s="102" customFormat="1" ht="75">
+      <c r="A52" s="2">
         <v>42463</v>
       </c>
-      <c r="B45" s="104" t="s">
+      <c r="B52" s="104" t="s">
         <v>497</v>
       </c>
-      <c r="C45" s="104" t="s">
+      <c r="C52" s="104" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A46" s="2">
+    <row r="53" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A53" s="2">
         <v>42463</v>
       </c>
-      <c r="B46" s="104" t="s">
+      <c r="B53" s="104" t="s">
         <v>499</v>
       </c>
-      <c r="C46" s="104" t="s">
+      <c r="C53" s="104" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="102" customFormat="1">
-      <c r="A47" s="2">
+    <row r="54" spans="1:3" s="102" customFormat="1">
+      <c r="A54" s="2">
         <v>42463</v>
       </c>
-      <c r="B47" s="104" t="s">
+      <c r="B54" s="104" t="s">
         <v>501</v>
       </c>
-      <c r="C47" s="104" t="s">
+      <c r="C54" s="104" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A48" s="2">
+    <row r="55" spans="1:3" s="102" customFormat="1" ht="150">
+      <c r="A55" s="2">
         <v>42463</v>
       </c>
-      <c r="B48" s="100" t="s">
+      <c r="B55" s="100" t="s">
         <v>493</v>
       </c>
-      <c r="C48" s="100" t="s">
+      <c r="C55" s="100" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="102" customFormat="1" ht="90">
-      <c r="A49" s="2">
+    <row r="56" spans="1:3" s="102" customFormat="1" ht="90">
+      <c r="A56" s="2">
         <v>42463</v>
       </c>
-      <c r="B49" s="103" t="s">
+      <c r="B56" s="103" t="s">
         <v>492</v>
       </c>
-      <c r="C49" s="103" t="s">
+      <c r="C56" s="103" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="102" customFormat="1" ht="30">
-      <c r="A50" s="2">
+    <row r="57" spans="1:3" s="102" customFormat="1" ht="30">
+      <c r="A57" s="2">
         <v>42463</v>
       </c>
-      <c r="B50" s="101" t="s">
+      <c r="B57" s="101" t="s">
         <v>489</v>
       </c>
-      <c r="C50" s="101" t="s">
+      <c r="C57" s="101" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="102" customFormat="1" ht="105">
-      <c r="A51" s="2">
+    <row r="58" spans="1:3" s="102" customFormat="1" ht="105">
+      <c r="A58" s="2">
         <v>42463</v>
       </c>
-      <c r="B51" s="101" t="s">
+      <c r="B58" s="101" t="s">
         <v>488</v>
       </c>
-      <c r="C51" s="101" t="s">
+      <c r="C58" s="101" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="102" customFormat="1" ht="150">
-      <c r="A52" s="2">
+    <row r="59" spans="1:3" s="102" customFormat="1" ht="150">
+      <c r="A59" s="2">
         <v>42462</v>
       </c>
-      <c r="B52" s="100" t="s">
+      <c r="B59" s="100" t="s">
         <v>486</v>
       </c>
-      <c r="C52" s="100" t="s">
+      <c r="C59" s="100" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="4" customFormat="1" ht="135">
-      <c r="A53" s="2">
+    <row r="60" spans="1:3" s="4" customFormat="1" ht="135">
+      <c r="A60" s="2">
         <v>42462</v>
       </c>
-      <c r="B53" s="100" t="s">
+      <c r="B60" s="100" t="s">
         <v>484</v>
       </c>
-      <c r="C53" s="100" t="s">
+      <c r="C60" s="100" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="4" customFormat="1" ht="240">
-      <c r="A54" s="2">
+    <row r="61" spans="1:3" s="4" customFormat="1" ht="240">
+      <c r="A61" s="2">
         <v>42462</v>
       </c>
-      <c r="B54" s="100" t="s">
+      <c r="B61" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="C54" s="100" t="s">
+      <c r="C61" s="100" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="4" customFormat="1" ht="120">
-      <c r="A55" s="2">
+    <row r="62" spans="1:3" s="4" customFormat="1" ht="120">
+      <c r="A62" s="2">
         <v>42462</v>
       </c>
-      <c r="B55" s="100" t="s">
+      <c r="B62" s="100" t="s">
         <v>480</v>
       </c>
-      <c r="C55" s="100" t="s">
+      <c r="C62" s="100" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="4" customFormat="1" ht="120">
-      <c r="A56" s="2">
+    <row r="63" spans="1:3" s="4" customFormat="1" ht="120">
+      <c r="A63" s="2">
         <v>42460</v>
       </c>
-      <c r="B56" s="99" t="s">
+      <c r="B63" s="99" t="s">
         <v>477</v>
       </c>
-      <c r="C56" s="99" t="s">
+      <c r="C63" s="99" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="4" customFormat="1" ht="30">
-      <c r="A57" s="2">
+    <row r="64" spans="1:3" s="4" customFormat="1" ht="30">
+      <c r="A64" s="2">
         <v>42460</v>
       </c>
-      <c r="B57" s="99" t="s">
+      <c r="B64" s="99" t="s">
         <v>476</v>
       </c>
-      <c r="C57" s="99" t="s">
+      <c r="C64" s="99" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="4" customFormat="1" ht="180">
-      <c r="A58" s="2">
+    <row r="65" spans="1:3" s="4" customFormat="1" ht="180">
+      <c r="A65" s="2">
         <v>42460</v>
       </c>
-      <c r="B58" s="99" t="s">
+      <c r="B65" s="99" t="s">
         <v>475</v>
       </c>
-      <c r="C58" s="99" t="s">
+      <c r="C65" s="99" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="4" customFormat="1" ht="60">
-      <c r="A59" s="2">
+    <row r="66" spans="1:3" s="4" customFormat="1" ht="60">
+      <c r="A66" s="2">
         <v>42460</v>
       </c>
-      <c r="B59" s="99" t="s">
+      <c r="B66" s="99" t="s">
         <v>478</v>
       </c>
-      <c r="C59" s="99" t="s">
+      <c r="C66" s="99" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="4" customFormat="1" ht="105">
-      <c r="A60" s="2">
+    <row r="67" spans="1:3" s="4" customFormat="1" ht="105">
+      <c r="A67" s="2">
         <v>42459</v>
       </c>
-      <c r="B60" s="99" t="s">
+      <c r="B67" s="99" t="s">
         <v>470</v>
       </c>
-      <c r="C60" s="98" t="s">
+      <c r="C67" s="98" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="60">
-      <c r="A61" s="2">
+    <row r="68" spans="1:3" ht="60">
+      <c r="A68" s="2">
         <v>42459</v>
       </c>
-      <c r="B61" s="99" t="s">
+      <c r="B68" s="99" t="s">
         <v>241</v>
       </c>
-      <c r="C61" s="99" t="s">
+      <c r="C68" s="99" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="2">
+    <row r="69" spans="1:3">
+      <c r="A69" s="2">
         <v>42458</v>
       </c>
-      <c r="B62" s="97" t="s">
+      <c r="B69" s="97" t="s">
         <v>470</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C69" s="8" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="105">
-      <c r="A63" s="2">
+    <row r="70" spans="1:3" ht="105">
+      <c r="A70" s="2">
         <v>42456</v>
       </c>
-      <c r="B63" s="96" t="s">
+      <c r="B70" s="96" t="s">
         <v>254</v>
       </c>
-      <c r="C63" s="100" t="s">
+      <c r="C70" s="100" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="60">
-      <c r="A64" s="2">
+    <row r="71" spans="1:3" ht="60">
+      <c r="A71" s="2">
         <v>42456</v>
       </c>
-      <c r="B64" s="96" t="s">
+      <c r="B71" s="96" t="s">
         <v>462</v>
       </c>
-      <c r="C64" s="44" t="s">
+      <c r="C71" s="44" t="s">
         <v>464</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="45">
-      <c r="A65" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B65" s="96" t="s">
-        <v>463</v>
-      </c>
-      <c r="C65" s="44" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="C66" s="44" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="45">
-      <c r="A67" s="2">
-        <v>42456</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="C67" s="44" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="77.25">
-      <c r="A68" s="79">
-        <v>42453</v>
-      </c>
-      <c r="B68" s="78" t="s">
-        <v>264</v>
-      </c>
-      <c r="C68" s="78" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="26.25">
-      <c r="A69" s="79">
-        <v>42453</v>
-      </c>
-      <c r="B69" s="78" t="s">
-        <v>262</v>
-      </c>
-      <c r="C69" s="78" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="39">
-      <c r="A70" s="79">
-        <v>42452</v>
-      </c>
-      <c r="B70" s="78" t="s">
-        <v>260</v>
-      </c>
-      <c r="C70" s="78" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="165">
-      <c r="A71" s="75">
-        <v>42451</v>
-      </c>
-      <c r="B71" s="74" t="s">
-        <v>247</v>
-      </c>
-      <c r="C71" s="100" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="45">
       <c r="A72" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B72" s="96" t="s">
+        <v>463</v>
+      </c>
+      <c r="C72" s="44" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C73" s="44" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="45">
+      <c r="A74" s="2">
+        <v>42456</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="C74" s="44" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="77.25">
+      <c r="A75" s="79">
+        <v>42453</v>
+      </c>
+      <c r="B75" s="78" t="s">
+        <v>264</v>
+      </c>
+      <c r="C75" s="78" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="26.25">
+      <c r="A76" s="79">
+        <v>42453</v>
+      </c>
+      <c r="B76" s="78" t="s">
+        <v>262</v>
+      </c>
+      <c r="C76" s="78" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="39">
+      <c r="A77" s="79">
+        <v>42452</v>
+      </c>
+      <c r="B77" s="78" t="s">
+        <v>260</v>
+      </c>
+      <c r="C77" s="78" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="165">
+      <c r="A78" s="75">
         <v>42451</v>
       </c>
-      <c r="B72" s="100" t="s">
+      <c r="B78" s="74" t="s">
+        <v>247</v>
+      </c>
+      <c r="C78" s="100" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="45">
+      <c r="A79" s="2">
+        <v>42451</v>
+      </c>
+      <c r="B79" s="100" t="s">
         <v>249</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="30">
-      <c r="A73" s="2">
+    <row r="80" spans="1:3" ht="30">
+      <c r="A80" s="2">
         <v>42451</v>
       </c>
-      <c r="B73" s="96" t="s">
+      <c r="B80" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="165">
-      <c r="A74" s="2">
+    <row r="81" spans="1:3" ht="165">
+      <c r="A81" s="2">
         <v>42451</v>
       </c>
-      <c r="B74" s="96" t="s">
+      <c r="B81" s="96" t="s">
         <v>253</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="64.5">
-      <c r="A75" s="79">
+    <row r="82" spans="1:3" ht="64.5">
+      <c r="A82" s="79">
         <v>42451</v>
       </c>
-      <c r="B75" s="78" t="s">
+      <c r="B82" s="78" t="s">
         <v>253</v>
       </c>
-      <c r="C75" s="78" t="s">
+      <c r="C82" s="78" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="64.5">
-      <c r="A76" s="79">
+    <row r="83" spans="1:3" ht="64.5">
+      <c r="A83" s="79">
         <v>42447</v>
       </c>
-      <c r="B76" s="78" t="s">
+      <c r="B83" s="78" t="s">
         <v>257</v>
       </c>
-      <c r="C76" s="78" t="s">
+      <c r="C83" s="78" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="2">
+    <row r="84" spans="1:3">
+      <c r="A84" s="2">
         <v>42440</v>
       </c>
-      <c r="B77" s="100" t="s">
+      <c r="B84" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="C77" s="100" t="s">
+      <c r="C84" s="100" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="75">
-      <c r="A78" s="2">
+    <row r="85" spans="1:3" ht="75">
+      <c r="A85" s="2">
         <v>42436</v>
       </c>
-      <c r="B78" s="96" t="s">
+      <c r="B85" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C85" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="39">
-      <c r="A79" s="79">
+    <row r="86" spans="1:3" ht="39">
+      <c r="A86" s="79">
         <v>42431</v>
       </c>
-      <c r="B79" s="78" t="s">
+      <c r="B86" s="78" t="s">
         <v>274</v>
       </c>
-      <c r="C79" s="78" t="s">
+      <c r="C86" s="78" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="26.25">
-      <c r="A80" s="79">
-        <v>42431</v>
-      </c>
-      <c r="B80" s="78" t="s">
-        <v>272</v>
-      </c>
-      <c r="C80" s="78" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="51.75">
-      <c r="A81" s="79">
-        <v>42430</v>
-      </c>
-      <c r="B81" s="78" t="s">
-        <v>270</v>
-      </c>
-      <c r="C81" s="78" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="26.25">
-      <c r="A82" s="79">
-        <v>42428</v>
-      </c>
-      <c r="B82" s="78" t="s">
-        <v>268</v>
-      </c>
-      <c r="C82" s="78" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="30">
-      <c r="A83" s="2">
-        <v>42426</v>
-      </c>
-      <c r="B83" s="100" t="s">
-        <v>186</v>
-      </c>
-      <c r="C83" s="100" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="77.25">
-      <c r="A84" s="79">
-        <v>42426</v>
-      </c>
-      <c r="B84" s="78" t="s">
-        <v>266</v>
-      </c>
-      <c r="C84" s="78" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="2">
-        <v>42425</v>
-      </c>
-      <c r="B85" s="100" t="s">
-        <v>241</v>
-      </c>
-      <c r="C85" s="100" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="2">
-        <v>42425</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="26.25">
       <c r="A87" s="79">
-        <v>42425</v>
+        <v>42431</v>
       </c>
       <c r="B87" s="78" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C87" s="78" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="51.75">
       <c r="A88" s="79">
-        <v>42425</v>
+        <v>42430</v>
       </c>
       <c r="B88" s="78" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C88" s="78" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="26.25">
       <c r="A89" s="79">
+        <v>42428</v>
+      </c>
+      <c r="B89" s="78" t="s">
+        <v>268</v>
+      </c>
+      <c r="C89" s="78" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="30">
+      <c r="A90" s="2">
+        <v>42426</v>
+      </c>
+      <c r="B90" s="100" t="s">
+        <v>186</v>
+      </c>
+      <c r="C90" s="100" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="77.25">
+      <c r="A91" s="79">
+        <v>42426</v>
+      </c>
+      <c r="B91" s="78" t="s">
+        <v>266</v>
+      </c>
+      <c r="C91" s="78" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="2">
         <v>42425</v>
       </c>
-      <c r="B89" s="78" t="s">
+      <c r="B92" s="100" t="s">
+        <v>241</v>
+      </c>
+      <c r="C92" s="100" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="2">
+        <v>42425</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="26.25">
+      <c r="A94" s="79">
+        <v>42425</v>
+      </c>
+      <c r="B94" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="C94" s="78" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="79">
+        <v>42425</v>
+      </c>
+      <c r="B95" s="78" t="s">
+        <v>276</v>
+      </c>
+      <c r="C95" s="78" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="26.25">
+      <c r="A96" s="79">
+        <v>42425</v>
+      </c>
+      <c r="B96" s="78" t="s">
         <v>279</v>
       </c>
-      <c r="C89" s="78" t="s">
+      <c r="C96" s="78" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="165">
-      <c r="A90" s="2">
+    <row r="97" spans="1:3" ht="165">
+      <c r="A97" s="2">
         <v>42424</v>
       </c>
-      <c r="B90" s="100" t="s">
+      <c r="B97" s="100" t="s">
         <v>239</v>
       </c>
-      <c r="C90" s="114" t="s">
+      <c r="C97" s="114" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="45">
-      <c r="A91" s="2">
+    <row r="98" spans="1:3" ht="45">
+      <c r="A98" s="2">
         <v>42423</v>
       </c>
-      <c r="B91" s="96" t="s">
+      <c r="B98" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="C98" s="11" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="79">
+    <row r="99" spans="1:3">
+      <c r="A99" s="79">
         <v>42423</v>
       </c>
-      <c r="B92" s="78" t="s">
+      <c r="B99" s="78" t="s">
         <v>281</v>
       </c>
-      <c r="C92" s="78" t="s">
+      <c r="C99" s="78" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="90">
-      <c r="A93" s="2">
+    <row r="100" spans="1:3" ht="90">
+      <c r="A100" s="2">
         <v>42422</v>
       </c>
-      <c r="B93" s="100" t="s">
+      <c r="B100" s="100" t="s">
         <v>236</v>
       </c>
-      <c r="C93" s="100" t="s">
+      <c r="C100" s="100" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="60">
-      <c r="A94" s="2">
+    <row r="101" spans="1:3" ht="60">
+      <c r="A101" s="2">
         <v>42419</v>
       </c>
-      <c r="B94" s="10" t="s">
+      <c r="B101" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="C94" s="36" t="s">
+      <c r="C101" s="36" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="195">
-      <c r="A95" s="2">
+    <row r="102" spans="1:3" ht="195">
+      <c r="A102" s="2">
         <v>42418</v>
       </c>
-      <c r="B95" s="10" t="s">
+      <c r="B102" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C95" s="18" t="s">
+      <c r="C102" s="18" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="45">
-      <c r="A96" s="2">
+    <row r="103" spans="1:3" ht="45">
+      <c r="A103" s="2">
         <v>42403</v>
       </c>
-      <c r="B96" s="96" t="s">
+      <c r="B103" s="96" t="s">
         <v>229</v>
       </c>
-      <c r="C96" s="12" t="s">
+      <c r="C103" s="12" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="75">
-      <c r="A97" s="2">
+    <row r="104" spans="1:3" ht="75">
+      <c r="A104" s="2">
         <v>42403</v>
       </c>
-      <c r="B97" s="12" t="s">
+      <c r="B104" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="C97" s="12" t="s">
+      <c r="C104" s="12" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="90">
-      <c r="A98" s="2">
+    <row r="105" spans="1:3" ht="90">
+      <c r="A105" s="2">
         <v>42403</v>
       </c>
-      <c r="B98" s="12"/>
-      <c r="C98" s="12" t="s">
+      <c r="B105" s="12"/>
+      <c r="C105" s="12" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="90">
-      <c r="A99" s="2">
+    <row r="106" spans="1:3" ht="90">
+      <c r="A106" s="2">
         <v>42398</v>
       </c>
-      <c r="B99" s="12" t="s">
+      <c r="B106" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C99" s="12" t="s">
+      <c r="C106" s="12" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="45">
-      <c r="A100" s="2">
+    <row r="107" spans="1:3" ht="45">
+      <c r="A107" s="2">
         <v>42398</v>
       </c>
-      <c r="B100" s="12" t="s">
+      <c r="B107" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="C100" s="12" t="s">
+      <c r="C107" s="12" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
-      <c r="A101" s="2">
+    <row r="108" spans="1:3">
+      <c r="A108" s="2">
         <v>42397</v>
       </c>
-      <c r="B101" s="96" t="s">
+      <c r="B108" s="96" t="s">
         <v>201</v>
       </c>
-      <c r="C101" s="14" t="s">
+      <c r="C108" s="14" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="45">
-      <c r="A102" s="2">
+    <row r="109" spans="1:3" ht="45">
+      <c r="A109" s="2">
         <v>42396</v>
       </c>
-      <c r="B102" s="12" t="s">
+      <c r="B109" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C102" s="12" t="s">
+      <c r="C109" s="12" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="30">
-      <c r="A103" s="2">
+    <row r="110" spans="1:3" ht="30">
+      <c r="A110" s="2">
         <v>42396</v>
       </c>
-      <c r="B103" s="96" t="s">
+      <c r="B110" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="C103" s="14" t="s">
+      <c r="C110" s="14" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="128.25">
-      <c r="A104" s="79">
+    <row r="111" spans="1:3" ht="128.25">
+      <c r="A111" s="79">
         <v>42386</v>
       </c>
-      <c r="B104" s="78" t="s">
+      <c r="B111" s="78" t="s">
         <v>283</v>
       </c>
-      <c r="C104" s="78" t="s">
+      <c r="C111" s="78" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="64.5">
-      <c r="A105" s="79">
+    <row r="112" spans="1:3" ht="64.5">
+      <c r="A112" s="79">
         <v>42386</v>
       </c>
-      <c r="B105" s="78" t="s">
+      <c r="B112" s="78" t="s">
         <v>285</v>
       </c>
-      <c r="C105" s="78" t="s">
+      <c r="C112" s="78" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="45">
-      <c r="A106" s="2">
+    <row r="113" spans="1:3" ht="45">
+      <c r="A113" s="2">
         <v>42384</v>
       </c>
-      <c r="B106" s="100" t="s">
+      <c r="B113" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="C106" s="100" t="s">
+      <c r="C113" s="100" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="180">
-      <c r="A107" s="2">
+    <row r="114" spans="1:3" ht="180">
+      <c r="A114" s="2">
         <v>42382</v>
       </c>
-      <c r="B107" s="14" t="s">
+      <c r="B114" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="C107" s="14" t="s">
+      <c r="C114" s="14" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="64.5">
-      <c r="A108" s="79">
+    <row r="115" spans="1:3" ht="64.5">
+      <c r="A115" s="79">
         <v>42382</v>
       </c>
-      <c r="B108" s="78" t="s">
+      <c r="B115" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="C108" s="78" t="s">
+      <c r="C115" s="78" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="30">
-      <c r="A109" s="2">
+    <row r="116" spans="1:3" ht="30">
+      <c r="A116" s="2">
         <v>42381</v>
       </c>
-      <c r="B109" s="100" t="s">
+      <c r="B116" s="100" t="s">
         <v>216</v>
       </c>
-      <c r="C109" s="100" t="s">
+      <c r="C116" s="100" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="45">
-      <c r="A110" s="2">
+    <row r="117" spans="1:3" ht="45">
+      <c r="A117" s="2">
         <v>42380</v>
       </c>
-      <c r="B110" s="16" t="s">
+      <c r="B117" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C110" s="16" t="s">
+      <c r="C117" s="16" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="75">
-      <c r="A111" s="2">
+    <row r="118" spans="1:3" ht="75">
+      <c r="A118" s="2">
         <v>42380</v>
       </c>
-      <c r="B111" s="50" t="s">
+      <c r="B118" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C111" s="17" t="s">
+      <c r="C118" s="17" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="180">
-      <c r="A112" s="2">
+    <row r="119" spans="1:3" ht="180">
+      <c r="A119" s="2">
         <v>42380</v>
       </c>
-      <c r="B112" s="50" t="s">
+      <c r="B119" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C112" s="18" t="s">
+      <c r="C119" s="18" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="217.5">
-      <c r="A113" s="79">
+    <row r="120" spans="1:3" ht="217.5">
+      <c r="A120" s="79">
         <v>42380</v>
       </c>
-      <c r="B113" s="78" t="s">
+      <c r="B120" s="78" t="s">
         <v>288</v>
       </c>
-      <c r="C113" s="78" t="s">
+      <c r="C120" s="78" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="102.75">
-      <c r="A114" s="79">
+    <row r="121" spans="1:3" ht="102.75">
+      <c r="A121" s="79">
         <v>42378</v>
       </c>
-      <c r="B114" s="78" t="s">
+      <c r="B121" s="78" t="s">
         <v>291</v>
       </c>
-      <c r="C114" s="78" t="s">
+      <c r="C121" s="78" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="102.75">
-      <c r="A115" s="79">
+    <row r="122" spans="1:3" ht="102.75">
+      <c r="A122" s="79">
         <v>42378</v>
       </c>
-      <c r="B115" s="78" t="s">
+      <c r="B122" s="78" t="s">
         <v>293</v>
       </c>
-      <c r="C115" s="78" t="s">
+      <c r="C122" s="78" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="141">
-      <c r="A116" s="79">
+    <row r="123" spans="1:3" ht="141">
+      <c r="A123" s="79">
         <v>42378</v>
       </c>
-      <c r="B116" s="78" t="s">
+      <c r="B123" s="78" t="s">
         <v>297</v>
       </c>
-      <c r="C116" s="78" t="s">
+      <c r="C123" s="78" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="77.25">
-      <c r="A117" s="79">
+    <row r="124" spans="1:3" ht="77.25">
+      <c r="A124" s="79">
         <v>42378</v>
       </c>
-      <c r="B117" s="78" t="s">
+      <c r="B124" s="78" t="s">
         <v>297</v>
       </c>
-      <c r="C117" s="78" t="s">
+      <c r="C124" s="78" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="102.75">
-      <c r="A118" s="79">
+    <row r="125" spans="1:3" ht="102.75">
+      <c r="A125" s="79">
         <v>42378</v>
       </c>
-      <c r="B118" s="78" t="s">
+      <c r="B125" s="78" t="s">
         <v>295</v>
       </c>
-      <c r="C118" s="78" t="s">
+      <c r="C125" s="78" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="60">
-      <c r="A119" s="2">
+    <row r="126" spans="1:3" ht="60">
+      <c r="A126" s="2">
         <v>42377</v>
       </c>
-      <c r="B119" s="100" t="s">
+      <c r="B126" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="C119" s="100" t="s">
+      <c r="C126" s="100" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="77.25">
-      <c r="A120" s="79">
+    <row r="127" spans="1:3" ht="77.25">
+      <c r="A127" s="79">
         <v>42376</v>
       </c>
-      <c r="B120" s="78" t="s">
+      <c r="B127" s="78" t="s">
         <v>300</v>
       </c>
-      <c r="C120" s="78" t="s">
+      <c r="C127" s="78" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="45">
-      <c r="A121" s="2">
+    <row r="128" spans="1:3" ht="45">
+      <c r="A128" s="2">
         <v>42375</v>
       </c>
-      <c r="B121" s="15" t="s">
+      <c r="B128" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C121" s="100" t="s">
+      <c r="C128" s="100" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
-      <c r="A122" s="2">
+    <row r="129" spans="1:3">
+      <c r="A129" s="2">
         <v>42369</v>
       </c>
-      <c r="B122" s="100" t="s">
+      <c r="B129" s="100" t="s">
         <v>202</v>
       </c>
-      <c r="C122" s="19" t="s">
+      <c r="C129" s="19" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="195">
-      <c r="A123" s="2">
+    <row r="130" spans="1:3" ht="195">
+      <c r="A130" s="2">
         <v>42368</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B130" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C123" s="19" t="s">
+      <c r="C130" s="19" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="135">
-      <c r="A124" s="2">
+    <row r="131" spans="1:3" ht="135">
+      <c r="A131" s="2">
         <v>42368</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B131" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C124" s="20" t="s">
+      <c r="C131" s="20" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="45">
-      <c r="A125" s="2">
+    <row r="132" spans="1:3" ht="45">
+      <c r="A132" s="2">
         <v>42368</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B132" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C125" s="20" t="s">
+      <c r="C132" s="20" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="30">
-      <c r="A126" s="2">
+    <row r="133" spans="1:3" ht="30">
+      <c r="A133" s="2">
         <v>42366</v>
       </c>
-      <c r="B126" s="20" t="s">
+      <c r="B133" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C126" s="20" t="s">
+      <c r="C133" s="20" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="30">
-      <c r="A127" s="2">
+    <row r="134" spans="1:3" ht="30">
+      <c r="A134" s="2">
         <v>42366</v>
       </c>
-      <c r="B127" s="20" t="s">
+      <c r="B134" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C127" s="20" t="s">
+      <c r="C134" s="20" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="150">
-      <c r="A128" s="2">
-        <v>42361</v>
-      </c>
-      <c r="C128" s="20" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="30">
-      <c r="A129" s="2">
-        <v>42361</v>
-      </c>
-      <c r="C129" s="20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="270">
-      <c r="A130" s="2">
-        <v>42361</v>
-      </c>
-      <c r="B130" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C130" s="22" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="30">
-      <c r="A131" s="2">
-        <v>42361</v>
-      </c>
-      <c r="B131" s="100" t="s">
-        <v>53</v>
-      </c>
-      <c r="C131" s="20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
-      <c r="A132" s="2">
-        <v>42361</v>
-      </c>
-      <c r="B132" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C132" s="21" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="225">
-      <c r="A133" s="2">
-        <v>42361</v>
-      </c>
-      <c r="B133" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C133" s="22" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="60">
-      <c r="A134" s="2">
-        <v>42361</v>
-      </c>
-      <c r="B134" s="100" t="s">
-        <v>49</v>
-      </c>
-      <c r="C134" s="22" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="90">
+    <row r="135" spans="1:3" ht="150">
       <c r="A135" s="2">
         <v>42361</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C135" s="22" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="60">
+      <c r="C135" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="30">
       <c r="A136" s="2">
         <v>42361</v>
       </c>
-      <c r="B136" s="24" t="s">
+      <c r="C136" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="270">
+      <c r="A137" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B137" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C137" s="22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="30">
+      <c r="A138" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B138" s="100" t="s">
+        <v>53</v>
+      </c>
+      <c r="C138" s="20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B139" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C139" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="225">
+      <c r="A140" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B140" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C140" s="22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="60">
+      <c r="A141" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B141" s="100" t="s">
+        <v>49</v>
+      </c>
+      <c r="C141" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="90">
+      <c r="A142" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C136" s="24" t="s">
+      <c r="C142" s="22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="60">
+      <c r="A143" s="2">
+        <v>42361</v>
+      </c>
+      <c r="B143" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C143" s="24" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
-      <c r="A137" s="40">
+    <row r="144" spans="1:3">
+      <c r="A144" s="40">
         <v>42360</v>
       </c>
-      <c r="B137" s="50" t="s">
+      <c r="B144" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C144" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
-      <c r="A138" s="40">
+    <row r="145" spans="1:3">
+      <c r="A145" s="40">
         <v>42360</v>
       </c>
-      <c r="B138" s="50" t="s">
+      <c r="B145" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C145" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="102.75">
-      <c r="A139" s="80">
+    <row r="146" spans="1:3" ht="102.75">
+      <c r="A146" s="80">
         <v>42360</v>
       </c>
-      <c r="B139" s="78" t="s">
+      <c r="B146" s="78" t="s">
         <v>302</v>
       </c>
-      <c r="C139" s="78" t="s">
+      <c r="C146" s="78" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="30">
-      <c r="A140" s="2">
+    <row r="147" spans="1:3" ht="30">
+      <c r="A147" s="2">
         <v>42356</v>
       </c>
-      <c r="B140" s="100" t="s">
+      <c r="B147" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="C140" s="100" t="s">
+      <c r="C147" s="100" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
-      <c r="A141" s="2">
+    <row r="148" spans="1:3">
+      <c r="A148" s="2">
         <v>42356</v>
       </c>
-      <c r="B141" s="23" t="s">
+      <c r="B148" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="C141" s="23" t="s">
+      <c r="C148" s="23" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
-      <c r="A142" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B142" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="C142" s="25" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="30">
-      <c r="A143" s="2">
-        <v>42356</v>
-      </c>
-      <c r="B143" s="96"/>
-      <c r="C143" s="25" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="60">
-      <c r="A144" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B144" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="C144" s="26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
-      <c r="A145" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B145" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C145" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="150">
-      <c r="A146" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B146" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C146" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" ht="120">
-      <c r="A147" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B147" s="100" t="s">
-        <v>168</v>
-      </c>
-      <c r="C147" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="30">
-      <c r="A148" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B148" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C148" s="28" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B149" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="C149" s="29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" ht="75">
+        <v>42356</v>
+      </c>
+      <c r="B149" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C149" s="25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="30">
       <c r="A150" s="2">
-        <v>42355</v>
-      </c>
-      <c r="B150" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C150" s="29" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="135">
+        <v>42356</v>
+      </c>
+      <c r="B150" s="96"/>
+      <c r="C150" s="25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="60">
       <c r="A151" s="2">
         <v>42355</v>
       </c>
-      <c r="B151" s="100" t="s">
-        <v>173</v>
-      </c>
-      <c r="C151" s="29" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="75">
+      <c r="B151" s="96" t="s">
+        <v>91</v>
+      </c>
+      <c r="C151" s="26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
       <c r="A152" s="2">
         <v>42355</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C152" s="42" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="30">
+      <c r="B152" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C152" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="150">
       <c r="A153" s="2">
         <v>42355</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C153" s="30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3">
+      <c r="B153" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C153" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="120">
       <c r="A154" s="2">
         <v>42355</v>
       </c>
-      <c r="C154" s="30" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3">
+      <c r="B154" s="100" t="s">
+        <v>168</v>
+      </c>
+      <c r="C154" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="30">
       <c r="A155" s="2">
         <v>42355</v>
       </c>
-      <c r="B155" s="42"/>
-      <c r="C155" s="30" t="s">
-        <v>179</v>
+      <c r="B155" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C155" s="28" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="2">
         <v>42355</v>
       </c>
-      <c r="B156" s="42"/>
-      <c r="C156" s="30" t="s">
-        <v>178</v>
+      <c r="B156" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C156" s="29" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="75">
       <c r="A157" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B157" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="C157" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="30">
+        <v>42355</v>
+      </c>
+      <c r="B157" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C157" s="29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="135">
       <c r="A158" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B158" s="26"/>
-      <c r="C158" s="31" t="s">
-        <v>65</v>
+        <v>42355</v>
+      </c>
+      <c r="B158" s="100" t="s">
+        <v>173</v>
+      </c>
+      <c r="C158" s="29" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="75">
       <c r="A159" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B159" s="26"/>
-      <c r="C159" s="70" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3">
+        <v>42355</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C159" s="42" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="30">
       <c r="A160" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B160" s="26"/>
-      <c r="C160" s="32" t="s">
-        <v>69</v>
+        <v>42355</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C160" s="30" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="161" spans="1:6">
       <c r="A161" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B161" s="96"/>
-      <c r="C161" s="33" t="s">
-        <v>75</v>
+        <v>42355</v>
+      </c>
+      <c r="C161" s="30" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="162" spans="1:6">
       <c r="A162" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B162" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C162" s="34" t="s">
-        <v>72</v>
+        <v>42355</v>
+      </c>
+      <c r="B162" s="42"/>
+      <c r="C162" s="30" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="163" spans="1:6">
       <c r="A163" s="2">
-        <v>42352</v>
-      </c>
-      <c r="B163" s="96"/>
-      <c r="C163" s="34" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6">
+        <v>42355</v>
+      </c>
+      <c r="B163" s="42"/>
+      <c r="C163" s="30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="75">
       <c r="A164" s="2">
         <v>42352</v>
       </c>
-      <c r="B164" s="96"/>
-      <c r="C164" s="37" t="s">
-        <v>74</v>
+      <c r="B164" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C164" s="30" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="30">
       <c r="A165" s="2">
         <v>42352</v>
       </c>
-      <c r="B165" s="37"/>
-      <c r="C165" s="37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="30">
+      <c r="B165" s="26"/>
+      <c r="C165" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="75">
       <c r="A166" s="2">
         <v>42352</v>
       </c>
-      <c r="B166" s="96"/>
-      <c r="C166" s="96" t="s">
-        <v>77</v>
-      </c>
-      <c r="F166" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="45">
+      <c r="B166" s="26"/>
+      <c r="C166" s="70" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
       <c r="A167" s="2">
         <v>42352</v>
       </c>
-      <c r="B167" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C167" s="96" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="45">
+      <c r="B167" s="26"/>
+      <c r="C167" s="32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
       <c r="A168" s="2">
         <v>42352</v>
       </c>
-      <c r="B168" s="100"/>
-      <c r="C168" s="39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="30">
+      <c r="B168" s="96"/>
+      <c r="C168" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
       <c r="A169" s="2">
         <v>42352</v>
       </c>
-      <c r="B169" s="38"/>
-      <c r="C169" s="56" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" ht="75">
+      <c r="B169" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C169" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
       <c r="A170" s="2">
         <v>42352</v>
       </c>
-      <c r="B170" s="41"/>
-      <c r="C170" s="41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" ht="45">
+      <c r="B170" s="96"/>
+      <c r="C170" s="34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
       <c r="A171" s="2">
         <v>42352</v>
       </c>
-      <c r="B171" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C171" s="41" t="s">
-        <v>90</v>
+      <c r="B171" s="96"/>
+      <c r="C171" s="37" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="30">
       <c r="A172" s="2">
         <v>42352</v>
       </c>
-      <c r="B172" s="43"/>
-      <c r="C172" s="43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" ht="45">
+      <c r="B172" s="37"/>
+      <c r="C172" s="37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="30">
       <c r="A173" s="2">
         <v>42352</v>
       </c>
-      <c r="B173" s="44"/>
-      <c r="C173" s="44" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" ht="30">
+      <c r="B173" s="96"/>
+      <c r="C173" s="96" t="s">
+        <v>77</v>
+      </c>
+      <c r="F173" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="45">
       <c r="A174" s="2">
         <v>42352</v>
       </c>
-      <c r="B174" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="C174" s="46" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" ht="30">
+      <c r="B174" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C174" s="96" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" ht="45">
       <c r="A175" s="2">
         <v>42352</v>
       </c>
-      <c r="B175" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C175" s="47" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6">
+      <c r="B175" s="100"/>
+      <c r="C175" s="39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="30">
       <c r="A176" s="2">
         <v>42352</v>
       </c>
-      <c r="B176" s="100" t="s">
-        <v>83</v>
-      </c>
-      <c r="C176" s="48" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" ht="135">
+      <c r="B176" s="38"/>
+      <c r="C176" s="56" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="75">
       <c r="A177" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B177" s="49"/>
-      <c r="C177" s="49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" ht="60">
+        <v>42352</v>
+      </c>
+      <c r="B177" s="41"/>
+      <c r="C177" s="41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="45">
       <c r="A178" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B178" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="C178" s="51" t="s">
-        <v>56</v>
+        <v>42352</v>
+      </c>
+      <c r="B178" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C178" s="41" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="30">
       <c r="A179" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B179" s="96"/>
-      <c r="C179" s="53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="120">
+        <v>42352</v>
+      </c>
+      <c r="B179" s="43"/>
+      <c r="C179" s="43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="45">
       <c r="A180" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B180" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C180" s="53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" ht="150">
+        <v>42352</v>
+      </c>
+      <c r="B180" s="44"/>
+      <c r="C180" s="44" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="30">
       <c r="A181" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B181" s="52"/>
-      <c r="C181" s="52" t="s">
-        <v>59</v>
+        <v>42352</v>
+      </c>
+      <c r="B181" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C181" s="46" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="30">
       <c r="A182" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B182" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C182" s="54" t="s">
-        <v>60</v>
+        <v>42352</v>
+      </c>
+      <c r="B182" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C182" s="47" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="2">
-        <v>42349</v>
-      </c>
-      <c r="B183" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C183" s="55" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3">
+        <v>42352</v>
+      </c>
+      <c r="B183" s="100" t="s">
+        <v>83</v>
+      </c>
+      <c r="C183" s="48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="135">
       <c r="A184" s="2">
         <v>42349</v>
       </c>
-      <c r="B184" s="100"/>
-      <c r="C184" s="57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
+      <c r="B184" s="49"/>
+      <c r="C184" s="49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="60">
       <c r="A185" s="2">
         <v>42349</v>
       </c>
-      <c r="B185" s="58"/>
-      <c r="C185" s="58" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3">
+      <c r="B185" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C185" s="51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="30">
       <c r="A186" s="2">
         <v>42349</v>
       </c>
-      <c r="B186" s="59"/>
-      <c r="C186" s="59" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3">
+      <c r="B186" s="96"/>
+      <c r="C186" s="53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="120">
       <c r="A187" s="2">
         <v>42349</v>
       </c>
-      <c r="B187" s="60"/>
-      <c r="C187" s="60" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3">
+      <c r="B187" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C187" s="53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="150">
       <c r="A188" s="2">
         <v>42349</v>
       </c>
-      <c r="B188" s="61"/>
-      <c r="C188" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" ht="60">
+      <c r="B188" s="52"/>
+      <c r="C188" s="52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="30">
       <c r="A189" s="2">
         <v>42349</v>
       </c>
-      <c r="B189" s="62" t="s">
-        <v>168</v>
-      </c>
-      <c r="C189" s="100" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" ht="90">
+      <c r="B189" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C189" s="54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
       <c r="A190" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B190" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C190" s="62" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" ht="30">
+        <v>42349</v>
+      </c>
+      <c r="B190" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C190" s="55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
       <c r="A191" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C191" s="62" t="s">
-        <v>36</v>
+        <v>42349</v>
+      </c>
+      <c r="B191" s="100"/>
+      <c r="C191" s="57" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B192" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C192" s="63" t="s">
-        <v>28</v>
+        <v>42349</v>
+      </c>
+      <c r="B192" s="58"/>
+      <c r="C192" s="58" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B193" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C193" s="64" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="30">
+        <v>42349</v>
+      </c>
+      <c r="B193" s="59"/>
+      <c r="C193" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
       <c r="A194" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B194" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C194" s="65" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="195">
+        <v>42349</v>
+      </c>
+      <c r="B194" s="60"/>
+      <c r="C194" s="60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
       <c r="A195" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B195" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C195" s="66" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" ht="135">
+        <v>42349</v>
+      </c>
+      <c r="B195" s="61"/>
+      <c r="C195" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="60">
       <c r="A196" s="2">
-        <v>42345</v>
-      </c>
-      <c r="B196" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="C196" s="67" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" ht="75">
+        <v>42349</v>
+      </c>
+      <c r="B196" s="62" t="s">
+        <v>168</v>
+      </c>
+      <c r="C196" s="100" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="90">
       <c r="A197" s="2">
         <v>42345</v>
       </c>
-      <c r="B197" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="C197" s="68" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" ht="75">
+      <c r="B197" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C197" s="62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="30">
       <c r="A198" s="2">
         <v>42345</v>
       </c>
-      <c r="B198" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C198" s="69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="30">
+      <c r="B198" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C198" s="62" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
       <c r="A199" s="2">
         <v>42345</v>
       </c>
-      <c r="B199" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="C199" s="73" t="s">
-        <v>37</v>
+      <c r="B199" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C199" s="63" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="2">
         <v>42345</v>
       </c>
-      <c r="B200" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="C200" s="73" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3">
+      <c r="B200" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C200" s="64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="30">
       <c r="A201" s="2">
         <v>42345</v>
       </c>
-      <c r="B201" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="C201" s="73" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="60">
+      <c r="B201" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C201" s="65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="195">
       <c r="A202" s="2">
         <v>42345</v>
       </c>
-      <c r="B202" s="96" t="s">
-        <v>39</v>
-      </c>
-      <c r="C202" s="73" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="150">
+      <c r="B202" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C202" s="66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="135">
       <c r="A203" s="2">
         <v>42345</v>
       </c>
-      <c r="B203" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C203" s="73" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="45">
+      <c r="B203" s="100" t="s">
+        <v>31</v>
+      </c>
+      <c r="C203" s="67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="75">
       <c r="A204" s="2">
         <v>42345</v>
       </c>
-      <c r="B204" s="100" t="s">
-        <v>39</v>
-      </c>
-      <c r="C204" s="76" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" ht="60">
+      <c r="B204" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C204" s="68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="75">
       <c r="A205" s="2">
         <v>42345</v>
       </c>
-      <c r="B205" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C205" s="77" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" ht="105">
+      <c r="B205" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C205" s="69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="30">
       <c r="A206" s="2">
         <v>42345</v>
       </c>
       <c r="B206" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="C206" s="1" t="s">
-        <v>48</v>
+      <c r="C206" s="73" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="2">
         <v>42345</v>
       </c>
-      <c r="B207" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C207" s="96" t="s">
-        <v>50</v>
+      <c r="B207" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="C207" s="73" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="2">
         <v>42345</v>
       </c>
-      <c r="B208" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C208" s="96" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="75">
+      <c r="B208" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C208" s="73" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="60">
       <c r="A209" s="2">
         <v>42345</v>
       </c>
       <c r="B209" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C209" s="96" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" ht="45">
+        <v>39</v>
+      </c>
+      <c r="C209" s="73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" ht="150">
       <c r="A210" s="2">
         <v>42345</v>
       </c>
-      <c r="B210" s="96" t="s">
-        <v>53</v>
-      </c>
-      <c r="C210" s="96" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" ht="141">
-      <c r="A211" s="80">
+      <c r="B210" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C210" s="73" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="45">
+      <c r="A211" s="2">
         <v>42345</v>
       </c>
-      <c r="B211" s="78" t="s">
-        <v>303</v>
-      </c>
-      <c r="C211" s="78" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" ht="105">
+      <c r="B211" s="100" t="s">
+        <v>39</v>
+      </c>
+      <c r="C211" s="76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="60">
       <c r="A212" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B212" s="2" t="s">
+        <v>42345</v>
+      </c>
+      <c r="B212" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C212" s="77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="105">
+      <c r="A213" s="2">
+        <v>42345</v>
+      </c>
+      <c r="B213" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="C212" s="100" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" ht="90">
-      <c r="A213" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C213" s="96" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" ht="75">
+      <c r="C213" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
       <c r="A214" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B214" s="2" t="s">
-        <v>15</v>
+        <v>42345</v>
+      </c>
+      <c r="B214" s="96" t="s">
+        <v>49</v>
       </c>
       <c r="C214" s="96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" ht="30">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
       <c r="A215" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>15</v>
+        <v>42345</v>
+      </c>
+      <c r="B215" s="96" t="s">
+        <v>49</v>
       </c>
       <c r="C215" s="96" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" ht="30">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="75">
       <c r="A216" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B216" s="2" t="s">
-        <v>15</v>
+        <v>42345</v>
+      </c>
+      <c r="B216" s="96" t="s">
+        <v>49</v>
       </c>
       <c r="C216" s="96" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="45">
       <c r="A217" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B217" s="2" t="s">
-        <v>15</v>
+        <v>42345</v>
+      </c>
+      <c r="B217" s="96" t="s">
+        <v>53</v>
       </c>
       <c r="C217" s="96" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="90">
-      <c r="A218" s="2">
-        <v>42341</v>
-      </c>
-      <c r="B218" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C218" s="96" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" ht="30">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="141">
+      <c r="A218" s="80">
+        <v>42345</v>
+      </c>
+      <c r="B218" s="78" t="s">
+        <v>303</v>
+      </c>
+      <c r="C218" s="78" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="105">
       <c r="A219" s="2">
         <v>42341</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C219" s="96" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" ht="150">
+        <v>12</v>
+      </c>
+      <c r="C219" s="100" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" ht="90">
       <c r="A220" s="2">
         <v>42341</v>
       </c>
@@ -6410,7 +6486,7 @@
         <v>15</v>
       </c>
       <c r="C220" s="96" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="75">
@@ -6421,95 +6497,95 @@
         <v>15</v>
       </c>
       <c r="C221" s="96" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="90">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" ht="30">
       <c r="A222" s="2">
         <v>42341</v>
       </c>
-      <c r="B222" s="100" t="s">
-        <v>12</v>
+      <c r="B222" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C222" s="96" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" ht="60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" ht="30">
       <c r="A223" s="2">
         <v>42341</v>
       </c>
-      <c r="B223" s="96" t="s">
+      <c r="B223" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C223" s="96" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" ht="45">
       <c r="A224" s="2">
         <v>42341</v>
       </c>
-      <c r="B224" s="96" t="s">
-        <v>12</v>
+      <c r="B224" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C224" s="96" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" ht="90">
       <c r="A225" s="2">
         <v>42341</v>
       </c>
-      <c r="B225" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C225" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3">
+      <c r="B225" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C225" s="96" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" ht="30">
       <c r="A226" s="2">
         <v>42341</v>
       </c>
-      <c r="B226" s="96" t="s">
+      <c r="B226" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C226" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3">
+      <c r="C226" s="96" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" ht="150">
       <c r="A227" s="2">
         <v>42341</v>
       </c>
-      <c r="B227" s="96" t="s">
+      <c r="B227" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C227" s="8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3">
+      <c r="C227" s="96" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" ht="75">
       <c r="A228" s="2">
         <v>42341</v>
       </c>
-      <c r="B228" s="96" t="s">
+      <c r="B228" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C228" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" ht="75">
+      <c r="C228" s="96" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="90">
       <c r="A229" s="2">
         <v>42341</v>
       </c>
-      <c r="B229" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C229" s="100" t="s">
-        <v>24</v>
+      <c r="B229" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C229" s="96" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="60">
@@ -6517,287 +6593,364 @@
         <v>42341</v>
       </c>
       <c r="B230" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C230" s="96" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B231" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C230" s="96" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" ht="60">
-      <c r="A231" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B231" s="96"/>
       <c r="C231" s="96" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" ht="45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
       <c r="A232" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B232" s="96"/>
-      <c r="C232" s="96" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" ht="60">
+        <v>42341</v>
+      </c>
+      <c r="B232" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C232" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
       <c r="A233" s="2">
-        <v>42340</v>
-      </c>
-      <c r="B233" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C233" s="96" t="s">
-        <v>4</v>
+        <v>42341</v>
+      </c>
+      <c r="B233" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C233" s="7" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" s="2">
-        <v>42339</v>
-      </c>
-      <c r="B234" s="2"/>
-      <c r="C234" s="96" t="s">
-        <v>0</v>
+        <v>42341</v>
+      </c>
+      <c r="B234" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C234" s="8" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B235" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C235" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" ht="75">
+      <c r="A236" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B236" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C236" s="100" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" ht="60">
+      <c r="A237" s="2">
+        <v>42341</v>
+      </c>
+      <c r="B237" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="C237" s="96" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" ht="60">
+      <c r="A238" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B238" s="96"/>
+      <c r="C238" s="96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" ht="45">
+      <c r="A239" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B239" s="96"/>
+      <c r="C239" s="96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" ht="60">
+      <c r="A240" s="2">
+        <v>42340</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C240" s="96" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" s="2">
         <v>42339</v>
       </c>
-      <c r="B235" s="2"/>
-      <c r="C235" s="96" t="s">
+      <c r="B241" s="2"/>
+      <c r="C241" s="96" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242" s="2">
+        <v>42339</v>
+      </c>
+      <c r="B242" s="2"/>
+      <c r="C242" s="96" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="64.5">
-      <c r="A236" s="80">
+    <row r="243" spans="1:3" ht="64.5">
+      <c r="A243" s="80">
         <v>42334</v>
       </c>
-      <c r="B236" s="78" t="s">
+      <c r="B243" s="78" t="s">
         <v>309</v>
       </c>
-      <c r="C236" s="78" t="s">
+      <c r="C243" s="78" t="s">
         <v>308</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" ht="26.25">
-      <c r="A237" s="80">
-        <v>42334</v>
-      </c>
-      <c r="B237" s="78" t="s">
-        <v>307</v>
-      </c>
-      <c r="C237" s="78" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" ht="39">
-      <c r="A238" s="80">
-        <v>42334</v>
-      </c>
-      <c r="B238" s="78" t="s">
-        <v>272</v>
-      </c>
-      <c r="C238" s="78" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" ht="128.25">
-      <c r="A239" s="80">
-        <v>42333</v>
-      </c>
-      <c r="B239" s="78" t="s">
-        <v>268</v>
-      </c>
-      <c r="C239" s="78" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" ht="51.75">
-      <c r="A240" s="80">
-        <v>42333</v>
-      </c>
-      <c r="B240" s="78" t="s">
-        <v>216</v>
-      </c>
-      <c r="C240" s="78" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" ht="26.25">
-      <c r="A241" s="80">
-        <v>42331</v>
-      </c>
-      <c r="B241" s="78" t="s">
-        <v>313</v>
-      </c>
-      <c r="C241" s="78" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" ht="39">
-      <c r="A242" s="80">
-        <v>42329</v>
-      </c>
-      <c r="B242" s="78" t="s">
-        <v>315</v>
-      </c>
-      <c r="C242" s="78" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" ht="39">
-      <c r="A243" s="80">
-        <v>42328</v>
-      </c>
-      <c r="B243" s="78" t="s">
-        <v>324</v>
-      </c>
-      <c r="C243" s="78" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="244" spans="1:3" ht="26.25">
       <c r="A244" s="80">
+        <v>42334</v>
+      </c>
+      <c r="B244" s="78" t="s">
+        <v>307</v>
+      </c>
+      <c r="C244" s="78" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" ht="39">
+      <c r="A245" s="80">
+        <v>42334</v>
+      </c>
+      <c r="B245" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="C245" s="78" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" ht="128.25">
+      <c r="A246" s="80">
+        <v>42333</v>
+      </c>
+      <c r="B246" s="78" t="s">
+        <v>268</v>
+      </c>
+      <c r="C246" s="78" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" ht="51.75">
+      <c r="A247" s="80">
+        <v>42333</v>
+      </c>
+      <c r="B247" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="C247" s="78" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" ht="26.25">
+      <c r="A248" s="80">
+        <v>42331</v>
+      </c>
+      <c r="B248" s="78" t="s">
+        <v>313</v>
+      </c>
+      <c r="C248" s="78" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" ht="39">
+      <c r="A249" s="80">
+        <v>42329</v>
+      </c>
+      <c r="B249" s="78" t="s">
+        <v>315</v>
+      </c>
+      <c r="C249" s="78" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" ht="39">
+      <c r="A250" s="80">
         <v>42328</v>
       </c>
-      <c r="B244" s="78" t="s">
+      <c r="B250" s="78" t="s">
+        <v>324</v>
+      </c>
+      <c r="C250" s="78" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" ht="26.25">
+      <c r="A251" s="80">
+        <v>42328</v>
+      </c>
+      <c r="B251" s="78" t="s">
         <v>322</v>
       </c>
-      <c r="C244" s="78" t="s">
+      <c r="C251" s="78" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="115.5">
-      <c r="A245" s="80">
+    <row r="252" spans="1:3" ht="115.5">
+      <c r="A252" s="80">
         <v>42328</v>
       </c>
-      <c r="B245" s="78" t="s">
+      <c r="B252" s="78" t="s">
         <v>320</v>
       </c>
-      <c r="C245" s="78" t="s">
+      <c r="C252" s="78" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="90">
-      <c r="A246" s="80">
+    <row r="253" spans="1:3" ht="90">
+      <c r="A253" s="80">
         <v>42328</v>
       </c>
-      <c r="B246" s="78" t="s">
+      <c r="B253" s="78" t="s">
         <v>317</v>
       </c>
-      <c r="C246" s="78" t="s">
+      <c r="C253" s="78" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="153.75">
-      <c r="A247" s="80">
+    <row r="254" spans="1:3" ht="153.75">
+      <c r="A254" s="80">
         <v>42328</v>
       </c>
-      <c r="B247" s="78" t="s">
+      <c r="B254" s="78" t="s">
         <v>317</v>
       </c>
-      <c r="C247" s="78" t="s">
+      <c r="C254" s="78" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="102.75">
-      <c r="A248" s="80">
+    <row r="255" spans="1:3" ht="102.75">
+      <c r="A255" s="80">
         <v>42324</v>
       </c>
-      <c r="B248" s="78" t="s">
+      <c r="B255" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="C248" s="78" t="s">
+      <c r="C255" s="78" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="90">
-      <c r="A249" s="80">
+    <row r="256" spans="1:3" ht="90">
+      <c r="A256" s="80">
         <v>42321</v>
       </c>
-      <c r="B249" s="78" t="s">
+      <c r="B256" s="78" t="s">
         <v>327</v>
       </c>
-      <c r="C249" s="78" t="s">
+      <c r="C256" s="78" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="26.25">
-      <c r="A250" s="80">
+    <row r="257" spans="1:3" ht="26.25">
+      <c r="A257" s="80">
         <v>42321</v>
       </c>
-      <c r="B250" s="78" t="s">
+      <c r="B257" s="78" t="s">
         <v>327</v>
       </c>
-      <c r="C250" s="78" t="s">
+      <c r="C257" s="78" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="77.25">
-      <c r="A251" s="79">
+    <row r="258" spans="1:3" ht="77.25">
+      <c r="A258" s="79">
         <v>42318</v>
       </c>
-      <c r="B251" s="78" t="s">
+      <c r="B258" s="78" t="s">
         <v>330</v>
       </c>
-      <c r="C251" s="78" t="s">
+      <c r="C258" s="78" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="115.5">
-      <c r="A252" s="79">
+    <row r="259" spans="1:3" ht="115.5">
+      <c r="A259" s="79">
         <v>42311</v>
       </c>
-      <c r="B252" s="78" t="s">
+      <c r="B259" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C252" s="78" t="s">
+      <c r="C259" s="78" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="253" spans="1:3" ht="77.25">
-      <c r="A253" s="79">
+    <row r="260" spans="1:3" ht="77.25">
+      <c r="A260" s="79">
         <v>42310</v>
       </c>
-      <c r="B253" s="78" t="s">
+      <c r="B260" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C253" s="78" t="s">
+      <c r="C260" s="78" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="51.75">
-      <c r="A254" s="79">
+    <row r="261" spans="1:3" ht="51.75">
+      <c r="A261" s="79">
         <v>42306</v>
       </c>
-      <c r="B254" s="78" t="s">
+      <c r="B261" s="78" t="s">
         <v>333</v>
       </c>
-      <c r="C254" s="78" t="s">
+      <c r="C261" s="78" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="255" spans="1:3">
-      <c r="A255" s="100"/>
-      <c r="B255" s="100"/>
-      <c r="C255" s="100"/>
+    <row r="262" spans="1:3">
+      <c r="A262" s="100"/>
+      <c r="B262" s="100"/>
+      <c r="C262" s="100"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C255">
+  <autoFilter ref="A1:C262">
     <sortState ref="A2:C201">
       <sortCondition descending="1" ref="A1:A201"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C227" r:id="rId1"/>
-    <hyperlink ref="C188" r:id="rId2"/>
-    <hyperlink ref="C228" r:id="rId3"/>
-    <hyperlink ref="C62" r:id="rId4"/>
-    <hyperlink ref="C47" r:id="rId5"/>
-    <hyperlink ref="C44" r:id="rId6"/>
+    <hyperlink ref="C234" r:id="rId1"/>
+    <hyperlink ref="C195" r:id="rId2"/>
+    <hyperlink ref="C235" r:id="rId3"/>
+    <hyperlink ref="C69" r:id="rId4"/>
+    <hyperlink ref="C54" r:id="rId5"/>
+    <hyperlink ref="C51" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -6817,16 +6970,16 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="60.75" customHeight="1">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="139" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add index entry on software engineering slogan, Add java entry on refactoring
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="760">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -4411,6 +4411,12 @@
       <t xml:space="preserve">. For example, if you're running a LAMP server you'd have apache listening on all IP addresses (so that your users can access it) while a mysql database could be configured to be accessible only from localhost (using it's bind=127.0.0.1 directive). This way php running on the same server will be able to access the database while external (and untrusted) users will not be able to access it.
 </t>
     </r>
+  </si>
+  <si>
+    <t>Slogan!</t>
+  </si>
+  <si>
+    <t>Give your desgin a "DRY but SOLID KISS"</t>
   </si>
 </sst>
 </file>
@@ -5614,8 +5620,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A326" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C335" sqref="C335"/>
+    <sheetView tabSelected="1" topLeftCell="A328" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C331" sqref="C331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="43.9" customHeight="1"/>
@@ -10590,8 +10596,21 @@
       </c>
     </row>
     <row r="330" spans="1:5" ht="43.9" customHeight="1">
-      <c r="A330" s="82"/>
-      <c r="E330" s="82"/>
+      <c r="A330" s="98">
+        <v>42870</v>
+      </c>
+      <c r="B330" s="115" t="s">
+        <v>579</v>
+      </c>
+      <c r="C330" s="122" t="s">
+        <v>758</v>
+      </c>
+      <c r="D330" s="122" t="s">
+        <v>596</v>
+      </c>
+      <c r="E330" s="120" t="s">
+        <v>759</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E330">

</xml_diff>

<commit_message>
Add index entry on NoSQL intro, Add python entry on basic
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'AS400 Version'!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$E$330</definedName>
-    <definedName name="CategoryOptions">options!$A$2:$A$14</definedName>
+    <definedName name="CategoryOptions">options!$A$2:$A$15</definedName>
     <definedName name="TagOptions">options!$B$2:$B$4</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="763">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -4417,6 +4417,17 @@
   </si>
   <si>
     <t>Give your desgin a "DRY but SOLID KISS"</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>Intro NoSQL</t>
+  </si>
+  <si>
+    <t>* NoSQL stands for Not Only SQL
+* Popular NoSQL implementations are MongoDB, CouchDB. 
+* Most NoSQL db use BSON (Binary representation of JSON) to store data/ object</t>
   </si>
 </sst>
 </file>
@@ -5618,10 +5629,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H330"/>
+  <dimension ref="A1:H331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A328" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C331" sqref="C331"/>
+    <sheetView tabSelected="1" topLeftCell="A326" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E332" sqref="E332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="43.9" customHeight="1"/>
@@ -10610,6 +10621,23 @@
       </c>
       <c r="E330" s="120" t="s">
         <v>759</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" ht="43.9" customHeight="1">
+      <c r="A331" s="98">
+        <v>42871</v>
+      </c>
+      <c r="B331" s="115" t="s">
+        <v>760</v>
+      </c>
+      <c r="C331" s="122" t="s">
+        <v>761</v>
+      </c>
+      <c r="D331" s="122" t="s">
+        <v>596</v>
+      </c>
+      <c r="E331" s="120" t="s">
+        <v>762</v>
       </c>
     </row>
   </sheetData>
@@ -10645,7 +10673,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -10691,51 +10719,56 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>579</v>
+        <v>760</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>575</v>
+        <v>587</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>689</v>
+        <v>575</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
         <v>580</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Use newer version of git that detect ^M difference of file
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="767">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -4428,6 +4428,40 @@
     <t>* NoSQL stands for Not Only SQL
 * Popular NoSQL implementations are MongoDB, CouchDB. 
 * Most NoSQL db use BSON (Binary representation of JSON) to store data/ object</t>
+  </si>
+  <si>
+    <t>cygwin</t>
+  </si>
+  <si>
+    <t># cygwin file structure
+* for linux / : map to the root directory of cygwin program
+* for linux ~: map to /home/username
+* for win drive C: map to /cygdrive/c</t>
+  </si>
+  <si>
+    <t># install package manager **apt-cyg** for cygwin
+## Intro to apt-cyg
+apt-cyg is simply a script that runs in /bin. So to install, we need only copy the script to /bin and make sure the x attribute is changed.
+## Installation
+1. svn --force export http://apt-cyg.googlecode.com/svn/trunk/ /bin/  __this project already moved to github, so no need svn__
+1. chmod +x /bin/apt-cyg
+1. sometimes when run the script, syntax error appears, use vim to set the fileformat to unix to fix the error
+## apt-cyg usage
+"apt-cyg install &lt;package names&gt;" to install packages 
+"apt-cyg remove &lt;package names&gt;" to remove packages 
+"apt-cyg update" to update setup.ini 
+"apt-cyg show" to show installed packages 
+"apt-cyg find &lt;pattern(s)&gt;" to find packages matching patterns 
+"apt-cyg describe &lt;pattern(s)&gt;" to describe packages matching patterns 
+"apt-cyg packageof &lt;commands or files&gt;" to locate parent packages</t>
+  </si>
+  <si>
+    <t># Reset cygwin
+## Reason of reset
+When we want to upgrade the version of cygwin, or when we want to install specific package that is only available in cygwin setup?
+## Step of reset
+* Invoke the setup.exe in / (aka the root of cygwin program in win OS C drive)
+* Select the needed packages in the setup</t>
   </si>
 </sst>
 </file>
@@ -5629,10 +5663,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H331"/>
+  <dimension ref="A1:H334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A326" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E332" sqref="E332"/>
+    <sheetView tabSelected="1" topLeftCell="C324" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E334" sqref="E334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="43.9" customHeight="1"/>
@@ -10638,6 +10672,57 @@
       </c>
       <c r="E331" s="120" t="s">
         <v>762</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" ht="43.9" customHeight="1">
+      <c r="A332" s="98">
+        <v>42879</v>
+      </c>
+      <c r="B332" s="115" t="s">
+        <v>577</v>
+      </c>
+      <c r="C332" s="122" t="s">
+        <v>763</v>
+      </c>
+      <c r="D332" s="122" t="s">
+        <v>596</v>
+      </c>
+      <c r="E332" s="120" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" ht="43.9" customHeight="1">
+      <c r="A333" s="98">
+        <v>42879</v>
+      </c>
+      <c r="B333" s="115" t="s">
+        <v>577</v>
+      </c>
+      <c r="C333" s="122" t="s">
+        <v>763</v>
+      </c>
+      <c r="D333" s="122" t="s">
+        <v>596</v>
+      </c>
+      <c r="E333" s="120" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" ht="43.9" customHeight="1">
+      <c r="A334" s="98">
+        <v>42879</v>
+      </c>
+      <c r="B334" s="115" t="s">
+        <v>577</v>
+      </c>
+      <c r="C334" s="122" t="s">
+        <v>763</v>
+      </c>
+      <c r="D334" s="122" t="s">
+        <v>596</v>
+      </c>
+      <c r="E334" s="120" t="s">
+        <v>766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add index entry on linux FHS
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="771">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -4462,6 +4462,79 @@
 ## Step of reset
 * Invoke the setup.exe in / (aka the root of cygwin program in win OS C drive)
 * Select the needed packages in the setup</t>
+  </si>
+  <si>
+    <t>FHS (File Hierarchy Standard)</t>
+  </si>
+  <si>
+    <r>
+      <t># What is FHS
+FHS is a set of standard for LFS(Linux File System), so that different distributions can follow
+# Detail of definition
+Download the PDF or html from http://refspecs.linuxfoundation.org/fhs.shtml
+# Brief Intro of main directory
+* /bin: Essential user command binaries (all users access)
+* /etc: Host-specific system config
+* /lib: Essential shared libraries and kernel modules
+* /opt: Add-on application software packages
+* /sbin: system binaries
+* /usr:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [static]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    * /usr/bin: Most user command
+    * /usr/sbin: Non-essential standard system binraries
+    * /usr/lib: Lib for programming and pakcages
+    * /usr/share: Architecture-independent data
+* /var: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[dynamic]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    * /var/log...</t>
+    </r>
+  </si>
+  <si>
+    <t>FHS impl</t>
+  </si>
+  <si>
+    <t># FHS Mindset Practice
+Say I want to install jdk on linux according to FHS suggestion. I will put the jdk folder under /usr/share because it is static and it is data. Then I might build a soft link in /usr/bin that link to $JAVA_HOME/bin (&lt;- but usually dont do that because if there is a java version update then all links need to be re-deploy)</t>
   </si>
 </sst>
 </file>
@@ -5663,10 +5736,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H334"/>
+  <dimension ref="A1:H336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C324" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E334" sqref="E334"/>
+    <sheetView tabSelected="1" topLeftCell="A330" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E337" sqref="E337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="43.9" customHeight="1"/>
@@ -10723,6 +10796,40 @@
       </c>
       <c r="E334" s="120" t="s">
         <v>766</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" ht="43.9" customHeight="1">
+      <c r="A335" s="98">
+        <v>42887</v>
+      </c>
+      <c r="B335" s="115" t="s">
+        <v>577</v>
+      </c>
+      <c r="C335" s="122" t="s">
+        <v>767</v>
+      </c>
+      <c r="D335" s="122" t="s">
+        <v>596</v>
+      </c>
+      <c r="E335" s="120" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" ht="43.9" customHeight="1">
+      <c r="A336" s="98">
+        <v>42887</v>
+      </c>
+      <c r="B336" s="115" t="s">
+        <v>577</v>
+      </c>
+      <c r="C336" s="122" t="s">
+        <v>769</v>
+      </c>
+      <c r="D336" s="122" t="s">
+        <v>596</v>
+      </c>
+      <c r="E336" s="120" t="s">
+        <v>770</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Modify index entry on Linux FHS impl 2. Add ai lib in markdown form 3. Add lisp lib in markdown form
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -4533,10 +4533,6 @@
     <t>FHS impl</t>
   </si>
   <si>
-    <t># FHS Mindset Practice
-Say I want to install jdk on linux according to FHS suggestion. I will put the jdk folder under /usr/share because it is static and it is data. Then I might build a soft link in /usr/bin that link to $JAVA_HOME/bin (&lt;- but usually dont do that because if there is a java version update then all links need to be re-deploy)</t>
-  </si>
-  <si>
     <t>jenkins</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -4733,6 +4729,16 @@
 * Lower failure rate of new releases
 * Shorten lead time between fixes
 * Faster mean time to recovery ( in event of a new releases crashing or otherwise disabling the current system)</t>
+  </si>
+  <si>
+    <t># FHS Mindset Practice
+Say I want to install jdk on linux according to FHS suggestion. I will put the jdk folder under:
+`/usr/share` ~ `/usr/share` ~ `/usr/local/share`
+because it is static and it is data. Then I might build a soft link in:
+`/usr/bin` ~ `/bin` ~ `/usr/local/bin`
+that link to:
+`$JAVA_HOME/bin` 
+p.s. but usually people dont practice this because if there is a java version update then all links need to be re-deploy</t>
   </si>
 </sst>
 </file>
@@ -5936,8 +5942,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A329" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E342" sqref="E342"/>
+    <sheetView tabSelected="1" topLeftCell="A335" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E336" sqref="E336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="43.9" customHeight="1"/>
@@ -11013,7 +11019,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="336" spans="1:5" ht="43.9" customHeight="1">
+    <row r="336" spans="1:5" ht="102.75" customHeight="1">
       <c r="A336" s="98">
         <v>42887</v>
       </c>
@@ -11027,7 +11033,7 @@
         <v>596</v>
       </c>
       <c r="E336" s="120" t="s">
-        <v>770</v>
+        <v>785</v>
       </c>
     </row>
     <row r="337" spans="1:5" ht="43.9" customHeight="1">
@@ -11035,16 +11041,16 @@
         <v>42889</v>
       </c>
       <c r="B337" s="115" t="s">
+        <v>770</v>
+      </c>
+      <c r="C337" s="122" t="s">
         <v>771</v>
       </c>
-      <c r="C337" s="122" t="s">
-        <v>772</v>
-      </c>
       <c r="D337" s="122" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E337" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="338" spans="1:5" ht="43.9" customHeight="1">
@@ -11052,16 +11058,16 @@
         <v>42889</v>
       </c>
       <c r="B338" s="115" t="s">
+        <v>772</v>
+      </c>
+      <c r="C338" s="122" t="s">
         <v>773</v>
       </c>
-      <c r="C338" s="122" t="s">
+      <c r="D338" s="122" t="s">
         <v>774</v>
       </c>
-      <c r="D338" s="122" t="s">
-        <v>775</v>
-      </c>
       <c r="E338" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="339" spans="1:5" ht="43.9" customHeight="1">
@@ -11069,16 +11075,16 @@
         <v>42889</v>
       </c>
       <c r="B339" s="115" t="s">
+        <v>775</v>
+      </c>
+      <c r="C339" s="122" t="s">
         <v>776</v>
       </c>
-      <c r="C339" s="122" t="s">
-        <v>777</v>
-      </c>
       <c r="D339" s="122" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E339" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="340" spans="1:5" ht="43.9" customHeight="1">
@@ -11086,16 +11092,16 @@
         <v>42889</v>
       </c>
       <c r="B340" s="115" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C340" s="122" t="s">
+        <v>779</v>
+      </c>
+      <c r="D340" s="122" t="s">
+        <v>774</v>
+      </c>
+      <c r="E340" s="1" t="s">
         <v>780</v>
-      </c>
-      <c r="D340" s="122" t="s">
-        <v>775</v>
-      </c>
-      <c r="E340" s="1" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="341" spans="1:5" ht="43.9" customHeight="1">
@@ -11103,16 +11109,16 @@
         <v>42891</v>
       </c>
       <c r="B341" s="115" t="s">
+        <v>782</v>
+      </c>
+      <c r="C341" s="122" t="s">
         <v>783</v>
-      </c>
-      <c r="C341" s="122" t="s">
-        <v>784</v>
       </c>
       <c r="D341" s="122" t="s">
         <v>596</v>
       </c>
       <c r="E341" s="120" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add index entry about today i learnt, and AI entry on problems
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="788">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -3846,10 +3846,6 @@
   </si>
   <si>
     <t>About Learning</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>最近學習多, Spring x Springboot我花了不少時間才基本上明白其理念和基本應用. 不談具體, 若談其學習過程, 我覺得重要是別怕盲人摸象, 要敢去判! 只有判錯了, 才能後來斷出正路. 要去習慣他, 重讀他. 也適用於Android, Spring Vaadin, Spring JPA, 哲學, 文學, 道學, 佛學, 音樂等等.</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
@@ -4739,6 +4735,15 @@
 that link to:
 `$JAVA_HOME/bin` 
 p.s. but usually people dont practice this because if there is a java version update then all links need to be re-deploy</t>
+  </si>
+  <si>
+    <t>最近學習多, Spring x Springboot我花了不少時間才基本上明白其理念和基本應用. 不談具體, 若談其學習過程, 我覺得重要是別怕盲人摸象, 要敢去判! 只有判錯了, 才能後來斷出正路. 要去習慣他, 重讀他. 也適用於Android, Spring Vaadin, Spring JPA, 哲學, 文學, 道學, 佛學, 音樂等等.</t>
+  </si>
+  <si>
+    <t>Today I learnt</t>
+  </si>
+  <si>
+    <t>Work as a Programmer for 1 and half year, I feel like the XP (extreme) programming concept is very relevant to my daily work. And when recently in Udacity AI course, teacher's motto saids, "Do the stupid way first, add intelligent only when necessary". And Martin Fowler also said, "Build MVP with least effort, refactor later"</t>
   </si>
 </sst>
 </file>
@@ -5584,7 +5589,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>53477</xdr:colOff>
+      <xdr:colOff>53478</xdr:colOff>
       <xdr:row>285</xdr:row>
       <xdr:rowOff>178663</xdr:rowOff>
     </xdr:to>
@@ -5940,16 +5945,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H341"/>
+  <dimension ref="A1:H342"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A335" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E336" sqref="E336"/>
+      <selection activeCell="E342" sqref="E342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="43.9" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="115" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="115" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" style="122" customWidth="1"/>
     <col min="4" max="4" width="10" style="122" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="115.5703125" style="1" customWidth="1"/>
@@ -10625,7 +10630,7 @@
         <v>714</v>
       </c>
       <c r="E312" s="120" t="s">
-        <v>718</v>
+        <v>785</v>
       </c>
     </row>
     <row r="313" spans="1:5" ht="43.9" customHeight="1">
@@ -10636,13 +10641,13 @@
         <v>715</v>
       </c>
       <c r="C313" s="120" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D313" s="120" t="s">
         <v>714</v>
       </c>
       <c r="E313" s="120" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="314" spans="1:5" ht="43.9" customHeight="1">
@@ -10653,13 +10658,13 @@
         <v>583</v>
       </c>
       <c r="C314" s="120" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D314" s="120" t="s">
         <v>598</v>
       </c>
       <c r="E314" s="120" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="315" spans="1:5" ht="43.9" customHeight="1">
@@ -10670,13 +10675,13 @@
         <v>583</v>
       </c>
       <c r="C315" s="120" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D315" s="120" t="s">
         <v>598</v>
       </c>
       <c r="E315" s="120" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="316" spans="1:5" ht="43.9" customHeight="1">
@@ -10684,16 +10689,16 @@
         <v>42851</v>
       </c>
       <c r="B316" s="115" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C316" s="120" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D316" s="120" t="s">
         <v>597</v>
       </c>
       <c r="E316" s="120" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="317" spans="1:5" ht="43.9" customHeight="1">
@@ -10701,16 +10706,16 @@
         <v>42851</v>
       </c>
       <c r="B317" s="115" t="s">
+        <v>730</v>
+      </c>
+      <c r="C317" s="120" t="s">
         <v>731</v>
-      </c>
-      <c r="C317" s="120" t="s">
-        <v>732</v>
       </c>
       <c r="D317" s="120" t="s">
         <v>596</v>
       </c>
       <c r="E317" s="120" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="318" spans="1:5" ht="43.9" customHeight="1">
@@ -10721,13 +10726,13 @@
         <v>583</v>
       </c>
       <c r="C318" s="120" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D318" s="120" t="s">
         <v>596</v>
       </c>
       <c r="E318" s="120" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="319" spans="1:5" ht="43.9" customHeight="1">
@@ -10738,13 +10743,13 @@
         <v>583</v>
       </c>
       <c r="C319" s="120" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D319" s="120" t="s">
         <v>596</v>
       </c>
       <c r="E319" s="120" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="320" spans="1:5" ht="43.9" customHeight="1">
@@ -10755,13 +10760,13 @@
         <v>583</v>
       </c>
       <c r="C320" s="120" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D320" s="120" t="s">
         <v>596</v>
       </c>
       <c r="E320" s="120" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="321" spans="1:5" ht="43.9" customHeight="1">
@@ -10772,13 +10777,13 @@
         <v>576</v>
       </c>
       <c r="C321" s="120" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D321" s="120" t="s">
         <v>598</v>
       </c>
       <c r="E321" s="120" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="322" spans="1:5" ht="43.9" customHeight="1">
@@ -10789,13 +10794,13 @@
         <v>576</v>
       </c>
       <c r="C322" s="120" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D322" s="120" t="s">
         <v>596</v>
       </c>
       <c r="E322" s="120" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="323" spans="1:5" ht="43.9" customHeight="1">
@@ -10806,13 +10811,13 @@
         <v>576</v>
       </c>
       <c r="C323" s="120" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D323" s="120" t="s">
         <v>596</v>
       </c>
       <c r="E323" s="120" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="324" spans="1:5" ht="43.9" customHeight="1">
@@ -10823,13 +10828,13 @@
         <v>576</v>
       </c>
       <c r="C324" s="120" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D324" s="120" t="s">
         <v>597</v>
       </c>
       <c r="E324" s="120" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="325" spans="1:5" ht="43.9" customHeight="1">
@@ -10840,13 +10845,13 @@
         <v>583</v>
       </c>
       <c r="C325" s="120" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D325" s="120" t="s">
         <v>597</v>
       </c>
       <c r="E325" s="120" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="326" spans="1:5" ht="43.9" customHeight="1">
@@ -10854,16 +10859,16 @@
         <v>42861</v>
       </c>
       <c r="B326" s="115" t="s">
+        <v>747</v>
+      </c>
+      <c r="C326" s="120" t="s">
         <v>748</v>
       </c>
-      <c r="C326" s="120" t="s">
+      <c r="D326" s="120" t="s">
         <v>749</v>
       </c>
-      <c r="D326" s="120" t="s">
+      <c r="E326" s="120" t="s">
         <v>750</v>
-      </c>
-      <c r="E326" s="120" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="327" spans="1:5" ht="43.9" customHeight="1">
@@ -10871,16 +10876,16 @@
         <v>42861</v>
       </c>
       <c r="B327" s="115" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C327" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D327" t="s">
         <v>596</v>
       </c>
       <c r="E327" s="120" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="328" spans="1:5" ht="43.9" customHeight="1">
@@ -10888,16 +10893,16 @@
         <v>42869</v>
       </c>
       <c r="B328" s="115" t="s">
+        <v>751</v>
+      </c>
+      <c r="C328" s="120" t="s">
+        <v>754</v>
+      </c>
+      <c r="D328" s="120" t="s">
         <v>752</v>
       </c>
-      <c r="C328" s="120" t="s">
-        <v>755</v>
-      </c>
-      <c r="D328" s="120" t="s">
+      <c r="E328" s="120" t="s">
         <v>753</v>
-      </c>
-      <c r="E328" s="120" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="329" spans="1:5" ht="43.9" customHeight="1">
@@ -10908,13 +10913,13 @@
         <v>577</v>
       </c>
       <c r="C329" s="120" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D329" s="120" t="s">
         <v>596</v>
       </c>
       <c r="E329" s="120" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="330" spans="1:5" ht="43.9" customHeight="1">
@@ -10925,13 +10930,13 @@
         <v>579</v>
       </c>
       <c r="C330" s="122" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D330" s="122" t="s">
         <v>596</v>
       </c>
       <c r="E330" s="120" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="331" spans="1:5" ht="43.9" customHeight="1">
@@ -10939,16 +10944,16 @@
         <v>42871</v>
       </c>
       <c r="B331" s="115" t="s">
+        <v>759</v>
+      </c>
+      <c r="C331" s="122" t="s">
         <v>760</v>
-      </c>
-      <c r="C331" s="122" t="s">
-        <v>761</v>
       </c>
       <c r="D331" s="122" t="s">
         <v>596</v>
       </c>
       <c r="E331" s="120" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="332" spans="1:5" ht="43.9" customHeight="1">
@@ -10959,13 +10964,13 @@
         <v>577</v>
       </c>
       <c r="C332" s="122" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D332" s="122" t="s">
         <v>596</v>
       </c>
       <c r="E332" s="120" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="333" spans="1:5" ht="43.9" customHeight="1">
@@ -10976,13 +10981,13 @@
         <v>577</v>
       </c>
       <c r="C333" s="122" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D333" s="122" t="s">
         <v>596</v>
       </c>
       <c r="E333" s="120" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="334" spans="1:5" ht="43.9" customHeight="1">
@@ -10993,13 +10998,13 @@
         <v>577</v>
       </c>
       <c r="C334" s="122" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D334" s="122" t="s">
         <v>596</v>
       </c>
       <c r="E334" s="120" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="335" spans="1:5" ht="43.9" customHeight="1">
@@ -11010,13 +11015,13 @@
         <v>577</v>
       </c>
       <c r="C335" s="122" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D335" s="122" t="s">
         <v>596</v>
       </c>
       <c r="E335" s="120" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="336" spans="1:5" ht="102.75" customHeight="1">
@@ -11027,13 +11032,13 @@
         <v>577</v>
       </c>
       <c r="C336" s="122" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D336" s="122" t="s">
         <v>596</v>
       </c>
       <c r="E336" s="120" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="337" spans="1:5" ht="43.9" customHeight="1">
@@ -11041,16 +11046,16 @@
         <v>42889</v>
       </c>
       <c r="B337" s="115" t="s">
+        <v>769</v>
+      </c>
+      <c r="C337" s="122" t="s">
         <v>770</v>
       </c>
-      <c r="C337" s="122" t="s">
-        <v>771</v>
-      </c>
       <c r="D337" s="122" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E337" s="1" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="338" spans="1:5" ht="43.9" customHeight="1">
@@ -11058,16 +11063,16 @@
         <v>42889</v>
       </c>
       <c r="B338" s="115" t="s">
+        <v>771</v>
+      </c>
+      <c r="C338" s="122" t="s">
         <v>772</v>
       </c>
-      <c r="C338" s="122" t="s">
+      <c r="D338" s="122" t="s">
         <v>773</v>
       </c>
-      <c r="D338" s="122" t="s">
-        <v>774</v>
-      </c>
       <c r="E338" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="339" spans="1:5" ht="43.9" customHeight="1">
@@ -11075,16 +11080,16 @@
         <v>42889</v>
       </c>
       <c r="B339" s="115" t="s">
+        <v>774</v>
+      </c>
+      <c r="C339" s="122" t="s">
         <v>775</v>
       </c>
-      <c r="C339" s="122" t="s">
-        <v>776</v>
-      </c>
       <c r="D339" s="122" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E339" s="1" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="340" spans="1:5" ht="43.9" customHeight="1">
@@ -11092,16 +11097,16 @@
         <v>42889</v>
       </c>
       <c r="B340" s="115" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C340" s="122" t="s">
+        <v>778</v>
+      </c>
+      <c r="D340" s="122" t="s">
+        <v>773</v>
+      </c>
+      <c r="E340" s="1" t="s">
         <v>779</v>
-      </c>
-      <c r="D340" s="122" t="s">
-        <v>774</v>
-      </c>
-      <c r="E340" s="1" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="341" spans="1:5" ht="43.9" customHeight="1">
@@ -11109,16 +11114,33 @@
         <v>42891</v>
       </c>
       <c r="B341" s="115" t="s">
+        <v>781</v>
+      </c>
+      <c r="C341" s="122" t="s">
         <v>782</v>
-      </c>
-      <c r="C341" s="122" t="s">
-        <v>783</v>
       </c>
       <c r="D341" s="122" t="s">
         <v>596</v>
       </c>
       <c r="E341" s="120" t="s">
-        <v>784</v>
+        <v>783</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5" ht="43.9" customHeight="1">
+      <c r="A342" s="98">
+        <v>42893</v>
+      </c>
+      <c r="B342" s="115" t="s">
+        <v>583</v>
+      </c>
+      <c r="C342" s="122" t="s">
+        <v>786</v>
+      </c>
+      <c r="D342" s="122" t="s">
+        <v>596</v>
+      </c>
+      <c r="E342" s="120" t="s">
+        <v>787</v>
       </c>
     </row>
   </sheetData>
@@ -11200,7 +11222,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="6" spans="1:2">

</xml_diff>

<commit_message>
Add index entry on Java message service/ RabbitMQ/ IBM MQ/ Kafka
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="792">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -4744,6 +4744,23 @@
   </si>
   <si>
     <t>Work as a Programmer for 1 and half year, I feel like the XP (extreme) programming concept is very relevant to my daily work. And when recently in Udacity AI course, teacher's motto saids, "Do the stupid way first, add intelligent only when necessary". And Martin Fowler also said, "Build MVP with least effort, refactor later"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are many Message Queue Product on market: RabbitMQ, Kafka, IBM MQ. In an article, message queue is discribe as the glue  between system components. Here is a vs table among these 3 products:
+https://techblog.xavient.com/messaging-what-to-choose-and-when/
+http://blog.itcentralstation.com/message-queue-reviews-face-off/ </t>
+  </si>
+  <si>
+    <t>Message Queue (1)</t>
+  </si>
+  <si>
+    <t>Message Queue (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Intro of concept
+The basic idea of mq is that a service (hardware/software) receive message from Sender/Publisher. The message then is stored in its queue. Later the service come back to delivery the queued message to its receiver/consumer
+# History
+First there is need for message service, then a industry specification comes in as MOM (Messgae Oriented Middleware). The JMS (Java Mesage Service) is the first wide known implementation of this specification. Then AMQP (Advanced Message Queuing Protocol) is published specification for async messaging. </t>
   </si>
 </sst>
 </file>
@@ -5945,10 +5962,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H342"/>
+  <dimension ref="A1:H344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E342" sqref="E342"/>
+    <sheetView tabSelected="1" topLeftCell="A342" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E345" sqref="E345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="43.9" customHeight="1"/>
@@ -11141,6 +11158,40 @@
       </c>
       <c r="E342" s="120" t="s">
         <v>787</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5" ht="43.9" customHeight="1">
+      <c r="A343" s="98">
+        <v>42907</v>
+      </c>
+      <c r="B343" s="115" t="s">
+        <v>587</v>
+      </c>
+      <c r="C343" s="122" t="s">
+        <v>789</v>
+      </c>
+      <c r="D343" s="122" t="s">
+        <v>596</v>
+      </c>
+      <c r="E343" s="120" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5" ht="43.9" customHeight="1">
+      <c r="A344" s="98">
+        <v>42907</v>
+      </c>
+      <c r="B344" s="115" t="s">
+        <v>587</v>
+      </c>
+      <c r="C344" s="122" t="s">
+        <v>790</v>
+      </c>
+      <c r="D344" s="122" t="s">
+        <v>596</v>
+      </c>
+      <c r="E344" s="120" t="s">
+        <v>791</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add index entry on TMUX usage
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="8145" windowHeight="9405"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="795">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -4761,6 +4761,23 @@
 The basic idea of mq is that a service (hardware/software) receive message from Sender/Publisher. The message then is stored in its queue. Later the service come back to delivery the queued message to its receiver/consumer
 # History
 First there is need for message service, then a industry specification comes in as MOM (Messgae Oriented Middleware). The JMS (Java Mesage Service) is the first wide known implementation of this specification. Then AMQP (Advanced Message Queuing Protocol) is published specification for async messaging. </t>
+  </si>
+  <si>
+    <t>tmux</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t># What is TMUX
+Tmux is a multi terminal. It can be install by apt-cyg.
+# Basic Usage
+* Launch tmux: tmux
+* Open new pane horizontally: Ctrl+B &gt; %
+* Open new pane vertically: Ctrl+B &gt; "
+* Iterate panes: Ctrl+B &gt; o
+* Next panes: Ctrl+B &gt; n
+* Previous panes: Ctrl+B &gt; p</t>
   </si>
 </sst>
 </file>
@@ -5962,7 +5979,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H344"/>
+  <dimension ref="A1:H345"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A342" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E345" sqref="E345"/>
@@ -11192,6 +11209,23 @@
       </c>
       <c r="E344" s="120" t="s">
         <v>791</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5" ht="43.9" customHeight="1">
+      <c r="A345" s="98">
+        <v>42985</v>
+      </c>
+      <c r="B345" s="115" t="s">
+        <v>792</v>
+      </c>
+      <c r="C345" s="122" t="s">
+        <v>793</v>
+      </c>
+      <c r="D345" s="122" t="s">
+        <v>596</v>
+      </c>
+      <c r="E345" s="120" t="s">
+        <v>794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add index entry on cygwin package procps-ng
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="797">
   <si>
     <t>General Induction of infrastructure</t>
   </si>
@@ -4778,6 +4778,12 @@
 * Iterate panes: Ctrl+B &gt; o
 * Next panes: Ctrl+B &gt; n
 * Previous panes: Ctrl+B &gt; p</t>
+  </si>
+  <si>
+    <t>pacakge procps-ng</t>
+  </si>
+  <si>
+    <t>On cygwin default util base, there is no command like "watch", "top", which are available in package "procps-ng". Simply install the package with `apt-cyg install procps-ng`.</t>
   </si>
 </sst>
 </file>
@@ -5979,10 +5985,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H345"/>
+  <dimension ref="A1:H346"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A342" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E345" sqref="E345"/>
+      <selection activeCell="B347" sqref="B347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="43.9" customHeight="1"/>
@@ -11226,6 +11232,23 @@
       </c>
       <c r="E345" s="120" t="s">
         <v>794</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5" ht="43.9" customHeight="1">
+      <c r="A346" s="98">
+        <v>42991</v>
+      </c>
+      <c r="B346" s="115" t="s">
+        <v>762</v>
+      </c>
+      <c r="C346" s="122" t="s">
+        <v>795</v>
+      </c>
+      <c r="D346" s="122" t="s">
+        <v>598</v>
+      </c>
+      <c r="E346" s="120" t="s">
+        <v>796</v>
       </c>
     </row>
   </sheetData>

</xml_diff>